<commit_message>
Automation - Projects and Products automation
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sueta\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA132DCE-325A-435A-804E-C51CCB01BB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DE393E-D6B4-46DB-A57A-52D632B394CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualContacts" sheetId="1" r:id="rId1"/>
     <sheet name="OrganizationContacts" sheetId="2" r:id="rId2"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="ProjectsProducts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="285">
   <si>
     <t>BillingAddressLine1</t>
   </si>
@@ -646,13 +648,262 @@
   </si>
   <si>
     <t>Surrey BC</t>
+  </si>
+  <si>
+    <t>Test Case description</t>
+  </si>
+  <si>
+    <t>MOTIRegion</t>
+  </si>
+  <si>
+    <t>CostEstimate</t>
+  </si>
+  <si>
+    <t>Objectives</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>ProductsCount</t>
+  </si>
+  <si>
+    <t>ProductsRowStart</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>UpdatedBy</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>Complete Project with 3 Products</t>
+  </si>
+  <si>
+    <t>Required only fields Project with no Products</t>
+  </si>
+  <si>
+    <t>Required only fields Project with 1 Product</t>
+  </si>
+  <si>
+    <t>Project with 10 Products</t>
+  </si>
+  <si>
+    <t>UpdateStatus</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>CodeName</t>
+  </si>
+  <si>
+    <t>UpdateName</t>
+  </si>
+  <si>
+    <t>UpdateNumber</t>
+  </si>
+  <si>
+    <t>UpdateCodeName</t>
+  </si>
+  <si>
+    <t>UpdateMOTIRegion</t>
+  </si>
+  <si>
+    <t>UpdateSummary</t>
+  </si>
+  <si>
+    <t>Automation Project 01</t>
+  </si>
+  <si>
+    <t>Automation Project 02</t>
+  </si>
+  <si>
+    <t>Automation Project 03</t>
+  </si>
+  <si>
+    <t>Automation Project 04</t>
+  </si>
+  <si>
+    <t>AU-0001</t>
+  </si>
+  <si>
+    <t>AU-0002</t>
+  </si>
+  <si>
+    <t>AU-0003</t>
+  </si>
+  <si>
+    <t>AU-0004</t>
+  </si>
+  <si>
+    <t>Active (AC)</t>
+  </si>
+  <si>
+    <t>Cancelled (CA)</t>
+  </si>
+  <si>
+    <t>Consolidated (CNCN)</t>
+  </si>
+  <si>
+    <t>Completed (CO)</t>
+  </si>
+  <si>
+    <t>South Coast Region</t>
+  </si>
+  <si>
+    <t>Southern Interior Region</t>
+  </si>
+  <si>
+    <t>Northern Region</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - 3 products associated</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - 1 products associated</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - no products associated</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - 10 products associated</t>
+  </si>
+  <si>
+    <t>TRANPSP1</t>
+  </si>
+  <si>
+    <t>Updated Automation Project 01</t>
+  </si>
+  <si>
+    <t>UPAU-0001</t>
+  </si>
+  <si>
+    <t>On Hold (HO)</t>
+  </si>
+  <si>
+    <t>Project updated by Automation Testing - 3 products associated</t>
+  </si>
+  <si>
+    <t>UpdateStartDate</t>
+  </si>
+  <si>
+    <t>UpdateCostEstimate</t>
+  </si>
+  <si>
+    <t>UpdateObjectives</t>
+  </si>
+  <si>
+    <t>UpdateScope</t>
+  </si>
+  <si>
+    <t>AU-0001-01</t>
+  </si>
+  <si>
+    <t>AU-0001-02</t>
+  </si>
+  <si>
+    <t>AU-0001-03</t>
+  </si>
+  <si>
+    <t>Automated Product 001</t>
+  </si>
+  <si>
+    <t>Automated Product 002</t>
+  </si>
+  <si>
+    <t>Automated Product 003</t>
+  </si>
+  <si>
+    <t>Regression Testing - create new products within a project</t>
+  </si>
+  <si>
+    <t>Most common cases of creating a product</t>
+  </si>
+  <si>
+    <t>UPAU-0001-01</t>
+  </si>
+  <si>
+    <t>UPAU-0001-02</t>
+  </si>
+  <si>
+    <t>UPAU-0001-03</t>
+  </si>
+  <si>
+    <t>Automated Product 001 - updated</t>
+  </si>
+  <si>
+    <t>Automated Product 002 - updated</t>
+  </si>
+  <si>
+    <t>Automated Product 003 -updated</t>
+  </si>
+  <si>
+    <t>Updated material product</t>
+  </si>
+  <si>
+    <t>AU-0001-01 Automated Product 001</t>
+  </si>
+  <si>
+    <t>AU-0001-02 Automated Product 002</t>
+  </si>
+  <si>
+    <t>AU-0001-03 Automated Product 003</t>
+  </si>
+  <si>
+    <t>UPAU-0001-01 Automated Product 001 - updated</t>
+  </si>
+  <si>
+    <t>UPAU-0001-02 Automated Product 002 - updated</t>
+  </si>
+  <si>
+    <t>UPAU-0001-03 Automated Product 003 -updated</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Updated new scope - Testing</t>
+  </si>
+  <si>
+    <t>ProductCodeName</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>UpdateProductCode</t>
+  </si>
+  <si>
+    <t>UpdateProductName</t>
+  </si>
+  <si>
+    <t>UpdateProductCodeName</t>
+  </si>
+  <si>
+    <t>EstimateDate</t>
+  </si>
+  <si>
+    <t>UpdateEstimateDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/dd/yy;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +923,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -698,13 +955,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -988,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -2099,4 +2359,476 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12A4D20-CBEC-42E3-9A24-C9C857FE01F3}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(C2," ",B2)</f>
+        <v>AU-0001 Automation Project 01</v>
+      </c>
+      <c r="E2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>247</v>
+      </c>
+      <c r="M2" t="s">
+        <v>248</v>
+      </c>
+      <c r="N2" t="str">
+        <f>CONCATENATE(M2," ",L2)</f>
+        <v>UPAU-0001 Updated Automation Project 01</v>
+      </c>
+      <c r="O2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D5" si="0">CONCATENATE(C3," ",B3)</f>
+        <v>AU-0002 Automation Project 02</v>
+      </c>
+      <c r="E3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I3" t="s">
+        <v>246</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>AU-0003 Automation Project 03</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I4" t="s">
+        <v>246</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>AU-0004 Automation Project 04</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5" t="s">
+        <v>246</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C337DBF-8E87-4911-96F1-55478D7291E8}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.77734375" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O1" t="s">
+        <v>253</v>
+      </c>
+      <c r="P1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44938</v>
+      </c>
+      <c r="E2" s="6">
+        <v>100</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44938</v>
+      </c>
+      <c r="G2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H2" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K2" t="s">
+        <v>273</v>
+      </c>
+      <c r="L2" s="4">
+        <v>44938</v>
+      </c>
+      <c r="M2" s="6">
+        <v>120</v>
+      </c>
+      <c r="N2" s="4">
+        <v>44969</v>
+      </c>
+      <c r="O2" t="s">
+        <v>269</v>
+      </c>
+      <c r="P2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44969</v>
+      </c>
+      <c r="E3" s="6">
+        <v>150.99</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44969</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" t="s">
+        <v>264</v>
+      </c>
+      <c r="J3" t="s">
+        <v>267</v>
+      </c>
+      <c r="K3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L3" s="4">
+        <v>44938</v>
+      </c>
+      <c r="M3" s="6">
+        <v>150.75</v>
+      </c>
+      <c r="N3" s="4">
+        <v>44969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44997</v>
+      </c>
+      <c r="E4" s="6">
+        <v>170.79</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44997</v>
+      </c>
+      <c r="G4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" t="s">
+        <v>265</v>
+      </c>
+      <c r="J4" t="s">
+        <v>268</v>
+      </c>
+      <c r="K4" t="s">
+        <v>275</v>
+      </c>
+      <c r="L4" s="4">
+        <v>44938</v>
+      </c>
+      <c r="M4" s="6">
+        <v>289</v>
+      </c>
+      <c r="N4" s="4">
+        <v>44969</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Automation - Projects and products (#3055)
* Automation Projects

* Automation - Projects and Products automation
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sueta\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA132DCE-325A-435A-804E-C51CCB01BB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DE393E-D6B4-46DB-A57A-52D632B394CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualContacts" sheetId="1" r:id="rId1"/>
     <sheet name="OrganizationContacts" sheetId="2" r:id="rId2"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="ProjectsProducts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="285">
   <si>
     <t>BillingAddressLine1</t>
   </si>
@@ -646,13 +648,262 @@
   </si>
   <si>
     <t>Surrey BC</t>
+  </si>
+  <si>
+    <t>Test Case description</t>
+  </si>
+  <si>
+    <t>MOTIRegion</t>
+  </si>
+  <si>
+    <t>CostEstimate</t>
+  </si>
+  <si>
+    <t>Objectives</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>ProductsCount</t>
+  </si>
+  <si>
+    <t>ProductsRowStart</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>UpdatedBy</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>Complete Project with 3 Products</t>
+  </si>
+  <si>
+    <t>Required only fields Project with no Products</t>
+  </si>
+  <si>
+    <t>Required only fields Project with 1 Product</t>
+  </si>
+  <si>
+    <t>Project with 10 Products</t>
+  </si>
+  <si>
+    <t>UpdateStatus</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>CodeName</t>
+  </si>
+  <si>
+    <t>UpdateName</t>
+  </si>
+  <si>
+    <t>UpdateNumber</t>
+  </si>
+  <si>
+    <t>UpdateCodeName</t>
+  </si>
+  <si>
+    <t>UpdateMOTIRegion</t>
+  </si>
+  <si>
+    <t>UpdateSummary</t>
+  </si>
+  <si>
+    <t>Automation Project 01</t>
+  </si>
+  <si>
+    <t>Automation Project 02</t>
+  </si>
+  <si>
+    <t>Automation Project 03</t>
+  </si>
+  <si>
+    <t>Automation Project 04</t>
+  </si>
+  <si>
+    <t>AU-0001</t>
+  </si>
+  <si>
+    <t>AU-0002</t>
+  </si>
+  <si>
+    <t>AU-0003</t>
+  </si>
+  <si>
+    <t>AU-0004</t>
+  </si>
+  <si>
+    <t>Active (AC)</t>
+  </si>
+  <si>
+    <t>Cancelled (CA)</t>
+  </si>
+  <si>
+    <t>Consolidated (CNCN)</t>
+  </si>
+  <si>
+    <t>Completed (CO)</t>
+  </si>
+  <si>
+    <t>South Coast Region</t>
+  </si>
+  <si>
+    <t>Southern Interior Region</t>
+  </si>
+  <si>
+    <t>Northern Region</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - 3 products associated</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - 1 products associated</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - no products associated</t>
+  </si>
+  <si>
+    <t>Project created by Automation Testing - 10 products associated</t>
+  </si>
+  <si>
+    <t>TRANPSP1</t>
+  </si>
+  <si>
+    <t>Updated Automation Project 01</t>
+  </si>
+  <si>
+    <t>UPAU-0001</t>
+  </si>
+  <si>
+    <t>On Hold (HO)</t>
+  </si>
+  <si>
+    <t>Project updated by Automation Testing - 3 products associated</t>
+  </si>
+  <si>
+    <t>UpdateStartDate</t>
+  </si>
+  <si>
+    <t>UpdateCostEstimate</t>
+  </si>
+  <si>
+    <t>UpdateObjectives</t>
+  </si>
+  <si>
+    <t>UpdateScope</t>
+  </si>
+  <si>
+    <t>AU-0001-01</t>
+  </si>
+  <si>
+    <t>AU-0001-02</t>
+  </si>
+  <si>
+    <t>AU-0001-03</t>
+  </si>
+  <si>
+    <t>Automated Product 001</t>
+  </si>
+  <si>
+    <t>Automated Product 002</t>
+  </si>
+  <si>
+    <t>Automated Product 003</t>
+  </si>
+  <si>
+    <t>Regression Testing - create new products within a project</t>
+  </si>
+  <si>
+    <t>Most common cases of creating a product</t>
+  </si>
+  <si>
+    <t>UPAU-0001-01</t>
+  </si>
+  <si>
+    <t>UPAU-0001-02</t>
+  </si>
+  <si>
+    <t>UPAU-0001-03</t>
+  </si>
+  <si>
+    <t>Automated Product 001 - updated</t>
+  </si>
+  <si>
+    <t>Automated Product 002 - updated</t>
+  </si>
+  <si>
+    <t>Automated Product 003 -updated</t>
+  </si>
+  <si>
+    <t>Updated material product</t>
+  </si>
+  <si>
+    <t>AU-0001-01 Automated Product 001</t>
+  </si>
+  <si>
+    <t>AU-0001-02 Automated Product 002</t>
+  </si>
+  <si>
+    <t>AU-0001-03 Automated Product 003</t>
+  </si>
+  <si>
+    <t>UPAU-0001-01 Automated Product 001 - updated</t>
+  </si>
+  <si>
+    <t>UPAU-0001-02 Automated Product 002 - updated</t>
+  </si>
+  <si>
+    <t>UPAU-0001-03 Automated Product 003 -updated</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Updated new scope - Testing</t>
+  </si>
+  <si>
+    <t>ProductCodeName</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>UpdateProductCode</t>
+  </si>
+  <si>
+    <t>UpdateProductName</t>
+  </si>
+  <si>
+    <t>UpdateProductCodeName</t>
+  </si>
+  <si>
+    <t>EstimateDate</t>
+  </si>
+  <si>
+    <t>UpdateEstimateDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/dd/yy;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +923,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -698,13 +955,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -988,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -2099,4 +2359,476 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12A4D20-CBEC-42E3-9A24-C9C857FE01F3}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(C2," ",B2)</f>
+        <v>AU-0001 Automation Project 01</v>
+      </c>
+      <c r="E2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>247</v>
+      </c>
+      <c r="M2" t="s">
+        <v>248</v>
+      </c>
+      <c r="N2" t="str">
+        <f>CONCATENATE(M2," ",L2)</f>
+        <v>UPAU-0001 Updated Automation Project 01</v>
+      </c>
+      <c r="O2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D5" si="0">CONCATENATE(C3," ",B3)</f>
+        <v>AU-0002 Automation Project 02</v>
+      </c>
+      <c r="E3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I3" t="s">
+        <v>246</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>AU-0003 Automation Project 03</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I4" t="s">
+        <v>246</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>AU-0004 Automation Project 04</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5" t="s">
+        <v>246</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C337DBF-8E87-4911-96F1-55478D7291E8}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.77734375" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O1" t="s">
+        <v>253</v>
+      </c>
+      <c r="P1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44938</v>
+      </c>
+      <c r="E2" s="6">
+        <v>100</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44938</v>
+      </c>
+      <c r="G2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H2" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K2" t="s">
+        <v>273</v>
+      </c>
+      <c r="L2" s="4">
+        <v>44938</v>
+      </c>
+      <c r="M2" s="6">
+        <v>120</v>
+      </c>
+      <c r="N2" s="4">
+        <v>44969</v>
+      </c>
+      <c r="O2" t="s">
+        <v>269</v>
+      </c>
+      <c r="P2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44969</v>
+      </c>
+      <c r="E3" s="6">
+        <v>150.99</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44969</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" t="s">
+        <v>264</v>
+      </c>
+      <c r="J3" t="s">
+        <v>267</v>
+      </c>
+      <c r="K3" t="s">
+        <v>274</v>
+      </c>
+      <c r="L3" s="4">
+        <v>44938</v>
+      </c>
+      <c r="M3" s="6">
+        <v>150.75</v>
+      </c>
+      <c r="N3" s="4">
+        <v>44969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44997</v>
+      </c>
+      <c r="E4" s="6">
+        <v>170.79</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44997</v>
+      </c>
+      <c r="G4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" t="s">
+        <v>265</v>
+      </c>
+      <c r="J4" t="s">
+        <v>268</v>
+      </c>
+      <c r="K4" t="s">
+        <v>275</v>
+      </c>
+      <c r="L4" s="4">
+        <v>44938</v>
+      </c>
+      <c r="M4" s="6">
+        <v>289</v>
+      </c>
+      <c r="N4" s="4">
+        <v>44969</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor on Research Files automation
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB33E2A-28E7-4344-B1DA-B1AAEEECCC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C06CC6-F4FE-40D2-83AD-202A49A1CB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" tabRatio="868" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualContacts" sheetId="1" r:id="rId1"/>
     <sheet name="OrganizationContacts" sheetId="2" r:id="rId2"/>
-    <sheet name="Projects" sheetId="3" r:id="rId3"/>
-    <sheet name="ProjectsProducts" sheetId="4" r:id="rId4"/>
-    <sheet name="ResearchFiles" sheetId="5" r:id="rId5"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId6"/>
-    <sheet name="PropertyResearch" sheetId="9" r:id="rId7"/>
-    <sheet name="Properties" sheetId="6" r:id="rId8"/>
+    <sheet name="FinancialCodes" sheetId="11" r:id="rId3"/>
+    <sheet name="Projects" sheetId="3" r:id="rId4"/>
+    <sheet name="ProjectsProducts" sheetId="4" r:id="rId5"/>
+    <sheet name="ResearchFiles" sheetId="5" r:id="rId6"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId7"/>
+    <sheet name="PropertyResearch" sheetId="9" r:id="rId8"/>
+    <sheet name="Properties" sheetId="6" r:id="rId9"/>
+    <sheet name="Notes" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="508">
   <si>
     <t>BillingAddressLine1</t>
   </si>
@@ -696,9 +698,6 @@
     <t>Project with 10 Products</t>
   </si>
   <si>
-    <t>UpdateStatus</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -708,21 +707,6 @@
     <t>CodeName</t>
   </si>
   <si>
-    <t>UpdateName</t>
-  </si>
-  <si>
-    <t>UpdateNumber</t>
-  </si>
-  <si>
-    <t>UpdateCodeName</t>
-  </si>
-  <si>
-    <t>UpdateMOTIRegion</t>
-  </si>
-  <si>
-    <t>UpdateSummary</t>
-  </si>
-  <si>
     <t>Automation Project 01</t>
   </si>
   <si>
@@ -783,9 +767,6 @@
     <t>TRANPSP1</t>
   </si>
   <si>
-    <t>Updated Automation Project 01</t>
-  </si>
-  <si>
     <t>UPAU-0001</t>
   </si>
   <si>
@@ -1101,18 +1082,12 @@
     <t>Automated updates on Property Information from Research File</t>
   </si>
   <si>
-    <t>Automated updates on Property Information from Research File - Changes added automatically</t>
-  </si>
-  <si>
     <t>AdjacentLandType</t>
   </si>
   <si>
     <t>Projects</t>
   </si>
   <si>
-    <t>NotesTab</t>
-  </si>
-  <si>
     <t>Automation Functional Testing - Note 1,Automation Functional Testing - Note 2,Automation Functional Testing - Note 3</t>
   </si>
   <si>
@@ -1257,9 +1232,6 @@
     <t>Automation Test - Editing Expropriation Notes</t>
   </si>
   <si>
-    <t>Automation Functional Testing - Note 1 edited to test notes edition is working successfully.</t>
-  </si>
-  <si>
     <t>Edit one Research Property</t>
   </si>
   <si>
@@ -1293,9 +1265,6 @@
     <t>Automation Test - Specific selected pin is not needed to acquire.</t>
   </si>
   <si>
-    <t>Automation Functional Testing - Research File created from a pin on a map</t>
-  </si>
-  <si>
     <t>Property Research from pin</t>
   </si>
   <si>
@@ -1362,9 +1331,6 @@
     <t>Cancel Changes</t>
   </si>
   <si>
-    <t>Automation Functional Testing - Update and cancel updates</t>
-  </si>
-  <si>
     <t>010-087-346</t>
   </si>
   <si>
@@ -1375,6 +1341,234 @@
   </si>
   <si>
     <t>Closed Road,Adjacent Land</t>
+  </si>
+  <si>
+    <t>Test case Description</t>
+  </si>
+  <si>
+    <t>Research File - Create new notes</t>
+  </si>
+  <si>
+    <t>Research File - Edit Note</t>
+  </si>
+  <si>
+    <t>Acquisition File - Create new notes</t>
+  </si>
+  <si>
+    <t>Acquisition File - Edit Notes</t>
+  </si>
+  <si>
+    <t>Automation Functional Testing - Note 1,Automation Functional Testing - Note 2,Automation Functional Testing - Note 3,Automation Functional Testing - Note 4,Automation Functional Testing - Note 5,Automation Functional Testing - Note 6,Automation Functional Testing - Note 7,Automation Functional Testing - Note 8,Automation Functional Testing - Note 9,Automation Functional Testing - Note 10,Automation Functional Testing - Note 11,Automation Functional Testing - Note 12</t>
+  </si>
+  <si>
+    <t>Automation Functional Testing - Note 1 edited to test notes from research file is working successfully.</t>
+  </si>
+  <si>
+    <t>Automation Functional Testing - Note edited to test notes from acquisition file is working successfully.</t>
+  </si>
+  <si>
+    <t>Update project</t>
+  </si>
+  <si>
+    <t>Unique Product for Project 1</t>
+  </si>
+  <si>
+    <t>Product 1 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 2 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 3 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 4 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 5 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 6 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 7 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 8 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 9 for Project 4</t>
+  </si>
+  <si>
+    <t>Product 10 for Project 4</t>
+  </si>
+  <si>
+    <t>UNIQUE-0001</t>
+  </si>
+  <si>
+    <t>Unique Product from Project 3</t>
+  </si>
+  <si>
+    <t>MULTI-0001</t>
+  </si>
+  <si>
+    <t>MULTI-0002</t>
+  </si>
+  <si>
+    <t>MULTI-0003</t>
+  </si>
+  <si>
+    <t>MULTI-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0005</t>
+  </si>
+  <si>
+    <t>MULTI-0006</t>
+  </si>
+  <si>
+    <t>MULTI-0007</t>
+  </si>
+  <si>
+    <t>MULTI-0008</t>
+  </si>
+  <si>
+    <t>MULTI-0009</t>
+  </si>
+  <si>
+    <t>MULTI-0010</t>
+  </si>
+  <si>
+    <t>Product 1 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 2 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 3 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 4 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 5 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 6 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 7 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 8 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 9 for AU-0004</t>
+  </si>
+  <si>
+    <t>Product 10 for AU-0004</t>
+  </si>
+  <si>
+    <t>UNIQUE-0001 Unique Product from Project 3</t>
+  </si>
+  <si>
+    <t>MULTI-0001 Product 1 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0002 Product 2 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0003 Product 3 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0004 Product 4 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0005 Product 5 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0006 Product 6 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0007 Product 7 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0008 Product 8 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0009 Product 9 for AU-0004</t>
+  </si>
+  <si>
+    <t>MULTI-0010 Product 10 for AU-0004</t>
+  </si>
+  <si>
+    <t>Testing of a project with 1 product</t>
+  </si>
+  <si>
+    <t>Testing a project with several products</t>
+  </si>
+  <si>
+    <t>Several products associated to 1 project</t>
+  </si>
+  <si>
+    <t>Main Search Properties</t>
+  </si>
+  <si>
+    <t>Edit Property from Map</t>
+  </si>
+  <si>
+    <t>123 Fake St.</t>
+  </si>
+  <si>
+    <t>Apt 305</t>
+  </si>
+  <si>
+    <t>V6Z 8H9</t>
+  </si>
+  <si>
+    <t>The Automated Zone from Properties Details</t>
+  </si>
+  <si>
+    <t>Main Search invalid PID</t>
+  </si>
+  <si>
+    <t>CodeType</t>
+  </si>
+  <si>
+    <t>CodeValue</t>
+  </si>
+  <si>
+    <t>CodeDescription</t>
+  </si>
+  <si>
+    <t>EffectiveDate</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>Create a new Financial Code</t>
+  </si>
+  <si>
+    <t>Edit Financial Code</t>
+  </si>
+  <si>
+    <t>Work activity</t>
+  </si>
+  <si>
+    <t>AUTO-TSTFINCODE</t>
+  </si>
+  <si>
+    <t>This is a Test Financial Code created by Automated programming</t>
+  </si>
+  <si>
+    <t>This is a Test Financial Code created by Automated programming - Edited automated form</t>
+  </si>
+  <si>
+    <t>Automated updates on Property Information from Property Information.</t>
   </si>
 </sst>
 </file>
@@ -1731,7 +1925,7 @@
   <dimension ref="A1:AW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1957,40 +2151,40 @@
         <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>108</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>130</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N2" t="s">
-        <v>131</v>
-      </c>
       <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>133</v>
+      </c>
+      <c r="R2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>112</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>132</v>
-      </c>
-      <c r="R2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" t="s">
-        <v>115</v>
-      </c>
-      <c r="T2" t="s">
-        <v>133</v>
       </c>
       <c r="U2" t="s">
         <v>31</v>
@@ -2094,7 +2288,7 @@
         <v>151</v>
       </c>
       <c r="H3" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>67</v>
@@ -2109,10 +2303,10 @@
         <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O3" t="s">
         <v>75</v>
@@ -2287,10 +2481,10 @@
         <v>183</v>
       </c>
       <c r="J5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>184</v>
@@ -2363,8 +2557,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{16C12AA1-ECCE-499E-9396-FFC7128B9E7E}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{3E5C643A-012D-4079-8C9C-CE03A2BB44C0}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{16C12AA1-ECCE-499E-9396-FFC7128B9E7E}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{3E5C643A-012D-4079-8C9C-CE03A2BB44C0}"/>
     <hyperlink ref="L3" r:id="rId3" xr:uid="{1CC1FCEE-4D1F-4BC0-B831-33526F37CA9E}"/>
     <hyperlink ref="I3" r:id="rId4" xr:uid="{749E9344-8D93-4BC6-9B68-CC2E0927EBF0}"/>
     <hyperlink ref="I5" r:id="rId5" xr:uid="{3BF8C400-BAC1-4978-8D41-326CBC17576E}"/>
@@ -2374,12 +2568,72 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC9B3A8-42C1-4A9C-B1C1-5E5E07CE0539}">
   <dimension ref="A1:AT5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2844,11 +3098,90 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C2" t="s">
+        <v>504</v>
+      </c>
+      <c r="D2" t="s">
+        <v>505</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45701</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C3" t="s">
+        <v>504</v>
+      </c>
+      <c r="D3" t="s">
+        <v>506</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12A4D20-CBEC-42E3-9A24-C9C857FE01F3}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2856,7 +3189,7 @@
     <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="55.1796875" bestFit="1" customWidth="1"/>
@@ -2864,26 +3197,20 @@
     <col min="9" max="9" width="11.54296875" customWidth="1"/>
     <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>202</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>118</v>
@@ -2906,53 +3233,35 @@
       <c r="K1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE(C2," ",B2)</f>
         <v>AU-0001 Automation Project 01</v>
       </c>
       <c r="E2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -2960,51 +3269,35 @@
       <c r="K2">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
-        <v>246</v>
-      </c>
-      <c r="M2" t="s">
-        <v>247</v>
-      </c>
-      <c r="N2" t="str">
-        <f>CONCATENATE(M2," ",L2)</f>
-        <v>UPAU-0001 Updated Automation Project 01</v>
-      </c>
-      <c r="O2" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D5" si="0">CONCATENATE(C3," ",B3)</f>
         <v>AU-0002 Automation Project 02</v>
       </c>
       <c r="E3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="G3" t="s">
-        <v>242</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>245</v>
-      </c>
       <c r="I3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J3">
         <v>4</v>
@@ -3013,34 +3306,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>AU-0003 Automation Project 03</v>
       </c>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -3049,40 +3342,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>AU-0004 Automation Project 04</v>
       </c>
       <c r="E5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J5">
         <v>5</v>
       </c>
       <c r="K5">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="str">
+        <f>CONCATENATE(C6," ",B6)</f>
+        <v>UPAU-0001 Automation Project 01</v>
+      </c>
+      <c r="E6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" t="s">
+        <v>242</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3092,12 +3421,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C337DBF-8E87-4911-96F1-55478D7291E8}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3118,13 +3447,13 @@
         <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>212</v>
@@ -3133,7 +3462,7 @@
         <v>204</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>205</v>
@@ -3144,16 +3473,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E2" s="4">
         <v>44938</v>
@@ -3165,24 +3494,24 @@
         <v>44938</v>
       </c>
       <c r="H2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="I2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E3" s="4">
         <v>44969</v>
@@ -3194,24 +3523,24 @@
         <v>44969</v>
       </c>
       <c r="H3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="I3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D4" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E4" s="4">
         <v>44997</v>
@@ -3223,84 +3552,367 @@
         <v>44997</v>
       </c>
       <c r="H4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="I4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>452</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>453</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>474</v>
       </c>
       <c r="E5" s="4">
-        <v>44938</v>
+        <v>45075</v>
       </c>
       <c r="F5" s="6">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="G5" s="4">
-        <v>44969</v>
+        <v>45076</v>
       </c>
       <c r="H5" t="s">
-        <v>264</v>
-      </c>
-      <c r="I5" t="s">
-        <v>272</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="B6" t="s">
-        <v>259</v>
+        <v>454</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>464</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>475</v>
       </c>
       <c r="E6" s="4">
-        <v>44938</v>
+        <v>43831</v>
       </c>
       <c r="F6" s="6">
-        <v>150.75</v>
+        <v>89.95</v>
       </c>
       <c r="G6" s="4">
-        <v>44969</v>
+        <v>43832</v>
+      </c>
+      <c r="H6" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="B7" t="s">
-        <v>260</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
+        <v>465</v>
+      </c>
+      <c r="D7" t="s">
+        <v>476</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43862</v>
+      </c>
+      <c r="F7" s="6">
+        <v>77.89</v>
+      </c>
+      <c r="G7" s="4">
+        <v>43863</v>
+      </c>
+      <c r="I7" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>444</v>
+      </c>
+      <c r="B8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C8" t="s">
+        <v>466</v>
+      </c>
+      <c r="D8" t="s">
+        <v>477</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43891</v>
+      </c>
+      <c r="F8" s="6">
+        <v>123.44</v>
+      </c>
+      <c r="G8" s="4">
+        <v>43892</v>
+      </c>
+      <c r="H8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>445</v>
+      </c>
+      <c r="B9" t="s">
+        <v>457</v>
+      </c>
+      <c r="C9" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" t="s">
+        <v>478</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43922</v>
+      </c>
+      <c r="F9" s="6">
+        <v>320.12</v>
+      </c>
+      <c r="G9" s="4">
+        <v>43923</v>
+      </c>
+      <c r="H9" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>446</v>
+      </c>
+      <c r="B10" t="s">
+        <v>458</v>
+      </c>
+      <c r="C10" t="s">
+        <v>468</v>
+      </c>
+      <c r="D10" t="s">
+        <v>479</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43952</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1500</v>
+      </c>
+      <c r="G10" s="4">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>447</v>
+      </c>
+      <c r="B11" t="s">
+        <v>459</v>
+      </c>
+      <c r="C11" t="s">
+        <v>469</v>
+      </c>
+      <c r="D11" t="s">
+        <v>480</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43983</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2.89</v>
+      </c>
+      <c r="G11" s="4">
+        <v>43984</v>
+      </c>
+      <c r="H11" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>448</v>
+      </c>
+      <c r="B12" t="s">
+        <v>460</v>
+      </c>
+      <c r="C12" t="s">
+        <v>470</v>
+      </c>
+      <c r="D12" t="s">
+        <v>481</v>
+      </c>
+      <c r="E12" s="4">
+        <v>44013</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5.9</v>
+      </c>
+      <c r="G12" s="4">
+        <v>44014</v>
+      </c>
+      <c r="H12" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>449</v>
+      </c>
+      <c r="B13" t="s">
+        <v>461</v>
+      </c>
+      <c r="C13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D13" t="s">
+        <v>482</v>
+      </c>
+      <c r="E13" s="4">
+        <v>44044</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6</v>
+      </c>
+      <c r="G13" s="4">
+        <v>44045</v>
+      </c>
+      <c r="I13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B14" t="s">
+        <v>462</v>
+      </c>
+      <c r="C14" t="s">
+        <v>472</v>
+      </c>
+      <c r="D14" t="s">
+        <v>483</v>
+      </c>
+      <c r="E14" s="4">
+        <v>44075</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="G14" s="4">
+        <v>44076</v>
+      </c>
+      <c r="H14" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>451</v>
+      </c>
+      <c r="B15" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" t="s">
+        <v>473</v>
+      </c>
+      <c r="D15" t="s">
+        <v>484</v>
+      </c>
+      <c r="E15" s="4">
+        <v>44105</v>
+      </c>
+      <c r="F15" s="6">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4">
+        <v>44106</v>
+      </c>
+      <c r="H15" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>421</v>
+      </c>
+      <c r="B16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" t="s">
+        <v>261</v>
+      </c>
+      <c r="E16" s="4">
+        <v>44938</v>
+      </c>
+      <c r="F16" s="6">
+        <v>120</v>
+      </c>
+      <c r="G16" s="4">
+        <v>44969</v>
+      </c>
+      <c r="H16" t="s">
+        <v>257</v>
+      </c>
+      <c r="I16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>422</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" s="4">
+        <v>44938</v>
+      </c>
+      <c r="F17" s="6">
+        <v>150.75</v>
+      </c>
+      <c r="G17" s="4">
+        <v>44969</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>423</v>
+      </c>
+      <c r="B18" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" t="s">
         <v>263</v>
       </c>
-      <c r="D7" t="s">
-        <v>270</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="E18" s="4">
         <v>44938</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F18" s="6">
         <v>289</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G18" s="4">
         <v>44969</v>
       </c>
     </row>
@@ -3311,12 +3923,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3C62D2-095D-41C7-8E12-52D5164F6230}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3330,159 +3942,152 @@
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="63.90625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="100.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>118</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>363</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" t="s">
         <v>313</v>
       </c>
-      <c r="C2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D2" t="s">
-        <v>441</v>
-      </c>
-      <c r="E2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F2" t="s">
-        <v>320</v>
-      </c>
       <c r="G2" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="H2" s="4">
         <v>44625</v>
       </c>
       <c r="I2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="J2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="K2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="L2" s="4">
         <v>44631</v>
       </c>
       <c r="M2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>325</v>
-      </c>
-      <c r="P2" t="s">
-        <v>356</v>
+        <v>318</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
       <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D3" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="F3" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="G3" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="J3" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K3" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="L3" s="4">
         <v>44651</v>
@@ -3491,126 +4096,117 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>403</v>
-      </c>
-      <c r="P3" t="s">
-        <v>404</v>
+        <v>394</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R3">
         <v>6</v>
       </c>
-      <c r="S3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C4" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="F4" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="G4" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="H4" s="4">
         <v>44254</v>
       </c>
       <c r="I4" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="J4" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="K4" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="L4" s="4">
         <v>44703</v>
       </c>
       <c r="M4" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="N4" t="b">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>416</v>
+      <c r="P4">
+        <v>4</v>
       </c>
       <c r="Q4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R4">
         <v>7</v>
       </c>
-      <c r="S4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C5" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="N5" t="b">
         <v>0</v>
       </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
       <c r="Q5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="B6" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="C6" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E6" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="N6" t="b">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
-        <v>439</v>
+      <c r="P6">
+        <v>5</v>
       </c>
       <c r="Q6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R6">
-        <v>6</v>
-      </c>
-      <c r="S6">
         <v>6</v>
       </c>
     </row>
@@ -3621,20 +4217,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
@@ -3660,98 +4256,120 @@
         <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C2">
         <v>8157500</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F2" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="B3" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B5" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="F6" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B9" t="s">
-        <v>328</v>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>488</v>
+      </c>
+      <c r="B10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10">
+        <v>90054791</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>494</v>
+      </c>
+      <c r="B11" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3759,12 +4377,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56704E8-1DAE-4D99-86A6-0D11D370D1F9}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3783,183 +4401,183 @@
         <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="F2" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="G2" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B3" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="C3" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="D3" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E3" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F3" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="G3" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C4" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="D4" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E4" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F4" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="G4" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" t="s">
         <v>378</v>
       </c>
-      <c r="B5" t="s">
-        <v>382</v>
-      </c>
-      <c r="C5" t="s">
-        <v>387</v>
-      </c>
       <c r="D5" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E5" t="s">
+        <v>380</v>
+      </c>
+      <c r="F5" t="s">
         <v>389</v>
       </c>
-      <c r="F5" t="s">
-        <v>398</v>
-      </c>
       <c r="G5" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C6" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E6" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F6" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="G6" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="B7" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="C7" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="D7" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E7" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F7" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G7" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="B8" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="C8" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="D8" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E8" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F8" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="G8" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -3968,12 +4586,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3991,7 +4609,7 @@
     <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.54296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="60" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.36328125" bestFit="1" customWidth="1"/>
@@ -4023,131 +4641,131 @@
         <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="B2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3" t="s">
+        <v>334</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" t="s">
+        <v>336</v>
+      </c>
+      <c r="J3" t="s">
+        <v>338</v>
+      </c>
+      <c r="K3" t="s">
+        <v>339</v>
+      </c>
+      <c r="L3" t="s">
+        <v>337</v>
+      </c>
+      <c r="M3" t="s">
+        <v>416</v>
+      </c>
+      <c r="N3" t="s">
+        <v>340</v>
+      </c>
+      <c r="O3" t="s">
+        <v>430</v>
+      </c>
+      <c r="P3" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>341</v>
+      </c>
+      <c r="S3" t="s">
         <v>342</v>
-      </c>
-      <c r="C3" t="s">
-        <v>338</v>
-      </c>
-      <c r="D3" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" t="s">
-        <v>340</v>
-      </c>
-      <c r="G3" t="s">
-        <v>341</v>
-      </c>
-      <c r="H3" t="s">
-        <v>238</v>
-      </c>
-      <c r="I3" t="s">
-        <v>343</v>
-      </c>
-      <c r="J3" t="s">
-        <v>345</v>
-      </c>
-      <c r="K3" t="s">
-        <v>346</v>
-      </c>
-      <c r="L3" t="s">
-        <v>344</v>
-      </c>
-      <c r="M3" t="s">
-        <v>427</v>
-      </c>
-      <c r="N3" t="s">
-        <v>347</v>
-      </c>
-      <c r="O3" t="s">
-        <v>442</v>
-      </c>
-      <c r="P3" t="s">
-        <v>443</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>348</v>
-      </c>
-      <c r="S3" t="s">
-        <v>349</v>
       </c>
       <c r="T3">
         <v>100</v>
@@ -4159,15 +4777,45 @@
         <v>50</v>
       </c>
       <c r="W3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="X3" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" t="s">
+        <v>490</v>
+      </c>
+      <c r="D4" t="s">
+        <v>491</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>492</v>
+      </c>
+      <c r="N4" t="s">
+        <v>493</v>
+      </c>
+      <c r="T4">
+        <v>65</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>103.59</v>
+      </c>
+      <c r="W4" t="s">
+        <v>343</v>
+      </c>
       <c r="X4" t="s">
-        <v>352</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automation - Digital Documents refactoring (#3147)
* Digital Documents refactoring

* Research File uncomment steps
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C06CC6-F4FE-40D2-83AD-202A49A1CB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4814C91-07EE-4F73-A421-EF825998BBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" tabRatio="868" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="868" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualContacts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="SearchProperties" sheetId="8" r:id="rId7"/>
     <sheet name="PropertyResearch" sheetId="9" r:id="rId8"/>
     <sheet name="Properties" sheetId="6" r:id="rId9"/>
-    <sheet name="Notes" sheetId="10" r:id="rId10"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId10"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId11"/>
+    <sheet name="Notes" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="754">
   <si>
     <t>BillingAddressLine1</t>
   </si>
@@ -1569,6 +1571,744 @@
   </si>
   <si>
     <t>Automated updates on Property Information from Property Information.</t>
+  </si>
+  <si>
+    <t>ShortDescriptor</t>
+  </si>
+  <si>
+    <t>CivicAddress</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>IndianReserveOrNationalPark</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>PropertyIdentifier</t>
+  </si>
+  <si>
+    <t>CrownGrant</t>
+  </si>
+  <si>
+    <t>HighwayDistrict</t>
+  </si>
+  <si>
+    <t>DistrictLot</t>
+  </si>
+  <si>
+    <t>FieldBook</t>
+  </si>
+  <si>
+    <t>LandDistrict</t>
+  </si>
+  <si>
+    <t>GazetteDate</t>
+  </si>
+  <si>
+    <t>GazettePage</t>
+  </si>
+  <si>
+    <t>GazettePublishedDate</t>
+  </si>
+  <si>
+    <t>GazetteType</t>
+  </si>
+  <si>
+    <t>LegalSurveyPlan</t>
+  </si>
+  <si>
+    <t>LTSAScheduleFiling</t>
+  </si>
+  <si>
+    <t>MoTIPlan</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>PhysicalLocation</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>PlanType</t>
+  </si>
+  <si>
+    <t>DateSigned</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MoTIFile</t>
+  </si>
+  <si>
+    <t>PublishedDate</t>
+  </si>
+  <si>
+    <t>RelatedGazette</t>
+  </si>
+  <si>
+    <t>OIC</t>
+  </si>
+  <si>
+    <t>OICRoute</t>
+  </si>
+  <si>
+    <t>OICType</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>PlanRevision</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>ProjectName</t>
+  </si>
+  <si>
+    <t>YearPrivyCouncil</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>CanadaLandSurvey</t>
+  </si>
+  <si>
+    <t>DigitalDocumentDetailsRowStart</t>
+  </si>
+  <si>
+    <t>DigitalDocumentsRowEnd</t>
+  </si>
+  <si>
+    <t>Insert Digital Documents into a Research File</t>
+  </si>
+  <si>
+    <t>Update Digital Documents in a Research File</t>
+  </si>
+  <si>
+    <t>Insert Digital Documents into a Lease/License</t>
+  </si>
+  <si>
+    <t>Update Digital Documents into a Lease/License</t>
+  </si>
+  <si>
+    <t>Insert Digital Documents into an Acquisition File</t>
+  </si>
+  <si>
+    <t>Update Digital Documents in an Acquisition File</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>Affidavit of service</t>
+  </si>
+  <si>
+    <t>Appraisal/Review</t>
+  </si>
+  <si>
+    <t>Approval of expropriation (From 5)</t>
+  </si>
+  <si>
+    <t>BC assessment search</t>
+  </si>
+  <si>
+    <t>Briefing notes</t>
+  </si>
+  <si>
+    <t>Canada lands survey</t>
+  </si>
+  <si>
+    <t>Certificate of Insurance (H0111)</t>
+  </si>
+  <si>
+    <t>Company search</t>
+  </si>
+  <si>
+    <t>Correspondence</t>
+  </si>
+  <si>
+    <t>Compensation cheque</t>
+  </si>
+  <si>
+    <t>Compensation requisition (H0120)</t>
+  </si>
+  <si>
+    <t>Condition of entry (H0443)</t>
+  </si>
+  <si>
+    <t>Conveyance closing documents (ex: PTT forms, Form A etc.)</t>
+  </si>
+  <si>
+    <t>Crown grant</t>
+  </si>
+  <si>
+    <t>District road register</t>
+  </si>
+  <si>
+    <t>Field notes</t>
+  </si>
+  <si>
+    <t>First nations consultation</t>
+  </si>
+  <si>
+    <t>Gazette</t>
+  </si>
+  <si>
+    <t>Historical file</t>
+  </si>
+  <si>
+    <t>Lease / License (H1005/H1005A)</t>
+  </si>
+  <si>
+    <t>Legal correspondence (ex: to AG/external lawyers)</t>
+  </si>
+  <si>
+    <t>Legal survey plan</t>
+  </si>
+  <si>
+    <t>Licensing approval/sign-off</t>
+  </si>
+  <si>
+    <t>LTSA documents and plans (except title search)</t>
+  </si>
+  <si>
+    <t>Ministerial order</t>
+  </si>
+  <si>
+    <t>Miscellaneous notes (LTSA)</t>
+  </si>
+  <si>
+    <t>MoTI plan</t>
+  </si>
+  <si>
+    <t>Notice of advanced payment (Form 8)</t>
+  </si>
+  <si>
+    <t>Notice of claims/Litigation documents</t>
+  </si>
+  <si>
+    <t>Notice of expropriation (Form 1)</t>
+  </si>
+  <si>
+    <t>Notice of possible entry (H0224)</t>
+  </si>
+  <si>
+    <t>Owner agreement/offer</t>
+  </si>
+  <si>
+    <t>PA plans / Design drawings</t>
+  </si>
+  <si>
+    <t>Photos / Images / Video</t>
+  </si>
+  <si>
+    <t>Privy council</t>
+  </si>
+  <si>
+    <t>Professional reports (ex: engineering, environmental etc.)</t>
+  </si>
+  <si>
+    <t>Record of negotiation</t>
+  </si>
+  <si>
+    <t>Release of claims</t>
+  </si>
+  <si>
+    <t>Spending authority approval (SAA)</t>
+  </si>
+  <si>
+    <t>Surplus property declaration</t>
+  </si>
+  <si>
+    <t>Tax notices and assessments</t>
+  </si>
+  <si>
+    <t>Temporary license for construction access (H0074)</t>
+  </si>
+  <si>
+    <t>Title search / Historical title</t>
+  </si>
+  <si>
+    <t>Transfer of administration</t>
+  </si>
+  <si>
+    <t>Vesting notice (Form 9)</t>
+  </si>
+  <si>
+    <t>Creating a Affidavit of service document type</t>
+  </si>
+  <si>
+    <t>Creating a Appraisal/Review document type</t>
+  </si>
+  <si>
+    <t>Creating a Approval of expropriation (From 5) document type</t>
+  </si>
+  <si>
+    <t>Creating a BC assessment search document type</t>
+  </si>
+  <si>
+    <t>Creating a Briefing notes document type</t>
+  </si>
+  <si>
+    <t>Creating a Canada lands survey document type</t>
+  </si>
+  <si>
+    <t>Creating a Certificate of Insurance (H0111) document type</t>
+  </si>
+  <si>
+    <t>Creating a Company search document type</t>
+  </si>
+  <si>
+    <t>Creating a Correspondence document type</t>
+  </si>
+  <si>
+    <t>Creating a Compensation cheque document type</t>
+  </si>
+  <si>
+    <t>Creating a Compensation requisition (H0120) document type</t>
+  </si>
+  <si>
+    <t>Creating a Condition of entry (H0443) document type</t>
+  </si>
+  <si>
+    <t>Creating a Conveyance closing documents (ex: PTT forms, Form A etc.) document type</t>
+  </si>
+  <si>
+    <t>Creating a Crown grant document type</t>
+  </si>
+  <si>
+    <t>Creating a District road register document type</t>
+  </si>
+  <si>
+    <t>Creating a Field notes document type</t>
+  </si>
+  <si>
+    <t>Creating a First nations consultation document type</t>
+  </si>
+  <si>
+    <t>Creating a Gazette document type</t>
+  </si>
+  <si>
+    <t>Creating a Historical file document type</t>
+  </si>
+  <si>
+    <t>Creating a Lease / License (H1005/H1005A) document type</t>
+  </si>
+  <si>
+    <t>Creating a Legal correspondence (ex: to AG/external lawyers) document type</t>
+  </si>
+  <si>
+    <t>Creating a Legal survey plan document type</t>
+  </si>
+  <si>
+    <t>Creating a Licensing approval/sign-off document type</t>
+  </si>
+  <si>
+    <t>Creating a LTSA documents and plans (except title search) document type</t>
+  </si>
+  <si>
+    <t>Creating a Ministerial order document type</t>
+  </si>
+  <si>
+    <t>Creating a Miscellaneous notes (LTSA) document type</t>
+  </si>
+  <si>
+    <t>Creating a MoTI plan document type</t>
+  </si>
+  <si>
+    <t>Creating a Notice of advanced payment (Form 8) document type</t>
+  </si>
+  <si>
+    <t>Creating a Notice of claims/Litigation documents document type</t>
+  </si>
+  <si>
+    <t>Creating a Notice of expropriation (Form 1) document type</t>
+  </si>
+  <si>
+    <t>Creating a Notice of possible entry (H0224) document type</t>
+  </si>
+  <si>
+    <t>Creating a OIC document type</t>
+  </si>
+  <si>
+    <t>Creating a Other document type</t>
+  </si>
+  <si>
+    <t>Creating a Owner agreement/offer document type</t>
+  </si>
+  <si>
+    <t>Creating a PA plans / Design drawings document type</t>
+  </si>
+  <si>
+    <t>Creating a Photos / Images / Video document type</t>
+  </si>
+  <si>
+    <t>Creating a Privy council document type</t>
+  </si>
+  <si>
+    <t>Creating a Professional reports (ex: engineering, environmental etc.) document type</t>
+  </si>
+  <si>
+    <t>Creating a Record of negotiation document type</t>
+  </si>
+  <si>
+    <t>Creating a Release of claims document type</t>
+  </si>
+  <si>
+    <t>Creating a Spending authority approval (SAA) document type</t>
+  </si>
+  <si>
+    <t>Creating a Surplus property declaration document type</t>
+  </si>
+  <si>
+    <t>Creating a Tax notices and assessments document type</t>
+  </si>
+  <si>
+    <t>Creating a Temporary license for construction access (H0074) document type</t>
+  </si>
+  <si>
+    <t>Creating a Title search / Historical title document type</t>
+  </si>
+  <si>
+    <t>Creating a Transfer of administration document type</t>
+  </si>
+  <si>
+    <t>Creating a Vesting notice (Form 9) document type</t>
+  </si>
+  <si>
+    <t>Create automatic Affidavit of service document</t>
+  </si>
+  <si>
+    <t>Create automatic Appraisal/Review document</t>
+  </si>
+  <si>
+    <t>Create automatic Approval of expropriation (From 5) document</t>
+  </si>
+  <si>
+    <t>Create automatic Briefing notes document</t>
+  </si>
+  <si>
+    <t>Create automatic Canada lands survey document</t>
+  </si>
+  <si>
+    <t>Create automatic Certificate of Insurance (H0111) document</t>
+  </si>
+  <si>
+    <t>Create automatic Company search document</t>
+  </si>
+  <si>
+    <t>Create automatic Correspondence document</t>
+  </si>
+  <si>
+    <t>Create automatic Compensation cheque document</t>
+  </si>
+  <si>
+    <t>Create automatic Compensation requisition (H0120) document</t>
+  </si>
+  <si>
+    <t>Create automatic Condition of entry (H0443) document</t>
+  </si>
+  <si>
+    <t>Create automatic Conveyance closing documents (ex: PTT forms, Form A etc.) document</t>
+  </si>
+  <si>
+    <t>Create automatic District road register document</t>
+  </si>
+  <si>
+    <t>Create automatic Field notes document</t>
+  </si>
+  <si>
+    <t>Create automatic First nations consultation document</t>
+  </si>
+  <si>
+    <t>Create automatic Lease / License (H1005/H1005A) document</t>
+  </si>
+  <si>
+    <t>Create automatic Legal correspondence (ex: to AG/external lawyers) document</t>
+  </si>
+  <si>
+    <t>Create automatic Licensing approval/sign-off document</t>
+  </si>
+  <si>
+    <t>Create automatic LTSA documents and plans (except title search) document</t>
+  </si>
+  <si>
+    <t>Create automatic MoTI plan document</t>
+  </si>
+  <si>
+    <t>Create automatic Notice of advanced payment (Form 8) document</t>
+  </si>
+  <si>
+    <t>Create automatic Notice of claims/Litigation documents document</t>
+  </si>
+  <si>
+    <t>Create automatic Notice of expropriation (Form 1) document</t>
+  </si>
+  <si>
+    <t>Create automatic Notice of possible entry (H0224) document</t>
+  </si>
+  <si>
+    <t>Create automatic Other document</t>
+  </si>
+  <si>
+    <t>Create automatic Owner agreement/offer document</t>
+  </si>
+  <si>
+    <t>Create automatic Photos / Images / Video document</t>
+  </si>
+  <si>
+    <t>Create automatic Professional reports (ex: engineering, environmental etc.) document</t>
+  </si>
+  <si>
+    <t>Create automatic Record of negotiation document</t>
+  </si>
+  <si>
+    <t>Create automatic Release of claims document</t>
+  </si>
+  <si>
+    <t>Create automatic Spending authority approval (SAA) document</t>
+  </si>
+  <si>
+    <t>Create automatic Surplus property declaration document</t>
+  </si>
+  <si>
+    <t>Create automatic Tax notices and assessments document</t>
+  </si>
+  <si>
+    <t>Create automatic Temporary license for construction access (H0074) document</t>
+  </si>
+  <si>
+    <t>Create automatic Vesting notice (Form 9) document</t>
+  </si>
+  <si>
+    <t>890 Main St.</t>
+  </si>
+  <si>
+    <t>123-456</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Amended</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>123-9090</t>
+  </si>
+  <si>
+    <t>Stanley Park</t>
+  </si>
+  <si>
+    <t>1233-1700 Fox St.</t>
+  </si>
+  <si>
+    <t>Allan Cooke</t>
+  </si>
+  <si>
+    <t>789-098-000</t>
+  </si>
+  <si>
+    <t>CR-000988-890</t>
+  </si>
+  <si>
+    <t>100 House Test</t>
+  </si>
+  <si>
+    <t>The Automation Road</t>
+  </si>
+  <si>
+    <t>2002-03</t>
+  </si>
+  <si>
+    <t>Nanaimo</t>
+  </si>
+  <si>
+    <t>Test Gazette</t>
+  </si>
+  <si>
+    <t>7889-000</t>
+  </si>
+  <si>
+    <t>LTSA 001-233</t>
+  </si>
+  <si>
+    <t>The Happy Automation Road</t>
+  </si>
+  <si>
+    <t>FL-12345678</t>
+  </si>
+  <si>
+    <t>At the Nartional Big Library</t>
+  </si>
+  <si>
+    <t>Sec 009-99345</t>
+  </si>
+  <si>
+    <t>7898887-099</t>
+  </si>
+  <si>
+    <t>Testing Plan</t>
+  </si>
+  <si>
+    <t>MF 90878-893466329</t>
+  </si>
+  <si>
+    <t>The Bernie Main Bridge</t>
+  </si>
+  <si>
+    <t>789-567-122</t>
+  </si>
+  <si>
+    <t>367273-000</t>
+  </si>
+  <si>
+    <t>8966554-98898</t>
+  </si>
+  <si>
+    <t>12334-7668</t>
+  </si>
+  <si>
+    <t>The main Gazette</t>
+  </si>
+  <si>
+    <t>4545-8437743</t>
+  </si>
+  <si>
+    <t>345-097436</t>
+  </si>
+  <si>
+    <t>Testing OIC</t>
+  </si>
+  <si>
+    <t>Burrard Bridge</t>
+  </si>
+  <si>
+    <t>345-097-000</t>
+  </si>
+  <si>
+    <t>The Main Canada Highway</t>
+  </si>
+  <si>
+    <t>2344-PA-8999</t>
+  </si>
+  <si>
+    <t>The plan was revisioned on May 2022</t>
+  </si>
+  <si>
+    <t>Automation Project</t>
+  </si>
+  <si>
+    <t>767 Main Beach Ave.</t>
+  </si>
+  <si>
+    <t>Joe Doe</t>
+  </si>
+  <si>
+    <t>456-090-900</t>
+  </si>
+  <si>
+    <t>Betty White</t>
+  </si>
+  <si>
+    <t>678-000-989</t>
+  </si>
+  <si>
+    <t>The automation creation of a Title search</t>
+  </si>
+  <si>
+    <t>123-909000</t>
+  </si>
+  <si>
+    <t>789-789-789</t>
+  </si>
+  <si>
+    <t>Yew St. New upcoming road</t>
+  </si>
+  <si>
+    <t>191-094-876363736-0-78</t>
+  </si>
+  <si>
+    <t>003-799-565</t>
+  </si>
+  <si>
+    <t>DocumentStatus</t>
+  </si>
+  <si>
+    <t>ContactStatus</t>
+  </si>
+  <si>
+    <t>ProjectStatus</t>
+  </si>
+  <si>
+    <t>PIDNumber</t>
+  </si>
+  <si>
+    <t>PINNumber</t>
+  </si>
+  <si>
+    <t>Updating a Affidavit of service document type</t>
+  </si>
+  <si>
+    <t>Update automatic Affidavit of service document - edited</t>
+  </si>
+  <si>
+    <t>Updating a Field notes document type</t>
+  </si>
+  <si>
+    <t>2002-11</t>
+  </si>
+  <si>
+    <t>Nanaimo Station</t>
+  </si>
+  <si>
+    <t>Updating automatic Field notes document</t>
+  </si>
+  <si>
+    <t>Updating a Notice of possible entry (H0224) document type</t>
+  </si>
+  <si>
+    <t>Updating automatic Notice of possible entry (H0224) document - edited</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +2370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1641,6 +2381,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1925,7 +2667,7 @@
   <dimension ref="A1:AW6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1936,7 +2678,7 @@
     <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="16.6328125" customWidth="1"/>
@@ -1996,7 +2738,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>118</v>
+        <v>742</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>15</v>
@@ -2569,6 +3311,1172 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>555</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B6">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>557</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
+  <dimension ref="A1:AX51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="75.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="19.1796875" customWidth="1"/>
+    <col min="16" max="16" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="19.1796875" customWidth="1"/>
+    <col min="19" max="19" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="30" width="19.1796875" customWidth="1"/>
+    <col min="31" max="31" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="19.1796875" customWidth="1"/>
+    <col min="35" max="35" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="41" width="19.1796875" customWidth="1"/>
+    <col min="42" max="42" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="19.1796875" customWidth="1"/>
+    <col min="45" max="45" width="77" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.26953125" customWidth="1"/>
+    <col min="47" max="47" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C2" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3" t="s">
+        <v>560</v>
+      </c>
+      <c r="C3" t="s">
+        <v>689</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>606</v>
+      </c>
+      <c r="B4" t="s">
+        <v>561</v>
+      </c>
+      <c r="C4" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>607</v>
+      </c>
+      <c r="B5" t="s">
+        <v>562</v>
+      </c>
+      <c r="C5" t="s">
+        <v>691</v>
+      </c>
+      <c r="E5" t="s">
+        <v>686</v>
+      </c>
+      <c r="T5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>687</v>
+      </c>
+      <c r="AW5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C6" t="s">
+        <v>692</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>609</v>
+      </c>
+      <c r="B7" t="s">
+        <v>564</v>
+      </c>
+      <c r="C7" t="s">
+        <v>693</v>
+      </c>
+      <c r="D7" t="s">
+        <v>695</v>
+      </c>
+      <c r="S7" t="s">
+        <v>696</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>610</v>
+      </c>
+      <c r="B8" t="s">
+        <v>565</v>
+      </c>
+      <c r="C8" t="s">
+        <v>694</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>611</v>
+      </c>
+      <c r="B9" t="s">
+        <v>566</v>
+      </c>
+      <c r="C9" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>612</v>
+      </c>
+      <c r="B10" t="s">
+        <v>567</v>
+      </c>
+      <c r="C10" t="s">
+        <v>689</v>
+      </c>
+      <c r="E10" t="s">
+        <v>697</v>
+      </c>
+      <c r="G10" s="4">
+        <v>37388</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>698</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>699</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>613</v>
+      </c>
+      <c r="B11" t="s">
+        <v>568</v>
+      </c>
+      <c r="C11" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>614</v>
+      </c>
+      <c r="B12" t="s">
+        <v>569</v>
+      </c>
+      <c r="C12" t="s">
+        <v>691</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>615</v>
+      </c>
+      <c r="B13" t="s">
+        <v>570</v>
+      </c>
+      <c r="C13" t="s">
+        <v>692</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>616</v>
+      </c>
+      <c r="B14" t="s">
+        <v>571</v>
+      </c>
+      <c r="C14" t="s">
+        <v>693</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>617</v>
+      </c>
+      <c r="B15" t="s">
+        <v>572</v>
+      </c>
+      <c r="C15" t="s">
+        <v>694</v>
+      </c>
+      <c r="F15" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>618</v>
+      </c>
+      <c r="B16" t="s">
+        <v>573</v>
+      </c>
+      <c r="C16" t="s">
+        <v>688</v>
+      </c>
+      <c r="J16" t="s">
+        <v>89</v>
+      </c>
+      <c r="R16" t="s">
+        <v>701</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>702</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>619</v>
+      </c>
+      <c r="B17" t="s">
+        <v>574</v>
+      </c>
+      <c r="C17" t="s">
+        <v>689</v>
+      </c>
+      <c r="I17" t="s">
+        <v>695</v>
+      </c>
+      <c r="L17" t="s">
+        <v>703</v>
+      </c>
+      <c r="U17" t="s">
+        <v>704</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>620</v>
+      </c>
+      <c r="B18" t="s">
+        <v>575</v>
+      </c>
+      <c r="C18" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>621</v>
+      </c>
+      <c r="B19" t="s">
+        <v>576</v>
+      </c>
+      <c r="C19" t="s">
+        <v>691</v>
+      </c>
+      <c r="N19" s="4">
+        <v>40128</v>
+      </c>
+      <c r="O19" s="8">
+        <v>12</v>
+      </c>
+      <c r="P19" s="4">
+        <v>40169</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>705</v>
+      </c>
+      <c r="V19" t="s">
+        <v>706</v>
+      </c>
+      <c r="W19" t="s">
+        <v>707</v>
+      </c>
+      <c r="Z19">
+        <v>1276877</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>622</v>
+      </c>
+      <c r="B20" t="s">
+        <v>577</v>
+      </c>
+      <c r="C20" t="s">
+        <v>692</v>
+      </c>
+      <c r="K20" s="4">
+        <v>36763</v>
+      </c>
+      <c r="M20" t="s">
+        <v>709</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>710</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>711</v>
+      </c>
+      <c r="AT20" s="4">
+        <v>36100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>623</v>
+      </c>
+      <c r="B21" t="s">
+        <v>578</v>
+      </c>
+      <c r="C21" t="s">
+        <v>693</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>624</v>
+      </c>
+      <c r="B22" t="s">
+        <v>579</v>
+      </c>
+      <c r="C22" t="s">
+        <v>694</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>625</v>
+      </c>
+      <c r="B23" t="s">
+        <v>580</v>
+      </c>
+      <c r="C23" t="s">
+        <v>688</v>
+      </c>
+      <c r="V23" t="s">
+        <v>712</v>
+      </c>
+      <c r="Z23">
+        <v>3435555</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>626</v>
+      </c>
+      <c r="B24" t="s">
+        <v>581</v>
+      </c>
+      <c r="C24" t="s">
+        <v>689</v>
+      </c>
+      <c r="AS24" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>627</v>
+      </c>
+      <c r="B25" t="s">
+        <v>582</v>
+      </c>
+      <c r="C25" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>628</v>
+      </c>
+      <c r="B26" t="s">
+        <v>583</v>
+      </c>
+      <c r="C26" t="s">
+        <v>691</v>
+      </c>
+      <c r="H26" s="4">
+        <v>36534</v>
+      </c>
+      <c r="X26">
+        <v>23456789</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>714</v>
+      </c>
+      <c r="AM26">
+        <v>2334568</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>629</v>
+      </c>
+      <c r="B27" t="s">
+        <v>584</v>
+      </c>
+      <c r="C27" t="s">
+        <v>692</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>717</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>718</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>719</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>716</v>
+      </c>
+      <c r="AN27" s="4">
+        <v>36412</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>630</v>
+      </c>
+      <c r="B28" t="s">
+        <v>585</v>
+      </c>
+      <c r="C28" t="s">
+        <v>693</v>
+      </c>
+      <c r="AS28" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>631</v>
+      </c>
+      <c r="B29" t="s">
+        <v>586</v>
+      </c>
+      <c r="C29" t="s">
+        <v>694</v>
+      </c>
+      <c r="AS29" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>632</v>
+      </c>
+      <c r="B30" t="s">
+        <v>587</v>
+      </c>
+      <c r="C30" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>633</v>
+      </c>
+      <c r="B31" t="s">
+        <v>588</v>
+      </c>
+      <c r="C31" t="s">
+        <v>689</v>
+      </c>
+      <c r="AS31" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>634</v>
+      </c>
+      <c r="B32" t="s">
+        <v>589</v>
+      </c>
+      <c r="C32" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS32" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="33" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>635</v>
+      </c>
+      <c r="B33" t="s">
+        <v>539</v>
+      </c>
+      <c r="C33" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>722</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>721</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>723</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>724</v>
+      </c>
+      <c r="AW33">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="34" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>636</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>692</v>
+      </c>
+      <c r="AG34">
+        <v>34567588</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>725</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>726</v>
+      </c>
+      <c r="AS34" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>637</v>
+      </c>
+      <c r="B35" t="s">
+        <v>590</v>
+      </c>
+      <c r="C35" t="s">
+        <v>693</v>
+      </c>
+      <c r="AS35" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>638</v>
+      </c>
+      <c r="B36" t="s">
+        <v>591</v>
+      </c>
+      <c r="C36" t="s">
+        <v>694</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>727</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>728</v>
+      </c>
+      <c r="AK36">
+        <v>9222</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="37" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>639</v>
+      </c>
+      <c r="B37" t="s">
+        <v>592</v>
+      </c>
+      <c r="C37" t="s">
+        <v>688</v>
+      </c>
+      <c r="E37" t="s">
+        <v>730</v>
+      </c>
+      <c r="G37" s="4">
+        <v>42239</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>731</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>732</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>640</v>
+      </c>
+      <c r="B38" t="s">
+        <v>593</v>
+      </c>
+      <c r="C38" t="s">
+        <v>689</v>
+      </c>
+      <c r="AX38">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>641</v>
+      </c>
+      <c r="B39" t="s">
+        <v>594</v>
+      </c>
+      <c r="C39" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS39" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="40" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>642</v>
+      </c>
+      <c r="B40" t="s">
+        <v>595</v>
+      </c>
+      <c r="C40" t="s">
+        <v>691</v>
+      </c>
+      <c r="AS40" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>643</v>
+      </c>
+      <c r="B41" t="s">
+        <v>596</v>
+      </c>
+      <c r="C41" t="s">
+        <v>692</v>
+      </c>
+      <c r="AS41" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>644</v>
+      </c>
+      <c r="B42" t="s">
+        <v>597</v>
+      </c>
+      <c r="C42" t="s">
+        <v>693</v>
+      </c>
+      <c r="AS42" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="43" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>645</v>
+      </c>
+      <c r="B43" t="s">
+        <v>598</v>
+      </c>
+      <c r="C43" t="s">
+        <v>694</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="44" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>646</v>
+      </c>
+      <c r="B44" t="s">
+        <v>599</v>
+      </c>
+      <c r="C44" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS44" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="45" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>647</v>
+      </c>
+      <c r="B45" t="s">
+        <v>600</v>
+      </c>
+      <c r="C45" t="s">
+        <v>689</v>
+      </c>
+      <c r="AS45" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="46" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>648</v>
+      </c>
+      <c r="B46" t="s">
+        <v>601</v>
+      </c>
+      <c r="C46" t="s">
+        <v>690</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>733</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>734</v>
+      </c>
+      <c r="AU46" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="47" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>649</v>
+      </c>
+      <c r="B47" t="s">
+        <v>602</v>
+      </c>
+      <c r="C47" t="s">
+        <v>691</v>
+      </c>
+      <c r="H47" s="4">
+        <v>36495</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>736</v>
+      </c>
+      <c r="AM47" t="s">
+        <v>737</v>
+      </c>
+      <c r="AP47" t="s">
+        <v>738</v>
+      </c>
+      <c r="AV47" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="48" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>650</v>
+      </c>
+      <c r="B48" t="s">
+        <v>603</v>
+      </c>
+      <c r="C48" t="s">
+        <v>692</v>
+      </c>
+      <c r="AS48" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>746</v>
+      </c>
+      <c r="B49" t="s">
+        <v>559</v>
+      </c>
+      <c r="C49" t="s">
+        <v>690</v>
+      </c>
+      <c r="AS49" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>748</v>
+      </c>
+      <c r="B50" t="s">
+        <v>574</v>
+      </c>
+      <c r="C50" t="s">
+        <v>692</v>
+      </c>
+      <c r="I50" t="s">
+        <v>695</v>
+      </c>
+      <c r="L50" t="s">
+        <v>749</v>
+      </c>
+      <c r="U50" t="s">
+        <v>750</v>
+      </c>
+      <c r="AS50" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>752</v>
+      </c>
+      <c r="B51" t="s">
+        <v>589</v>
+      </c>
+      <c r="C51" t="s">
+        <v>694</v>
+      </c>
+      <c r="AS51" t="s">
+        <v>753</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2633,7 +4541,7 @@
   <dimension ref="A1:AT5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2695,7 +4603,7 @@
         <v>87</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>118</v>
+        <v>742</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>40</v>
@@ -3181,7 +5089,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3213,7 +5121,7 @@
         <v>219</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>118</v>
+        <v>743</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>203</v>
@@ -3928,7 +5836,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4222,7 +6130,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4276,7 +6184,7 @@
         <v>352</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>740</v>
       </c>
       <c r="C2">
         <v>8157500</v>
@@ -4590,8 +6498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Automation - Lease Licenses refactoring (#3188)
* Automation Projects

* Automation - Projects and Products automation

* Leases refactoring

* Leases refactoring
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4814C91-07EE-4F73-A421-EF825998BBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934CED0E-0604-4AE7-A36B-B854BF09258F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="868" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="934" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualContacts" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,18 @@
     <sheet name="FinancialCodes" sheetId="11" r:id="rId3"/>
     <sheet name="Projects" sheetId="3" r:id="rId4"/>
     <sheet name="ProjectsProducts" sheetId="4" r:id="rId5"/>
-    <sheet name="ResearchFiles" sheetId="5" r:id="rId6"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId7"/>
+    <sheet name="Leases" sheetId="14" r:id="rId6"/>
+    <sheet name="ResearchFiles" sheetId="5" r:id="rId7"/>
     <sheet name="PropertyResearch" sheetId="9" r:id="rId8"/>
-    <sheet name="Properties" sheetId="6" r:id="rId9"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId10"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId11"/>
-    <sheet name="Notes" sheetId="10" r:id="rId12"/>
+    <sheet name="LeasesTenants" sheetId="15" r:id="rId9"/>
+    <sheet name="LeasesDeposits" sheetId="16" r:id="rId10"/>
+    <sheet name="LeasesTerms" sheetId="17" r:id="rId11"/>
+    <sheet name="LeasesPayments" sheetId="18" r:id="rId12"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId13"/>
+    <sheet name="Properties" sheetId="6" r:id="rId14"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId15"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId16"/>
+    <sheet name="Notes" sheetId="10" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="992">
   <si>
     <t>BillingAddressLine1</t>
   </si>
@@ -2309,14 +2314,729 @@
   </si>
   <si>
     <t>Updating automatic Notice of possible entry (H0224) document - edited</t>
+  </si>
+  <si>
+    <t>MinistryProject</t>
+  </si>
+  <si>
+    <t>LeaseStatus</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>LeaseStartDate</t>
+  </si>
+  <si>
+    <t>LeaseExpiryDate</t>
+  </si>
+  <si>
+    <t>MOTIContact</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>ProgramOther</t>
+  </si>
+  <si>
+    <t>AdminType</t>
+  </si>
+  <si>
+    <t>TypeOther</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>CategoryOther</t>
+  </si>
+  <si>
+    <t>PurposeOther</t>
+  </si>
+  <si>
+    <t>Initiator</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>IntendedUse</t>
+  </si>
+  <si>
+    <t>FirstNation</t>
+  </si>
+  <si>
+    <t>StrategicRealEstate</t>
+  </si>
+  <si>
+    <t>RegionalPlanning</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Headquarter</t>
+  </si>
+  <si>
+    <t>ConsultationOther</t>
+  </si>
+  <si>
+    <t>ConsultationOtherDetails</t>
+  </si>
+  <si>
+    <t>PhysicalLeaseExist</t>
+  </si>
+  <si>
+    <t>DigitalLeaseExist</t>
+  </si>
+  <si>
+    <t>DocumentLocation</t>
+  </si>
+  <si>
+    <t>LISNumber</t>
+  </si>
+  <si>
+    <t>PSNumber</t>
+  </si>
+  <si>
+    <t>LeaseNotes</t>
+  </si>
+  <si>
+    <t>TenantsStartRow</t>
+  </si>
+  <si>
+    <t>TenantsQuantity</t>
+  </si>
+  <si>
+    <t>TenantsNumber</t>
+  </si>
+  <si>
+    <t>RepresentativeNumber</t>
+  </si>
+  <si>
+    <t>PropertyManagerNumber</t>
+  </si>
+  <si>
+    <t>UnknownNumber</t>
+  </si>
+  <si>
+    <t>CommercialImprovementUnit</t>
+  </si>
+  <si>
+    <t>CommercialImprovementBuildingSize</t>
+  </si>
+  <si>
+    <t>CommercialImprovementDescription</t>
+  </si>
+  <si>
+    <t>AircraftInsuranceInPlace</t>
+  </si>
+  <si>
+    <t>AircraftLimit</t>
+  </si>
+  <si>
+    <t>AircraftPolicyExpiryDate</t>
+  </si>
+  <si>
+    <t>AircraftDescriptionCoverage</t>
+  </si>
+  <si>
+    <t>CGLInsuranceInPlace</t>
+  </si>
+  <si>
+    <t>CGLLimit</t>
+  </si>
+  <si>
+    <t>CGLPolicyExpiryDate</t>
+  </si>
+  <si>
+    <t>CGLDescriptionCoverage</t>
+  </si>
+  <si>
+    <t>MarineInsuranceInPlace</t>
+  </si>
+  <si>
+    <t>MarineLimit</t>
+  </si>
+  <si>
+    <t>MarinePolicyExpiryDate</t>
+  </si>
+  <si>
+    <t>MarineDescriptionCoverage</t>
+  </si>
+  <si>
+    <t>VehicleInsuranceInPlace</t>
+  </si>
+  <si>
+    <t>VehicleLimit</t>
+  </si>
+  <si>
+    <t>VehiclePolicyExpiryDate</t>
+  </si>
+  <si>
+    <t>VehicleDescriptionCoverage</t>
+  </si>
+  <si>
+    <t>OtherInsuranceType</t>
+  </si>
+  <si>
+    <t>OtherInsuranceInPlace</t>
+  </si>
+  <si>
+    <t>OtherLimit</t>
+  </si>
+  <si>
+    <t>OtherPolicyExpiryDate</t>
+  </si>
+  <si>
+    <t>OtherDescriptionCoverage</t>
+  </si>
+  <si>
+    <t>DepositNotes</t>
+  </si>
+  <si>
+    <t>DepositsStartRow</t>
+  </si>
+  <si>
+    <t>DepositsCount</t>
+  </si>
+  <si>
+    <t>TermsStartRow</t>
+  </si>
+  <si>
+    <t>TermsCount</t>
+  </si>
+  <si>
+    <t>PaymentsStartRow</t>
+  </si>
+  <si>
+    <t>PaymentsCount</t>
+  </si>
+  <si>
+    <t>Create a new complete lease</t>
+  </si>
+  <si>
+    <t>Payable (BCTFA as tenant)</t>
+  </si>
+  <si>
+    <t>Automation Test</t>
+  </si>
+  <si>
+    <t>BC Ferries</t>
+  </si>
+  <si>
+    <t>MOTI Project Use License</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Headquarters</t>
+  </si>
+  <si>
+    <t>Automation Test Intention of use</t>
+  </si>
+  <si>
+    <t>Required, not completed</t>
+  </si>
+  <si>
+    <t>Required, completed</t>
+  </si>
+  <si>
+    <t>Not required</t>
+  </si>
+  <si>
+    <t>Other required documents</t>
+  </si>
+  <si>
+    <t>The documents has been scanned and saved on the main server</t>
+  </si>
+  <si>
+    <t>1948-0000-1</t>
+  </si>
+  <si>
+    <t>135-256-001</t>
+  </si>
+  <si>
+    <t>Automation Test Notes</t>
+  </si>
+  <si>
+    <t>1688 Blanshard St. Victoria, BC, V7C 1B7</t>
+  </si>
+  <si>
+    <t>256 sqft</t>
+  </si>
+  <si>
+    <t>Automation Test - Commercial Improvement Description</t>
+  </si>
+  <si>
+    <t>2301-1155 Nanaimo St. Vancouver, BC V6Z 2C7</t>
+  </si>
+  <si>
+    <t>175.69 sqft</t>
+  </si>
+  <si>
+    <t>Automation Test - Residential Improvement Description</t>
+  </si>
+  <si>
+    <t>Stanley Park, Vancouver, BC, V6Z 8J9</t>
+  </si>
+  <si>
+    <t>2256 sqft</t>
+  </si>
+  <si>
+    <t>Automation Test - Other Improvement Description</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Automation Test - Aircraft Insurance Description</t>
+  </si>
+  <si>
+    <t>Automation Test - Commercial General Liability Insurance Description</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Automation Test - Marine Insurance Description</t>
+  </si>
+  <si>
+    <t>Automation Test - Vehicle Insurance Description</t>
+  </si>
+  <si>
+    <t>Pets Insurance</t>
+  </si>
+  <si>
+    <t>Pet insurance pending by the tenant to acquire</t>
+  </si>
+  <si>
+    <t>Automation Test - Deposit Notes</t>
+  </si>
+  <si>
+    <t>Edit lease</t>
+  </si>
+  <si>
+    <t>Automation Test Intented use - Edited by automation</t>
+  </si>
+  <si>
+    <t>Automation Test Notes - Edited by automation</t>
+  </si>
+  <si>
+    <t>Vancouver Aquarium, Vancouver, BC, V6Z 8J9</t>
+  </si>
+  <si>
+    <t>225 sqft</t>
+  </si>
+  <si>
+    <t>Automation Test Edition - Other Improvement Description edited</t>
+  </si>
+  <si>
+    <t>Automation Test - Vehicle Insurance no longer in place.</t>
+  </si>
+  <si>
+    <t>Automation Test Edition - Deposit Description edited</t>
+  </si>
+  <si>
+    <t>Create minimum lease</t>
+  </si>
+  <si>
+    <t>Payable (MOTI as tenant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>TMEP</t>
+  </si>
+  <si>
+    <t>Automated Purpose</t>
+  </si>
+  <si>
+    <t>1663 Fox St. Nanaimo, BC, B9N 2H8</t>
+  </si>
+  <si>
+    <t>54 sqft</t>
+  </si>
+  <si>
+    <t>Automation Test - Minimum Lease creation</t>
+  </si>
+  <si>
+    <t>Automation Test - Minimum Insurance test</t>
+  </si>
+  <si>
+    <t>Automation Test - Creating minimum lease with one deposit</t>
+  </si>
+  <si>
+    <t>Create a lease from a green pin</t>
+  </si>
+  <si>
+    <t>Receivable</t>
+  </si>
+  <si>
+    <t>Create a lease from a blue pin</t>
+  </si>
+  <si>
+    <t>Terminated</t>
+  </si>
+  <si>
+    <t>Create a lease from a purple pin</t>
+  </si>
+  <si>
+    <t>Discarded</t>
+  </si>
+  <si>
+    <t>ContactType</t>
+  </si>
+  <si>
+    <t>PrimaryContact</t>
+  </si>
+  <si>
+    <t>TenantType</t>
+  </si>
+  <si>
+    <t>Create Complete Lease</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Tenant</t>
+  </si>
+  <si>
+    <t>District of Saanich</t>
+  </si>
+  <si>
+    <t>Chris Pease</t>
+  </si>
+  <si>
+    <t>Sakwi Creek Hydro LP</t>
+  </si>
+  <si>
+    <t>Paul Schincariol</t>
+  </si>
+  <si>
+    <t>Property manager</t>
+  </si>
+  <si>
+    <t>Bishop of Victoria</t>
+  </si>
+  <si>
+    <t>No contacts available</t>
+  </si>
+  <si>
+    <t>Representative</t>
+  </si>
+  <si>
+    <t>Edit Lease</t>
+  </si>
+  <si>
+    <t>Create minimum Lease</t>
+  </si>
+  <si>
+    <t>Pauline Faulkes</t>
+  </si>
+  <si>
+    <t>DepositType</t>
+  </si>
+  <si>
+    <t>DepositTypeOther</t>
+  </si>
+  <si>
+    <t>DepositDescription</t>
+  </si>
+  <si>
+    <t>DepositAmount</t>
+  </si>
+  <si>
+    <t>DepositPaidDate</t>
+  </si>
+  <si>
+    <t>DepositHolder</t>
+  </si>
+  <si>
+    <t>ReturnTerminationDate</t>
+  </si>
+  <si>
+    <t>TerminationClaimDeposit</t>
+  </si>
+  <si>
+    <t>ReturnedAmount</t>
+  </si>
+  <si>
+    <t>ReturnInterestPaid</t>
+  </si>
+  <si>
+    <t>ReturnedDate</t>
+  </si>
+  <si>
+    <t>ReturnPayeeName</t>
+  </si>
+  <si>
+    <t>Security deposit</t>
+  </si>
+  <si>
+    <t>Automation Test - Deposit Description</t>
+  </si>
+  <si>
+    <t>Other deposit</t>
+  </si>
+  <si>
+    <t>Special Levy</t>
+  </si>
+  <si>
+    <t>Automation - Special Levy required on the first payment</t>
+  </si>
+  <si>
+    <t>Pet deposit</t>
+  </si>
+  <si>
+    <t>Automation - Minimum lease with one insurance</t>
+  </si>
+  <si>
+    <t>Bernadette Miller</t>
+  </si>
+  <si>
+    <t>Alicia Ortega</t>
+  </si>
+  <si>
+    <t>TermStartDate</t>
+  </si>
+  <si>
+    <t>TermEndDate</t>
+  </si>
+  <si>
+    <t>TermPaymentFrequency</t>
+  </si>
+  <si>
+    <t>TermAgreedPayment</t>
+  </si>
+  <si>
+    <t>TermPaymentsDue</t>
+  </si>
+  <si>
+    <t>PaymentGST</t>
+  </si>
+  <si>
+    <t>TermStatus</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Every Friday</t>
+  </si>
+  <si>
+    <t>Exercised</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Every 15th of the month</t>
+  </si>
+  <si>
+    <t>Not Exercised</t>
+  </si>
+  <si>
+    <t>Edit a lease</t>
+  </si>
+  <si>
+    <t>Annually</t>
+  </si>
+  <si>
+    <t>January 1st</t>
+  </si>
+  <si>
+    <t>PaymentSentDate</t>
+  </si>
+  <si>
+    <t>PaymentMethod</t>
+  </si>
+  <si>
+    <t>PaymentTotalReceived</t>
+  </si>
+  <si>
+    <t>PaymentExpectedPayment</t>
+  </si>
+  <si>
+    <t>PaymentStatus</t>
+  </si>
+  <si>
+    <t>ParentTerm</t>
+  </si>
+  <si>
+    <t>Create new complete lease</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Credit / Debit</t>
+  </si>
+  <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>Edit created lease</t>
+  </si>
+  <si>
+    <t>EFT</t>
+  </si>
+  <si>
+    <t>H120</t>
+  </si>
+  <si>
+    <t>Create new Lease</t>
+  </si>
+  <si>
+    <t>001-192-396</t>
+  </si>
+  <si>
+    <t>2525 Mill Bay Rd</t>
+  </si>
+  <si>
+    <t>VAP7495</t>
+  </si>
+  <si>
+    <t>LOT 3 DISTRICT LOT 118 GROUP 1</t>
+  </si>
+  <si>
+    <t>010-598-103</t>
+  </si>
+  <si>
+    <t>Create Lease from green pin</t>
+  </si>
+  <si>
+    <t>015-254-241</t>
+  </si>
+  <si>
+    <t>Create Lease from blue pin</t>
+  </si>
+  <si>
+    <t>Create Lease from purple pin</t>
+  </si>
+  <si>
+    <t>000-228-729</t>
+  </si>
+  <si>
+    <t>Leases - Create new notes</t>
+  </si>
+  <si>
+    <t>Leases Automation Functional Testing - Note 1,Leases Automation Functional Testing - Note 2,Leases Automation Functional Testing - Note 3,Leases Automation Functional Testing - Note 4,Leases Automation Functional Testing - Note 5,Leases Automation Functional Testing - Note 6,Leases Automation Functional Testing - Note 7,Leases Automation Functional Testing - Note 8,Leases Automation Functional Testing - Note 9,Leases Automation Functional Testing - Note 10,Leases Automation Functional Testing - Note 11,Leases Automation Functional Testing - Note 12</t>
+  </si>
+  <si>
+    <t>Every Monday</t>
+  </si>
+  <si>
+    <t>RegionalPropertyService</t>
+  </si>
+  <si>
+    <t>ResidentialImprovementUnit</t>
+  </si>
+  <si>
+    <t>ResidentialImprovementBuildingSize</t>
+  </si>
+  <si>
+    <t>ResidentialImprovementDescription</t>
+  </si>
+  <si>
+    <t>OtherImprovementUnit</t>
+  </si>
+  <si>
+    <t>OtherImprovementBuildingSize</t>
+  </si>
+  <si>
+    <t>OtherImprovementDescription</t>
+  </si>
+  <si>
+    <t>Automation - Update previously created Deposit</t>
+  </si>
+  <si>
+    <t>Jacqueline Pamela Baker</t>
+  </si>
+  <si>
+    <t>IsGSTEligible</t>
+  </si>
+  <si>
+    <t>Overpayment</t>
+  </si>
+  <si>
+    <t>Create from green pin</t>
+  </si>
+  <si>
+    <t>Mid June</t>
+  </si>
+  <si>
+    <t>Post-dated cheque</t>
+  </si>
+  <si>
+    <t>Local Government/RCMP</t>
+  </si>
+  <si>
+    <t>Rail Trails</t>
+  </si>
+  <si>
+    <t>Automation Program</t>
+  </si>
+  <si>
+    <t>Ground Lease</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
+  </si>
+  <si>
+    <t>Park and Ride</t>
+  </si>
+  <si>
+    <t>Road Crossing</t>
+  </si>
+  <si>
+    <t>Maintenance Yard</t>
+  </si>
+  <si>
+    <t>TransLink</t>
+  </si>
+  <si>
+    <t>Lease - Unregistered</t>
+  </si>
+  <si>
+    <t>Gov't to Gov't</t>
+  </si>
+  <si>
+    <t>Encroachment</t>
+  </si>
+  <si>
+    <t>Other Licencing</t>
+  </si>
+  <si>
+    <t>MinistryProjectCode</t>
+  </si>
+  <si>
+    <t>TotalImprovementCount</t>
+  </si>
+  <si>
+    <t>TotalInsuranceCount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/dd/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2370,7 +3090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2383,6 +3103,10 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3311,11 +4035,1053 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59063E35-2744-4A83-A0B3-24C7FD044C62}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>904</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>905</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B2" t="s">
+        <v>909</v>
+      </c>
+      <c r="D2" t="s">
+        <v>910</v>
+      </c>
+      <c r="E2" s="11">
+        <v>250</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44617</v>
+      </c>
+      <c r="G2" t="s">
+        <v>883</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44645</v>
+      </c>
+      <c r="I2" s="11">
+        <v>75</v>
+      </c>
+      <c r="J2" s="11">
+        <v>50</v>
+      </c>
+      <c r="K2" s="11">
+        <v>25</v>
+      </c>
+      <c r="L2" s="4">
+        <v>44650</v>
+      </c>
+      <c r="M2" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>820</v>
+      </c>
+      <c r="B3" t="s">
+        <v>911</v>
+      </c>
+      <c r="C3" t="s">
+        <v>912</v>
+      </c>
+      <c r="D3" t="s">
+        <v>913</v>
+      </c>
+      <c r="E3" s="11">
+        <v>632</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44645</v>
+      </c>
+      <c r="G3" t="s">
+        <v>970</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44666</v>
+      </c>
+      <c r="I3" s="11">
+        <v>150</v>
+      </c>
+      <c r="J3" s="11">
+        <v>150</v>
+      </c>
+      <c r="K3" s="11">
+        <v>50</v>
+      </c>
+      <c r="L3" s="4">
+        <v>44681</v>
+      </c>
+      <c r="M3" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>894</v>
+      </c>
+      <c r="B4" t="s">
+        <v>914</v>
+      </c>
+      <c r="D4" t="s">
+        <v>969</v>
+      </c>
+      <c r="E4" s="11">
+        <v>50.99</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44645</v>
+      </c>
+      <c r="G4" t="s">
+        <v>970</v>
+      </c>
+      <c r="H4" s="4">
+        <v>44666</v>
+      </c>
+      <c r="I4" s="11">
+        <v>150</v>
+      </c>
+      <c r="J4" s="11">
+        <v>150</v>
+      </c>
+      <c r="K4" s="11">
+        <v>50</v>
+      </c>
+      <c r="L4" s="4">
+        <v>44681</v>
+      </c>
+      <c r="M4" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>862</v>
+      </c>
+      <c r="B5" t="s">
+        <v>909</v>
+      </c>
+      <c r="D5" t="s">
+        <v>915</v>
+      </c>
+      <c r="E5" s="11">
+        <v>3500.79</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45058</v>
+      </c>
+      <c r="G5" t="s">
+        <v>916</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45076</v>
+      </c>
+      <c r="I5" s="11">
+        <v>3000</v>
+      </c>
+      <c r="J5" s="11">
+        <v>3000</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>45078</v>
+      </c>
+      <c r="M5" t="s">
+        <v>917</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC2A471-385A-4133-9FB5-E00CEEFCFD2D}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44614</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44673</v>
+      </c>
+      <c r="D2" t="s">
+        <v>925</v>
+      </c>
+      <c r="E2">
+        <v>2500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>926</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>820</v>
+      </c>
+      <c r="B3" s="4">
+        <v>44703</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44742</v>
+      </c>
+      <c r="D3" t="s">
+        <v>928</v>
+      </c>
+      <c r="E3">
+        <v>3500</v>
+      </c>
+      <c r="F3" t="s">
+        <v>929</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>931</v>
+      </c>
+      <c r="B4" s="4">
+        <v>44614</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44673</v>
+      </c>
+      <c r="D4" t="s">
+        <v>925</v>
+      </c>
+      <c r="E4">
+        <v>3000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>961</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>862</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45058</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45424</v>
+      </c>
+      <c r="D5" t="s">
+        <v>932</v>
+      </c>
+      <c r="E5">
+        <v>120000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>933</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>973</v>
+      </c>
+      <c r="B6" s="4">
+        <v>36690</v>
+      </c>
+      <c r="C6" s="4">
+        <v>36720</v>
+      </c>
+      <c r="D6" t="s">
+        <v>928</v>
+      </c>
+      <c r="E6">
+        <v>3000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>974</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>927</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4E3335-5C1A-476B-8F34-CC44F557D991}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>940</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44616</v>
+      </c>
+      <c r="C2" t="s">
+        <v>941</v>
+      </c>
+      <c r="D2">
+        <v>2625</v>
+      </c>
+      <c r="E2">
+        <v>2500</v>
+      </c>
+      <c r="F2">
+        <f>D2-E2</f>
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>942</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>940</v>
+      </c>
+      <c r="B3" s="4">
+        <v>44623</v>
+      </c>
+      <c r="C3" t="s">
+        <v>943</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3">
+        <v>285.70999999999998</v>
+      </c>
+      <c r="F3">
+        <v>14.29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>944</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>945</v>
+      </c>
+      <c r="B4" s="4">
+        <v>44630</v>
+      </c>
+      <c r="C4" t="s">
+        <v>946</v>
+      </c>
+      <c r="D4">
+        <v>3000</v>
+      </c>
+      <c r="E4">
+        <v>2857.14</v>
+      </c>
+      <c r="F4">
+        <v>142.86000000000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>972</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>862</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45061</v>
+      </c>
+      <c r="C5" t="s">
+        <v>947</v>
+      </c>
+      <c r="D5">
+        <v>130000</v>
+      </c>
+      <c r="E5">
+        <v>123809.52</v>
+      </c>
+      <c r="F5">
+        <v>6190.48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>972</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>973</v>
+      </c>
+      <c r="B6" s="4">
+        <v>36692</v>
+      </c>
+      <c r="C6" t="s">
+        <v>975</v>
+      </c>
+      <c r="D6">
+        <v>3000</v>
+      </c>
+      <c r="E6">
+        <v>3000</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>942</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C2">
+        <v>8157500</v>
+      </c>
+      <c r="D2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" t="s">
+        <v>361</v>
+      </c>
+      <c r="F6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>488</v>
+      </c>
+      <c r="B10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10">
+        <v>90054791</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>494</v>
+      </c>
+      <c r="B11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>948</v>
+      </c>
+      <c r="B12" t="s">
+        <v>949</v>
+      </c>
+      <c r="C12">
+        <v>553490</v>
+      </c>
+      <c r="D12" t="s">
+        <v>950</v>
+      </c>
+      <c r="E12" t="s">
+        <v>951</v>
+      </c>
+      <c r="F12" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>894</v>
+      </c>
+      <c r="B13" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>954</v>
+      </c>
+      <c r="B14" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>956</v>
+      </c>
+      <c r="B15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>957</v>
+      </c>
+      <c r="B16" t="s">
+        <v>958</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="60" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="27.36328125" customWidth="1"/>
+    <col min="20" max="20" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="83.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3" t="s">
+        <v>334</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" t="s">
+        <v>336</v>
+      </c>
+      <c r="J3" t="s">
+        <v>338</v>
+      </c>
+      <c r="K3" t="s">
+        <v>339</v>
+      </c>
+      <c r="L3" t="s">
+        <v>337</v>
+      </c>
+      <c r="M3" t="s">
+        <v>416</v>
+      </c>
+      <c r="N3" t="s">
+        <v>340</v>
+      </c>
+      <c r="O3" t="s">
+        <v>430</v>
+      </c>
+      <c r="P3" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>341</v>
+      </c>
+      <c r="S3" t="s">
+        <v>342</v>
+      </c>
+      <c r="T3">
+        <v>100</v>
+      </c>
+      <c r="U3" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>50</v>
+      </c>
+      <c r="W3" t="s">
+        <v>343</v>
+      </c>
+      <c r="X3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" t="s">
+        <v>490</v>
+      </c>
+      <c r="D4" t="s">
+        <v>491</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>492</v>
+      </c>
+      <c r="N4" t="s">
+        <v>493</v>
+      </c>
+      <c r="T4">
+        <v>65</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>103.59</v>
+      </c>
+      <c r="W4" t="s">
+        <v>343</v>
+      </c>
+      <c r="X4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3407,12 +5173,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3420,8 +5186,14 @@
     <col min="1" max="1" width="75.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="15" width="19.1796875" customWidth="1"/>
-    <col min="16" max="16" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="8" width="19.1796875" style="13" customWidth="1"/>
+    <col min="9" max="10" width="19.1796875" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="13" customWidth="1"/>
+    <col min="12" max="13" width="19.1796875" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" style="13" customWidth="1"/>
+    <col min="15" max="15" width="19.1796875" customWidth="1"/>
+    <col min="16" max="16" width="20.1796875" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="19.1796875" customWidth="1"/>
     <col min="19" max="19" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="20" max="30" width="19.1796875" customWidth="1"/>
@@ -3432,7 +5204,7 @@
     <col min="42" max="42" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="43" max="44" width="19.1796875" customWidth="1"/>
     <col min="45" max="45" width="77" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.26953125" customWidth="1"/>
+    <col min="46" max="46" width="14.26953125" style="13" customWidth="1"/>
     <col min="47" max="47" width="36.26953125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="15.26953125" bestFit="1" customWidth="1"/>
@@ -3457,10 +5229,10 @@
       <c r="F1" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="12" t="s">
         <v>514</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="12" t="s">
         <v>534</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -3469,7 +5241,7 @@
       <c r="J1" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="12" t="s">
         <v>529</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -3478,13 +5250,13 @@
       <c r="M1" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="12" t="s">
         <v>522</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="12" t="s">
         <v>524</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -3574,7 +5346,7 @@
       <c r="AS1" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="12" t="s">
         <v>212</v>
       </c>
       <c r="AU1" s="3" t="s">
@@ -3730,7 +5502,7 @@
       <c r="E10" t="s">
         <v>697</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="13">
         <v>37388</v>
       </c>
       <c r="AD10" t="s">
@@ -3883,13 +5655,13 @@
       <c r="C19" t="s">
         <v>691</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19" s="13">
         <v>40128</v>
       </c>
       <c r="O19" s="8">
         <v>12</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="13">
         <v>40169</v>
       </c>
       <c r="Q19" t="s">
@@ -3918,7 +5690,7 @@
       <c r="C20" t="s">
         <v>692</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="13">
         <v>36763</v>
       </c>
       <c r="M20" t="s">
@@ -3930,7 +5702,7 @@
       <c r="AR20" t="s">
         <v>711</v>
       </c>
-      <c r="AT20" s="4">
+      <c r="AT20" s="13">
         <v>36100</v>
       </c>
     </row>
@@ -4020,7 +5792,7 @@
       <c r="C26" t="s">
         <v>691</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="13">
         <v>36534</v>
       </c>
       <c r="X26">
@@ -4234,7 +6006,7 @@
       <c r="E37" t="s">
         <v>730</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="13">
         <v>42239</v>
       </c>
       <c r="AD37" t="s">
@@ -4389,7 +6161,7 @@
       <c r="C47" t="s">
         <v>691</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="13">
         <v>36495</v>
       </c>
       <c r="Y47" t="s">
@@ -4476,12 +6248,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4528,6 +6300,14 @@
       </c>
       <c r="B5" t="s">
         <v>439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>959</v>
+      </c>
+      <c r="B6" t="s">
+        <v>960</v>
       </c>
     </row>
   </sheetData>
@@ -5832,11 +7612,993 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
+  <dimension ref="A1:CC7"/>
+  <sheetViews>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="22.453125" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="56" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="50" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="49.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.6328125" customWidth="1"/>
+    <col min="60" max="60" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="42.26953125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="53.26953125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="17" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:81" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="BD1" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="BE1" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="2" spans="1:81" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" t="s">
+        <v>689</v>
+      </c>
+      <c r="E2" t="s">
+        <v>821</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44614</v>
+      </c>
+      <c r="G2" s="4">
+        <v>45373</v>
+      </c>
+      <c r="H2" t="s">
+        <v>822</v>
+      </c>
+      <c r="I2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J2" t="s">
+        <v>823</v>
+      </c>
+      <c r="L2" t="s">
+        <v>824</v>
+      </c>
+      <c r="P2" t="s">
+        <v>825</v>
+      </c>
+      <c r="R2" t="s">
+        <v>826</v>
+      </c>
+      <c r="S2" t="s">
+        <v>544</v>
+      </c>
+      <c r="T2" s="4">
+        <v>44615</v>
+      </c>
+      <c r="U2" t="s">
+        <v>827</v>
+      </c>
+      <c r="V2" t="s">
+        <v>828</v>
+      </c>
+      <c r="W2" t="s">
+        <v>380</v>
+      </c>
+      <c r="X2" t="s">
+        <v>829</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>830</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>828</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>380</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>828</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>831</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>337</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>339</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>832</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>833</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>834</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>835</v>
+      </c>
+      <c r="AJ2">
+        <v>11</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>4</v>
+      </c>
+      <c r="AM2">
+        <v>2</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AO2">
+        <v>1</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>836</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>837</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>838</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>839</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>840</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>841</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>842</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>843</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>844</v>
+      </c>
+      <c r="AZ2">
+        <v>3</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>845</v>
+      </c>
+      <c r="BB2">
+        <v>25000</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>46003</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>846</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>845</v>
+      </c>
+      <c r="BF2">
+        <v>205000</v>
+      </c>
+      <c r="BG2" s="4">
+        <v>46368</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>847</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>848</v>
+      </c>
+      <c r="BJ2">
+        <v>125000</v>
+      </c>
+      <c r="BK2" s="4">
+        <v>46733</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>849</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>845</v>
+      </c>
+      <c r="BN2">
+        <v>11000</v>
+      </c>
+      <c r="BO2" s="4">
+        <v>45272</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>850</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>851</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>848</v>
+      </c>
+      <c r="BS2">
+        <v>100000</v>
+      </c>
+      <c r="BT2" s="4">
+        <v>45729</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>852</v>
+      </c>
+      <c r="BV2">
+        <v>5</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>853</v>
+      </c>
+      <c r="BX2">
+        <v>1</v>
+      </c>
+      <c r="BY2">
+        <v>2</v>
+      </c>
+      <c r="BZ2">
+        <v>1</v>
+      </c>
+      <c r="CA2">
+        <v>2</v>
+      </c>
+      <c r="CB2">
+        <v>1</v>
+      </c>
+      <c r="CC2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:81" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>854</v>
+      </c>
+      <c r="D3" t="s">
+        <v>875</v>
+      </c>
+      <c r="U3" t="s">
+        <v>855</v>
+      </c>
+      <c r="V3" t="s">
+        <v>830</v>
+      </c>
+      <c r="W3" t="s">
+        <v>830</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>337</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>856</v>
+      </c>
+      <c r="AJ3">
+        <v>12</v>
+      </c>
+      <c r="AK3">
+        <v>5</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>857</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>859</v>
+      </c>
+      <c r="AZ3">
+        <v>3</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>848</v>
+      </c>
+      <c r="BN3">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="4">
+        <v>44897</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>860</v>
+      </c>
+      <c r="BV3">
+        <v>4</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>861</v>
+      </c>
+      <c r="BX3">
+        <v>3</v>
+      </c>
+      <c r="BY3">
+        <v>1</v>
+      </c>
+      <c r="BZ3">
+        <v>0</v>
+      </c>
+      <c r="CA3">
+        <v>0</v>
+      </c>
+      <c r="CB3">
+        <v>3</v>
+      </c>
+      <c r="CC3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:81" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>862</v>
+      </c>
+      <c r="D4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" t="s">
+        <v>863</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45058</v>
+      </c>
+      <c r="G4" t="s">
+        <v>864</v>
+      </c>
+      <c r="I4" t="s">
+        <v>233</v>
+      </c>
+      <c r="J4" t="s">
+        <v>865</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>822</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>866</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>6</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>867</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>868</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>869</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>845</v>
+      </c>
+      <c r="BN4">
+        <v>35000</v>
+      </c>
+      <c r="BO4" s="4">
+        <v>45650</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>870</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>871</v>
+      </c>
+      <c r="BX4">
+        <v>4</v>
+      </c>
+      <c r="BY4">
+        <v>1</v>
+      </c>
+      <c r="BZ4">
+        <v>3</v>
+      </c>
+      <c r="CA4">
+        <v>1</v>
+      </c>
+      <c r="CB4">
+        <v>3</v>
+      </c>
+      <c r="CC4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:81" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>872</v>
+      </c>
+      <c r="D5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" t="s">
+        <v>873</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45064</v>
+      </c>
+      <c r="J5" t="s">
+        <v>988</v>
+      </c>
+      <c r="K5" t="s">
+        <v>978</v>
+      </c>
+      <c r="L5" t="s">
+        <v>979</v>
+      </c>
+      <c r="N5" t="s">
+        <v>980</v>
+      </c>
+      <c r="P5" t="s">
+        <v>981</v>
+      </c>
+      <c r="AJ5">
+        <v>13</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BX5">
+        <v>0</v>
+      </c>
+      <c r="BY5">
+        <v>0</v>
+      </c>
+      <c r="BZ5">
+        <v>0</v>
+      </c>
+      <c r="CA5">
+        <v>1</v>
+      </c>
+      <c r="CB5">
+        <v>4</v>
+      </c>
+      <c r="CC5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:81" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>874</v>
+      </c>
+      <c r="D6" t="s">
+        <v>875</v>
+      </c>
+      <c r="E6" t="s">
+        <v>873</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45063</v>
+      </c>
+      <c r="J6" t="s">
+        <v>976</v>
+      </c>
+      <c r="L6" t="s">
+        <v>982</v>
+      </c>
+      <c r="P6" t="s">
+        <v>983</v>
+      </c>
+      <c r="AJ6">
+        <v>14</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BV6">
+        <v>0</v>
+      </c>
+      <c r="BX6">
+        <v>0</v>
+      </c>
+      <c r="BY6">
+        <v>0</v>
+      </c>
+      <c r="BZ6">
+        <v>0</v>
+      </c>
+      <c r="CA6">
+        <v>0</v>
+      </c>
+      <c r="CB6">
+        <v>0</v>
+      </c>
+      <c r="CC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:81" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>876</v>
+      </c>
+      <c r="D7" t="s">
+        <v>877</v>
+      </c>
+      <c r="E7" t="s">
+        <v>821</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45062</v>
+      </c>
+      <c r="J7" t="s">
+        <v>977</v>
+      </c>
+      <c r="K7" t="s">
+        <v>984</v>
+      </c>
+      <c r="L7" t="s">
+        <v>985</v>
+      </c>
+      <c r="N7" t="s">
+        <v>986</v>
+      </c>
+      <c r="P7" t="s">
+        <v>987</v>
+      </c>
+      <c r="AJ7">
+        <v>15</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BV7">
+        <v>0</v>
+      </c>
+      <c r="BX7">
+        <v>0</v>
+      </c>
+      <c r="BY7">
+        <v>0</v>
+      </c>
+      <c r="BZ7">
+        <v>0</v>
+      </c>
+      <c r="CA7">
+        <v>0</v>
+      </c>
+      <c r="CB7">
+        <v>0</v>
+      </c>
+      <c r="CC7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3C62D2-095D-41C7-8E12-52D5164F6230}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6125,172 +8887,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B2" t="s">
-        <v>740</v>
-      </c>
-      <c r="C2">
-        <v>8157500</v>
-      </c>
-      <c r="D2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E2" t="s">
-        <v>325</v>
-      </c>
-      <c r="F2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>413</v>
-      </c>
-      <c r="B3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B4" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B5" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>360</v>
-      </c>
-      <c r="B6" t="s">
-        <v>361</v>
-      </c>
-      <c r="F6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>351</v>
-      </c>
-      <c r="B7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>349</v>
-      </c>
-      <c r="B8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>350</v>
-      </c>
-      <c r="B9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>488</v>
-      </c>
-      <c r="B10" t="s">
-        <v>324</v>
-      </c>
-      <c r="C10">
-        <v>90054791</v>
-      </c>
-      <c r="D10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>494</v>
-      </c>
-      <c r="B11" t="s">
-        <v>361</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56704E8-1DAE-4D99-86A6-0D11D370D1F9}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6495,239 +9097,142 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
-  <dimension ref="A1:X4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E3AF99-B285-4872-B012-0C94F438EBF8}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="60" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="27.36328125" customWidth="1"/>
-    <col min="20" max="20" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="83.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>329</v>
+        <v>878</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>283</v>
+        <v>209</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>284</v>
+        <v>879</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>411</v>
+        <v>881</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+        <v>882</v>
+      </c>
+      <c r="C2" t="s">
+        <v>883</v>
+      </c>
+      <c r="D2" t="s">
+        <v>884</v>
+      </c>
+      <c r="E2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>881</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>331</v>
+        <v>886</v>
       </c>
       <c r="D3" t="s">
-        <v>332</v>
-      </c>
-      <c r="F3" t="s">
-        <v>333</v>
-      </c>
-      <c r="G3" t="s">
-        <v>334</v>
-      </c>
-      <c r="H3" t="s">
-        <v>232</v>
-      </c>
-      <c r="I3" t="s">
-        <v>336</v>
-      </c>
-      <c r="J3" t="s">
-        <v>338</v>
-      </c>
-      <c r="K3" t="s">
-        <v>339</v>
-      </c>
-      <c r="L3" t="s">
-        <v>337</v>
-      </c>
-      <c r="M3" t="s">
-        <v>416</v>
-      </c>
-      <c r="N3" t="s">
-        <v>340</v>
-      </c>
-      <c r="O3" t="s">
-        <v>430</v>
-      </c>
-      <c r="P3" t="s">
-        <v>431</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>341</v>
-      </c>
-      <c r="S3" t="s">
-        <v>342</v>
-      </c>
-      <c r="T3">
-        <v>100</v>
-      </c>
-      <c r="U3" t="b">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>50</v>
-      </c>
-      <c r="W3" t="s">
-        <v>343</v>
-      </c>
-      <c r="X3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+        <v>887</v>
+      </c>
+      <c r="E3" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>489</v>
+        <v>881</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>490</v>
+        <v>888</v>
       </c>
       <c r="D4" t="s">
-        <v>491</v>
-      </c>
-      <c r="F4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" t="s">
-        <v>492</v>
-      </c>
-      <c r="N4" t="s">
-        <v>493</v>
-      </c>
-      <c r="T4">
-        <v>65</v>
-      </c>
-      <c r="U4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V4">
-        <v>103.59</v>
-      </c>
-      <c r="W4" t="s">
-        <v>343</v>
-      </c>
-      <c r="X4" t="s">
-        <v>507</v>
+        <v>889</v>
+      </c>
+      <c r="E4" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>881</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>891</v>
+      </c>
+      <c r="D5" t="s">
+        <v>892</v>
+      </c>
+      <c r="E5" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>894</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>888</v>
+      </c>
+      <c r="D6" t="s">
+        <v>889</v>
+      </c>
+      <c r="E6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>895</v>
+      </c>
+      <c r="B7" t="s">
+        <v>882</v>
+      </c>
+      <c r="C7" t="s">
+        <v>896</v>
+      </c>
+      <c r="D7" t="s">
+        <v>884</v>
+      </c>
+      <c r="E7" t="s">
+        <v>890</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nuget package updates, refactoring Contacts, Help desk and AF Checklist
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE484E5-3112-43F7-BF1C-E1F7430A9D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4D5F1E-B35E-47EB-AEB4-573E19F0F583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="934" firstSheet="9" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="934" firstSheet="3" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="1482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="1490">
   <si>
     <t>FirstName</t>
   </si>
@@ -3176,12 +3176,6 @@
     <t>Update existing Individual</t>
   </si>
   <si>
-    <t>Seline</t>
-  </si>
-  <si>
-    <t>seline.white2@yahoo.com</t>
-  </si>
-  <si>
     <t>(778) 567-5555</t>
   </si>
   <si>
@@ -3203,9 +3197,6 @@
     <t>2835 12TH AVE E</t>
   </si>
   <si>
-    <t>Update existing Organization contact</t>
-  </si>
-  <si>
     <t>Automation Test Corp III</t>
   </si>
   <si>
@@ -3392,9 +3383,6 @@
     <t>Section3AgreementSelect9</t>
   </si>
   <si>
-    <t>Section3AgreementSelect10</t>
-  </si>
-  <si>
     <t>AcquisitionCompletionSelect1</t>
   </si>
   <si>
@@ -4127,9 +4115,6 @@
     <t>Editing existing Acquisition File</t>
   </si>
   <si>
-    <t>Devin Smith(MoTI Solicitor)</t>
-  </si>
-  <si>
     <t>010-344-250</t>
   </si>
   <si>
@@ -4512,6 +4497,45 @@
   </si>
   <si>
     <t>Permanent SRW</t>
+  </si>
+  <si>
+    <t>Update complete Individual contact</t>
+  </si>
+  <si>
+    <t>Update existing Individual all Addresses</t>
+  </si>
+  <si>
+    <t>Update complete Individual contact with "Other" addresses</t>
+  </si>
+  <si>
+    <t>Update complete contact form</t>
+  </si>
+  <si>
+    <t>info@testcorp.ca</t>
+  </si>
+  <si>
+    <t>(779) 700-3000</t>
+  </si>
+  <si>
+    <t>Automated update on complete Organization contact</t>
+  </si>
+  <si>
+    <t>Update minimum Organization contact</t>
+  </si>
+  <si>
+    <t>Gral. Manuel Baquedano 079</t>
+  </si>
+  <si>
+    <t>(236) 900-7000</t>
+  </si>
+  <si>
+    <t>Section6ExpropriationSelect12</t>
+  </si>
+  <si>
+    <t>Automated Research File Creation - File Details</t>
+  </si>
+  <si>
+    <t>Devin Smith (MoTI Solicitor)</t>
   </si>
 </sst>
 </file>
@@ -4916,19 +4940,19 @@
         <v>619</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>175</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>176</v>
@@ -4967,13 +4991,13 @@
         <v>201</v>
       </c>
       <c r="H2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I2" t="s">
         <v>1058</v>
       </c>
-      <c r="I2" t="s">
-        <v>1061</v>
-      </c>
       <c r="J2" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>205</v>
@@ -5012,7 +5036,7 @@
         <v>202</v>
       </c>
       <c r="H3" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>205</v>
@@ -5051,7 +5075,7 @@
         <v>203</v>
       </c>
       <c r="I4" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>205</v>
@@ -5090,7 +5114,7 @@
         <v>204</v>
       </c>
       <c r="J5" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>205</v>
@@ -5335,7 +5359,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5371,7 +5395,7 @@
         <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1356</v>
+        <v>1351</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>307</v>
@@ -5416,21 +5440,21 @@
         <v>329</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>1355</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1357</v>
+        <v>1352</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>1488</v>
       </c>
       <c r="C2" t="s">
         <v>275</v>
       </c>
       <c r="E2" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="F2" t="s">
         <v>276</v>
@@ -5463,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>1361</v>
+        <v>1356</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5477,10 +5501,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1358</v>
+        <v>1353</v>
       </c>
       <c r="B3" t="s">
-        <v>1395</v>
+        <v>1390</v>
       </c>
       <c r="C3" t="s">
         <v>273</v>
@@ -5505,10 +5529,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1397</v>
+        <v>1392</v>
       </c>
       <c r="B4" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
       <c r="C4" t="s">
         <v>273</v>
@@ -5530,16 +5554,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1360</v>
+        <v>1355</v>
       </c>
       <c r="B5" t="s">
-        <v>1396</v>
+        <v>1391</v>
       </c>
       <c r="C5" t="s">
         <v>274</v>
       </c>
       <c r="E5" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="G5" t="s">
         <v>282</v>
@@ -5571,10 +5595,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1359</v>
+        <v>1354</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>1390</v>
       </c>
       <c r="C6" t="s">
         <v>273</v>
@@ -5610,7 +5634,7 @@
         <v>199</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="F7" t="s">
         <v>361</v>
@@ -5981,7 +6005,7 @@
         <v>922</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>861</v>
@@ -6014,7 +6038,7 @@
         <v>868</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>870</v>
@@ -6032,54 +6056,54 @@
         <v>899</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>1126</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>1130</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>314</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
       <c r="B2" t="s">
         <v>879</v>
@@ -6091,10 +6115,10 @@
         <v>873</v>
       </c>
       <c r="E2" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F2" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G2" t="s">
         <v>877</v>
@@ -6107,7 +6131,7 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="M2" t="s">
         <v>876</v>
@@ -6137,10 +6161,10 @@
         <v>900</v>
       </c>
       <c r="V2" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W2" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X2">
         <v>17</v>
@@ -6184,29 +6208,29 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
       <c r="B3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C3" s="14">
         <v>5500001</v>
       </c>
       <c r="D3" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E3" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="F3" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="G3" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45225</v>
+        <v>45231</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -6215,7 +6239,7 @@
         <v>45352</v>
       </c>
       <c r="L3" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
       <c r="O3" t="s">
         <v>944</v>
@@ -6239,10 +6263,10 @@
         <v>354</v>
       </c>
       <c r="V3" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="W3" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="X3">
         <v>18</v>
@@ -6286,7 +6310,7 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
       <c r="B4" t="s">
         <v>273</v>
@@ -6298,10 +6322,10 @@
         <v>873</v>
       </c>
       <c r="E4" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F4" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G4" t="s">
         <v>877</v>
@@ -6314,7 +6338,7 @@
       </c>
       <c r="K4" s="4"/>
       <c r="L4" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
       <c r="M4" t="s">
         <v>876</v>
@@ -6344,10 +6368,10 @@
         <v>900</v>
       </c>
       <c r="V4" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W4" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X4">
         <v>17</v>
@@ -6391,29 +6415,29 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1410</v>
+        <v>1405</v>
       </c>
       <c r="B5" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C5" s="14">
         <v>5500001</v>
       </c>
       <c r="D5" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E5" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="F5" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="G5" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45225</v>
+        <v>45231</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -6422,7 +6446,7 @@
         <v>45352</v>
       </c>
       <c r="L5" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
       <c r="O5" t="s">
         <v>944</v>
@@ -6446,10 +6470,10 @@
         <v>354</v>
       </c>
       <c r="V5" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="W5" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="X5">
         <v>18</v>
@@ -6493,7 +6517,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
       <c r="B6" t="s">
         <v>273</v>
@@ -6505,10 +6529,10 @@
         <v>873</v>
       </c>
       <c r="E6" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F6" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G6" t="s">
         <v>877</v>
@@ -6521,7 +6545,7 @@
       </c>
       <c r="K6" s="4"/>
       <c r="L6" t="s">
-        <v>1411</v>
+        <v>1406</v>
       </c>
       <c r="M6" t="s">
         <v>876</v>
@@ -6551,10 +6575,10 @@
         <v>900</v>
       </c>
       <c r="V6" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W6" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X6">
         <v>17</v>
@@ -6598,7 +6622,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
       <c r="B7" t="s">
         <v>273</v>
@@ -6607,20 +6631,20 @@
         <v>5500001</v>
       </c>
       <c r="D7" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E7" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="F7" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="G7" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45225</v>
+        <v>45231</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -6629,7 +6653,7 @@
         <v>45352</v>
       </c>
       <c r="L7" t="s">
-        <v>1430</v>
+        <v>1425</v>
       </c>
       <c r="O7" t="s">
         <v>944</v>
@@ -6653,10 +6677,10 @@
         <v>354</v>
       </c>
       <c r="V7" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="W7" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="X7">
         <v>18</v>
@@ -6700,7 +6724,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
       <c r="B8" t="s">
         <v>273</v>
@@ -6712,10 +6736,10 @@
         <v>873</v>
       </c>
       <c r="E8" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F8" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G8" t="s">
         <v>877</v>
@@ -6728,7 +6752,7 @@
       </c>
       <c r="K8" s="4"/>
       <c r="L8" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="M8" t="s">
         <v>876</v>
@@ -6758,10 +6782,10 @@
         <v>900</v>
       </c>
       <c r="V8" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W8" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X8">
         <v>17</v>
@@ -6805,7 +6829,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1414</v>
+        <v>1409</v>
       </c>
       <c r="B9" t="s">
         <v>273</v>
@@ -6817,10 +6841,10 @@
         <v>873</v>
       </c>
       <c r="E9" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F9" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G9" t="s">
         <v>877</v>
@@ -6833,7 +6857,7 @@
       </c>
       <c r="K9" s="4"/>
       <c r="L9" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
       <c r="M9" t="s">
         <v>876</v>
@@ -6863,10 +6887,10 @@
         <v>900</v>
       </c>
       <c r="V9" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W9" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X9">
         <v>17</v>
@@ -6910,7 +6934,7 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
       <c r="B10" t="s">
         <v>273</v>
@@ -6922,10 +6946,10 @@
         <v>873</v>
       </c>
       <c r="E10" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F10" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G10" t="s">
         <v>877</v>
@@ -6938,7 +6962,7 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="M10" t="s">
         <v>876</v>
@@ -6968,10 +6992,10 @@
         <v>900</v>
       </c>
       <c r="V10" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W10" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X10">
         <v>17</v>
@@ -7015,7 +7039,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="B11" t="s">
         <v>273</v>
@@ -7027,10 +7051,10 @@
         <v>873</v>
       </c>
       <c r="E11" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F11" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G11" t="s">
         <v>877</v>
@@ -7043,7 +7067,7 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" t="s">
-        <v>1420</v>
+        <v>1415</v>
       </c>
       <c r="M11" t="s">
         <v>876</v>
@@ -7073,10 +7097,10 @@
         <v>900</v>
       </c>
       <c r="V11" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W11" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X11">
         <v>17</v>
@@ -7120,29 +7144,29 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="B12" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C12" s="14">
         <v>5500001</v>
       </c>
       <c r="D12" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E12" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="F12" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="G12" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45225</v>
+        <v>45231</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -7151,7 +7175,7 @@
         <v>45352</v>
       </c>
       <c r="L12" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
       <c r="O12" t="s">
         <v>944</v>
@@ -7175,10 +7199,10 @@
         <v>354</v>
       </c>
       <c r="V12" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="W12" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="X12">
         <v>18</v>
@@ -7222,7 +7246,7 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
       <c r="B13" t="s">
         <v>273</v>
@@ -7234,10 +7258,10 @@
         <v>873</v>
       </c>
       <c r="E13" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F13" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G13" t="s">
         <v>877</v>
@@ -7250,7 +7274,7 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
       <c r="M13" t="s">
         <v>876</v>
@@ -7280,10 +7304,10 @@
         <v>900</v>
       </c>
       <c r="V13" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W13" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X13">
         <v>17</v>
@@ -7327,7 +7351,7 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1424</v>
+        <v>1419</v>
       </c>
       <c r="B14" t="s">
         <v>273</v>
@@ -7339,10 +7363,10 @@
         <v>873</v>
       </c>
       <c r="E14" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="F14" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="G14" t="s">
         <v>877</v>
@@ -7355,7 +7379,7 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="M14" t="s">
         <v>876</v>
@@ -7385,10 +7409,10 @@
         <v>900</v>
       </c>
       <c r="V14" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="W14" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="X14">
         <v>17</v>
@@ -7432,7 +7456,7 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
       <c r="B15" t="s">
         <v>273</v>
@@ -7441,20 +7465,20 @@
         <v>5500001</v>
       </c>
       <c r="D15" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E15" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="F15" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="G15" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45225</v>
+        <v>45231</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -7463,7 +7487,7 @@
         <v>45352</v>
       </c>
       <c r="L15" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
       <c r="O15" t="s">
         <v>944</v>
@@ -7487,10 +7511,10 @@
         <v>354</v>
       </c>
       <c r="V15" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="W15" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="X15">
         <v>18</v>
@@ -7534,13 +7558,13 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="B16" t="s">
         <v>273</v>
       </c>
       <c r="L16" t="s">
-        <v>1431</v>
+        <v>1426</v>
       </c>
       <c r="O16" t="s">
         <v>944</v>
@@ -7561,13 +7585,13 @@
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
       <c r="V16" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
       <c r="W16" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
       <c r="X16">
         <v>17</v>
@@ -7611,13 +7635,13 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="B17" t="s">
         <v>273</v>
       </c>
       <c r="L17" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
       <c r="O17" t="s">
         <v>918</v>
@@ -7919,35 +7943,35 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="B8" t="s">
         <v>884</v>
       </c>
       <c r="C8" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="B9" t="s">
         <v>945</v>
       </c>
       <c r="C9" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="B10" t="s">
         <v>884</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
     </row>
   </sheetData>
@@ -8172,7 +8196,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="B5" t="s">
         <v>753</v>
@@ -8181,16 +8205,16 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="E5" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="J5" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="K5" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="M5" t="s">
         <v>36</v>
@@ -8202,10 +8226,10 @@
         <v>37</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="S5">
         <v>7896778787</v>
@@ -8213,7 +8237,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -8222,22 +8246,22 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1232</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1233</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1234</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1236</v>
+      </c>
+      <c r="N6" t="s">
         <v>1235</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1236</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1237</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1238</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1240</v>
-      </c>
-      <c r="N6" t="s">
-        <v>1239</v>
       </c>
       <c r="O6" t="s">
         <v>20</v>
@@ -8246,7 +8270,7 @@
         <v>19706</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="S6">
         <v>7780991098</v>
@@ -8254,7 +8278,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="B7" t="s">
         <v>753</v>
@@ -8266,13 +8290,13 @@
         <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
       <c r="J7" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
       <c r="K7" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
       <c r="M7" t="s">
         <v>72</v>
@@ -8284,10 +8308,10 @@
         <v>37</v>
       </c>
       <c r="Q7" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="S7">
         <v>7089090655</v>
@@ -8311,8 +8335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD9027E-311F-43F3-971B-D6244D52A1F4}">
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AR2" sqref="AR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8323,10 +8347,9 @@
     <col min="16" max="23" width="28.36328125" bestFit="1" customWidth="1"/>
     <col min="24" max="26" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="27" max="35" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="45" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.54296875" customWidth="1"/>
+    <col min="36" max="44" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="26.54296875" customWidth="1"/>
     <col min="48" max="48" width="27.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8335,288 +8358,288 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1074</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1075</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1076</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1077</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1078</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1079</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1080</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1081</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1082</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1083</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1084</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1085</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1086</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1087</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1088</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1089</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1090</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>1091</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>1092</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>1093</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1094</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1095</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1096</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1097</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1098</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1099</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1100</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1102</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1103</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1104</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="AV1" s="3" t="s">
         <v>1105</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>1106</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>1107</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>1108</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>1115</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>1116</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>1117</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>1118</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>1119</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>1120</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>1121</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>1122</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>1123</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>1125</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="B2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="C2" t="s">
         <v>755</v>
       </c>
       <c r="D2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="E2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="F2" t="s">
         <v>755</v>
       </c>
       <c r="G2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="H2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="I2" t="s">
         <v>755</v>
       </c>
       <c r="J2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="K2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="L2" t="s">
         <v>755</v>
       </c>
       <c r="M2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="N2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="O2" t="s">
         <v>755</v>
       </c>
       <c r="P2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="Q2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="R2" t="s">
         <v>755</v>
       </c>
       <c r="S2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="T2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="U2" t="s">
         <v>755</v>
       </c>
       <c r="V2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="W2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="X2" t="s">
         <v>755</v>
       </c>
       <c r="Y2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="Z2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="AA2" t="s">
         <v>755</v>
       </c>
       <c r="AB2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="AC2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="AD2" t="s">
         <v>755</v>
       </c>
       <c r="AE2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="AF2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="AG2" t="s">
         <v>755</v>
       </c>
       <c r="AH2" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="AI2" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="AJ2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AL2" t="s">
         <v>755</v>
       </c>
-      <c r="AK2" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>1111</v>
-      </c>
       <c r="AM2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AO2" t="s">
         <v>755</v>
       </c>
-      <c r="AN2" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>1111</v>
-      </c>
       <c r="AP2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AR2" t="s">
         <v>755</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>1111</v>
-      </c>
       <c r="AS2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AU2" t="s">
         <v>755</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>1112</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>1111</v>
       </c>
       <c r="AV2" t="s">
         <v>755</v>
@@ -8624,22 +8647,22 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="B3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C3" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="X3" t="s">
-        <v>1111</v>
-      </c>
-      <c r="AL3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AK3" t="s">
         <v>755</v>
       </c>
       <c r="AV3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
     </row>
   </sheetData>
@@ -8677,48 +8700,48 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1134</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1135</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1136</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1137</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>1147</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1138</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1139</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1141</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="B2" t="s">
         <v>569</v>
       </c>
       <c r="C2" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="D2" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="E2" s="4">
         <v>44440</v>
@@ -8741,16 +8764,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="B3" t="s">
         <v>569</v>
       </c>
       <c r="C3" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="D3" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="E3" s="4">
         <v>44806</v>
@@ -8773,16 +8796,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="B4" t="s">
         <v>569</v>
       </c>
       <c r="C4" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="D4" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="E4" s="4">
         <v>44809</v>
@@ -8805,16 +8828,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="B5" t="s">
         <v>572</v>
       </c>
       <c r="C5" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="D5" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="E5" s="4">
         <v>44810</v>
@@ -8840,16 +8863,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="B6" t="s">
         <v>569</v>
       </c>
       <c r="C6" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="D6" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="E6" s="4">
         <v>44811</v>
@@ -8872,16 +8895,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="B7" t="s">
         <v>569</v>
       </c>
       <c r="C7" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="D7" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="E7" s="4">
         <v>44819</v>
@@ -8932,45 +8955,45 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>750</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B2" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="F2" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="G2" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -8978,22 +9001,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B3" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C3" t="s">
         <v>753</v>
       </c>
       <c r="E3" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="G3" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -9001,22 +9024,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B4" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="F4" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="G4" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -9024,22 +9047,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B5" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C5" t="s">
         <v>753</v>
       </c>
       <c r="E5" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="G5" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -9047,22 +9070,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B6" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C6" t="s">
         <v>753</v>
       </c>
       <c r="E6" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="G6" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="H6">
         <v>4</v>
@@ -9070,16 +9093,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B7" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -9087,16 +9110,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B8" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -9104,16 +9127,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B9" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C9" t="s">
         <v>753</v>
       </c>
       <c r="D9" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -9121,16 +9144,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B10" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C10" t="s">
         <v>753</v>
       </c>
       <c r="D10" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="H10">
         <v>3</v>
@@ -9138,16 +9161,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B11" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C11" t="s">
         <v>753</v>
       </c>
       <c r="D11" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -9155,16 +9178,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="B12" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C12" t="s">
         <v>753</v>
       </c>
       <c r="D12" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -9172,22 +9195,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="B13" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="F13" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="G13" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -9195,16 +9218,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="B14" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -9212,22 +9235,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="B15" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C15" t="s">
         <v>753</v>
       </c>
       <c r="E15" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="F15" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="G15" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -9245,8 +9268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CC3795-F36B-4D0F-8244-A4F4C3935686}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9279,69 +9302,69 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>1257</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>1191</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1252</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1192</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1193</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>1194</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1195</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1196</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1197</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1198</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1199</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>1261</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1201</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>1202</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>1203</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>1204</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="B2">
         <v>1256918.8700000001</v>
@@ -9356,7 +9379,7 @@
         <v>569</v>
       </c>
       <c r="F2" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="G2" s="4">
         <v>45176</v>
@@ -9368,22 +9391,22 @@
         <v>45149</v>
       </c>
       <c r="J2" t="s">
+        <v>1213</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1214</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1216</v>
+      </c>
+      <c r="N2" t="s">
         <v>1217</v>
       </c>
-      <c r="K2" t="s">
-        <v>1218</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1219</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1220</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1221</v>
-      </c>
       <c r="O2" t="s">
-        <v>1353</v>
+        <v>1489</v>
       </c>
       <c r="P2" t="s">
         <v>278</v>
@@ -9395,7 +9418,7 @@
         <v>12345</v>
       </c>
       <c r="S2" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="T2">
         <v>1</v>
@@ -9406,7 +9429,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="E3" t="s">
         <v>572</v>
@@ -9415,7 +9438,7 @@
         <v>45178</v>
       </c>
       <c r="J3" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="Q3" t="b">
         <v>0</v>
@@ -9955,27 +9978,27 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1206</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1207</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1208</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1210</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="B2" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="C2">
         <v>128.88999999999999</v>
@@ -9992,10 +10015,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="B3" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="C3">
         <v>1200000</v>
@@ -10009,10 +10032,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="B4" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C4">
         <v>56789.98</v>
@@ -10029,10 +10052,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="B5" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="C5">
         <v>1000</v>
@@ -10074,39 +10097,39 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1433</v>
+        <v>1428</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1480</v>
+        <v>1475</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1434</v>
+        <v>1429</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1435</v>
+        <v>1430</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B2" t="s">
         <v>1454</v>
       </c>
-      <c r="B2" t="s">
-        <v>1459</v>
-      </c>
       <c r="C2" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
       <c r="D2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E2" t="s">
         <v>1463</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1468</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -10117,19 +10140,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="B3" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="C3" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
       <c r="D3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E3" t="s">
         <v>1464</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1469</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -10140,19 +10163,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="B4" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="C4" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="D4" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="E4" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -10163,19 +10186,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="B5" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="C5" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="D5" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
       <c r="E5" t="s">
-        <v>1472</v>
+        <v>1467</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -10193,7 +10216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9467DD6-431B-4487-B73A-065D683A7274}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -10212,27 +10235,27 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1473</v>
+        <v>1468</v>
       </c>
       <c r="B2" t="s">
-        <v>1476</v>
+        <v>1471</v>
       </c>
       <c r="C2" s="11">
         <v>78990</v>
@@ -10249,10 +10272,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1473</v>
+        <v>1468</v>
       </c>
       <c r="B3" t="s">
-        <v>1477</v>
+        <v>1472</v>
       </c>
       <c r="C3" s="11">
         <v>789.39</v>
@@ -10269,10 +10292,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B4" t="s">
         <v>1473</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1478</v>
       </c>
       <c r="C4" s="11">
         <v>2000</v>
@@ -10289,10 +10312,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1474</v>
+        <v>1469</v>
       </c>
       <c r="B5" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="C5" s="11">
         <v>8989.8700000000008</v>
@@ -10309,10 +10332,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1475</v>
+        <v>1470</v>
       </c>
       <c r="B6" t="s">
-        <v>1479</v>
+        <v>1474</v>
       </c>
       <c r="C6" s="11">
         <v>1800.48</v>
@@ -10338,7 +10361,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10412,7 +10435,7 @@
         <v>374</v>
       </c>
       <c r="B3" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="C3">
         <v>2000000</v>
@@ -10477,13 +10500,13 @@
         <v>442</v>
       </c>
       <c r="B10" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="C10">
         <v>90077451</v>
       </c>
       <c r="D10" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -10527,7 +10550,7 @@
         <v>824</v>
       </c>
       <c r="B14" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -10559,7 +10582,7 @@
         <v>901</v>
       </c>
       <c r="B18" t="s">
-        <v>1354</v>
+        <v>1349</v>
       </c>
       <c r="C18">
         <v>90077451</v>
@@ -10568,10 +10591,10 @@
         <v>902</v>
       </c>
       <c r="E18" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="F18" t="s">
-        <v>1429</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -10611,26 +10634,26 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B23" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="B24" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="B25" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
     </row>
   </sheetData>
@@ -10809,7 +10832,7 @@
         <v>385</v>
       </c>
       <c r="P3" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="Q3" t="s">
         <v>303</v>
@@ -10900,7 +10923,7 @@
         <v>941</v>
       </c>
       <c r="R5" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="T5">
         <v>89.87</v>
@@ -10959,103 +10982,103 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1362</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1363</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1364</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1365</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1366</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1367</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1368</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1369</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1370</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1371</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1372</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1373</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1374</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>1375</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>1376</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>1377</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>1378</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>1379</v>
-      </c>
       <c r="T1" s="3" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>814</v>
       </c>
       <c r="C2" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="D2" t="s">
         <v>301</v>
       </c>
       <c r="E2" t="s">
-        <v>1385</v>
+        <v>1380</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="K2" t="s">
-        <v>1389</v>
+        <v>1384</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="4">
         <v>36841</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="O2" s="6"/>
       <c r="Q2" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="R2" s="6"/>
       <c r="S2">
@@ -11067,10 +11090,10 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="B3" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="C3" t="s">
         <v>574</v>
@@ -11079,25 +11102,25 @@
         <v>341</v>
       </c>
       <c r="E3" t="s">
-        <v>1386</v>
+        <v>1381</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="G3" s="6">
         <v>1200</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="I3" s="6">
         <v>1178</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="K3" t="s">
-        <v>1390</v>
+        <v>1385</v>
       </c>
       <c r="L3" s="6">
         <v>3207</v>
@@ -11106,7 +11129,7 @@
         <v>39077</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="O3" s="6">
         <v>1289.99</v>
@@ -11115,7 +11138,7 @@
         <v>45408</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="R3" s="6">
         <v>1335.88</v>
@@ -11129,41 +11152,41 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="B4" t="s">
         <v>814</v>
       </c>
       <c r="C4" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="D4" t="s">
         <v>299</v>
       </c>
       <c r="E4" t="s">
-        <v>1388</v>
+        <v>1383</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="G4" s="6">
         <v>1604</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="4"/>
       <c r="N4" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="O4" s="6"/>
       <c r="Q4" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="R4" s="6">
         <v>2566.66</v>
@@ -11177,40 +11200,40 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="B5" t="s">
         <v>814</v>
       </c>
       <c r="C5" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="D5" t="s">
         <v>301</v>
       </c>
       <c r="E5" t="s">
-        <v>1393</v>
+        <v>1388</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="I5" s="6">
         <v>1888.88</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="L5" s="6"/>
       <c r="N5" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="O5" s="6"/>
       <c r="Q5" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5">
@@ -11222,10 +11245,10 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="B6" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="C6" t="s">
         <v>574</v>
@@ -11234,34 +11257,34 @@
         <v>341</v>
       </c>
       <c r="E6" t="s">
-        <v>1394</v>
+        <v>1389</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="G6" s="6">
         <v>2205.3000000000002</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="K6" t="s">
-        <v>1391</v>
+        <v>1386</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="4">
         <v>45147</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="O6" s="6"/>
       <c r="Q6" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="R6" s="6"/>
       <c r="S6">
@@ -11273,36 +11296,36 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1387</v>
+        <v>1382</v>
       </c>
       <c r="B7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="C7" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="D7" t="s">
         <v>301</v>
       </c>
       <c r="E7" t="s">
-        <v>1392</v>
+        <v>1387</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="G7" s="6">
         <v>3800.9</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="15" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="L7" s="6"/>
       <c r="N7" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="O7" s="6">
         <v>8790.7900000000009</v>
@@ -11311,7 +11334,7 @@
         <v>39270</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="R7" s="6">
         <v>9000</v>
@@ -11478,7 +11501,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="B13">
         <v>65</v>
@@ -12605,7 +12628,7 @@
         <v>959</v>
       </c>
       <c r="AS51" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="52" spans="1:47" x14ac:dyDescent="0.35">
@@ -12845,7 +12868,7 @@
         <v>678998</v>
       </c>
       <c r="AS63" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="64" spans="1:47" x14ac:dyDescent="0.35">
@@ -12887,7 +12910,7 @@
         <v>568</v>
       </c>
       <c r="AS66" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
     </row>
   </sheetData>
@@ -13045,10 +13068,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW7"/>
+  <dimension ref="A1:AW9"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13072,14 +13095,15 @@
     <col min="18" max="18" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.453125" customWidth="1"/>
-    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.453125" bestFit="1" customWidth="1"/>
@@ -13124,127 +13148,127 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1262</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1263</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1264</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1265</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1266</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1267</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1268</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1269</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1270</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>1271</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>1272</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>1273</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1274</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1275</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1276</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1277</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1278</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1279</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1280</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1282</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1283</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1284</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>1285</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>1286</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>1287</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>1288</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>1289</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>1290</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>1291</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>1292</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>1293</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>1294</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>1295</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>1296</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>1297</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>1298</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>1299</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>1300</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>1301</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.35">
@@ -13389,156 +13413,49 @@
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" t="s">
-        <v>382</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" t="s">
-        <v>89</v>
-      </c>
-      <c r="N3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>101</v>
-      </c>
+        <v>1035</v>
+      </c>
+      <c r="L3" s="1"/>
       <c r="R3" t="s">
-        <v>57</v>
+        <v>1486</v>
       </c>
       <c r="S3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T3" t="s">
-        <v>120</v>
-      </c>
-      <c r="U3" t="s">
-        <v>53</v>
-      </c>
-      <c r="X3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD3">
-        <v>3500</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM3">
-        <v>10089</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>118</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="AW3" t="s">
-        <v>48</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
       </c>
       <c r="G4" t="s">
         <v>121</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>382</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s">
         <v>90</v>
@@ -13546,126 +13463,134 @@
       <c r="K4" t="s">
         <v>101</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" t="s">
+        <v>100</v>
+      </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="P4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="Q4" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+      <c r="R4" t="s">
+        <v>57</v>
+      </c>
+      <c r="S4" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" t="s">
+        <v>120</v>
       </c>
       <c r="U4" t="s">
-        <v>35</v>
-      </c>
-      <c r="V4" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="X4" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="Y4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="AA4" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="AB4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4">
+        <v>3500</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4">
+        <v>10089</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>45</v>
       </c>
       <c r="AW4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J5" t="s">
-        <v>90</v>
-      </c>
-      <c r="K5" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="M5" t="s">
-        <v>89</v>
-      </c>
-      <c r="N5" t="s">
-        <v>100</v>
-      </c>
-      <c r="O5" t="s">
-        <v>151</v>
-      </c>
-      <c r="P5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>119</v>
-      </c>
-      <c r="R5" t="s">
-        <v>152</v>
-      </c>
-      <c r="S5" t="s">
-        <v>93</v>
-      </c>
-      <c r="T5" t="s">
-        <v>120</v>
-      </c>
-      <c r="U5" t="s">
-        <v>153</v>
-      </c>
-      <c r="V5" t="s">
-        <v>154</v>
-      </c>
-      <c r="X5" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>157</v>
+        <v>1478</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="AE5" t="s">
+        <v>1485</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM5">
+        <v>10089</v>
       </c>
       <c r="AW5" t="s">
-        <v>158</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1035</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
         <v>146</v>
@@ -13676,14 +13601,11 @@
       <c r="E6" t="s">
         <v>148</v>
       </c>
-      <c r="F6" t="s">
-        <v>1036</v>
-      </c>
       <c r="G6" t="s">
         <v>121</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1037</v>
+        <v>149</v>
       </c>
       <c r="J6" t="s">
         <v>90</v>
@@ -13691,9 +13613,26 @@
       <c r="K6" t="s">
         <v>101</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" t="s">
+        <v>151</v>
+      </c>
+      <c r="P6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>119</v>
+      </c>
       <c r="R6" t="s">
-        <v>1038</v>
+        <v>152</v>
       </c>
       <c r="S6" t="s">
         <v>93</v>
@@ -13702,10 +13641,10 @@
         <v>120</v>
       </c>
       <c r="U6" t="s">
-        <v>1039</v>
+        <v>153</v>
       </c>
       <c r="V6" t="s">
-        <v>1040</v>
+        <v>154</v>
       </c>
       <c r="X6" t="s">
         <v>155</v>
@@ -13726,32 +13665,148 @@
         <v>157</v>
       </c>
       <c r="AW6" t="s">
-        <v>1041</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="R7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="S7" t="s">
+        <v>93</v>
+      </c>
+      <c r="T7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>1037</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>1038</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>119</v>
+      </c>
+      <c r="U8" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" t="s">
+        <v>106</v>
+      </c>
+      <c r="X8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>145</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>159</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>160</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E9" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{16C12AA1-ECCE-499E-9396-FFC7128B9E7E}"/>
     <hyperlink ref="I2" r:id="rId2" xr:uid="{3E5C643A-012D-4079-8C9C-CE03A2BB44C0}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{1CC1FCEE-4D1F-4BC0-B831-33526F37CA9E}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{749E9344-8D93-4BC6-9B68-CC2E0927EBF0}"/>
-    <hyperlink ref="I5" r:id="rId5" xr:uid="{3BF8C400-BAC1-4978-8D41-326CBC17576E}"/>
-    <hyperlink ref="L5" r:id="rId6" xr:uid="{9CA6DE06-BA42-496F-902B-6B9113678CE6}"/>
-    <hyperlink ref="I6" r:id="rId7" xr:uid="{B25FEFEA-0800-4243-A177-1E1D3B4F1661}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{1CC1FCEE-4D1F-4BC0-B831-33526F37CA9E}"/>
+    <hyperlink ref="I4" r:id="rId4" xr:uid="{749E9344-8D93-4BC6-9B68-CC2E0927EBF0}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{3BF8C400-BAC1-4978-8D41-326CBC17576E}"/>
+    <hyperlink ref="L6" r:id="rId6" xr:uid="{9CA6DE06-BA42-496F-902B-6B9113678CE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13759,17 +13814,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC9B3A8-42C1-4A9C-B1C1-5E5E07CE0539}">
-  <dimension ref="A1:AT6"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1"/>
@@ -13828,127 +13883,127 @@
         <v>618</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>1303</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1304</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1305</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1306</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1307</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1308</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1309</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1310</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1311</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1312</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1313</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1314</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>1315</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>1316</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>1317</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1318</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1319</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1320</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1323</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1324</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1325</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1326</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1327</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1328</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>1329</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>1330</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>1331</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>1332</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>1333</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>1334</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>1335</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>1336</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>1337</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>1338</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>1339</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>1340</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>1341</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.35">
@@ -14084,55 +14139,31 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
+        <v>1480</v>
       </c>
       <c r="E3" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="J3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1482</v>
+      </c>
+      <c r="M3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" t="s">
         <v>101</v>
       </c>
-      <c r="L3" t="s">
-        <v>88</v>
-      </c>
-      <c r="M3" t="s">
-        <v>94</v>
-      </c>
-      <c r="N3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R3" t="s">
-        <v>83</v>
-      </c>
-      <c r="U3" t="s">
-        <v>84</v>
-      </c>
-      <c r="V3" t="s">
-        <v>85</v>
-      </c>
-      <c r="W3" t="s">
-        <v>86</v>
-      </c>
-      <c r="X3" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA3">
-        <v>33323</v>
-      </c>
       <c r="AT3" t="s">
-        <v>81</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.35">
@@ -14140,7 +14171,7 @@
         <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="E4" t="s">
         <v>121</v>
@@ -14208,23 +14239,23 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D5" t="s">
         <v>1045</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1048</v>
       </c>
       <c r="E5" t="s">
         <v>121</v>
       </c>
       <c r="F5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="J5" t="s">
         <v>89</v>
@@ -14233,7 +14264,7 @@
         <v>100</v>
       </c>
       <c r="L5" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="M5" t="s">
         <v>94</v>
@@ -14242,10 +14273,10 @@
         <v>103</v>
       </c>
       <c r="AB5" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="AC5" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="AE5" t="s">
         <v>43</v>
@@ -14260,17 +14291,70 @@
         <v>44</v>
       </c>
       <c r="AJ5" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="AT5" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N6" t="s">
+        <v>103</v>
+      </c>
+      <c r="R6" t="s">
+        <v>83</v>
+      </c>
+      <c r="U6" t="s">
+        <v>84</v>
+      </c>
+      <c r="V6" t="s">
+        <v>85</v>
+      </c>
+      <c r="W6" t="s">
+        <v>86</v>
+      </c>
+      <c r="X6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6">
+        <v>33323</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>162</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>163</v>
       </c>
     </row>
@@ -14278,13 +14362,14 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{EABDD7EF-9E20-4FD0-91D9-4DE7B815FF35}"/>
     <hyperlink ref="I2" r:id="rId2" xr:uid="{A0A05DFE-6C79-4ADA-B136-085505F633B4}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{7537BC25-0749-4A34-9FD8-9F423E0202C6}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{7537BC25-0749-4A34-9FD8-9F423E0202C6}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{4078AD70-0085-443C-BDA0-BD2ECBB8DD3B}"/>
     <hyperlink ref="I4" r:id="rId5" xr:uid="{ED87B454-F8FB-4903-82F0-44C2BB74A551}"/>
     <hyperlink ref="I5" r:id="rId6" xr:uid="{C2EB0E13-A168-49C4-8001-C198483226AD}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{30233657-0EC2-4B08-BA0D-0862260E6F8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -14292,8 +14377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CC7"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14628,10 +14713,10 @@
         <v>692</v>
       </c>
       <c r="B2" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="C2" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="D2" t="s">
         <v>569</v>
@@ -15326,7 +15411,7 @@
         <v>753</v>
       </c>
       <c r="C2" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="D2" t="s">
         <v>755</v>

</xml_diff>

<commit_message>
Automation refactoring to update new modals and typehead fields
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CECA63-B8BF-43B5-A336-B2BF304FD057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC88636-CB28-4750-B6F6-03A54350E6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="934" firstSheet="12" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="934" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -5006,7 +5006,7 @@
         <v>191</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE(C2," ",B2)</f>
+        <f t="shared" ref="D2:D8" si="0">CONCATENATE(C2," ",B2)</f>
         <v>AU-0002 Automation Project 02</v>
       </c>
       <c r="E2" t="s">
@@ -5045,7 +5045,7 @@
         <v>192</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE(C3," ",B3)</f>
+        <f t="shared" si="0"/>
         <v>AU-0003 Automation Project 03</v>
       </c>
       <c r="E3" t="s">
@@ -5084,7 +5084,7 @@
         <v>193</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE(C4," ",B4)</f>
+        <f t="shared" si="0"/>
         <v>AU-0004 Automation Project 04</v>
       </c>
       <c r="E4" t="s">
@@ -5123,7 +5123,7 @@
         <v>190</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE(C5," ",B5)</f>
+        <f t="shared" si="0"/>
         <v>AU-0001 Automation Project 01</v>
       </c>
       <c r="E5" t="s">
@@ -5168,7 +5168,7 @@
         <v>206</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE(C6," ",B6)</f>
+        <f t="shared" si="0"/>
         <v>UPAU-0001 Automation Project 01</v>
       </c>
       <c r="E6" t="s">
@@ -5204,7 +5204,7 @@
         <v>1488</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE(C7," ",B7)</f>
+        <f t="shared" si="0"/>
         <v>AU-0005 Automation Project 05</v>
       </c>
       <c r="E7" t="s">
@@ -5240,7 +5240,7 @@
         <v>1491</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE(C8," ",B8)</f>
+        <f t="shared" si="0"/>
         <v>AU-0006 Automation Project 06</v>
       </c>
       <c r="E8" t="s">
@@ -5458,8 +5458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3C62D2-095D-41C7-8E12-52D5164F6230}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5551,7 +5551,7 @@
         <v>1471</v>
       </c>
       <c r="C2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E2" t="s">
         <v>1059</v>
@@ -6048,8 +6048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -7269,7 +7269,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -12997,7 +12997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed the disposition bug 7582
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FB010D-B48E-493A-8686-655D89019F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B642EF1A-C48C-4A3D-88FB-3DBFB92738B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="1711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="1712">
   <si>
     <t>FirstName</t>
   </si>
@@ -5205,6 +5205,9 @@
   </si>
   <si>
     <t>SaleInformationSelect6</t>
+  </si>
+  <si>
+    <t>DirectSaleRoadClosureSelect9</t>
   </si>
 </sst>
 </file>
@@ -7024,7 +7027,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7234,7 +7237,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7441,7 +7444,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -7963,7 +7966,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8275,7 +8278,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8859,7 +8862,7 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="D4" s="4">
         <v>45352</v>
@@ -8921,10 +8924,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6959299-8109-4A66-918B-3B215FFD6F08}">
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8934,13 +8937,15 @@
     <col min="6" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="16" width="29.54296875" bestFit="1" customWidth="1"/>
     <col min="17" max="22" width="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="31" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="26.54296875" customWidth="1"/>
-    <col min="35" max="35" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.54296875" customWidth="1"/>
+    <col min="26" max="32" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="26.54296875" customWidth="1"/>
+    <col min="36" max="36" width="27.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -9014,40 +9019,43 @@
         <v>1698</v>
       </c>
       <c r="Y1" s="3" t="s">
+        <v>1711</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>1699</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1700</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1701</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1702</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1703</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1710</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1704</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1705</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1706</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1707</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>1708</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1084</v>
       </c>
@@ -9121,40 +9129,43 @@
         <v>742</v>
       </c>
       <c r="Y2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="Z2" t="s">
         <v>1086</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>1085</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>742</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>1086</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>1085</v>
       </c>
       <c r="AD2" t="s">
         <v>1085</v>
       </c>
       <c r="AE2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="AF2" t="s">
         <v>742</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>1086</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>1085</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>742</v>
       </c>
       <c r="AI2" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1087</v>
       </c>
@@ -9170,11 +9181,11 @@
       <c r="W3" t="s">
         <v>742</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>1086</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1590</v>
       </c>
@@ -9247,9 +9258,6 @@
       <c r="X4" t="s">
         <v>1085</v>
       </c>
-      <c r="Y4" t="s">
-        <v>1085</v>
-      </c>
       <c r="Z4" t="s">
         <v>1085</v>
       </c>
@@ -9278,6 +9286,9 @@
         <v>1085</v>
       </c>
       <c r="AI4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>1085</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Offers and sales tab automation
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9843A973-8EFC-4930-9811-366DCD96E162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4771DE-12AB-484F-81A5-2CA1710B90E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,28 +27,29 @@
     <sheet name="PropertyResearch" sheetId="9" r:id="rId12"/>
     <sheet name="AcquisitionFiles" sheetId="19" r:id="rId13"/>
     <sheet name="DispositionFiles" sheetId="34" r:id="rId14"/>
-    <sheet name="AcquisitionTeams" sheetId="20" r:id="rId15"/>
-    <sheet name="AcquisitionOwners" sheetId="21" r:id="rId16"/>
-    <sheet name="AcquisitionChecklist" sheetId="22" r:id="rId17"/>
-    <sheet name="AcquisitionAgreement" sheetId="23" r:id="rId18"/>
-    <sheet name="AcquisitionStakeholder" sheetId="24" r:id="rId19"/>
-    <sheet name="AcquisitionCompensation" sheetId="25" r:id="rId20"/>
-    <sheet name="CompensationActivities" sheetId="26" r:id="rId21"/>
-    <sheet name="AcquisitionExpropriationForm8" sheetId="28" r:id="rId22"/>
-    <sheet name="ExpropriationPayment" sheetId="29" r:id="rId23"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId24"/>
-    <sheet name="Properties" sheetId="6" r:id="rId25"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId26"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId27"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId28"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId29"/>
-    <sheet name="Takes" sheetId="27" r:id="rId30"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId31"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId32"/>
-    <sheet name="Notes" sheetId="10" r:id="rId33"/>
+    <sheet name="DispositionOfferSale" sheetId="35" r:id="rId15"/>
+    <sheet name="AcquisitionTeams" sheetId="20" r:id="rId16"/>
+    <sheet name="AcquisitionOwners" sheetId="21" r:id="rId17"/>
+    <sheet name="AcquisitionChecklist" sheetId="22" r:id="rId18"/>
+    <sheet name="AcquisitionAgreement" sheetId="23" r:id="rId19"/>
+    <sheet name="AcquisitionStakeholder" sheetId="24" r:id="rId20"/>
+    <sheet name="AcquisitionCompensation" sheetId="25" r:id="rId21"/>
+    <sheet name="CompensationActivities" sheetId="26" r:id="rId22"/>
+    <sheet name="AcquisitionExpropriationForm8" sheetId="28" r:id="rId23"/>
+    <sheet name="ExpropriationPayment" sheetId="29" r:id="rId24"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId25"/>
+    <sheet name="Properties" sheetId="6" r:id="rId26"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId27"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId28"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId29"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId30"/>
+    <sheet name="Takes" sheetId="27" r:id="rId31"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId32"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId33"/>
+    <sheet name="Notes" sheetId="10" r:id="rId34"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="1680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2570" uniqueCount="1702">
   <si>
     <t>FirstName</t>
   </si>
@@ -5111,6 +5112,72 @@
   </si>
   <si>
     <t>Amin Devji</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentAppraisalValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentAppraisalDate</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentBcAssessmentValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentBcAssessmentRollYear</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentListPrice</t>
+  </si>
+  <si>
+    <t>OfferOfferStatus</t>
+  </si>
+  <si>
+    <t>OfferOfferName</t>
+  </si>
+  <si>
+    <t>OfferOfferDate</t>
+  </si>
+  <si>
+    <t>OfferOfferExpiryDate</t>
+  </si>
+  <si>
+    <t>OfferPrice</t>
+  </si>
+  <si>
+    <t>OfferNotes</t>
+  </si>
+  <si>
+    <t>Create AppraisalAndAssessment Section</t>
+  </si>
+  <si>
+    <t>Update AppraisalAndAssessment Section</t>
+  </si>
+  <si>
+    <t>Create Offers Section</t>
+  </si>
+  <si>
+    <t>Update Offers Section</t>
+  </si>
+  <si>
+    <t>Basic OffersAndSales Test</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>automated Offer name</t>
+  </si>
+  <si>
+    <t>automated Offer name Updated</t>
+  </si>
+  <si>
+    <t>Test Offer Notes</t>
+  </si>
+  <si>
+    <t>Test Offer Notes Updated</t>
   </si>
 </sst>
 </file>
@@ -5173,7 +5240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5199,6 +5266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6648,8 +6716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6930,7 +6998,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45310</v>
+        <v>45318</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7140,7 +7208,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45310</v>
+        <v>45318</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7347,7 +7415,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45310</v>
+        <v>45318</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -7869,7 +7937,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45310</v>
+        <v>45318</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8181,7 +8249,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45310</v>
+        <v>45318</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8571,7 +8639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -8758,7 +8826,7 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45310</v>
+        <v>45318</v>
       </c>
       <c r="D4" s="4">
         <v>45352</v>
@@ -8815,10 +8883,188 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941E3E0A-6CC8-48F3-AEE4-7C111D1D460B}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1683</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1684</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1685</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1686</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1687</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B2">
+        <v>1000000.99</v>
+      </c>
+      <c r="C2" s="4">
+        <v>45170</v>
+      </c>
+      <c r="D2" s="19">
+        <v>4560</v>
+      </c>
+      <c r="E2" s="19">
+        <v>2024</v>
+      </c>
+      <c r="F2" s="19">
+        <v>4560</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B3">
+        <v>120000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>45192</v>
+      </c>
+      <c r="D3" s="19">
+        <v>5435</v>
+      </c>
+      <c r="E3" s="19">
+        <v>2025</v>
+      </c>
+      <c r="F3" s="19">
+        <v>6500</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>1696</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>1698</v>
+      </c>
+      <c r="I4" s="4">
+        <v>45352</v>
+      </c>
+      <c r="J4" s="4">
+        <v>45427</v>
+      </c>
+      <c r="K4" s="6">
+        <v>550000</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1694</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>1697</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>1699</v>
+      </c>
+      <c r="I5" s="4">
+        <v>45463</v>
+      </c>
+      <c r="J5" s="4">
+        <v>45442</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1200.5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -9002,7 +9248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5453F532-21B6-4188-9011-0BA56E95151F}">
   <dimension ref="A1:S8"/>
   <sheetViews>
@@ -9396,7 +9642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD9027E-311F-43F3-971B-D6244D52A1F4}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
@@ -9883,7 +10129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247DFAE7-4496-4934-B20F-D611E033A94F}">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -10170,363 +10416,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073F58F-6509-4BF3-843F-237D06AC55C6}">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1135</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>737</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1136</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1158</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>740</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1157</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1152</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1143</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1158</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1153</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>740</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1145</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C6" t="s">
-        <v>740</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1147</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1155</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1141</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1142</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C9" t="s">
-        <v>740</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1144</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C10" t="s">
-        <v>740</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1146</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C11" t="s">
-        <v>740</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1148</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>740</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1216</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1217</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1218</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1232</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1419</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C15" t="s">
-        <v>740</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1417</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1418</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>1593</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C16" t="s">
-        <v>740</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1157</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1152</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
-    <sortCondition ref="B2:B11"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11034,6 +10923,363 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073F58F-6509-4BF3-843F-237D06AC55C6}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>740</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>740</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>740</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C10" t="s">
+        <v>740</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1146</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>740</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>740</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1216</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1232</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1419</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C15" t="s">
+        <v>740</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1417</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1418</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C16" t="s">
+        <v>740</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+    <sortCondition ref="B2:B11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CC3795-F36B-4D0F-8244-A4F4C3935686}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -11299,7 +11545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A39253E-76F9-426F-AB51-5E3DB6377515}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -11437,7 +11683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE31339F-895D-48D8-9AD6-CFA457625F2E}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -11599,7 +11845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9467DD6-431B-4487-B73A-065D683A7274}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -11763,7 +12009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -12082,7 +12328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:X5"/>
   <sheetViews>
@@ -12376,7 +12622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -12529,7 +12775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -12636,7 +12882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -12911,7 +13157,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1616</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1617</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45701</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C3" t="s">
+        <v>449</v>
+      </c>
+      <c r="D3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -13024,86 +13349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1614</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1615</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1616</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1617</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>446</v>
-      </c>
-      <c r="B2" t="s">
-        <v>448</v>
-      </c>
-      <c r="C2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F2" s="4">
-        <v>45701</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>447</v>
-      </c>
-      <c r="C3" t="s">
-        <v>449</v>
-      </c>
-      <c r="D3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -13571,7 +13817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -13723,7 +13969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX72"/>
   <sheetViews>
@@ -15214,7 +15460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
disposition offers and sales tab
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B642EF1A-C48C-4A3D-88FB-3DBFB92738B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76395606-AB81-4A4A-BA68-C65974115D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -28,28 +28,29 @@
     <sheet name="AcquisitionFiles" sheetId="19" r:id="rId13"/>
     <sheet name="DispositionFiles" sheetId="34" r:id="rId14"/>
     <sheet name="DispositionChecklist" sheetId="35" r:id="rId15"/>
-    <sheet name="AcquisitionTeams" sheetId="20" r:id="rId16"/>
-    <sheet name="AcquisitionOwners" sheetId="21" r:id="rId17"/>
-    <sheet name="AcquisitionChecklist" sheetId="22" r:id="rId18"/>
-    <sheet name="AcquisitionAgreement" sheetId="23" r:id="rId19"/>
-    <sheet name="AcquisitionStakeholder" sheetId="24" r:id="rId20"/>
-    <sheet name="AcquisitionCompensation" sheetId="25" r:id="rId21"/>
-    <sheet name="CompensationActivities" sheetId="26" r:id="rId22"/>
-    <sheet name="AcquisitionExpropriationForm8" sheetId="28" r:id="rId23"/>
-    <sheet name="ExpropriationPayment" sheetId="29" r:id="rId24"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId25"/>
-    <sheet name="Properties" sheetId="6" r:id="rId26"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId27"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId28"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId29"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId30"/>
-    <sheet name="Takes" sheetId="27" r:id="rId31"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId32"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId33"/>
-    <sheet name="Notes" sheetId="10" r:id="rId34"/>
+    <sheet name="DispositionOfferSale" sheetId="36" r:id="rId16"/>
+    <sheet name="AcquisitionTeams" sheetId="20" r:id="rId17"/>
+    <sheet name="AcquisitionOwners" sheetId="21" r:id="rId18"/>
+    <sheet name="AcquisitionChecklist" sheetId="22" r:id="rId19"/>
+    <sheet name="AcquisitionAgreement" sheetId="23" r:id="rId20"/>
+    <sheet name="AcquisitionStakeholder" sheetId="24" r:id="rId21"/>
+    <sheet name="AcquisitionCompensation" sheetId="25" r:id="rId22"/>
+    <sheet name="CompensationActivities" sheetId="26" r:id="rId23"/>
+    <sheet name="AcquisitionExpropriationForm8" sheetId="28" r:id="rId24"/>
+    <sheet name="ExpropriationPayment" sheetId="29" r:id="rId25"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId26"/>
+    <sheet name="Properties" sheetId="6" r:id="rId27"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId28"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId29"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId30"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId31"/>
+    <sheet name="Takes" sheetId="27" r:id="rId32"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId33"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId34"/>
+    <sheet name="Notes" sheetId="10" r:id="rId35"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="1712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="1738">
   <si>
     <t>FirstName</t>
   </si>
@@ -5208,6 +5209,84 @@
   </si>
   <si>
     <t>DirectSaleRoadClosureSelect9</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentAppraisalValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentAppraisalDate</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentBcAssessmentValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentBcAssessmentRollYear</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentListPrice</t>
+  </si>
+  <si>
+    <t>OfferOfferStatus</t>
+  </si>
+  <si>
+    <t>OfferOfferName</t>
+  </si>
+  <si>
+    <t>OfferOfferDate</t>
+  </si>
+  <si>
+    <t>OfferOfferExpiryDate</t>
+  </si>
+  <si>
+    <t>OfferPrice</t>
+  </si>
+  <si>
+    <t>OfferNotes</t>
+  </si>
+  <si>
+    <t>Create Offers Section</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Update Offers Section</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>automated Offer name Updated</t>
+  </si>
+  <si>
+    <t>Test Offer Notes Updated</t>
+  </si>
+  <si>
+    <t>OfferSaleStartRow</t>
+  </si>
+  <si>
+    <t>New Disposition File to test Offers and sale</t>
+  </si>
+  <si>
+    <t>Offers and sale Disposition File - Automated</t>
+  </si>
+  <si>
+    <t>OfferSaleTotalCount</t>
+  </si>
+  <si>
+    <t>automated Offer name 1</t>
+  </si>
+  <si>
+    <t>automated Offer name 2</t>
+  </si>
+  <si>
+    <t>Test Offer Notes 2</t>
+  </si>
+  <si>
+    <t>Test Offer Notes 1</t>
+  </si>
+  <si>
+    <t>Update Disposition File to test Offers and sale</t>
   </si>
 </sst>
 </file>
@@ -6745,8 +6824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="V7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7027,7 +7106,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7237,7 +7316,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7444,7 +7523,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -7966,7 +8045,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8278,7 +8357,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8666,10 +8745,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8689,26 +8768,24 @@
     <col min="15" max="15" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.54296875" customWidth="1"/>
-    <col min="23" max="23" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -8760,8 +8837,29 @@
       <c r="Q1" s="3" t="s">
         <v>1709</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="R1" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>1716</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1658</v>
       </c>
@@ -8798,10 +8896,16 @@
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2" s="8"/>
-      <c r="AF2" s="6"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="S2" s="4"/>
+      <c r="W2" s="8">
+        <v>1</v>
+      </c>
+      <c r="X2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="6"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1657</v>
       </c>
@@ -8850,10 +8954,15 @@
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="AF3" s="6"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="W3" s="8">
+        <v>0</v>
+      </c>
+      <c r="X3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="6"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1656</v>
       </c>
@@ -8862,7 +8971,7 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45315</v>
+        <v>45320</v>
       </c>
       <c r="D4" s="4">
         <v>45352</v>
@@ -8885,10 +8994,15 @@
       <c r="Q4">
         <v>1</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="AF4" s="6"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="W4" s="8">
+        <v>0</v>
+      </c>
+      <c r="X4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="6"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1659</v>
       </c>
@@ -8913,8 +9027,108 @@
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="AF5" s="6"/>
+      <c r="W5" s="8">
+        <v>0</v>
+      </c>
+      <c r="X5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="6"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F6">
+        <v>77665544</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1671</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1672</v>
+      </c>
+      <c r="L6" t="s">
+        <v>925</v>
+      </c>
+      <c r="M6" t="s">
+        <v>863</v>
+      </c>
+      <c r="N6" t="s">
+        <v>200</v>
+      </c>
+      <c r="O6" s="8">
+        <v>10</v>
+      </c>
+      <c r="P6" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1000000.99</v>
+      </c>
+      <c r="S6" s="4">
+        <v>45170</v>
+      </c>
+      <c r="T6">
+        <v>4560</v>
+      </c>
+      <c r="U6">
+        <v>2024</v>
+      </c>
+      <c r="V6">
+        <v>4560</v>
+      </c>
+      <c r="W6" s="8">
+        <v>1</v>
+      </c>
+      <c r="X6" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="6"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1737</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>10500.99</v>
+      </c>
+      <c r="S7" s="4">
+        <v>45536</v>
+      </c>
+      <c r="T7">
+        <v>4560</v>
+      </c>
+      <c r="U7">
+        <v>2024</v>
+      </c>
+      <c r="V7">
+        <v>4600</v>
+      </c>
+      <c r="W7" s="8">
+        <v>3</v>
+      </c>
+      <c r="X7" s="8">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8926,7 +9140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6959299-8109-4A66-918B-3B215FFD6F08}">
   <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
@@ -9299,11 +9513,134 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E92D2C-114B-4B89-8045-FD4BA7A40A1C}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1721</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45352</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45427</v>
+      </c>
+      <c r="F2" s="6">
+        <v>550000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45352</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45427</v>
+      </c>
+      <c r="F3" s="6">
+        <v>550000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45463</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45442</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1200.5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9486,7 +9823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5453F532-21B6-4188-9011-0BA56E95151F}">
   <dimension ref="A1:S8"/>
   <sheetViews>
@@ -9880,7 +10217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD9027E-311F-43F3-971B-D6244D52A1F4}">
   <dimension ref="A1:AV4"/>
   <sheetViews>
@@ -10364,297 +10701,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247DFAE7-4496-4934-B20F-D611E033A94F}">
-  <dimension ref="A1:K8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1107</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1110</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1120</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1111</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1112</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>1113</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1114</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B2" t="s">
-        <v>560</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E2" s="4">
-        <v>44440</v>
-      </c>
-      <c r="G2" s="4">
-        <v>44470</v>
-      </c>
-      <c r="H2" s="4">
-        <v>44471</v>
-      </c>
-      <c r="I2" s="6">
-        <v>25000000</v>
-      </c>
-      <c r="J2" s="8">
-        <v>30</v>
-      </c>
-      <c r="K2" s="6">
-        <v>1000000.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>560</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E3" s="4">
-        <v>44806</v>
-      </c>
-      <c r="G3" s="4">
-        <v>45201</v>
-      </c>
-      <c r="H3" s="4">
-        <v>45202</v>
-      </c>
-      <c r="I3" s="6">
-        <v>2000000</v>
-      </c>
-      <c r="J3" s="8">
-        <v>60</v>
-      </c>
-      <c r="K3" s="6">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1118</v>
-      </c>
-      <c r="B4" t="s">
-        <v>560</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1130</v>
-      </c>
-      <c r="E4" s="4">
-        <v>44809</v>
-      </c>
-      <c r="G4" s="4">
-        <v>44907</v>
-      </c>
-      <c r="H4" s="4">
-        <v>44908</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1000000.79</v>
-      </c>
-      <c r="J4" s="8">
-        <v>90</v>
-      </c>
-      <c r="K4" s="6">
-        <v>550000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B5" t="s">
-        <v>563</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1131</v>
-      </c>
-      <c r="E5" s="4">
-        <v>44810</v>
-      </c>
-      <c r="F5" s="4">
-        <v>44819</v>
-      </c>
-      <c r="G5" s="4">
-        <v>45541</v>
-      </c>
-      <c r="H5" s="4">
-        <v>45542</v>
-      </c>
-      <c r="I5" s="6">
-        <v>120225.7</v>
-      </c>
-      <c r="J5" s="8">
-        <v>120</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1200.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B6" t="s">
-        <v>560</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E6" s="4">
-        <v>44811</v>
-      </c>
-      <c r="G6" s="4">
-        <v>45184</v>
-      </c>
-      <c r="H6" s="4">
-        <v>45185</v>
-      </c>
-      <c r="I6" s="6">
-        <v>200000.9</v>
-      </c>
-      <c r="J6" s="8">
-        <v>30</v>
-      </c>
-      <c r="K6" s="6">
-        <v>190000.95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>1121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>560</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E7" s="4">
-        <v>44819</v>
-      </c>
-      <c r="G7" s="4">
-        <v>45563</v>
-      </c>
-      <c r="H7" s="4">
-        <v>45564</v>
-      </c>
-      <c r="I7" s="6">
-        <v>15000.9</v>
-      </c>
-      <c r="J7" s="8">
-        <v>45</v>
-      </c>
-      <c r="K7" s="6">
-        <v>12000.89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1591</v>
-      </c>
-      <c r="B8" t="s">
-        <v>560</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1592</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E8" s="4">
-        <v>45265</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4">
-        <v>45638</v>
-      </c>
-      <c r="H8" s="4">
-        <v>45638</v>
-      </c>
-      <c r="I8" s="6">
-        <v>10000</v>
-      </c>
-      <c r="J8" s="8">
-        <v>30</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11161,6 +11207,297 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247DFAE7-4496-4934-B20F-D611E033A94F}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44440</v>
+      </c>
+      <c r="G2" s="4">
+        <v>44470</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44471</v>
+      </c>
+      <c r="I2" s="6">
+        <v>25000000</v>
+      </c>
+      <c r="J2" s="8">
+        <v>30</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1000000.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>560</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44806</v>
+      </c>
+      <c r="G3" s="4">
+        <v>45201</v>
+      </c>
+      <c r="H3" s="4">
+        <v>45202</v>
+      </c>
+      <c r="I3" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="J3" s="8">
+        <v>60</v>
+      </c>
+      <c r="K3" s="6">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>560</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44809</v>
+      </c>
+      <c r="G4" s="4">
+        <v>44907</v>
+      </c>
+      <c r="H4" s="4">
+        <v>44908</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1000000.79</v>
+      </c>
+      <c r="J4" s="8">
+        <v>90</v>
+      </c>
+      <c r="K4" s="6">
+        <v>550000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>563</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44810</v>
+      </c>
+      <c r="F5" s="4">
+        <v>44819</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45541</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45542</v>
+      </c>
+      <c r="I5" s="6">
+        <v>120225.7</v>
+      </c>
+      <c r="J5" s="8">
+        <v>120</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1200.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>560</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44811</v>
+      </c>
+      <c r="G6" s="4">
+        <v>45184</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45185</v>
+      </c>
+      <c r="I6" s="6">
+        <v>200000.9</v>
+      </c>
+      <c r="J6" s="8">
+        <v>30</v>
+      </c>
+      <c r="K6" s="6">
+        <v>190000.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>560</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44819</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45563</v>
+      </c>
+      <c r="H7" s="4">
+        <v>45564</v>
+      </c>
+      <c r="I7" s="6">
+        <v>15000.9</v>
+      </c>
+      <c r="J7" s="8">
+        <v>45</v>
+      </c>
+      <c r="K7" s="6">
+        <v>12000.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B8" t="s">
+        <v>560</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45265</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
+        <v>45638</v>
+      </c>
+      <c r="H8" s="4">
+        <v>45638</v>
+      </c>
+      <c r="I8" s="6">
+        <v>10000</v>
+      </c>
+      <c r="J8" s="8">
+        <v>30</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073F58F-6509-4BF3-843F-237D06AC55C6}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -11517,7 +11854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CC3795-F36B-4D0F-8244-A4F4C3935686}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -11783,7 +12120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A39253E-76F9-426F-AB51-5E3DB6377515}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -11921,7 +12258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE31339F-895D-48D8-9AD6-CFA457625F2E}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -12083,7 +12420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9467DD6-431B-4487-B73A-065D683A7274}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -12247,7 +12584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -12566,7 +12903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:X5"/>
   <sheetViews>
@@ -12860,7 +13197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -13013,7 +13350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -13120,7 +13457,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1616</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1617</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45701</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C3" t="s">
+        <v>449</v>
+      </c>
+      <c r="D3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -13395,86 +13811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1614</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1615</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1616</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1617</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>446</v>
-      </c>
-      <c r="B2" t="s">
-        <v>448</v>
-      </c>
-      <c r="C2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F2" s="4">
-        <v>45701</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>447</v>
-      </c>
-      <c r="C3" t="s">
-        <v>449</v>
-      </c>
-      <c r="D3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -13587,7 +13924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -14055,7 +14392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -14207,7 +14544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX72"/>
   <sheetViews>
@@ -15698,7 +16035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Refactoring and Disposition file automation
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F9BBFF-EC84-4C86-859C-F96074DE2991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8354805A-4DAD-4770-A295-B839A7F7B411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="11" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -36,20 +36,21 @@
     <sheet name="ExpropriationPayment" sheetId="29" r:id="rId21"/>
     <sheet name="DispositionFiles" sheetId="34" r:id="rId22"/>
     <sheet name="DispositionChecklist" sheetId="35" r:id="rId23"/>
-    <sheet name="TeamMembers" sheetId="20" r:id="rId24"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId25"/>
-    <sheet name="Properties" sheetId="6" r:id="rId26"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId27"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId28"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId29"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId30"/>
-    <sheet name="Takes" sheetId="27" r:id="rId31"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId32"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId33"/>
-    <sheet name="Notes" sheetId="10" r:id="rId34"/>
+    <sheet name="DispositionOfferSale" sheetId="36" r:id="rId24"/>
+    <sheet name="TeamMembers" sheetId="20" r:id="rId25"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId26"/>
+    <sheet name="Properties" sheetId="6" r:id="rId27"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId28"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId29"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId30"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId31"/>
+    <sheet name="Takes" sheetId="27" r:id="rId32"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId33"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId34"/>
+    <sheet name="Notes" sheetId="10" r:id="rId35"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="1819">
   <si>
     <t>FirstName</t>
   </si>
@@ -5351,9 +5352,6 @@
     <t>Disposition Files - Field notes</t>
   </si>
   <si>
-    <t>Appraisal/ Reviews</t>
-  </si>
-  <si>
     <t>1233-AGB</t>
   </si>
   <si>
@@ -5400,6 +5398,138 @@
   </si>
   <si>
     <t>MoTI Lead</t>
+  </si>
+  <si>
+    <t>Disposition Files - Briefing notes</t>
+  </si>
+  <si>
+    <t>Disposition Files - Correspondence</t>
+  </si>
+  <si>
+    <t>Disposition Files - Legal correspondence (ex: to AG/external lawyers)</t>
+  </si>
+  <si>
+    <t>Disposition Files - First nations consultation</t>
+  </si>
+  <si>
+    <t>Disposition Files - Ministerial order</t>
+  </si>
+  <si>
+    <t>Disposition Files - Miscellaneous notes (LTSA)</t>
+  </si>
+  <si>
+    <t>1222-9090</t>
+  </si>
+  <si>
+    <t>2309-1178 Burrard St.</t>
+  </si>
+  <si>
+    <t>Africa Smithe</t>
+  </si>
+  <si>
+    <t>909-890-887</t>
+  </si>
+  <si>
+    <t>Create a new Correspondece Document in a Disposition File</t>
+  </si>
+  <si>
+    <t>Create a Document of type Legal correspondence for Disposition File</t>
+  </si>
+  <si>
+    <t>First Nation consultation within an automated Disposition File</t>
+  </si>
+  <si>
+    <t>02-099897-88</t>
+  </si>
+  <si>
+    <t>233-900-899</t>
+  </si>
+  <si>
+    <t>W37 Main Road</t>
+  </si>
+  <si>
+    <t>900-003-123</t>
+  </si>
+  <si>
+    <t>OfferOfferStatus</t>
+  </si>
+  <si>
+    <t>OfferOfferName</t>
+  </si>
+  <si>
+    <t>OfferOfferDate</t>
+  </si>
+  <si>
+    <t>OfferOfferExpiryDate</t>
+  </si>
+  <si>
+    <t>OfferPrice</t>
+  </si>
+  <si>
+    <t>OfferNotes</t>
+  </si>
+  <si>
+    <t>Create Offers Section</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>automated Offer name 1</t>
+  </si>
+  <si>
+    <t>Test Offer Notes 1</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>automated Offer name 2</t>
+  </si>
+  <si>
+    <t>Test Offer Notes 2</t>
+  </si>
+  <si>
+    <t>Update Offers Section</t>
+  </si>
+  <si>
+    <t>automated Offer name Updated</t>
+  </si>
+  <si>
+    <t>Test Offer Notes Updated</t>
+  </si>
+  <si>
+    <t>New Disposition File to test Offers and sale</t>
+  </si>
+  <si>
+    <t>Update Disposition File to test Offers and sale</t>
+  </si>
+  <si>
+    <t>Automated Disposition Files - Offers and Sales</t>
+  </si>
+  <si>
+    <t>Update Automated Disposition File Offers and Sales</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentAppraisalValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentAppraisalDate</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentBcAssessmentValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentBcAssessmentRollYear</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentListPrice</t>
+  </si>
+  <si>
+    <t>OfferSaleStartRow</t>
+  </si>
+  <si>
+    <t>OfferSaleTotalCount</t>
   </si>
 </sst>
 </file>
@@ -5477,7 +5607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5505,6 +5635,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7237,7 +7368,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45320</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7447,7 +7578,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45320</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7654,7 +7785,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45320</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8176,7 +8307,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45320</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8488,7 +8619,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45320</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -11617,10 +11748,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11629,7 +11760,7 @@
     <col min="2" max="2" width="19.1796875" customWidth="1"/>
     <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="5" max="5" width="39.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.1796875" customWidth="1"/>
@@ -11644,13 +11775,13 @@
     <col min="18" max="18" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.54296875" customWidth="1"/>
-    <col min="25" max="25" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
@@ -11670,7 +11801,7 @@
         <v>1642</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>994</v>
@@ -11691,7 +11822,7 @@
         <v>1628</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1629</v>
@@ -11722,6 +11853,27 @@
       </c>
       <c r="T1" s="3" t="s">
         <v>1722</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>1812</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>1813</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>1814</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>1815</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>1816</v>
+      </c>
+      <c r="Z1" s="19" t="s">
+        <v>1817</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>1818</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.35">
@@ -11761,6 +11913,12 @@
       <c r="T2" s="8">
         <v>0</v>
       </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
       <c r="AH2" s="6"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
@@ -11792,13 +11950,13 @@
         <v>1728</v>
       </c>
       <c r="J3" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="M3" s="4">
         <v>45323</v>
@@ -11822,6 +11980,12 @@
         <v>0</v>
       </c>
       <c r="T3" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
         <v>0</v>
       </c>
       <c r="AH3" s="6"/>
@@ -11835,7 +11999,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45320</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -11865,6 +12029,12 @@
         <v>0</v>
       </c>
       <c r="T4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
         <v>0</v>
       </c>
       <c r="AH4" s="6"/>
@@ -11900,6 +12070,12 @@
       <c r="T5" s="8">
         <v>0</v>
       </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.35">
@@ -11936,6 +12112,12 @@
       <c r="T6" s="8">
         <v>0</v>
       </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -11968,100 +12150,257 @@
       <c r="T7" s="8">
         <v>0</v>
       </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="20" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="F8" t="s">
-        <v>1724</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1725</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="F8" s="20" t="s">
+        <v>1810</v>
+      </c>
+      <c r="G8" s="20">
+        <v>77665544</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>1647</v>
       </c>
-      <c r="P8" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
-        <v>0</v>
-      </c>
-      <c r="T8">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="N8" s="20" t="s">
+        <v>906</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>846</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>0</v>
+      </c>
+      <c r="R8" s="20">
+        <v>0</v>
+      </c>
+      <c r="S8" s="20">
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="20">
+        <v>1000000.99</v>
+      </c>
+      <c r="V8" s="21">
+        <v>45170</v>
+      </c>
+      <c r="W8" s="20">
+        <v>4560</v>
+      </c>
+      <c r="X8" s="20">
+        <v>2024</v>
+      </c>
+      <c r="Y8" s="20">
+        <v>4560</v>
+      </c>
+      <c r="Z8" s="20">
         <v>1</v>
       </c>
+      <c r="AA8" s="20">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1746</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="20" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="F9" t="s">
-        <v>1748</v>
-      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>1811</v>
+      </c>
+      <c r="G9" s="20"/>
       <c r="H9" t="s">
-        <v>1646</v>
+        <v>1641</v>
       </c>
       <c r="I9" t="s">
-        <v>1647</v>
-      </c>
-      <c r="P9" t="s">
+        <v>1727</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="Q9" s="8">
-        <v>0</v>
-      </c>
-      <c r="R9" s="8">
-        <v>0</v>
-      </c>
-      <c r="S9" s="8">
+      <c r="Q9" s="20">
+        <v>0</v>
+      </c>
+      <c r="R9" s="20">
+        <v>0</v>
+      </c>
+      <c r="S9" s="20">
         <v>0</v>
       </c>
       <c r="T9" s="8">
         <v>0</v>
       </c>
+      <c r="U9" s="20">
+        <v>10500.99</v>
+      </c>
+      <c r="V9" s="21">
+        <v>45536</v>
+      </c>
+      <c r="W9" s="20">
+        <v>4560</v>
+      </c>
+      <c r="X9" s="20">
+        <v>2024</v>
+      </c>
+      <c r="Y9" s="20">
+        <v>4600</v>
+      </c>
+      <c r="Z9" s="20">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="20">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1747</v>
+        <v>1723</v>
       </c>
       <c r="B10" t="s">
         <v>273</v>
       </c>
       <c r="F10" t="s">
+        <v>1724</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1725</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1647</v>
+      </c>
+      <c r="P10" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>0</v>
+      </c>
+      <c r="R10" s="8">
+        <v>0</v>
+      </c>
+      <c r="S10" s="8">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B11" t="s">
+        <v>273</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1748</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1647</v>
+      </c>
+      <c r="P11" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0</v>
+      </c>
+      <c r="R11" s="8">
+        <v>0</v>
+      </c>
+      <c r="S11" s="8">
+        <v>0</v>
+      </c>
+      <c r="T11" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B12" t="s">
+        <v>273</v>
+      </c>
+      <c r="F12" t="s">
         <v>1749</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H12" t="s">
         <v>1641</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I12" t="s">
         <v>1727</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P12" t="s">
         <v>200</v>
       </c>
-      <c r="Q10" s="8">
-        <v>0</v>
-      </c>
-      <c r="R10" s="8">
-        <v>0</v>
-      </c>
-      <c r="S10" s="8">
-        <v>0</v>
-      </c>
-      <c r="T10" s="8">
+      <c r="Q12" s="8">
+        <v>0</v>
+      </c>
+      <c r="R12" s="8">
+        <v>0</v>
+      </c>
+      <c r="S12" s="8">
+        <v>0</v>
+      </c>
+      <c r="T12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
         <v>0</v>
       </c>
     </row>
@@ -12474,10 +12813,135 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>1794</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>1796</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>1800</v>
+      </c>
+      <c r="D2" s="21">
+        <v>45352</v>
+      </c>
+      <c r="E2" s="21">
+        <v>45427</v>
+      </c>
+      <c r="F2" s="20">
+        <v>550000</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D3" s="21">
+        <v>45352</v>
+      </c>
+      <c r="E3" s="21">
+        <v>45427</v>
+      </c>
+      <c r="F3" s="20">
+        <v>550000</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D4" s="21">
+        <v>45463</v>
+      </c>
+      <c r="E4" s="21">
+        <v>45442</v>
+      </c>
+      <c r="F4" s="20">
+        <v>1200.5</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -12689,7 +13153,7 @@
         <v>1709</v>
       </c>
       <c r="B14" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="C14" t="s">
         <v>1711</v>
@@ -12785,7 +13249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -13135,7 +13599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
@@ -13498,7 +13962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -13651,7 +14115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -13758,7 +14222,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1594</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1595</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" t="s">
+        <v>449</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45701</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -14033,86 +14576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776329E-4018-44A5-82B8-B8248C5C0C9C}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1591</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1592</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1593</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1594</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1595</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>445</v>
-      </c>
-      <c r="B2" t="s">
-        <v>447</v>
-      </c>
-      <c r="C2" t="s">
-        <v>448</v>
-      </c>
-      <c r="D2" t="s">
-        <v>449</v>
-      </c>
-      <c r="F2" s="4">
-        <v>45701</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>446</v>
-      </c>
-      <c r="C3" t="s">
-        <v>448</v>
-      </c>
-      <c r="D3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -14225,7 +14689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -14693,12 +15157,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14848,7 +15312,7 @@
         <v>72</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -14856,7 +15320,7 @@
         <v>1745</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -14867,13 +15331,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
-  <dimension ref="A1:AX78"/>
+  <dimension ref="A1:AX84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16375,16 +16839,16 @@
         <v>12</v>
       </c>
       <c r="V73" t="s">
+        <v>1759</v>
+      </c>
+      <c r="W73" t="s">
         <v>1760</v>
       </c>
-      <c r="W73" t="s">
+      <c r="Z73" t="s">
         <v>1761</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="AP73" t="s">
         <v>1762</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>1763</v>
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
@@ -16409,7 +16873,7 @@
         <v>561</v>
       </c>
       <c r="E75" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="T75" t="s">
         <v>574</v>
@@ -16426,21 +16890,21 @@
         <v>1757</v>
       </c>
       <c r="B76" t="s">
-        <v>1759</v>
+        <v>922</v>
       </c>
       <c r="C76" t="s">
         <v>562</v>
       </c>
       <c r="AS76" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1758</v>
+        <v>1775</v>
       </c>
       <c r="B77" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="C77" t="s">
         <v>563</v>
@@ -16452,42 +16916,156 @@
         <v>123</v>
       </c>
       <c r="U77" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B78" t="s">
+        <v>511</v>
+      </c>
+      <c r="C78" t="s">
+        <v>563</v>
+      </c>
+      <c r="I78">
+        <v>900</v>
+      </c>
+      <c r="L78" t="s">
+        <v>1781</v>
+      </c>
+      <c r="U78" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="79" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B79" t="s">
+        <v>507</v>
+      </c>
+      <c r="C79" t="s">
+        <v>564</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1782</v>
+      </c>
+      <c r="G79" s="13">
+        <v>44053</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>1783</v>
+      </c>
+      <c r="AM79" t="s">
+        <v>1784</v>
+      </c>
+      <c r="AS79" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="80" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B80" t="s">
+        <v>516</v>
+      </c>
+      <c r="C80" t="s">
+        <v>559</v>
+      </c>
+      <c r="AS80" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="81" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B81" t="s">
+        <v>512</v>
+      </c>
+      <c r="C81" t="s">
+        <v>560</v>
+      </c>
+      <c r="AS81" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="82" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B82" t="s">
+        <v>520</v>
+      </c>
+      <c r="C82" t="s">
+        <v>561</v>
+      </c>
+      <c r="H82" s="13">
+        <v>44813</v>
+      </c>
+      <c r="X82">
+        <v>8900999</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>1788</v>
+      </c>
+      <c r="AF82" t="s">
+        <v>1789</v>
+      </c>
+      <c r="AP82" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="83" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B83" t="s">
+        <v>521</v>
+      </c>
+      <c r="C83" t="s">
+        <v>562</v>
+      </c>
+      <c r="AF83" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="84" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>1750</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B84" t="s">
         <v>513</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C84" t="s">
         <v>564</v>
       </c>
-      <c r="N78" s="13">
+      <c r="N84" s="13">
         <v>45210</v>
       </c>
-      <c r="O78">
+      <c r="O84">
         <v>4</v>
       </c>
-      <c r="P78" s="13">
+      <c r="P84" s="13">
         <v>44866</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="Q84" t="s">
+        <v>1766</v>
+      </c>
+      <c r="V84" t="s">
         <v>1767</v>
       </c>
-      <c r="V78" t="s">
+      <c r="W84" t="s">
         <v>1768</v>
       </c>
-      <c r="W78" t="s">
+      <c r="Z84">
+        <v>909000</v>
+      </c>
+      <c r="AP84" t="s">
         <v>1769</v>
-      </c>
-      <c r="Z78">
-        <v>909000</v>
-      </c>
-      <c r="AP78" t="s">
-        <v>1770</v>
       </c>
     </row>
   </sheetData>
@@ -16496,7 +17074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B11"/>
   <sheetViews>

</xml_diff>

<commit_message>
Merge conflicts between local and remote
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8354805A-4DAD-4770-A295-B839A7F7B411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1481B0E0-4155-4B7F-82CE-F5FCCCC34EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11751,7 +11751,7 @@
   <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12158,100 +12158,74 @@
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
-        <v>1808</v>
-      </c>
-      <c r="B8" s="20" t="s">
+      <c r="A8" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B8" t="s">
         <v>273</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="F8" s="20" t="s">
-        <v>1810</v>
-      </c>
-      <c r="G8" s="20">
-        <v>77665544</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>1646</v>
-      </c>
-      <c r="I8" s="20" t="s">
+      <c r="F8" t="s">
+        <v>1724</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1725</v>
+      </c>
+      <c r="I8" t="s">
         <v>1647</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="N8" s="20" t="s">
-        <v>906</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>846</v>
-      </c>
-      <c r="P8" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q8" s="20">
-        <v>0</v>
-      </c>
-      <c r="R8" s="20">
-        <v>0</v>
-      </c>
-      <c r="S8" s="20">
-        <v>0</v>
-      </c>
-      <c r="T8" s="8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="20">
-        <v>1000000.99</v>
-      </c>
-      <c r="V8" s="21">
-        <v>45170</v>
-      </c>
-      <c r="W8" s="20">
-        <v>4560</v>
-      </c>
-      <c r="X8" s="20">
-        <v>2024</v>
-      </c>
-      <c r="Y8" s="20">
-        <v>4560</v>
-      </c>
-      <c r="Z8" s="20">
+      <c r="P8" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>1</v>
       </c>
-      <c r="AA8" s="20">
-        <v>2</v>
-      </c>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20"/>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>273</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>1811</v>
-      </c>
-      <c r="G9" s="20"/>
-      <c r="H9" t="s">
-        <v>1641</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1727</v>
+        <v>1810</v>
+      </c>
+      <c r="G9" s="20">
+        <v>77665544</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>1647</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
+      <c r="N9" s="20" t="s">
+        <v>906</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>846</v>
+      </c>
       <c r="P9" s="20" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Q9" s="20">
         <v>0</v>
@@ -12266,10 +12240,10 @@
         <v>0</v>
       </c>
       <c r="U9" s="20">
-        <v>10500.99</v>
+        <v>1000000.99</v>
       </c>
       <c r="V9" s="21">
-        <v>45536</v>
+        <v>45170</v>
       </c>
       <c r="W9" s="20">
         <v>4560</v>
@@ -12278,55 +12252,81 @@
         <v>2024</v>
       </c>
       <c r="Y9" s="20">
-        <v>4600</v>
+        <v>4560</v>
       </c>
       <c r="Z9" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB9" s="20"/>
       <c r="AC9" s="20"/>
       <c r="AD9" s="20"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="20" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="F10" t="s">
-        <v>1724</v>
-      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>1811</v>
+      </c>
+      <c r="G10" s="20"/>
       <c r="H10" t="s">
-        <v>1725</v>
+        <v>1641</v>
       </c>
       <c r="I10" t="s">
-        <v>1647</v>
-      </c>
-      <c r="P10" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>0</v>
-      </c>
-      <c r="R10" s="8">
-        <v>0</v>
-      </c>
-      <c r="S10" s="8">
-        <v>0</v>
-      </c>
-      <c r="T10">
+        <v>1727</v>
+      </c>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>0</v>
+      </c>
+      <c r="R10" s="20">
+        <v>0</v>
+      </c>
+      <c r="S10" s="20">
+        <v>0</v>
+      </c>
+      <c r="T10" s="8">
+        <v>0</v>
+      </c>
+      <c r="U10" s="20">
+        <v>10500.99</v>
+      </c>
+      <c r="V10" s="21">
+        <v>45536</v>
+      </c>
+      <c r="W10" s="20">
+        <v>4560</v>
+      </c>
+      <c r="X10" s="20">
+        <v>2024</v>
+      </c>
+      <c r="Y10" s="20">
+        <v>4600</v>
+      </c>
+      <c r="Z10" s="20">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="20">
         <v>1</v>
       </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Disposition files - Offers and sale create and update
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1481B0E0-4155-4B7F-82CE-F5FCCCC34EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156757EA-199F-4A1C-9C20-4F1B375AFC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -5475,27 +5475,18 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>automated Offer name 1</t>
-  </si>
-  <si>
     <t>Test Offer Notes 1</t>
   </si>
   <si>
     <t>Open</t>
   </si>
   <si>
-    <t>automated Offer name 2</t>
-  </si>
-  <si>
     <t>Test Offer Notes 2</t>
   </si>
   <si>
     <t>Update Offers Section</t>
   </si>
   <si>
-    <t>automated Offer name Updated</t>
-  </si>
-  <si>
     <t>Test Offer Notes Updated</t>
   </si>
   <si>
@@ -5530,6 +5521,15 @@
   </si>
   <si>
     <t>OfferSaleTotalCount</t>
+  </si>
+  <si>
+    <t>Automated Offer name 1</t>
+  </si>
+  <si>
+    <t>Automated Offer name 2</t>
+  </si>
+  <si>
+    <t>Automated Offer name Updated</t>
   </si>
 </sst>
 </file>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8307,7 +8307,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -11750,8 +11750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
   <dimension ref="A1:AH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11855,25 +11855,25 @@
         <v>1722</v>
       </c>
       <c r="U1" s="19" t="s">
+        <v>1809</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>1810</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>1811</v>
+      </c>
+      <c r="X1" s="19" t="s">
         <v>1812</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1813</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1814</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1815</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>1816</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>1817</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>1818</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.35">
@@ -11999,7 +11999,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12197,7 +12197,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>273</v>
@@ -12205,7 +12205,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
       <c r="G9" s="20">
         <v>77665544</v>
@@ -12266,7 +12266,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>273</v>
@@ -12275,7 +12275,7 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" t="s">
@@ -12309,12 +12309,8 @@
       <c r="V10" s="21">
         <v>45536</v>
       </c>
-      <c r="W10" s="20">
-        <v>4560</v>
-      </c>
-      <c r="X10" s="20">
-        <v>2024</v>
-      </c>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
       <c r="Y10" s="20">
         <v>4600</v>
       </c>
@@ -12816,8 +12812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12862,7 +12858,7 @@
         <v>1799</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>1800</v>
+        <v>1816</v>
       </c>
       <c r="D2" s="21">
         <v>45352</v>
@@ -12874,7 +12870,7 @@
         <v>550000</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -12882,10 +12878,10 @@
         <v>1798</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>1803</v>
+        <v>1817</v>
       </c>
       <c r="D3" s="21">
         <v>45352</v>
@@ -12897,18 +12893,18 @@
         <v>550000</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1806</v>
+        <v>1818</v>
       </c>
       <c r="D4" s="21">
         <v>45463</v>
@@ -12920,7 +12916,7 @@
         <v>1200.5</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Automation refactoring - Change of models and functions to avois warning messages
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156757EA-199F-4A1C-9C20-4F1B375AFC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C5776-416D-424A-AB16-D457D116C78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45780" yWindow="2445" windowWidth="21885" windowHeight="15315" tabRatio="950" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8307,7 +8307,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -11999,7 +11999,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12812,7 +12812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -19338,7 +19338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E3AF99-B285-4872-B012-0C94F438EBF8}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Automation refactoring - Change of models and functions to avois warning messages (#3764)
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156757EA-199F-4A1C-9C20-4F1B375AFC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C5776-416D-424A-AB16-D457D116C78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45780" yWindow="2445" windowWidth="21885" windowHeight="15315" tabRatio="950" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7578,7 +7578,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8307,7 +8307,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -11999,7 +11999,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12812,7 +12812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -19338,7 +19338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E3AF99-B285-4872-B012-0C94F438EBF8}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
disposition offers and sales
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156757EA-199F-4A1C-9C20-4F1B375AFC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2892B51E-66C3-4866-B76B-CB1EAED233A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="19" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="1819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2869" uniqueCount="1834">
   <si>
     <t>FirstName</t>
   </si>
@@ -5530,6 +5530,51 @@
   </si>
   <si>
     <t>Automated Offer name Updated</t>
+  </si>
+  <si>
+    <t>SalesDetailsContactType</t>
+  </si>
+  <si>
+    <t>PurchaserAgent</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitor</t>
+  </si>
+  <si>
+    <t>LastConditionRemovalDate</t>
+  </si>
+  <si>
+    <t>SaleCompletionDate</t>
+  </si>
+  <si>
+    <t>FiscalYearOfSale</t>
+  </si>
+  <si>
+    <t>FinalSalePrice</t>
+  </si>
+  <si>
+    <t>RealtorCommission</t>
+  </si>
+  <si>
+    <t>GSTRequired</t>
+  </si>
+  <si>
+    <t>GSTCollected</t>
+  </si>
+  <si>
+    <t>NetBookValue</t>
+  </si>
+  <si>
+    <t>TotalCostOfSales</t>
+  </si>
+  <si>
+    <t>SPPAmount</t>
+  </si>
+  <si>
+    <t>RemediationCost</t>
+  </si>
+  <si>
+    <t>PurchaserName</t>
   </si>
 </sst>
 </file>
@@ -5607,7 +5652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5636,6 +5681,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7368,7 +7414,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7578,7 +7624,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7785,7 +7831,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8307,7 +8353,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8619,7 +8665,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -9870,7 +9916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247DFAE7-4496-4934-B20F-D611E033A94F}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -10161,8 +10207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073F58F-6509-4BF3-843F-237D06AC55C6}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10518,7 +10564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CC3795-F36B-4D0F-8244-A4F4C3935686}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -11748,10 +11794,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AQ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11782,18 +11828,25 @@
     <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.54296875" customWidth="1"/>
+    <col min="30" max="30" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -11875,8 +11928,56 @@
       <c r="AA1" s="19" t="s">
         <v>1815</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB1" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>1820</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>1821</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>1822</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>1824</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>1825</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>1827</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1829</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>1831</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1635</v>
       </c>
@@ -11919,9 +12020,9 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AH2" s="6"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AJ2" s="6"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1634</v>
       </c>
@@ -11988,9 +12089,9 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AJ3" s="6"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1633</v>
       </c>
@@ -11999,7 +12100,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45321</v>
+        <v>45324</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12037,9 +12138,9 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AJ4" s="6"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1636</v>
       </c>
@@ -12076,9 +12177,9 @@
       <c r="AA5">
         <v>0</v>
       </c>
-      <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AJ5" s="6"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1719</v>
       </c>
@@ -12119,7 +12220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1718</v>
       </c>
@@ -12157,7 +12258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1723</v>
       </c>
@@ -12195,7 +12296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>1805</v>
       </c>
@@ -12260,11 +12361,45 @@
       <c r="AA9" s="20">
         <v>2</v>
       </c>
-      <c r="AB9" s="20"/>
+      <c r="AB9" s="20" t="s">
+        <v>736</v>
+      </c>
       <c r="AC9" s="20"/>
       <c r="AD9" s="20"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="4">
+        <v>45352</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>45505</v>
+      </c>
+      <c r="AI9">
+        <v>2024</v>
+      </c>
+      <c r="AJ9" s="22">
+        <v>50000</v>
+      </c>
+      <c r="AK9" s="22">
+        <v>10000</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>703</v>
+      </c>
+      <c r="AN9">
+        <v>750000</v>
+      </c>
+      <c r="AO9">
+        <v>800000</v>
+      </c>
+      <c r="AP9">
+        <v>67000</v>
+      </c>
+      <c r="AQ9">
+        <v>29000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>1806</v>
       </c>
@@ -12323,8 +12458,10 @@
       <c r="AB10" s="20"/>
       <c r="AC10" s="20"/>
       <c r="AD10" s="20"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1746</v>
       </c>
@@ -12362,7 +12499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1747</v>
       </c>
@@ -12812,7 +12949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sales Details object creations
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C5776-416D-424A-AB16-D457D116C78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B58EF78-0322-41F8-9C32-E234072C6578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45780" yWindow="2445" windowWidth="21885" windowHeight="15315" tabRatio="950" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="20" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -37,22 +37,24 @@
     <sheet name="DispositionFiles" sheetId="34" r:id="rId22"/>
     <sheet name="DispositionChecklist" sheetId="35" r:id="rId23"/>
     <sheet name="DispositionOfferSale" sheetId="36" r:id="rId24"/>
-    <sheet name="TeamMembers" sheetId="20" r:id="rId25"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId26"/>
-    <sheet name="Properties" sheetId="6" r:id="rId27"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId28"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId29"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId30"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId31"/>
-    <sheet name="Takes" sheetId="27" r:id="rId32"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId33"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId34"/>
-    <sheet name="Notes" sheetId="10" r:id="rId35"/>
+    <sheet name="PurchaserNames" sheetId="38" r:id="rId25"/>
+    <sheet name="TeamMembers" sheetId="20" r:id="rId26"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId27"/>
+    <sheet name="Properties" sheetId="6" r:id="rId28"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId29"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId30"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId31"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId32"/>
+    <sheet name="Takes" sheetId="27" r:id="rId33"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId34"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId35"/>
+    <sheet name="Notes" sheetId="10" r:id="rId36"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="1819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2883" uniqueCount="1840">
   <si>
     <t>FirstName</t>
   </si>
@@ -5530,6 +5532,69 @@
   </si>
   <si>
     <t>Automated Offer name Updated</t>
+  </si>
+  <si>
+    <t>SalesDetailsContactType</t>
+  </si>
+  <si>
+    <t>PurchaserName</t>
+  </si>
+  <si>
+    <t>PurchaserAgent</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitor</t>
+  </si>
+  <si>
+    <t>LastConditionRemovalDate</t>
+  </si>
+  <si>
+    <t>SaleCompletionDate</t>
+  </si>
+  <si>
+    <t>FiscalYearOfSale</t>
+  </si>
+  <si>
+    <t>FinalSalePrice</t>
+  </si>
+  <si>
+    <t>RealtorCommission</t>
+  </si>
+  <si>
+    <t>GSTRequired</t>
+  </si>
+  <si>
+    <t>GSTCollected</t>
+  </si>
+  <si>
+    <t>NetBookValue</t>
+  </si>
+  <si>
+    <t>TotalCostOfSales</t>
+  </si>
+  <si>
+    <t>SPPAmount</t>
+  </si>
+  <si>
+    <t>RemediationCost</t>
+  </si>
+  <si>
+    <t>PurchaseMemberContactType</t>
+  </si>
+  <si>
+    <t>PurchaseMemberPrimaryContact</t>
+  </si>
+  <si>
+    <t>PurchaseNameStartRow</t>
+  </si>
+  <si>
+    <t>PurchaseNameTotalCount</t>
+  </si>
+  <si>
+    <t>Purchase 1</t>
+  </si>
+  <si>
+    <t>Purchase 2</t>
   </si>
 </sst>
 </file>
@@ -7085,8 +7150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7368,7 +7433,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45326</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7578,7 +7643,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45326</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7785,7 +7850,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45326</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8307,7 +8372,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45326</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8619,7 +8684,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45326</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -10162,7 +10227,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11748,10 +11813,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AR12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11782,18 +11847,26 @@
     <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -11875,8 +11948,59 @@
       <c r="AA1" s="19" t="s">
         <v>1815</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB1" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>1836</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>1837</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>1821</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>1822</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>1824</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>1825</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>1827</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1829</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>1831</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>1832</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1635</v>
       </c>
@@ -11919,9 +12043,15 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AH2" s="6"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="6"/>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1634</v>
       </c>
@@ -11988,9 +12118,15 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="6"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1633</v>
       </c>
@@ -11999,7 +12135,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45326</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12037,9 +12173,15 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="6"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1636</v>
       </c>
@@ -12076,9 +12218,15 @@
       <c r="AA5">
         <v>0</v>
       </c>
-      <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="6"/>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1719</v>
       </c>
@@ -12118,8 +12266,14 @@
       <c r="AA6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1718</v>
       </c>
@@ -12156,8 +12310,14 @@
       <c r="AA7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1723</v>
       </c>
@@ -12194,8 +12354,14 @@
       <c r="AA8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>1805</v>
       </c>
@@ -12260,11 +12426,56 @@
       <c r="AA9" s="20">
         <v>2</v>
       </c>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB9" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="AC9" s="20">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="20">
+        <v>2</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AF9" s="20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="AG9" s="20" t="s">
+        <v>1139</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>45352</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>45505</v>
+      </c>
+      <c r="AJ9">
+        <v>2024</v>
+      </c>
+      <c r="AK9">
+        <v>50000</v>
+      </c>
+      <c r="AL9">
+        <v>10000</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>301</v>
+      </c>
+      <c r="AO9">
+        <v>750000</v>
+      </c>
+      <c r="AP9">
+        <v>800000</v>
+      </c>
+      <c r="AQ9">
+        <v>67000</v>
+      </c>
+      <c r="AR9">
+        <v>29000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>1806</v>
       </c>
@@ -12321,10 +12532,16 @@
         <v>1</v>
       </c>
       <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1746</v>
       </c>
@@ -12361,8 +12578,14 @@
       <c r="AA11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1747</v>
       </c>
@@ -12397,6 +12620,12 @@
         <v>0</v>
       </c>
       <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
         <v>0</v>
       </c>
     </row>
@@ -12411,7 +12640,7 @@
   <dimension ref="A1:AJ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12934,11 +13163,68 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FABE200-F318-4425-94AC-190989D6516A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13245,7 +13531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -13595,12 +13881,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13958,7 +14244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -14107,113 +14393,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1469</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1527</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1491</v>
-      </c>
-      <c r="C2" t="s">
-        <v>736</v>
-      </c>
-      <c r="D2" t="s">
-        <v>738</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>856</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C4" t="s">
-        <v>736</v>
-      </c>
-      <c r="D4" t="s">
-        <v>738</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C5" t="s">
-        <v>736</v>
-      </c>
-      <c r="D5" t="s">
-        <v>738</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14298,6 +14477,113 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C2" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2" t="s">
+        <v>738</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D4" t="s">
+        <v>738</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C5" t="s">
+        <v>736</v>
+      </c>
+      <c r="D5" t="s">
+        <v>738</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -14572,7 +14858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -14685,7 +14971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -15153,7 +15439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -15327,7 +15613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX84"/>
   <sheetViews>
@@ -17070,7 +17356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -19338,7 +19624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E3AF99-B285-4872-B012-0C94F438EBF8}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Automation fixes related to new modals
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C5776-416D-424A-AB16-D457D116C78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E08ADF-C39F-4060-B0F9-883BF2101C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45780" yWindow="2445" windowWidth="21885" windowHeight="15315" tabRatio="950" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="13" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -53,6 +53,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="1819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1820">
   <si>
     <t>FirstName</t>
   </si>
@@ -4635,9 +4636,6 @@
     <t>ManagementPropertyActivitiesCount</t>
   </si>
   <si>
-    <t>009-536-892</t>
-  </si>
-  <si>
     <t>ManagementPropertyActivityInvoicesStartRow</t>
   </si>
   <si>
@@ -5530,6 +5528,12 @@
   </si>
   <si>
     <t>Automated Offer name Updated</t>
+  </si>
+  <si>
+    <t>DF From PIN</t>
+  </si>
+  <si>
+    <t>Automated Disposition File - From PIN</t>
   </si>
 </sst>
 </file>
@@ -6522,7 +6526,7 @@
         <v>314</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>326</v>
@@ -6815,10 +6819,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B10" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="C10" t="s">
         <v>273</v>
@@ -6876,7 +6880,7 @@
         <v>321</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>322</v>
@@ -6899,7 +6903,7 @@
         <v>328</v>
       </c>
       <c r="C2" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D2" t="s">
         <v>299</v>
@@ -6922,7 +6926,7 @@
         <v>329</v>
       </c>
       <c r="C3" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D3" t="s">
         <v>301</v>
@@ -7054,13 +7058,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B9" t="s">
         <v>1545</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>1546</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1547</v>
       </c>
       <c r="D9" t="s">
         <v>301</v>
@@ -7069,10 +7073,10 @@
         <v>301</v>
       </c>
       <c r="F9" t="s">
+        <v>1549</v>
+      </c>
+      <c r="G9" t="s">
         <v>1550</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1551</v>
       </c>
     </row>
   </sheetData>
@@ -7086,7 +7090,7 @@
   <dimension ref="A1:AJ19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7134,7 +7138,7 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>916</v>
@@ -7200,7 +7204,7 @@
         <v>1083</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>1322</v>
@@ -7355,20 +7359,20 @@
         <v>5500502</v>
       </c>
       <c r="D3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F3" t="s">
         <v>1619</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1620</v>
       </c>
       <c r="G3" t="s">
         <v>1178</v>
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7565,7 +7569,7 @@
         <v>5503710</v>
       </c>
       <c r="D5" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="E5" t="s">
         <v>1176</v>
@@ -7578,7 +7582,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7772,20 +7776,20 @@
         <v>5500502</v>
       </c>
       <c r="D7" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F7" t="s">
         <v>1619</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1620</v>
       </c>
       <c r="G7" t="s">
         <v>1178</v>
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8294,20 +8298,20 @@
         <v>5500502</v>
       </c>
       <c r="D12" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F12" t="s">
         <v>1619</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1620</v>
       </c>
       <c r="G12" t="s">
         <v>1178</v>
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8606,20 +8610,20 @@
         <v>5500502</v>
       </c>
       <c r="D15" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F15" t="s">
         <v>1619</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1620</v>
       </c>
       <c r="G15" t="s">
         <v>1178</v>
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8927,16 +8931,16 @@
         <v>5500502</v>
       </c>
       <c r="D19" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F19" t="s">
         <v>1619</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1620</v>
-      </c>
       <c r="G19" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="L19" t="s">
         <v>881</v>
@@ -9345,7 +9349,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -9354,16 +9358,16 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
+        <v>1558</v>
+      </c>
+      <c r="H8" t="s">
         <v>1559</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>1560</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>1561</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1562</v>
       </c>
       <c r="M8" t="s">
         <v>72</v>
@@ -9375,10 +9379,10 @@
         <v>37</v>
       </c>
       <c r="Q8" t="s">
+        <v>1562</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>1563</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>1564</v>
       </c>
       <c r="S8">
         <v>7080009876</v>
@@ -9715,7 +9719,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B3" t="s">
         <v>1066</v>
@@ -10121,13 +10125,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B8" t="s">
         <v>559</v>
       </c>
       <c r="C8" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D8" t="s">
         <v>1109</v>
@@ -10485,7 +10489,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B16" t="s">
         <v>1130</v>
@@ -10577,7 +10581,7 @@
         <v>1147</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1148</v>
@@ -10633,7 +10637,7 @@
         <v>559</v>
       </c>
       <c r="F2" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G2" s="4">
         <v>45176</v>
@@ -10709,7 +10713,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -10724,7 +10728,7 @@
         <v>559</v>
       </c>
       <c r="F4" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G4" s="4">
         <v>45272</v>
@@ -10739,25 +10743,25 @@
         <v>45181</v>
       </c>
       <c r="K4" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="L4" t="s">
         <v>1171</v>
       </c>
       <c r="M4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="N4" t="s">
         <v>1573</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>1574</v>
       </c>
-      <c r="O4" t="s">
-        <v>1575</v>
-      </c>
       <c r="P4" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="Q4" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="R4" t="b">
         <v>1</v>
@@ -10766,7 +10770,7 @@
         <v>145556</v>
       </c>
       <c r="T4" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="U4">
         <v>5</v>
@@ -10894,10 +10898,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B6" t="s">
         <v>1577</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1578</v>
       </c>
       <c r="C6">
         <v>10000</v>
@@ -11556,19 +11560,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B6" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="C6" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D6" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E6" t="s">
         <v>1579</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1580</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -11722,10 +11726,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B7" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C7" s="11">
         <v>1000</v>
@@ -11748,10 +11752,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11798,102 +11802,102 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>994</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>1624</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1625</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1626</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1627</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>1770</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>1628</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>1771</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>1643</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1629</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1644</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>1630</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>836</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>1621</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>1622</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1623</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>1624</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="U1" s="19" t="s">
+        <v>1808</v>
+      </c>
+      <c r="V1" s="19" t="s">
         <v>1809</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>1810</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>1811</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1812</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1813</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1814</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>1815</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B2" t="s">
         <v>273</v>
       </c>
       <c r="F2" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="H2" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="I2" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="K2" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="O2" t="s">
         <v>846</v>
@@ -11923,13 +11927,13 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="B3" t="s">
         <v>847</v>
       </c>
       <c r="C3" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D3" s="4">
         <v>45170</v>
@@ -11938,25 +11942,25 @@
         <v>45366</v>
       </c>
       <c r="F3" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="G3" t="s">
         <v>845</v>
       </c>
       <c r="H3" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I3" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="J3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="M3" s="4">
         <v>45323</v>
@@ -11965,7 +11969,7 @@
         <v>273</v>
       </c>
       <c r="O3" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="P3" t="s">
         <v>198</v>
@@ -11992,23 +11996,23 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="B4" t="s">
         <v>1066</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45323</v>
+        <v>45328</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
       </c>
       <c r="F4" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="G4" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="H4" t="s">
         <v>1500</v>
@@ -12041,19 +12045,19 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="B5" t="s">
         <v>559</v>
       </c>
       <c r="F5" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="H5" t="s">
+        <v>1725</v>
+      </c>
+      <c r="I5" t="s">
         <v>1726</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1727</v>
       </c>
       <c r="P5" t="s">
         <v>199</v>
@@ -12080,22 +12084,22 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B6" t="s">
         <v>273</v>
       </c>
       <c r="F6" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="H6" t="s">
         <v>336</v>
       </c>
       <c r="I6" t="s">
+        <v>1727</v>
+      </c>
+      <c r="J6" t="s">
         <v>1728</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1729</v>
       </c>
       <c r="P6" t="s">
         <v>198</v>
@@ -12121,16 +12125,16 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B7" t="s">
         <v>273</v>
       </c>
       <c r="F7" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="H7" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I7" t="s">
         <v>364</v>
@@ -12159,19 +12163,19 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B8" t="s">
         <v>273</v>
       </c>
       <c r="F8" t="s">
+        <v>1723</v>
+      </c>
+      <c r="H8" t="s">
         <v>1724</v>
       </c>
-      <c r="H8" t="s">
-        <v>1725</v>
-      </c>
       <c r="I8" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="P8" t="s">
         <v>199</v>
@@ -12197,7 +12201,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>273</v>
@@ -12205,16 +12209,16 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="G9" s="20">
         <v>77665544</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>1645</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>1646</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>1647</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
@@ -12266,7 +12270,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>273</v>
@@ -12275,14 +12279,14 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I10" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -12326,19 +12330,19 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B11" t="s">
         <v>273</v>
       </c>
       <c r="F11" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="H11" t="s">
+        <v>1645</v>
+      </c>
+      <c r="I11" t="s">
         <v>1646</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1647</v>
       </c>
       <c r="P11" t="s">
         <v>198</v>
@@ -12364,19 +12368,19 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B12" t="s">
         <v>273</v>
       </c>
       <c r="F12" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="H12" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I12" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="P12" t="s">
         <v>200</v>
@@ -12397,6 +12401,44 @@
         <v>0</v>
       </c>
       <c r="AA12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B13" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1500</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P13" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0</v>
+      </c>
+      <c r="S13" s="8">
+        <v>24</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
         <v>0</v>
       </c>
     </row>
@@ -12442,97 +12484,97 @@
         <v>1032</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>1667</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>1668</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>1669</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>1670</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>1671</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>1672</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>1673</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>1674</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>1675</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="19" t="s">
         <v>1676</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>1677</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>1678</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>1679</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>1680</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>1681</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>1682</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>1683</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>1684</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>1685</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1686</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1687</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1688</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>1689</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>1690</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>1691</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>1692</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>1693</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>1694</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>1695</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>1696</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>1697</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
@@ -12697,7 +12739,7 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>1066</v>
@@ -12832,33 +12874,33 @@
         <v>112</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1792</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>1793</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>1794</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>1795</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>1796</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1797</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>1798</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>1799</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D2" s="21">
         <v>45352</v>
@@ -12870,18 +12912,18 @@
         <v>550000</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D3" s="21">
         <v>45352</v>
@@ -12893,18 +12935,18 @@
         <v>550000</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D4" s="21">
         <v>45463</v>
@@ -12916,7 +12958,7 @@
         <v>1200.5</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -12938,7 +12980,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12955,16 +12997,16 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1648</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1649</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1650</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1651</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -13034,13 +13076,13 @@
         <v>853</v>
       </c>
       <c r="C6" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -13079,13 +13121,13 @@
         <v>908</v>
       </c>
       <c r="C9" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -13104,13 +13146,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B11" t="s">
         <v>850</v>
       </c>
       <c r="C11" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D11" t="s">
         <v>736</v>
@@ -13118,10 +13160,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B12" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="C12" t="s">
         <v>1385</v>
@@ -13132,13 +13174,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B13" t="s">
         <v>850</v>
       </c>
       <c r="C13" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D13" t="s">
         <v>736</v>
@@ -13146,13 +13188,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B14" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C14" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D14" t="s">
         <v>736</v>
@@ -13160,7 +13202,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B15" t="s">
         <v>851</v>
@@ -13177,13 +13219,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B16" t="s">
         <v>908</v>
       </c>
       <c r="C16" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -13194,30 +13236,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B17" t="s">
         <v>853</v>
       </c>
       <c r="C17" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B18" t="s">
         <v>852</v>
       </c>
       <c r="C18" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -13228,13 +13270,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C19" t="s">
         <v>1716</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1717</v>
       </c>
       <c r="D19" t="s">
         <v>736</v>
@@ -13249,8 +13291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13398,7 +13440,7 @@
         <v>1002</v>
       </c>
       <c r="E10" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -13411,7 +13453,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B12" t="s">
         <v>800</v>
@@ -13431,7 +13473,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B13" t="s">
         <v>804</v>
@@ -13439,7 +13481,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B14" t="s">
         <v>379</v>
@@ -13447,7 +13489,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B15" t="s">
         <v>925</v>
@@ -13475,7 +13517,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B17" t="s">
         <v>878</v>
@@ -13486,7 +13528,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B18" t="s">
         <v>884</v>
@@ -13502,7 +13544,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B20" t="s">
         <v>379</v>
@@ -13510,7 +13552,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B21" t="s">
         <v>1129</v>
@@ -13518,7 +13560,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B22" t="s">
         <v>1201</v>
@@ -13526,7 +13568,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B23" t="s">
         <v>1202</v>
@@ -13534,23 +13576,23 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B24" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B25" t="s">
-        <v>1520</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B26" t="s">
         <v>1303</v>
@@ -13562,12 +13604,12 @@
         <v>801</v>
       </c>
       <c r="E26" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B27" t="s">
         <v>804</v>
@@ -13575,7 +13617,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B28" t="s">
         <v>925</v>
@@ -13583,7 +13625,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B29" t="s">
         <v>379</v>
@@ -13669,7 +13711,7 @@
         <v>253</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>254</v>
@@ -13813,10 +13855,10 @@
         <v>442</v>
       </c>
       <c r="P4" t="s">
+        <v>1596</v>
+      </c>
+      <c r="Q4" t="s">
         <v>1597</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1598</v>
       </c>
       <c r="U4">
         <v>65</v>
@@ -13889,31 +13931,31 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B6" t="s">
         <v>1731</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>1732</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1733</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1734</v>
       </c>
       <c r="F6" t="s">
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="I6" t="s">
         <v>198</v>
       </c>
       <c r="J6" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="K6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="L6" t="s">
         <v>301</v>
@@ -13922,16 +13964,16 @@
         <v>301</v>
       </c>
       <c r="N6" t="s">
+        <v>1738</v>
+      </c>
+      <c r="O6" t="s">
         <v>1739</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>1740</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>1741</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1742</v>
       </c>
       <c r="R6" t="s">
         <v>303</v>
@@ -13949,7 +13991,7 @@
         <v>874</v>
       </c>
       <c r="Y6" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
   </sheetData>
@@ -13962,8 +14004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14039,7 +14081,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B3" t="s">
         <v>681</v>
@@ -14051,7 +14093,7 @@
         <v>299</v>
       </c>
       <c r="E3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -14068,7 +14110,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="C4" t="s">
         <v>336</v>
@@ -14091,7 +14133,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -14135,7 +14177,7 @@
         <v>1469</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1514</v>
@@ -14197,7 +14239,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B5" t="s">
         <v>1492</v>
@@ -14209,7 +14251,7 @@
         <v>738</v>
       </c>
       <c r="E5" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
   </sheetData>
@@ -14242,22 +14284,22 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1591</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1592</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1593</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1594</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1595</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1596</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -14361,22 +14403,22 @@
         <v>1479</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1521</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1522</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1523</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1524</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1525</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>1526</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -14387,10 +14429,10 @@
         <v>1497</v>
       </c>
       <c r="C2" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D2" t="s">
         <v>1528</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1529</v>
       </c>
       <c r="E2" s="4">
         <v>45257</v>
@@ -14481,34 +14523,34 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B4" t="s">
         <v>1535</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1536</v>
       </c>
-      <c r="C4" t="s">
-        <v>1537</v>
-      </c>
       <c r="D4" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E4" s="4">
         <v>45265</v>
       </c>
       <c r="G4" t="s">
+        <v>1537</v>
+      </c>
+      <c r="H4" t="s">
         <v>1538</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>1539</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="K4" t="s">
         <v>1540</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1542</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1541</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -14531,22 +14573,22 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B5" t="s">
         <v>1614</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>1615</v>
       </c>
-      <c r="C5" t="s">
-        <v>1616</v>
-      </c>
       <c r="D5" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E5" s="4">
         <v>44962</v>
       </c>
       <c r="G5" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -14690,7 +14732,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15108,7 +15150,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B8" t="s">
         <v>796</v>
@@ -15120,7 +15162,7 @@
         <v>301</v>
       </c>
       <c r="E8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>1341</v>
@@ -15280,7 +15322,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B11">
         <v>66</v>
@@ -15291,7 +15333,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B12">
         <v>67</v>
@@ -15302,7 +15344,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B13">
         <v>72</v>
@@ -15313,7 +15355,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B14">
         <v>83</v>
@@ -16709,7 +16751,7 @@
     </row>
     <row r="67" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B67" t="s">
         <v>502</v>
@@ -16718,13 +16760,13 @@
         <v>559</v>
       </c>
       <c r="E67" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="T67" t="s">
         <v>72</v>
       </c>
       <c r="AQ67" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="AW67">
         <v>1993</v>
@@ -16732,7 +16774,7 @@
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B68" t="s">
         <v>922</v>
@@ -16741,12 +16783,12 @@
         <v>560</v>
       </c>
       <c r="AS68" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="69" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B69" t="s">
         <v>503</v>
@@ -16755,12 +16797,12 @@
         <v>561</v>
       </c>
       <c r="AS69" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="70" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="B70" t="s">
         <v>506</v>
@@ -16769,12 +16811,12 @@
         <v>562</v>
       </c>
       <c r="AS70" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="71" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B71" t="s">
         <v>919</v>
@@ -16783,7 +16825,7 @@
         <v>563</v>
       </c>
       <c r="AA71" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="AB71">
         <v>123445</v>
@@ -16792,7 +16834,7 @@
         <v>12</v>
       </c>
       <c r="AP71" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="AW71">
         <v>1987</v>
@@ -16800,7 +16842,7 @@
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B72" t="s">
         <v>532</v>
@@ -16809,12 +16851,12 @@
         <v>564</v>
       </c>
       <c r="AD72" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B73" t="s">
         <v>513</v>
@@ -16835,21 +16877,21 @@
         <v>12</v>
       </c>
       <c r="V73" t="s">
+        <v>1758</v>
+      </c>
+      <c r="W73" t="s">
         <v>1759</v>
       </c>
-      <c r="W73" t="s">
+      <c r="Z73" t="s">
         <v>1760</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="AP73" t="s">
         <v>1761</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>1762</v>
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B74" t="s">
         <v>510</v>
@@ -16860,7 +16902,7 @@
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B75" t="s">
         <v>502</v>
@@ -16869,7 +16911,7 @@
         <v>561</v>
       </c>
       <c r="E75" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="T75" t="s">
         <v>574</v>
@@ -16883,7 +16925,7 @@
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B76" t="s">
         <v>922</v>
@@ -16892,12 +16934,12 @@
         <v>562</v>
       </c>
       <c r="AS76" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B77" t="s">
         <v>503</v>
@@ -16912,12 +16954,12 @@
         <v>123</v>
       </c>
       <c r="U77" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B78" t="s">
         <v>511</v>
@@ -16929,7 +16971,7 @@
         <v>900</v>
       </c>
       <c r="L78" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="U78" t="s">
         <v>574</v>
@@ -16937,7 +16979,7 @@
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B79" t="s">
         <v>507</v>
@@ -16946,24 +16988,24 @@
         <v>564</v>
       </c>
       <c r="E79" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="G79" s="13">
         <v>44053</v>
       </c>
       <c r="AD79" t="s">
+        <v>1782</v>
+      </c>
+      <c r="AM79" t="s">
         <v>1783</v>
       </c>
-      <c r="AM79" t="s">
+      <c r="AS79" t="s">
         <v>1784</v>
-      </c>
-      <c r="AS79" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B80" t="s">
         <v>516</v>
@@ -16972,12 +17014,12 @@
         <v>559</v>
       </c>
       <c r="AS80" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B81" t="s">
         <v>512</v>
@@ -16986,12 +17028,12 @@
         <v>560</v>
       </c>
       <c r="AS81" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B82" t="s">
         <v>520</v>
@@ -17006,18 +17048,18 @@
         <v>8900999</v>
       </c>
       <c r="Y82" t="s">
+        <v>1787</v>
+      </c>
+      <c r="AF82" t="s">
         <v>1788</v>
       </c>
-      <c r="AF82" t="s">
+      <c r="AP82" t="s">
         <v>1789</v>
-      </c>
-      <c r="AP82" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B83" t="s">
         <v>521</v>
@@ -17026,12 +17068,12 @@
         <v>562</v>
       </c>
       <c r="AF83" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B84" t="s">
         <v>513</v>
@@ -17049,19 +17091,19 @@
         <v>44866</v>
       </c>
       <c r="Q84" t="s">
+        <v>1765</v>
+      </c>
+      <c r="V84" t="s">
         <v>1766</v>
       </c>
-      <c r="V84" t="s">
+      <c r="W84" t="s">
         <v>1767</v>
-      </c>
-      <c r="W84" t="s">
-        <v>1768</v>
       </c>
       <c r="Z84">
         <v>909000</v>
       </c>
       <c r="AP84" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
   </sheetData>
@@ -17150,15 +17192,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B9" t="s">
         <v>1556</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1557</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B10" t="s">
         <v>386</v>
@@ -17166,10 +17208,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B11" t="s">
         <v>1752</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1753</v>
       </c>
     </row>
   </sheetData>
@@ -18489,8 +18531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CC5"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18622,7 +18664,7 @@
         <v>623</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>624</v>
@@ -18682,7 +18724,7 @@
         <v>640</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="AK1" s="3" t="s">
         <v>641</v>
@@ -19338,7 +19380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E3AF99-B285-4872-B012-0C94F438EBF8}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -19692,7 +19734,7 @@
         <v>45078</v>
       </c>
       <c r="M5" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PSP-7731: Automation fixes (#3778)
* Automation refactoring - Change of models and functions to avois warning messages

* Automation refactoring - Change of models and functions to avois warning messages

* Automation fixes related to new modals

---------

Co-authored-by: devinleighsmith <41091511+devinleighsmith@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSP\testing\PIMS.Tests.Automation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B58EF78-0322-41F8-9C32-E234072C6578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E08ADF-C39F-4060-B0F9-883BF2101C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="950" firstSheet="20" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="13" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -37,21 +37,20 @@
     <sheet name="DispositionFiles" sheetId="34" r:id="rId22"/>
     <sheet name="DispositionChecklist" sheetId="35" r:id="rId23"/>
     <sheet name="DispositionOfferSale" sheetId="36" r:id="rId24"/>
-    <sheet name="PurchaserNames" sheetId="38" r:id="rId25"/>
-    <sheet name="TeamMembers" sheetId="20" r:id="rId26"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId27"/>
-    <sheet name="Properties" sheetId="6" r:id="rId28"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId29"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId30"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId31"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId32"/>
-    <sheet name="Takes" sheetId="27" r:id="rId33"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId34"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId35"/>
-    <sheet name="Notes" sheetId="10" r:id="rId36"/>
+    <sheet name="TeamMembers" sheetId="20" r:id="rId25"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId26"/>
+    <sheet name="Properties" sheetId="6" r:id="rId27"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId28"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId29"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId30"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId31"/>
+    <sheet name="Takes" sheetId="27" r:id="rId32"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId33"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId34"/>
+    <sheet name="Notes" sheetId="10" r:id="rId35"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2883" uniqueCount="1840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1820">
   <si>
     <t>FirstName</t>
   </si>
@@ -4637,9 +4636,6 @@
     <t>ManagementPropertyActivitiesCount</t>
   </si>
   <si>
-    <t>009-536-892</t>
-  </si>
-  <si>
     <t>ManagementPropertyActivityInvoicesStartRow</t>
   </si>
   <si>
@@ -5534,67 +5530,10 @@
     <t>Automated Offer name Updated</t>
   </si>
   <si>
-    <t>SalesDetailsContactType</t>
-  </si>
-  <si>
-    <t>PurchaserName</t>
-  </si>
-  <si>
-    <t>PurchaserAgent</t>
-  </si>
-  <si>
-    <t>PurchaserSolicitor</t>
-  </si>
-  <si>
-    <t>LastConditionRemovalDate</t>
-  </si>
-  <si>
-    <t>SaleCompletionDate</t>
-  </si>
-  <si>
-    <t>FiscalYearOfSale</t>
-  </si>
-  <si>
-    <t>FinalSalePrice</t>
-  </si>
-  <si>
-    <t>RealtorCommission</t>
-  </si>
-  <si>
-    <t>GSTRequired</t>
-  </si>
-  <si>
-    <t>GSTCollected</t>
-  </si>
-  <si>
-    <t>NetBookValue</t>
-  </si>
-  <si>
-    <t>TotalCostOfSales</t>
-  </si>
-  <si>
-    <t>SPPAmount</t>
-  </si>
-  <si>
-    <t>RemediationCost</t>
-  </si>
-  <si>
-    <t>PurchaseMemberContactType</t>
-  </si>
-  <si>
-    <t>PurchaseMemberPrimaryContact</t>
-  </si>
-  <si>
-    <t>PurchaseNameStartRow</t>
-  </si>
-  <si>
-    <t>PurchaseNameTotalCount</t>
-  </si>
-  <si>
-    <t>Purchase 1</t>
-  </si>
-  <si>
-    <t>Purchase 2</t>
+    <t>DF From PIN</t>
+  </si>
+  <si>
+    <t>Automated Disposition File - From PIN</t>
   </si>
 </sst>
 </file>
@@ -6587,7 +6526,7 @@
         <v>314</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>326</v>
@@ -6880,10 +6819,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B10" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="C10" t="s">
         <v>273</v>
@@ -6941,7 +6880,7 @@
         <v>321</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>322</v>
@@ -6964,7 +6903,7 @@
         <v>328</v>
       </c>
       <c r="C2" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D2" t="s">
         <v>299</v>
@@ -6987,7 +6926,7 @@
         <v>329</v>
       </c>
       <c r="C3" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D3" t="s">
         <v>301</v>
@@ -7119,13 +7058,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B9" t="s">
         <v>1545</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>1546</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1547</v>
       </c>
       <c r="D9" t="s">
         <v>301</v>
@@ -7134,10 +7073,10 @@
         <v>301</v>
       </c>
       <c r="F9" t="s">
+        <v>1549</v>
+      </c>
+      <c r="G9" t="s">
         <v>1550</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1551</v>
       </c>
     </row>
   </sheetData>
@@ -7150,8 +7089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7199,7 +7138,7 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>916</v>
@@ -7265,7 +7204,7 @@
         <v>1083</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>1322</v>
@@ -7420,20 +7359,20 @@
         <v>5500502</v>
       </c>
       <c r="D3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F3" t="s">
         <v>1619</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1620</v>
       </c>
       <c r="G3" t="s">
         <v>1178</v>
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45326</v>
+        <v>45328</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7630,7 +7569,7 @@
         <v>5503710</v>
       </c>
       <c r="D5" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="E5" t="s">
         <v>1176</v>
@@ -7643,7 +7582,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45326</v>
+        <v>45328</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7837,20 +7776,20 @@
         <v>5500502</v>
       </c>
       <c r="D7" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F7" t="s">
         <v>1619</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1620</v>
       </c>
       <c r="G7" t="s">
         <v>1178</v>
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45326</v>
+        <v>45328</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8359,20 +8298,20 @@
         <v>5500502</v>
       </c>
       <c r="D12" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F12" t="s">
         <v>1619</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1620</v>
       </c>
       <c r="G12" t="s">
         <v>1178</v>
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45326</v>
+        <v>45328</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8671,20 +8610,20 @@
         <v>5500502</v>
       </c>
       <c r="D15" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F15" t="s">
         <v>1619</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1620</v>
       </c>
       <c r="G15" t="s">
         <v>1178</v>
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45326</v>
+        <v>45328</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8992,16 +8931,16 @@
         <v>5500502</v>
       </c>
       <c r="D19" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>1620</v>
+      </c>
+      <c r="F19" t="s">
         <v>1619</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1620</v>
-      </c>
       <c r="G19" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="L19" t="s">
         <v>881</v>
@@ -9410,7 +9349,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -9419,16 +9358,16 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
+        <v>1558</v>
+      </c>
+      <c r="H8" t="s">
         <v>1559</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>1560</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>1561</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1562</v>
       </c>
       <c r="M8" t="s">
         <v>72</v>
@@ -9440,10 +9379,10 @@
         <v>37</v>
       </c>
       <c r="Q8" t="s">
+        <v>1562</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>1563</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>1564</v>
       </c>
       <c r="S8">
         <v>7080009876</v>
@@ -9780,7 +9719,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B3" t="s">
         <v>1066</v>
@@ -10186,13 +10125,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B8" t="s">
         <v>559</v>
       </c>
       <c r="C8" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D8" t="s">
         <v>1109</v>
@@ -10227,7 +10166,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10550,7 +10489,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B16" t="s">
         <v>1130</v>
@@ -10642,7 +10581,7 @@
         <v>1147</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1148</v>
@@ -10698,7 +10637,7 @@
         <v>559</v>
       </c>
       <c r="F2" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G2" s="4">
         <v>45176</v>
@@ -10774,7 +10713,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -10789,7 +10728,7 @@
         <v>559</v>
       </c>
       <c r="F4" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G4" s="4">
         <v>45272</v>
@@ -10804,25 +10743,25 @@
         <v>45181</v>
       </c>
       <c r="K4" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="L4" t="s">
         <v>1171</v>
       </c>
       <c r="M4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="N4" t="s">
         <v>1573</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>1574</v>
       </c>
-      <c r="O4" t="s">
-        <v>1575</v>
-      </c>
       <c r="P4" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="Q4" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="R4" t="b">
         <v>1</v>
@@ -10831,7 +10770,7 @@
         <v>145556</v>
       </c>
       <c r="T4" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="U4">
         <v>5</v>
@@ -10959,10 +10898,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B6" t="s">
         <v>1577</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1578</v>
       </c>
       <c r="C6">
         <v>10000</v>
@@ -11621,19 +11560,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B6" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="C6" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D6" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E6" t="s">
         <v>1579</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1580</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -11787,10 +11726,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B7" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C7" s="11">
         <v>1000</v>
@@ -11813,10 +11752,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AC18" sqref="AC18"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11847,177 +11786,118 @@
     <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>994</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>1624</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1625</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1626</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1627</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>1770</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>1628</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>1771</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>1643</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1629</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1644</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>1630</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>836</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>1621</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>1622</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1623</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>1624</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="U1" s="19" t="s">
+        <v>1808</v>
+      </c>
+      <c r="V1" s="19" t="s">
         <v>1809</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>1810</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>1811</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1812</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1813</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1814</v>
       </c>
-      <c r="AA1" s="19" t="s">
-        <v>1815</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>1819</v>
-      </c>
-      <c r="AC1" s="19" t="s">
-        <v>1836</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>1837</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>1821</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>1822</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>1823</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>1824</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>1825</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>1826</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>1827</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>1828</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>1829</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>1830</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>1831</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>1832</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B2" t="s">
         <v>273</v>
       </c>
       <c r="F2" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="H2" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="I2" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="K2" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="O2" t="s">
         <v>846</v>
@@ -12043,23 +11923,17 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="6"/>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AH2" s="6"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="B3" t="s">
         <v>847</v>
       </c>
       <c r="C3" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D3" s="4">
         <v>45170</v>
@@ -12068,25 +11942,25 @@
         <v>45366</v>
       </c>
       <c r="F3" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="G3" t="s">
         <v>845</v>
       </c>
       <c r="H3" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I3" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="J3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="M3" s="4">
         <v>45323</v>
@@ -12095,7 +11969,7 @@
         <v>273</v>
       </c>
       <c r="O3" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="P3" t="s">
         <v>198</v>
@@ -12118,33 +11992,27 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="6"/>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AH3" s="6"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="B4" t="s">
         <v>1066</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45326</v>
+        <v>45328</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
       </c>
       <c r="F4" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="G4" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="H4" t="s">
         <v>1500</v>
@@ -12173,29 +12041,23 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="6"/>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AH4" s="6"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="B5" t="s">
         <v>559</v>
       </c>
       <c r="F5" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="H5" t="s">
+        <v>1725</v>
+      </c>
+      <c r="I5" t="s">
         <v>1726</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1727</v>
       </c>
       <c r="P5" t="s">
         <v>199</v>
@@ -12218,32 +12080,26 @@
       <c r="AA5">
         <v>0</v>
       </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="6"/>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AH5" s="6"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B6" t="s">
         <v>273</v>
       </c>
       <c r="F6" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="H6" t="s">
         <v>336</v>
       </c>
       <c r="I6" t="s">
+        <v>1727</v>
+      </c>
+      <c r="J6" t="s">
         <v>1728</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1729</v>
       </c>
       <c r="P6" t="s">
         <v>198</v>
@@ -12266,25 +12122,19 @@
       <c r="AA6">
         <v>0</v>
       </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B7" t="s">
         <v>273</v>
       </c>
       <c r="F7" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="H7" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I7" t="s">
         <v>364</v>
@@ -12310,28 +12160,22 @@
       <c r="AA7">
         <v>0</v>
       </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B8" t="s">
         <v>273</v>
       </c>
       <c r="F8" t="s">
+        <v>1723</v>
+      </c>
+      <c r="H8" t="s">
         <v>1724</v>
       </c>
-      <c r="H8" t="s">
-        <v>1725</v>
-      </c>
       <c r="I8" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="P8" t="s">
         <v>199</v>
@@ -12354,16 +12198,10 @@
       <c r="AA8">
         <v>0</v>
       </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>273</v>
@@ -12371,16 +12209,16 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="G9" s="20">
         <v>77665544</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>1645</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>1646</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>1647</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
@@ -12426,58 +12264,13 @@
       <c r="AA9" s="20">
         <v>2</v>
       </c>
-      <c r="AB9" s="20" t="s">
-        <v>736</v>
-      </c>
-      <c r="AC9" s="20">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="20">
-        <v>2</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="AF9" s="20" t="s">
-        <v>1203</v>
-      </c>
-      <c r="AG9" s="20" t="s">
-        <v>1139</v>
-      </c>
-      <c r="AH9" s="4">
-        <v>45352</v>
-      </c>
-      <c r="AI9" s="4">
-        <v>45505</v>
-      </c>
-      <c r="AJ9">
-        <v>2024</v>
-      </c>
-      <c r="AK9">
-        <v>50000</v>
-      </c>
-      <c r="AL9">
-        <v>10000</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>301</v>
-      </c>
-      <c r="AO9">
-        <v>750000</v>
-      </c>
-      <c r="AP9">
-        <v>800000</v>
-      </c>
-      <c r="AQ9">
-        <v>67000</v>
-      </c>
-      <c r="AR9">
-        <v>29000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>273</v>
@@ -12486,14 +12279,14 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I10" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -12532,30 +12325,24 @@
         <v>1</v>
       </c>
       <c r="AB10" s="20"/>
-      <c r="AC10" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="20">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="20"/>
-      <c r="AG10" s="20"/>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B11" t="s">
         <v>273</v>
       </c>
       <c r="F11" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="H11" t="s">
+        <v>1645</v>
+      </c>
+      <c r="I11" t="s">
         <v>1646</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1647</v>
       </c>
       <c r="P11" t="s">
         <v>198</v>
@@ -12578,28 +12365,22 @@
       <c r="AA11">
         <v>0</v>
       </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B12" t="s">
         <v>273</v>
       </c>
       <c r="F12" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="H12" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I12" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="P12" t="s">
         <v>200</v>
@@ -12622,10 +12403,42 @@
       <c r="AA12">
         <v>0</v>
       </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B13" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1819</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1500</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P13" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0</v>
+      </c>
+      <c r="S13" s="8">
+        <v>24</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
         <v>0</v>
       </c>
     </row>
@@ -12640,7 +12453,7 @@
   <dimension ref="A1:AJ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12671,97 +12484,97 @@
         <v>1032</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>1667</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>1668</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>1669</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>1670</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>1671</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>1672</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>1673</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>1674</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>1675</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="19" t="s">
         <v>1676</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>1677</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>1678</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>1679</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>1680</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>1681</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>1682</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>1683</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>1684</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>1685</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1686</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1687</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1688</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>1689</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>1690</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>1691</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
         <v>1692</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>1693</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>1694</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>1695</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>1696</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AJ1" s="19" t="s">
         <v>1697</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
@@ -12926,7 +12739,7 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>1066</v>
@@ -13061,33 +12874,33 @@
         <v>112</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1792</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>1793</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>1794</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>1795</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>1796</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1797</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>1798</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>1799</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D2" s="21">
         <v>45352</v>
@@ -13099,18 +12912,18 @@
         <v>550000</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D3" s="21">
         <v>45352</v>
@@ -13122,18 +12935,18 @@
         <v>550000</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D4" s="21">
         <v>45463</v>
@@ -13145,7 +12958,7 @@
         <v>1200.5</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -13163,68 +12976,11 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FABE200-F318-4425-94AC-190989D6516A}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1820</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1834</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1835</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1838</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1711</v>
-      </c>
-      <c r="C2" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1839</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="C3" t="s">
-        <v>736</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13241,16 +12997,16 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1648</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1649</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1650</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1651</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -13320,13 +13076,13 @@
         <v>853</v>
       </c>
       <c r="C6" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -13365,13 +13121,13 @@
         <v>908</v>
       </c>
       <c r="C9" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -13390,13 +13146,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B11" t="s">
         <v>850</v>
       </c>
       <c r="C11" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D11" t="s">
         <v>736</v>
@@ -13404,10 +13160,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B12" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="C12" t="s">
         <v>1385</v>
@@ -13418,13 +13174,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B13" t="s">
         <v>850</v>
       </c>
       <c r="C13" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D13" t="s">
         <v>736</v>
@@ -13432,13 +13188,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B14" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="C14" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D14" t="s">
         <v>736</v>
@@ -13446,7 +13202,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B15" t="s">
         <v>851</v>
@@ -13463,13 +13219,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B16" t="s">
         <v>908</v>
       </c>
       <c r="C16" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -13480,30 +13236,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B17" t="s">
         <v>853</v>
       </c>
       <c r="C17" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B18" t="s">
         <v>852</v>
       </c>
       <c r="C18" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -13514,13 +13270,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C19" t="s">
         <v>1716</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1717</v>
       </c>
       <c r="D19" t="s">
         <v>736</v>
@@ -13531,12 +13287,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13684,7 +13440,7 @@
         <v>1002</v>
       </c>
       <c r="E10" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -13697,7 +13453,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B12" t="s">
         <v>800</v>
@@ -13717,7 +13473,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B13" t="s">
         <v>804</v>
@@ -13725,7 +13481,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B14" t="s">
         <v>379</v>
@@ -13733,7 +13489,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B15" t="s">
         <v>925</v>
@@ -13761,7 +13517,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B17" t="s">
         <v>878</v>
@@ -13772,7 +13528,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B18" t="s">
         <v>884</v>
@@ -13788,7 +13544,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B20" t="s">
         <v>379</v>
@@ -13796,7 +13552,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B21" t="s">
         <v>1129</v>
@@ -13804,7 +13560,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B22" t="s">
         <v>1201</v>
@@ -13812,7 +13568,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B23" t="s">
         <v>1202</v>
@@ -13820,23 +13576,23 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B24" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B25" t="s">
-        <v>1520</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B26" t="s">
         <v>1303</v>
@@ -13848,12 +13604,12 @@
         <v>801</v>
       </c>
       <c r="E26" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B27" t="s">
         <v>804</v>
@@ -13861,7 +13617,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B28" t="s">
         <v>925</v>
@@ -13869,7 +13625,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B29" t="s">
         <v>379</v>
@@ -13881,12 +13637,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13955,7 +13711,7 @@
         <v>253</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>254</v>
@@ -14099,10 +13855,10 @@
         <v>442</v>
       </c>
       <c r="P4" t="s">
+        <v>1596</v>
+      </c>
+      <c r="Q4" t="s">
         <v>1597</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1598</v>
       </c>
       <c r="U4">
         <v>65</v>
@@ -14175,31 +13931,31 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B6" t="s">
         <v>1731</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>1732</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1733</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1734</v>
       </c>
       <c r="F6" t="s">
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="I6" t="s">
         <v>198</v>
       </c>
       <c r="J6" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="K6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="L6" t="s">
         <v>301</v>
@@ -14208,16 +13964,16 @@
         <v>301</v>
       </c>
       <c r="N6" t="s">
+        <v>1738</v>
+      </c>
+      <c r="O6" t="s">
         <v>1739</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>1740</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>1741</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1742</v>
       </c>
       <c r="R6" t="s">
         <v>303</v>
@@ -14235,7 +13991,7 @@
         <v>874</v>
       </c>
       <c r="Y6" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
   </sheetData>
@@ -14244,12 +14000,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14325,7 +14081,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B3" t="s">
         <v>681</v>
@@ -14337,7 +14093,7 @@
         <v>299</v>
       </c>
       <c r="E3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -14354,7 +14110,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="C4" t="s">
         <v>336</v>
@@ -14377,7 +14133,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -14393,6 +14149,113 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C2" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2" t="s">
+        <v>738</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D4" t="s">
+        <v>738</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C5" t="s">
+        <v>736</v>
+      </c>
+      <c r="D5" t="s">
+        <v>738</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14421,22 +14284,22 @@
         <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1591</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1592</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1593</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1594</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1595</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1596</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -14477,113 +14340,6 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1469</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1527</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1491</v>
-      </c>
-      <c r="C2" t="s">
-        <v>736</v>
-      </c>
-      <c r="D2" t="s">
-        <v>738</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>856</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C4" t="s">
-        <v>736</v>
-      </c>
-      <c r="D4" t="s">
-        <v>738</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C5" t="s">
-        <v>736</v>
-      </c>
-      <c r="D5" t="s">
-        <v>738</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -14647,22 +14403,22 @@
         <v>1479</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1521</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1522</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1523</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1524</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1525</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>1526</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -14673,10 +14429,10 @@
         <v>1497</v>
       </c>
       <c r="C2" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D2" t="s">
         <v>1528</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1529</v>
       </c>
       <c r="E2" s="4">
         <v>45257</v>
@@ -14767,34 +14523,34 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B4" t="s">
         <v>1535</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1536</v>
       </c>
-      <c r="C4" t="s">
-        <v>1537</v>
-      </c>
       <c r="D4" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E4" s="4">
         <v>45265</v>
       </c>
       <c r="G4" t="s">
+        <v>1537</v>
+      </c>
+      <c r="H4" t="s">
         <v>1538</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>1539</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>1541</v>
+      </c>
+      <c r="K4" t="s">
         <v>1540</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1542</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1541</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -14817,22 +14573,22 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B5" t="s">
         <v>1614</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>1615</v>
       </c>
-      <c r="C5" t="s">
-        <v>1616</v>
-      </c>
       <c r="D5" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E5" s="4">
         <v>44962</v>
       </c>
       <c r="G5" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -14858,7 +14614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -14971,12 +14727,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15394,7 +15150,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B8" t="s">
         <v>796</v>
@@ -15406,7 +15162,7 @@
         <v>301</v>
       </c>
       <c r="E8" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>1341</v>
@@ -15439,7 +15195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -15566,7 +15322,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B11">
         <v>66</v>
@@ -15577,7 +15333,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B12">
         <v>67</v>
@@ -15588,7 +15344,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B13">
         <v>72</v>
@@ -15599,7 +15355,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B14">
         <v>83</v>
@@ -15613,7 +15369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX84"/>
   <sheetViews>
@@ -16995,7 +16751,7 @@
     </row>
     <row r="67" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B67" t="s">
         <v>502</v>
@@ -17004,13 +16760,13 @@
         <v>559</v>
       </c>
       <c r="E67" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="T67" t="s">
         <v>72</v>
       </c>
       <c r="AQ67" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="AW67">
         <v>1993</v>
@@ -17018,7 +16774,7 @@
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B68" t="s">
         <v>922</v>
@@ -17027,12 +16783,12 @@
         <v>560</v>
       </c>
       <c r="AS68" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="69" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B69" t="s">
         <v>503</v>
@@ -17041,12 +16797,12 @@
         <v>561</v>
       </c>
       <c r="AS69" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="70" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="B70" t="s">
         <v>506</v>
@@ -17055,12 +16811,12 @@
         <v>562</v>
       </c>
       <c r="AS70" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="71" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B71" t="s">
         <v>919</v>
@@ -17069,7 +16825,7 @@
         <v>563</v>
       </c>
       <c r="AA71" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="AB71">
         <v>123445</v>
@@ -17078,7 +16834,7 @@
         <v>12</v>
       </c>
       <c r="AP71" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="AW71">
         <v>1987</v>
@@ -17086,7 +16842,7 @@
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B72" t="s">
         <v>532</v>
@@ -17095,12 +16851,12 @@
         <v>564</v>
       </c>
       <c r="AD72" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B73" t="s">
         <v>513</v>
@@ -17121,21 +16877,21 @@
         <v>12</v>
       </c>
       <c r="V73" t="s">
+        <v>1758</v>
+      </c>
+      <c r="W73" t="s">
         <v>1759</v>
       </c>
-      <c r="W73" t="s">
+      <c r="Z73" t="s">
         <v>1760</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="AP73" t="s">
         <v>1761</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>1762</v>
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B74" t="s">
         <v>510</v>
@@ -17146,7 +16902,7 @@
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B75" t="s">
         <v>502</v>
@@ -17155,7 +16911,7 @@
         <v>561</v>
       </c>
       <c r="E75" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="T75" t="s">
         <v>574</v>
@@ -17169,7 +16925,7 @@
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B76" t="s">
         <v>922</v>
@@ -17178,12 +16934,12 @@
         <v>562</v>
       </c>
       <c r="AS76" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B77" t="s">
         <v>503</v>
@@ -17198,12 +16954,12 @@
         <v>123</v>
       </c>
       <c r="U77" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B78" t="s">
         <v>511</v>
@@ -17215,7 +16971,7 @@
         <v>900</v>
       </c>
       <c r="L78" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="U78" t="s">
         <v>574</v>
@@ -17223,7 +16979,7 @@
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B79" t="s">
         <v>507</v>
@@ -17232,24 +16988,24 @@
         <v>564</v>
       </c>
       <c r="E79" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="G79" s="13">
         <v>44053</v>
       </c>
       <c r="AD79" t="s">
+        <v>1782</v>
+      </c>
+      <c r="AM79" t="s">
         <v>1783</v>
       </c>
-      <c r="AM79" t="s">
+      <c r="AS79" t="s">
         <v>1784</v>
-      </c>
-      <c r="AS79" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B80" t="s">
         <v>516</v>
@@ -17258,12 +17014,12 @@
         <v>559</v>
       </c>
       <c r="AS80" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B81" t="s">
         <v>512</v>
@@ -17272,12 +17028,12 @@
         <v>560</v>
       </c>
       <c r="AS81" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B82" t="s">
         <v>520</v>
@@ -17292,18 +17048,18 @@
         <v>8900999</v>
       </c>
       <c r="Y82" t="s">
+        <v>1787</v>
+      </c>
+      <c r="AF82" t="s">
         <v>1788</v>
       </c>
-      <c r="AF82" t="s">
+      <c r="AP82" t="s">
         <v>1789</v>
-      </c>
-      <c r="AP82" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B83" t="s">
         <v>521</v>
@@ -17312,12 +17068,12 @@
         <v>562</v>
       </c>
       <c r="AF83" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B84" t="s">
         <v>513</v>
@@ -17335,19 +17091,19 @@
         <v>44866</v>
       </c>
       <c r="Q84" t="s">
+        <v>1765</v>
+      </c>
+      <c r="V84" t="s">
         <v>1766</v>
       </c>
-      <c r="V84" t="s">
+      <c r="W84" t="s">
         <v>1767</v>
-      </c>
-      <c r="W84" t="s">
-        <v>1768</v>
       </c>
       <c r="Z84">
         <v>909000</v>
       </c>
       <c r="AP84" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
   </sheetData>
@@ -17356,7 +17112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -17436,15 +17192,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B9" t="s">
         <v>1556</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1557</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B10" t="s">
         <v>386</v>
@@ -17452,10 +17208,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B11" t="s">
         <v>1752</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1753</v>
       </c>
     </row>
   </sheetData>
@@ -18775,8 +18531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CC5"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18908,7 +18664,7 @@
         <v>623</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>624</v>
@@ -18968,7 +18724,7 @@
         <v>640</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="AK1" s="3" t="s">
         <v>641</v>
@@ -19978,7 +19734,7 @@
         <v>45078</v>
       </c>
       <c r="M5" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disposition Files - Offers and Sale Tab
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E08ADF-C39F-4060-B0F9-883BF2101C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A672A3-863C-466A-9FCD-8B60D8AD5BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="13" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="12" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -37,23 +37,23 @@
     <sheet name="DispositionFiles" sheetId="34" r:id="rId22"/>
     <sheet name="DispositionChecklist" sheetId="35" r:id="rId23"/>
     <sheet name="DispositionOfferSale" sheetId="36" r:id="rId24"/>
-    <sheet name="TeamMembers" sheetId="20" r:id="rId25"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId26"/>
-    <sheet name="Properties" sheetId="6" r:id="rId27"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId28"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId29"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId30"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId31"/>
-    <sheet name="Takes" sheetId="27" r:id="rId32"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId33"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId34"/>
-    <sheet name="Notes" sheetId="10" r:id="rId35"/>
+    <sheet name="PurchaserNames" sheetId="37" r:id="rId25"/>
+    <sheet name="TeamMembers" sheetId="20" r:id="rId26"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId27"/>
+    <sheet name="Properties" sheetId="6" r:id="rId28"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId29"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId30"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId31"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId32"/>
+    <sheet name="Takes" sheetId="27" r:id="rId33"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId34"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId35"/>
+    <sheet name="Notes" sheetId="10" r:id="rId36"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1854">
   <si>
     <t>FirstName</t>
   </si>
@@ -5173,9 +5173,6 @@
     <t>AcqSearchPropertiesIndex</t>
   </si>
   <si>
-    <t>DisSearchPropertiesIndex</t>
-  </si>
-  <si>
     <t>LeaseSearchPropertiesIndex</t>
   </si>
   <si>
@@ -5500,12 +5497,6 @@
     <t>Update Automated Disposition File Offers and Sales</t>
   </si>
   <si>
-    <t>AppraisalAndAssessmentAppraisalValue</t>
-  </si>
-  <si>
-    <t>AppraisalAndAssessmentAppraisalDate</t>
-  </si>
-  <si>
     <t>AppraisalAndAssessmentBcAssessmentValue</t>
   </si>
   <si>
@@ -5534,6 +5525,117 @@
   </si>
   <si>
     <t>Automated Disposition File - From PIN</t>
+  </si>
+  <si>
+    <t>PurchaseNameStartRow</t>
+  </si>
+  <si>
+    <t>PurchaseNameTotalCount</t>
+  </si>
+  <si>
+    <t>PurchaserName</t>
+  </si>
+  <si>
+    <t>PurchaseMemberContactType</t>
+  </si>
+  <si>
+    <t>PurchaseMemberPrimaryContact</t>
+  </si>
+  <si>
+    <t>Create DF with Offer and Sales Tab</t>
+  </si>
+  <si>
+    <t>Edit DF with Offer and Sales Tab</t>
+  </si>
+  <si>
+    <t>Al Dommasch</t>
+  </si>
+  <si>
+    <t>Al Radke</t>
+  </si>
+  <si>
+    <t>PurchaserAgent</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitor</t>
+  </si>
+  <si>
+    <t>LastConditionRemovalDate</t>
+  </si>
+  <si>
+    <t>SaleCompletionDate</t>
+  </si>
+  <si>
+    <t>FiscalYearOfSale</t>
+  </si>
+  <si>
+    <t>FinalSalePrice</t>
+  </si>
+  <si>
+    <t>RealtorCommission</t>
+  </si>
+  <si>
+    <t>GSTRequired</t>
+  </si>
+  <si>
+    <t>NetBookValue</t>
+  </si>
+  <si>
+    <t>TotalCostOfSales</t>
+  </si>
+  <si>
+    <t>SPPAmount</t>
+  </si>
+  <si>
+    <t>RemediationCost</t>
+  </si>
+  <si>
+    <t>NetProceedsBeforeSPP</t>
+  </si>
+  <si>
+    <t>NetProceedsAfterSPP</t>
+  </si>
+  <si>
+    <t>OwnerSolicitorPrimaryContact</t>
+  </si>
+  <si>
+    <t>Joahn Eyles</t>
+  </si>
+  <si>
+    <t>PurchaserAgentPrimaryContact</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitorPrimaryContact</t>
+  </si>
+  <si>
+    <t>Aalten Richard MINERS</t>
+  </si>
+  <si>
+    <t>YASUSHI NOMA</t>
+  </si>
+  <si>
+    <t>PurchaserAgentType</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitorType</t>
+  </si>
+  <si>
+    <t>GSTCollected</t>
+  </si>
+  <si>
+    <t>DispositionAssignedDate</t>
+  </si>
+  <si>
+    <t>DispositionPhysicalFileStatus</t>
+  </si>
+  <si>
+    <t>DispositionSearchPropertiesIndex</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentDate</t>
   </si>
 </sst>
 </file>
@@ -6526,7 +6628,7 @@
         <v>314</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>326</v>
@@ -7087,10 +7189,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
-  <dimension ref="A1:AJ19"/>
+  <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7115,25 +7217,26 @@
     <col min="18" max="18" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -7198,52 +7301,55 @@
         <v>864</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>1840</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>1080</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>1083</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1698</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1068</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1085</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1086</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1112</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1113</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1199</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>1377</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>1378</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1343</v>
       </c>
@@ -7300,55 +7406,58 @@
         <v>2</v>
       </c>
       <c r="U2" t="s">
-        <v>865</v>
+        <v>1651</v>
       </c>
       <c r="V2" t="s">
+        <v>1653</v>
+      </c>
+      <c r="W2" t="s">
         <v>1084</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>1081</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>15</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>5</v>
       </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
       <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
         <v>1</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>4</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>10</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
       </c>
       <c r="AG2">
         <v>1</v>
       </c>
-      <c r="AH2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI2">
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="6">
         <v>0</v>
       </c>
       <c r="AJ2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1344</v>
       </c>
@@ -7372,7 +7481,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7407,18 +7516,15 @@
       <c r="U3" t="s">
         <v>349</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>1203</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>1302</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>16</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
       <c r="Z3">
         <v>0</v>
       </c>
@@ -7426,34 +7532,37 @@
         <v>0</v>
       </c>
       <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
         <v>5</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>2</v>
       </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
         <v>2</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>1</v>
       </c>
-      <c r="AH3" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI3">
+      <c r="AI3" s="6">
         <v>0</v>
       </c>
       <c r="AJ3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1350</v>
       </c>
@@ -7510,55 +7619,58 @@
         <v>2</v>
       </c>
       <c r="U4" t="s">
-        <v>865</v>
+        <v>1651</v>
       </c>
       <c r="V4" t="s">
+        <v>1841</v>
+      </c>
+      <c r="W4" t="s">
         <v>1084</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>1081</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>15</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>1</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>5</v>
       </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
       <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
         <v>1</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>4</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>1</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>10</v>
-      </c>
-      <c r="AF4">
-        <v>1</v>
       </c>
       <c r="AG4">
         <v>1</v>
       </c>
-      <c r="AH4" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI4">
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="6">
         <v>0</v>
       </c>
       <c r="AJ4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1351</v>
       </c>
@@ -7582,7 +7694,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7614,18 +7726,15 @@
       <c r="U5" t="s">
         <v>349</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>1203</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>1302</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>16</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
       <c r="Z5">
         <v>0</v>
       </c>
@@ -7633,34 +7742,37 @@
         <v>0</v>
       </c>
       <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
         <v>5</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>2</v>
       </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
         <v>2</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>1</v>
       </c>
-      <c r="AH5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI5">
+      <c r="AI5" s="6">
         <v>0</v>
       </c>
       <c r="AJ5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1349</v>
       </c>
@@ -7719,53 +7831,53 @@
       <c r="U6" t="s">
         <v>865</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>1084</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>1081</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>15</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>1</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>5</v>
       </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
       <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
         <v>1</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>4</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>1</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>10</v>
-      </c>
-      <c r="AF6">
-        <v>1</v>
       </c>
       <c r="AG6">
         <v>1</v>
       </c>
-      <c r="AH6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="6">
         <v>0</v>
       </c>
       <c r="AJ6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1344</v>
       </c>
@@ -7789,7 +7901,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -7821,53 +7933,53 @@
       <c r="U7" t="s">
         <v>349</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>1203</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>1302</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>18</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>6</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>1</v>
       </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
       <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
         <v>5</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>2</v>
       </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <v>2</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <v>1</v>
       </c>
-      <c r="AH7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI7">
+      <c r="AI7" s="6">
         <v>0</v>
       </c>
       <c r="AJ7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1353</v>
       </c>
@@ -7926,53 +8038,53 @@
       <c r="U8" t="s">
         <v>865</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>1084</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>1081</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>15</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>1</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>5</v>
-      </c>
-      <c r="AA8">
-        <v>1</v>
       </c>
       <c r="AB8">
         <v>1</v>
       </c>
       <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
         <v>4</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>1</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>10</v>
-      </c>
-      <c r="AF8">
-        <v>1</v>
       </c>
       <c r="AG8">
         <v>1</v>
       </c>
-      <c r="AH8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI8">
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="6">
         <v>0</v>
       </c>
       <c r="AJ8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1355</v>
       </c>
@@ -8029,55 +8141,58 @@
         <v>2</v>
       </c>
       <c r="U9" t="s">
-        <v>865</v>
+        <v>1651</v>
       </c>
       <c r="V9" t="s">
+        <v>278</v>
+      </c>
+      <c r="W9" t="s">
         <v>1084</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>1081</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>15</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>1</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>5</v>
       </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
       <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
         <v>1</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>4</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>1</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>10</v>
-      </c>
-      <c r="AF9">
-        <v>1</v>
       </c>
       <c r="AG9">
         <v>1</v>
       </c>
-      <c r="AH9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI9">
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="6">
         <v>0</v>
       </c>
       <c r="AJ9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1357</v>
       </c>
@@ -8136,53 +8251,53 @@
       <c r="U10" t="s">
         <v>865</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>1084</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>1081</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>15</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>1</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>5</v>
       </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
       <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
         <v>1</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>4</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>1</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>10</v>
-      </c>
-      <c r="AF10">
-        <v>1</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
-      <c r="AH10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI10">
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="6">
         <v>0</v>
       </c>
       <c r="AJ10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1359</v>
       </c>
@@ -8241,53 +8356,53 @@
       <c r="U11" t="s">
         <v>865</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>1084</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>1081</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>15</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>1</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>5</v>
       </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
       <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
         <v>1</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>4</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>1</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>10</v>
-      </c>
-      <c r="AF11">
-        <v>1</v>
       </c>
       <c r="AG11">
         <v>1</v>
       </c>
-      <c r="AH11" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI11">
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="6">
         <v>0</v>
       </c>
       <c r="AJ11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1360</v>
       </c>
@@ -8311,7 +8426,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8341,20 +8456,20 @@
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>349</v>
+        <v>1651</v>
       </c>
       <c r="V12" t="s">
+        <v>1652</v>
+      </c>
+      <c r="W12" t="s">
         <v>1203</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>1302</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>16</v>
       </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
       <c r="Z12">
         <v>0</v>
       </c>
@@ -8362,34 +8477,37 @@
         <v>0</v>
       </c>
       <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
         <v>5</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>2</v>
       </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
       <c r="AE12">
         <v>0</v>
       </c>
       <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
         <v>2</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>1</v>
       </c>
-      <c r="AH12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI12">
+      <c r="AI12" s="6">
         <v>0</v>
       </c>
       <c r="AJ12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1363</v>
       </c>
@@ -8448,53 +8566,53 @@
       <c r="U13" t="s">
         <v>865</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>1084</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>1081</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>20</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>1</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>5</v>
       </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
       <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>1</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>4</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>1</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>10</v>
-      </c>
-      <c r="AF13">
-        <v>1</v>
       </c>
       <c r="AG13">
         <v>1</v>
       </c>
-      <c r="AH13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI13">
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="6">
         <v>0</v>
       </c>
       <c r="AJ13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1365</v>
       </c>
@@ -8553,53 +8671,53 @@
       <c r="U14" t="s">
         <v>865</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>1084</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>1081</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>21</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>1</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>5</v>
       </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
       <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
         <v>1</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>4</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>1</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>10</v>
-      </c>
-      <c r="AF14">
-        <v>1</v>
       </c>
       <c r="AG14">
         <v>1</v>
       </c>
-      <c r="AH14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI14">
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="6">
         <v>0</v>
       </c>
       <c r="AJ14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1366</v>
       </c>
@@ -8623,7 +8741,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8655,18 +8773,15 @@
       <c r="U15" t="s">
         <v>349</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>1203</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>1302</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>22</v>
       </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
       <c r="Z15">
         <v>0</v>
       </c>
@@ -8674,34 +8789,37 @@
         <v>0</v>
       </c>
       <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
         <v>5</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>2</v>
       </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
         <v>2</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI15">
+      <c r="AI15" s="6">
         <v>0</v>
       </c>
       <c r="AJ15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1082</v>
       </c>
@@ -8732,18 +8850,15 @@
       <c r="U16" t="s">
         <v>1384</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>1385</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>1393</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>16</v>
       </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
       <c r="Z16">
         <v>0</v>
       </c>
@@ -8757,28 +8872,31 @@
         <v>0</v>
       </c>
       <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
         <v>13</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>2</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
       <c r="AG16">
         <v>0</v>
       </c>
-      <c r="AH16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI16">
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
         <v>1</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1114</v>
       </c>
@@ -8806,9 +8924,6 @@
       <c r="T17" s="8">
         <v>0</v>
       </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
       <c r="Y17">
         <v>0</v>
       </c>
@@ -8836,17 +8951,20 @@
       <c r="AG17">
         <v>0</v>
       </c>
-      <c r="AH17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI17">
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
         <v>4</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>879</v>
       </c>
@@ -8880,12 +8998,9 @@
       <c r="U18" t="s">
         <v>883</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>19</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
       <c r="Z18">
         <v>0</v>
       </c>
@@ -8910,17 +9025,20 @@
       <c r="AG18">
         <v>0</v>
       </c>
-      <c r="AH18" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI18">
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="6">
         <v>0</v>
       </c>
       <c r="AJ18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>880</v>
       </c>
@@ -8963,43 +9081,43 @@
       <c r="T19" s="8">
         <v>1</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>17</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>7</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>1</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>2</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>7</v>
       </c>
-      <c r="AC19">
+      <c r="AD19">
         <v>1</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>15</v>
       </c>
-      <c r="AE19">
+      <c r="AF19">
         <v>1</v>
       </c>
-      <c r="AF19">
+      <c r="AG19">
         <v>3</v>
       </c>
-      <c r="AG19">
+      <c r="AH19">
         <v>1</v>
       </c>
-      <c r="AH19" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI19">
+      <c r="AI19" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
         <v>5</v>
       </c>
-      <c r="AJ19">
+      <c r="AK19">
         <v>1</v>
       </c>
     </row>
@@ -11752,10 +11870,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11763,8 +11881,8 @@
     <col min="1" max="1" width="41.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1796875" customWidth="1"/>
     <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.1796875" customWidth="1"/>
@@ -11772,32 +11890,44 @@
     <col min="11" max="11" width="19.1796875" customWidth="1"/>
     <col min="12" max="12" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.453125" customWidth="1"/>
-    <col min="14" max="14" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.1796875" customWidth="1"/>
     <col min="16" max="16" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.36328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="40.36328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="42.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.54296875" customWidth="1"/>
+    <col min="35" max="35" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12" customWidth="1"/>
+    <col min="43" max="43" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -11805,10 +11935,10 @@
         <v>1641</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>994</v>
+        <v>1849</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1631</v>
@@ -11826,7 +11956,7 @@
         <v>1627</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1628</v>
@@ -11838,7 +11968,7 @@
         <v>1629</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>836</v>
+        <v>1850</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>1630</v>
@@ -11853,34 +11983,97 @@
         <v>1623</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>1699</v>
+        <v>1851</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="U1" s="19" t="s">
+        <v>1852</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>1853</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>1807</v>
+      </c>
+      <c r="X1" s="19" t="s">
         <v>1808</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1809</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1810</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1811</v>
       </c>
-      <c r="Y1" s="19" t="s">
-        <v>1812</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>1813</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB1" s="3" t="s">
+        <v>1817</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>1818</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>1846</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>1842</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>1827</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>1847</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>1843</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>1829</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>1831</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1832</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>1848</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>1835</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>1838</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>1836</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>1839</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1634</v>
       </c>
@@ -11894,7 +12087,7 @@
         <v>1645</v>
       </c>
       <c r="I2" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="K2" t="s">
         <v>1642</v>
@@ -11923,9 +12116,15 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AH2" s="6"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="6"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1633</v>
       </c>
@@ -11951,16 +12150,16 @@
         <v>1640</v>
       </c>
       <c r="I3" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J3" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="M3" s="4">
         <v>45323</v>
@@ -11992,9 +12191,15 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="6"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1632</v>
       </c>
@@ -12003,7 +12208,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12012,7 +12217,7 @@
         <v>1637</v>
       </c>
       <c r="G4" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="H4" t="s">
         <v>1500</v>
@@ -12041,9 +12246,15 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="6"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1635</v>
       </c>
@@ -12054,10 +12265,10 @@
         <v>1638</v>
       </c>
       <c r="H5" t="s">
+        <v>1724</v>
+      </c>
+      <c r="I5" t="s">
         <v>1725</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1726</v>
       </c>
       <c r="P5" t="s">
         <v>199</v>
@@ -12080,26 +12291,32 @@
       <c r="AA5">
         <v>0</v>
       </c>
-      <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="6"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B6" t="s">
         <v>273</v>
       </c>
       <c r="F6" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="H6" t="s">
         <v>336</v>
       </c>
       <c r="I6" t="s">
+        <v>1726</v>
+      </c>
+      <c r="J6" t="s">
         <v>1727</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1728</v>
       </c>
       <c r="P6" t="s">
         <v>198</v>
@@ -12122,16 +12339,22 @@
       <c r="AA6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B7" t="s">
         <v>273</v>
       </c>
       <c r="F7" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="H7" t="s">
         <v>1640</v>
@@ -12160,19 +12383,25 @@
       <c r="AA7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B8" t="s">
         <v>273</v>
       </c>
       <c r="F8" t="s">
+        <v>1722</v>
+      </c>
+      <c r="H8" t="s">
         <v>1723</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1724</v>
       </c>
       <c r="I8" t="s">
         <v>1646</v>
@@ -12198,10 +12427,16 @@
       <c r="AA8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>273</v>
@@ -12209,7 +12444,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="G9" s="20">
         <v>77665544</v>
@@ -12264,13 +12499,70 @@
       <c r="AA9" s="20">
         <v>2</v>
       </c>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB9" s="20">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="20" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AE9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1841</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>1844</v>
+      </c>
+      <c r="AH9" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>45513</v>
+      </c>
+      <c r="AK9" s="4">
+        <v>45482</v>
+      </c>
+      <c r="AL9">
+        <v>2024</v>
+      </c>
+      <c r="AM9">
+        <v>1000000</v>
+      </c>
+      <c r="AN9">
+        <v>10000</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP9">
+        <v>50000</v>
+      </c>
+      <c r="AQ9">
+        <v>25000</v>
+      </c>
+      <c r="AR9">
+        <v>12000.99</v>
+      </c>
+      <c r="AS9">
+        <v>902999.01</v>
+      </c>
+      <c r="AT9">
+        <v>1200</v>
+      </c>
+      <c r="AU9">
+        <v>901799.01</v>
+      </c>
+      <c r="AV9">
+        <v>1988.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>273</v>
@@ -12279,14 +12571,14 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" t="s">
         <v>1640</v>
       </c>
       <c r="I10" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -12324,19 +12616,56 @@
       <c r="AA10" s="20">
         <v>1</v>
       </c>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB10" s="20">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="20">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="20" t="s">
+        <v>1845</v>
+      </c>
+      <c r="AE10" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="AF10" s="20"/>
+      <c r="AG10" t="s">
+        <v>1711</v>
+      </c>
+      <c r="AH10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>1712</v>
+      </c>
+      <c r="AJ10" s="21">
+        <v>45209</v>
+      </c>
+      <c r="AK10" s="4">
+        <v>46368</v>
+      </c>
+      <c r="AL10">
+        <v>2026</v>
+      </c>
+      <c r="AM10">
+        <v>544900</v>
+      </c>
+      <c r="AN10">
+        <v>4900</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B11" t="s">
         <v>273</v>
       </c>
       <c r="F11" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="H11" t="s">
         <v>1645</v>
@@ -12365,22 +12694,28 @@
       <c r="AA11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B12" t="s">
         <v>273</v>
       </c>
       <c r="F12" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="H12" t="s">
         <v>1640</v>
       </c>
       <c r="I12" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="P12" t="s">
         <v>200</v>
@@ -12403,16 +12738,22 @@
       <c r="AA12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="B13" t="s">
         <v>273</v>
       </c>
       <c r="F13" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="H13" t="s">
         <v>1500</v>
@@ -12439,6 +12780,12 @@
         <v>0</v>
       </c>
       <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>0</v>
       </c>
     </row>
@@ -12854,9 +13201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12874,33 +13219,33 @@
         <v>112</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1791</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>1792</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>1793</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>1794</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>1795</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1796</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>1797</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>1798</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="D2" s="21">
         <v>45352</v>
@@ -12912,18 +13257,18 @@
         <v>550000</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="D3" s="21">
         <v>45352</v>
@@ -12935,18 +13280,18 @@
         <v>550000</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="D4" s="21">
         <v>45463</v>
@@ -12958,7 +13303,7 @@
         <v>1200.5</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -12976,11 +13321,121 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAD653A-DB80-460C-86DB-ACD85A6EF957}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C5" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13160,10 +13615,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B12" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="C12" t="s">
         <v>1385</v>
@@ -13174,13 +13629,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B13" t="s">
         <v>850</v>
       </c>
       <c r="C13" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D13" t="s">
         <v>736</v>
@@ -13188,13 +13643,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B14" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C14" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D14" t="s">
         <v>736</v>
@@ -13202,7 +13657,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B15" t="s">
         <v>851</v>
@@ -13219,13 +13674,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B16" t="s">
         <v>908</v>
       </c>
       <c r="C16" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -13236,30 +13691,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B17" t="s">
         <v>853</v>
       </c>
       <c r="C17" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B18" t="s">
         <v>852</v>
       </c>
       <c r="C18" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -13270,13 +13725,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C19" t="s">
         <v>1715</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1716</v>
       </c>
       <c r="D19" t="s">
         <v>736</v>
@@ -13287,12 +13742,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13440,7 +13895,7 @@
         <v>1002</v>
       </c>
       <c r="E10" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -13592,7 +14047,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B26" t="s">
         <v>1303</v>
@@ -13604,12 +14059,12 @@
         <v>801</v>
       </c>
       <c r="E26" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B27" t="s">
         <v>804</v>
@@ -13617,7 +14072,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B28" t="s">
         <v>925</v>
@@ -13625,7 +14080,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B29" t="s">
         <v>379</v>
@@ -13637,7 +14092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
@@ -13711,7 +14166,7 @@
         <v>253</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>254</v>
@@ -13931,31 +14386,31 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B6" t="s">
         <v>1730</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>1731</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1732</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1733</v>
       </c>
       <c r="F6" t="s">
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="I6" t="s">
         <v>198</v>
       </c>
       <c r="J6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="K6" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="L6" t="s">
         <v>301</v>
@@ -13964,16 +14419,16 @@
         <v>301</v>
       </c>
       <c r="N6" t="s">
+        <v>1737</v>
+      </c>
+      <c r="O6" t="s">
         <v>1738</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>1739</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>1740</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1741</v>
       </c>
       <c r="R6" t="s">
         <v>303</v>
@@ -13991,7 +14446,7 @@
         <v>874</v>
       </c>
       <c r="Y6" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
   </sheetData>
@@ -14000,7 +14455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -14149,113 +14604,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1469</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1526</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1491</v>
-      </c>
-      <c r="C2" t="s">
-        <v>736</v>
-      </c>
-      <c r="D2" t="s">
-        <v>738</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>856</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C4" t="s">
-        <v>736</v>
-      </c>
-      <c r="D4" t="s">
-        <v>738</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1532</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C5" t="s">
-        <v>736</v>
-      </c>
-      <c r="D5" t="s">
-        <v>738</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14340,6 +14688,113 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C2" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2" t="s">
+        <v>738</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D4" t="s">
+        <v>738</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C5" t="s">
+        <v>736</v>
+      </c>
+      <c r="D5" t="s">
+        <v>738</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -14614,7 +15069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -14727,7 +15182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -15195,7 +15650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -15344,7 +15799,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B13">
         <v>72</v>
@@ -15355,7 +15810,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B14">
         <v>83</v>
@@ -15369,7 +15824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX84"/>
   <sheetViews>
@@ -16856,7 +17311,7 @@
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="B73" t="s">
         <v>513</v>
@@ -16877,21 +17332,21 @@
         <v>12</v>
       </c>
       <c r="V73" t="s">
+        <v>1757</v>
+      </c>
+      <c r="W73" t="s">
         <v>1758</v>
       </c>
-      <c r="W73" t="s">
+      <c r="Z73" t="s">
         <v>1759</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="AP73" t="s">
         <v>1760</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>1761</v>
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B74" t="s">
         <v>510</v>
@@ -16902,7 +17357,7 @@
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B75" t="s">
         <v>502</v>
@@ -16911,7 +17366,7 @@
         <v>561</v>
       </c>
       <c r="E75" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="T75" t="s">
         <v>574</v>
@@ -16925,7 +17380,7 @@
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B76" t="s">
         <v>922</v>
@@ -16934,12 +17389,12 @@
         <v>562</v>
       </c>
       <c r="AS76" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B77" t="s">
         <v>503</v>
@@ -16954,12 +17409,12 @@
         <v>123</v>
       </c>
       <c r="U77" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B78" t="s">
         <v>511</v>
@@ -16971,7 +17426,7 @@
         <v>900</v>
       </c>
       <c r="L78" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="U78" t="s">
         <v>574</v>
@@ -16979,7 +17434,7 @@
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B79" t="s">
         <v>507</v>
@@ -16988,24 +17443,24 @@
         <v>564</v>
       </c>
       <c r="E79" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="G79" s="13">
         <v>44053</v>
       </c>
       <c r="AD79" t="s">
+        <v>1781</v>
+      </c>
+      <c r="AM79" t="s">
         <v>1782</v>
       </c>
-      <c r="AM79" t="s">
+      <c r="AS79" t="s">
         <v>1783</v>
-      </c>
-      <c r="AS79" t="s">
-        <v>1784</v>
       </c>
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B80" t="s">
         <v>516</v>
@@ -17014,12 +17469,12 @@
         <v>559</v>
       </c>
       <c r="AS80" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B81" t="s">
         <v>512</v>
@@ -17028,12 +17483,12 @@
         <v>560</v>
       </c>
       <c r="AS81" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B82" t="s">
         <v>520</v>
@@ -17048,18 +17503,18 @@
         <v>8900999</v>
       </c>
       <c r="Y82" t="s">
+        <v>1786</v>
+      </c>
+      <c r="AF82" t="s">
         <v>1787</v>
       </c>
-      <c r="AF82" t="s">
+      <c r="AP82" t="s">
         <v>1788</v>
-      </c>
-      <c r="AP82" t="s">
-        <v>1789</v>
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B83" t="s">
         <v>521</v>
@@ -17068,12 +17523,12 @@
         <v>562</v>
       </c>
       <c r="AF83" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="B84" t="s">
         <v>513</v>
@@ -17091,19 +17546,19 @@
         <v>44866</v>
       </c>
       <c r="Q84" t="s">
+        <v>1764</v>
+      </c>
+      <c r="V84" t="s">
         <v>1765</v>
       </c>
-      <c r="V84" t="s">
+      <c r="W84" t="s">
         <v>1766</v>
-      </c>
-      <c r="W84" t="s">
-        <v>1767</v>
       </c>
       <c r="Z84">
         <v>909000</v>
       </c>
       <c r="AP84" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
   </sheetData>
@@ -17112,7 +17567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -17200,7 +17655,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B10" t="s">
         <v>386</v>
@@ -17208,10 +17663,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B11" t="s">
         <v>1751</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1752</v>
       </c>
     </row>
   </sheetData>
@@ -18724,7 +19179,7 @@
         <v>640</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="AK1" s="3" t="s">
         <v>641</v>

</xml_diff>

<commit_message>
PSP-7731: Automation Task (#3784)
* Automation refactoring - Change of models and functions to avois warning messages

* Automation refactoring - Change of models and functions to avois warning messages

* Automation fixes related to new modals

* Disposition Files - Offers and Sale Tab

* Disposition Files - Offers and Sale Tab

---------

Co-authored-by: devinleighsmith <41091511+devinleighsmith@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\Quartech Projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E08ADF-C39F-4060-B0F9-883BF2101C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A672A3-863C-466A-9FCD-8B60D8AD5BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="13" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="950" firstSheet="12" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -37,23 +37,23 @@
     <sheet name="DispositionFiles" sheetId="34" r:id="rId22"/>
     <sheet name="DispositionChecklist" sheetId="35" r:id="rId23"/>
     <sheet name="DispositionOfferSale" sheetId="36" r:id="rId24"/>
-    <sheet name="TeamMembers" sheetId="20" r:id="rId25"/>
-    <sheet name="SearchProperties" sheetId="8" r:id="rId26"/>
-    <sheet name="Properties" sheetId="6" r:id="rId27"/>
-    <sheet name="PropertyManagement" sheetId="30" r:id="rId28"/>
-    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId29"/>
-    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId30"/>
-    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId31"/>
-    <sheet name="Takes" sheetId="27" r:id="rId32"/>
-    <sheet name="DocumentsIndex" sheetId="13" r:id="rId33"/>
-    <sheet name="DocumentsDetails" sheetId="12" r:id="rId34"/>
-    <sheet name="Notes" sheetId="10" r:id="rId35"/>
+    <sheet name="PurchaserNames" sheetId="37" r:id="rId25"/>
+    <sheet name="TeamMembers" sheetId="20" r:id="rId26"/>
+    <sheet name="SearchProperties" sheetId="8" r:id="rId27"/>
+    <sheet name="Properties" sheetId="6" r:id="rId28"/>
+    <sheet name="PropertyManagement" sheetId="30" r:id="rId29"/>
+    <sheet name="PropertyManagementContact" sheetId="31" r:id="rId30"/>
+    <sheet name="PropertyManagementActivity" sheetId="32" r:id="rId31"/>
+    <sheet name="ManagementPropActivityInvoice" sheetId="33" r:id="rId32"/>
+    <sheet name="Takes" sheetId="27" r:id="rId33"/>
+    <sheet name="DocumentsIndex" sheetId="13" r:id="rId34"/>
+    <sheet name="DocumentsDetails" sheetId="12" r:id="rId35"/>
+    <sheet name="Notes" sheetId="10" r:id="rId36"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">DocumentsDetails!$A$1:$AX$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1854">
   <si>
     <t>FirstName</t>
   </si>
@@ -5173,9 +5173,6 @@
     <t>AcqSearchPropertiesIndex</t>
   </si>
   <si>
-    <t>DisSearchPropertiesIndex</t>
-  </si>
-  <si>
     <t>LeaseSearchPropertiesIndex</t>
   </si>
   <si>
@@ -5500,12 +5497,6 @@
     <t>Update Automated Disposition File Offers and Sales</t>
   </si>
   <si>
-    <t>AppraisalAndAssessmentAppraisalValue</t>
-  </si>
-  <si>
-    <t>AppraisalAndAssessmentAppraisalDate</t>
-  </si>
-  <si>
     <t>AppraisalAndAssessmentBcAssessmentValue</t>
   </si>
   <si>
@@ -5534,6 +5525,117 @@
   </si>
   <si>
     <t>Automated Disposition File - From PIN</t>
+  </si>
+  <si>
+    <t>PurchaseNameStartRow</t>
+  </si>
+  <si>
+    <t>PurchaseNameTotalCount</t>
+  </si>
+  <si>
+    <t>PurchaserName</t>
+  </si>
+  <si>
+    <t>PurchaseMemberContactType</t>
+  </si>
+  <si>
+    <t>PurchaseMemberPrimaryContact</t>
+  </si>
+  <si>
+    <t>Create DF with Offer and Sales Tab</t>
+  </si>
+  <si>
+    <t>Edit DF with Offer and Sales Tab</t>
+  </si>
+  <si>
+    <t>Al Dommasch</t>
+  </si>
+  <si>
+    <t>Al Radke</t>
+  </si>
+  <si>
+    <t>PurchaserAgent</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitor</t>
+  </si>
+  <si>
+    <t>LastConditionRemovalDate</t>
+  </si>
+  <si>
+    <t>SaleCompletionDate</t>
+  </si>
+  <si>
+    <t>FiscalYearOfSale</t>
+  </si>
+  <si>
+    <t>FinalSalePrice</t>
+  </si>
+  <si>
+    <t>RealtorCommission</t>
+  </si>
+  <si>
+    <t>GSTRequired</t>
+  </si>
+  <si>
+    <t>NetBookValue</t>
+  </si>
+  <si>
+    <t>TotalCostOfSales</t>
+  </si>
+  <si>
+    <t>SPPAmount</t>
+  </si>
+  <si>
+    <t>RemediationCost</t>
+  </si>
+  <si>
+    <t>NetProceedsBeforeSPP</t>
+  </si>
+  <si>
+    <t>NetProceedsAfterSPP</t>
+  </si>
+  <si>
+    <t>OwnerSolicitorPrimaryContact</t>
+  </si>
+  <si>
+    <t>Joahn Eyles</t>
+  </si>
+  <si>
+    <t>PurchaserAgentPrimaryContact</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitorPrimaryContact</t>
+  </si>
+  <si>
+    <t>Aalten Richard MINERS</t>
+  </si>
+  <si>
+    <t>YASUSHI NOMA</t>
+  </si>
+  <si>
+    <t>PurchaserAgentType</t>
+  </si>
+  <si>
+    <t>PurchaserSolicitorType</t>
+  </si>
+  <si>
+    <t>GSTCollected</t>
+  </si>
+  <si>
+    <t>DispositionAssignedDate</t>
+  </si>
+  <si>
+    <t>DispositionPhysicalFileStatus</t>
+  </si>
+  <si>
+    <t>DispositionSearchPropertiesIndex</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentValue</t>
+  </si>
+  <si>
+    <t>AppraisalAndAssessmentDate</t>
   </si>
 </sst>
 </file>
@@ -6526,7 +6628,7 @@
         <v>314</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>326</v>
@@ -7087,10 +7189,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
-  <dimension ref="A1:AJ19"/>
+  <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7115,25 +7217,26 @@
     <col min="18" max="18" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -7198,52 +7301,55 @@
         <v>864</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>1840</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>1080</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>1083</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1698</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1068</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1085</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1086</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>1112</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>1113</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1199</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>1377</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>1378</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1343</v>
       </c>
@@ -7300,55 +7406,58 @@
         <v>2</v>
       </c>
       <c r="U2" t="s">
-        <v>865</v>
+        <v>1651</v>
       </c>
       <c r="V2" t="s">
+        <v>1653</v>
+      </c>
+      <c r="W2" t="s">
         <v>1084</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>1081</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>15</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>5</v>
       </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
       <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
         <v>1</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>4</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>10</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
       </c>
       <c r="AG2">
         <v>1</v>
       </c>
-      <c r="AH2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI2">
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="6">
         <v>0</v>
       </c>
       <c r="AJ2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1344</v>
       </c>
@@ -7372,7 +7481,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7407,18 +7516,15 @@
       <c r="U3" t="s">
         <v>349</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>1203</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>1302</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>16</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
       <c r="Z3">
         <v>0</v>
       </c>
@@ -7426,34 +7532,37 @@
         <v>0</v>
       </c>
       <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
         <v>5</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>2</v>
       </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
         <v>2</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>1</v>
       </c>
-      <c r="AH3" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI3">
+      <c r="AI3" s="6">
         <v>0</v>
       </c>
       <c r="AJ3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1350</v>
       </c>
@@ -7510,55 +7619,58 @@
         <v>2</v>
       </c>
       <c r="U4" t="s">
-        <v>865</v>
+        <v>1651</v>
       </c>
       <c r="V4" t="s">
+        <v>1841</v>
+      </c>
+      <c r="W4" t="s">
         <v>1084</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>1081</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>15</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>1</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>5</v>
       </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
       <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
         <v>1</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>4</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>1</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>10</v>
-      </c>
-      <c r="AF4">
-        <v>1</v>
       </c>
       <c r="AG4">
         <v>1</v>
       </c>
-      <c r="AH4" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI4">
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="6">
         <v>0</v>
       </c>
       <c r="AJ4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1351</v>
       </c>
@@ -7582,7 +7694,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7614,18 +7726,15 @@
       <c r="U5" t="s">
         <v>349</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>1203</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>1302</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>16</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
       <c r="Z5">
         <v>0</v>
       </c>
@@ -7633,34 +7742,37 @@
         <v>0</v>
       </c>
       <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
         <v>5</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>2</v>
       </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
         <v>2</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>1</v>
       </c>
-      <c r="AH5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI5">
+      <c r="AI5" s="6">
         <v>0</v>
       </c>
       <c r="AJ5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1349</v>
       </c>
@@ -7719,53 +7831,53 @@
       <c r="U6" t="s">
         <v>865</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>1084</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>1081</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>15</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>1</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>5</v>
       </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
       <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
         <v>1</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>4</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>1</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>10</v>
-      </c>
-      <c r="AF6">
-        <v>1</v>
       </c>
       <c r="AG6">
         <v>1</v>
       </c>
-      <c r="AH6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="6">
         <v>0</v>
       </c>
       <c r="AJ6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1344</v>
       </c>
@@ -7789,7 +7901,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -7821,53 +7933,53 @@
       <c r="U7" t="s">
         <v>349</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>1203</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>1302</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>18</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>6</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>1</v>
       </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
       <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
         <v>5</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>2</v>
       </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <v>2</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <v>1</v>
       </c>
-      <c r="AH7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI7">
+      <c r="AI7" s="6">
         <v>0</v>
       </c>
       <c r="AJ7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1353</v>
       </c>
@@ -7926,53 +8038,53 @@
       <c r="U8" t="s">
         <v>865</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>1084</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>1081</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>15</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>1</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>5</v>
-      </c>
-      <c r="AA8">
-        <v>1</v>
       </c>
       <c r="AB8">
         <v>1</v>
       </c>
       <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
         <v>4</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>1</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>10</v>
-      </c>
-      <c r="AF8">
-        <v>1</v>
       </c>
       <c r="AG8">
         <v>1</v>
       </c>
-      <c r="AH8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI8">
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="6">
         <v>0</v>
       </c>
       <c r="AJ8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1355</v>
       </c>
@@ -8029,55 +8141,58 @@
         <v>2</v>
       </c>
       <c r="U9" t="s">
-        <v>865</v>
+        <v>1651</v>
       </c>
       <c r="V9" t="s">
+        <v>278</v>
+      </c>
+      <c r="W9" t="s">
         <v>1084</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>1081</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>15</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>1</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>5</v>
       </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
       <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
         <v>1</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>4</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>1</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>10</v>
-      </c>
-      <c r="AF9">
-        <v>1</v>
       </c>
       <c r="AG9">
         <v>1</v>
       </c>
-      <c r="AH9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI9">
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="6">
         <v>0</v>
       </c>
       <c r="AJ9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1357</v>
       </c>
@@ -8136,53 +8251,53 @@
       <c r="U10" t="s">
         <v>865</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>1084</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>1081</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>15</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>1</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>5</v>
       </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
       <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
         <v>1</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>4</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>1</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>10</v>
-      </c>
-      <c r="AF10">
-        <v>1</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
-      <c r="AH10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI10">
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="6">
         <v>0</v>
       </c>
       <c r="AJ10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1359</v>
       </c>
@@ -8241,53 +8356,53 @@
       <c r="U11" t="s">
         <v>865</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>1084</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>1081</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>15</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>1</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>5</v>
       </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
       <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
         <v>1</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>4</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>1</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>10</v>
-      </c>
-      <c r="AF11">
-        <v>1</v>
       </c>
       <c r="AG11">
         <v>1</v>
       </c>
-      <c r="AH11" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI11">
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="6">
         <v>0</v>
       </c>
       <c r="AJ11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1360</v>
       </c>
@@ -8311,7 +8426,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8341,20 +8456,20 @@
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>349</v>
+        <v>1651</v>
       </c>
       <c r="V12" t="s">
+        <v>1652</v>
+      </c>
+      <c r="W12" t="s">
         <v>1203</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>1302</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>16</v>
       </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
       <c r="Z12">
         <v>0</v>
       </c>
@@ -8362,34 +8477,37 @@
         <v>0</v>
       </c>
       <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
         <v>5</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>2</v>
       </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
       <c r="AE12">
         <v>0</v>
       </c>
       <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
         <v>2</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>1</v>
       </c>
-      <c r="AH12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI12">
+      <c r="AI12" s="6">
         <v>0</v>
       </c>
       <c r="AJ12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1363</v>
       </c>
@@ -8448,53 +8566,53 @@
       <c r="U13" t="s">
         <v>865</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>1084</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>1081</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>20</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>1</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>5</v>
       </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
       <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>1</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>4</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>1</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>10</v>
-      </c>
-      <c r="AF13">
-        <v>1</v>
       </c>
       <c r="AG13">
         <v>1</v>
       </c>
-      <c r="AH13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI13">
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="6">
         <v>0</v>
       </c>
       <c r="AJ13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1365</v>
       </c>
@@ -8553,53 +8671,53 @@
       <c r="U14" t="s">
         <v>865</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>1084</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>1081</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>21</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>1</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>5</v>
       </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
       <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
         <v>1</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>4</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>1</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>10</v>
-      </c>
-      <c r="AF14">
-        <v>1</v>
       </c>
       <c r="AG14">
         <v>1</v>
       </c>
-      <c r="AH14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI14">
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="6">
         <v>0</v>
       </c>
       <c r="AJ14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1366</v>
       </c>
@@ -8623,7 +8741,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -8655,18 +8773,15 @@
       <c r="U15" t="s">
         <v>349</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>1203</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>1302</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>22</v>
       </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
       <c r="Z15">
         <v>0</v>
       </c>
@@ -8674,34 +8789,37 @@
         <v>0</v>
       </c>
       <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
         <v>5</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>2</v>
       </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
       <c r="AE15">
         <v>0</v>
       </c>
       <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
         <v>2</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>1</v>
       </c>
-      <c r="AH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI15">
+      <c r="AI15" s="6">
         <v>0</v>
       </c>
       <c r="AJ15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1082</v>
       </c>
@@ -8732,18 +8850,15 @@
       <c r="U16" t="s">
         <v>1384</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>1385</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>1393</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>16</v>
       </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
       <c r="Z16">
         <v>0</v>
       </c>
@@ -8757,28 +8872,31 @@
         <v>0</v>
       </c>
       <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
         <v>13</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>2</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
       <c r="AG16">
         <v>0</v>
       </c>
-      <c r="AH16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI16">
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
         <v>1</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1114</v>
       </c>
@@ -8806,9 +8924,6 @@
       <c r="T17" s="8">
         <v>0</v>
       </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
       <c r="Y17">
         <v>0</v>
       </c>
@@ -8836,17 +8951,20 @@
       <c r="AG17">
         <v>0</v>
       </c>
-      <c r="AH17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI17">
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
         <v>4</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>879</v>
       </c>
@@ -8880,12 +8998,9 @@
       <c r="U18" t="s">
         <v>883</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>19</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
       <c r="Z18">
         <v>0</v>
       </c>
@@ -8910,17 +9025,20 @@
       <c r="AG18">
         <v>0</v>
       </c>
-      <c r="AH18" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI18">
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="6">
         <v>0</v>
       </c>
       <c r="AJ18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>880</v>
       </c>
@@ -8963,43 +9081,43 @@
       <c r="T19" s="8">
         <v>1</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>17</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>7</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>1</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>2</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>7</v>
       </c>
-      <c r="AC19">
+      <c r="AD19">
         <v>1</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>15</v>
       </c>
-      <c r="AE19">
+      <c r="AF19">
         <v>1</v>
       </c>
-      <c r="AF19">
+      <c r="AG19">
         <v>3</v>
       </c>
-      <c r="AG19">
+      <c r="AH19">
         <v>1</v>
       </c>
-      <c r="AH19" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI19">
+      <c r="AI19" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
         <v>5</v>
       </c>
-      <c r="AJ19">
+      <c r="AK19">
         <v>1</v>
       </c>
     </row>
@@ -11752,10 +11870,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63446AF6-E41F-4CAA-9C6A-F4588DBEF458}">
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AV13"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11763,8 +11881,8 @@
     <col min="1" max="1" width="41.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1796875" customWidth="1"/>
     <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
-    <col min="5" max="5" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.1796875" customWidth="1"/>
@@ -11772,32 +11890,44 @@
     <col min="11" max="11" width="19.1796875" customWidth="1"/>
     <col min="12" max="12" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.453125" customWidth="1"/>
-    <col min="14" max="14" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.1796875" customWidth="1"/>
     <col min="16" max="16" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.36328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="40.36328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="42.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.54296875" customWidth="1"/>
+    <col min="35" max="35" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12" customWidth="1"/>
+    <col min="43" max="43" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
@@ -11805,10 +11935,10 @@
         <v>1641</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>994</v>
+        <v>1849</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1631</v>
@@ -11826,7 +11956,7 @@
         <v>1627</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1628</v>
@@ -11838,7 +11968,7 @@
         <v>1629</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>836</v>
+        <v>1850</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>1630</v>
@@ -11853,34 +11983,97 @@
         <v>1623</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>1699</v>
+        <v>1851</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="U1" s="19" t="s">
+        <v>1852</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>1853</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>1807</v>
+      </c>
+      <c r="X1" s="19" t="s">
         <v>1808</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>1809</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>1810</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>1811</v>
       </c>
-      <c r="Y1" s="19" t="s">
-        <v>1812</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>1813</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB1" s="3" t="s">
+        <v>1817</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>1818</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>1846</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>1842</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>1827</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>1847</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>1843</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>1829</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>1831</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1832</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>1848</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>1835</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>1838</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>1836</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>1839</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1634</v>
       </c>
@@ -11894,7 +12087,7 @@
         <v>1645</v>
       </c>
       <c r="I2" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="K2" t="s">
         <v>1642</v>
@@ -11923,9 +12116,15 @@
       <c r="AA2">
         <v>0</v>
       </c>
-      <c r="AH2" s="6"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="6"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1633</v>
       </c>
@@ -11951,16 +12150,16 @@
         <v>1640</v>
       </c>
       <c r="I3" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J3" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="M3" s="4">
         <v>45323</v>
@@ -11992,9 +12191,15 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="6"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1632</v>
       </c>
@@ -12003,7 +12208,7 @@
       </c>
       <c r="D4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45328</v>
+        <v>45331</v>
       </c>
       <c r="E4" s="4">
         <v>45352</v>
@@ -12012,7 +12217,7 @@
         <v>1637</v>
       </c>
       <c r="G4" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="H4" t="s">
         <v>1500</v>
@@ -12041,9 +12246,15 @@
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="6"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1635</v>
       </c>
@@ -12054,10 +12265,10 @@
         <v>1638</v>
       </c>
       <c r="H5" t="s">
+        <v>1724</v>
+      </c>
+      <c r="I5" t="s">
         <v>1725</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1726</v>
       </c>
       <c r="P5" t="s">
         <v>199</v>
@@ -12080,26 +12291,32 @@
       <c r="AA5">
         <v>0</v>
       </c>
-      <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="6"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B6" t="s">
         <v>273</v>
       </c>
       <c r="F6" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="H6" t="s">
         <v>336</v>
       </c>
       <c r="I6" t="s">
+        <v>1726</v>
+      </c>
+      <c r="J6" t="s">
         <v>1727</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1728</v>
       </c>
       <c r="P6" t="s">
         <v>198</v>
@@ -12122,16 +12339,22 @@
       <c r="AA6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B7" t="s">
         <v>273</v>
       </c>
       <c r="F7" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="H7" t="s">
         <v>1640</v>
@@ -12160,19 +12383,25 @@
       <c r="AA7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B8" t="s">
         <v>273</v>
       </c>
       <c r="F8" t="s">
+        <v>1722</v>
+      </c>
+      <c r="H8" t="s">
         <v>1723</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1724</v>
       </c>
       <c r="I8" t="s">
         <v>1646</v>
@@ -12198,10 +12427,16 @@
       <c r="AA8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>273</v>
@@ -12209,7 +12444,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="F9" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="G9" s="20">
         <v>77665544</v>
@@ -12264,13 +12499,70 @@
       <c r="AA9" s="20">
         <v>2</v>
       </c>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB9" s="20">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="20">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="20" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AE9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1841</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>1844</v>
+      </c>
+      <c r="AH9" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>45513</v>
+      </c>
+      <c r="AK9" s="4">
+        <v>45482</v>
+      </c>
+      <c r="AL9">
+        <v>2024</v>
+      </c>
+      <c r="AM9">
+        <v>1000000</v>
+      </c>
+      <c r="AN9">
+        <v>10000</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>299</v>
+      </c>
+      <c r="AP9">
+        <v>50000</v>
+      </c>
+      <c r="AQ9">
+        <v>25000</v>
+      </c>
+      <c r="AR9">
+        <v>12000.99</v>
+      </c>
+      <c r="AS9">
+        <v>902999.01</v>
+      </c>
+      <c r="AT9">
+        <v>1200</v>
+      </c>
+      <c r="AU9">
+        <v>901799.01</v>
+      </c>
+      <c r="AV9">
+        <v>1988.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>273</v>
@@ -12279,14 +12571,14 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" t="s">
         <v>1640</v>
       </c>
       <c r="I10" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -12324,19 +12616,56 @@
       <c r="AA10" s="20">
         <v>1</v>
       </c>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB10" s="20">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="20">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="20" t="s">
+        <v>1845</v>
+      </c>
+      <c r="AE10" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="AF10" s="20"/>
+      <c r="AG10" t="s">
+        <v>1711</v>
+      </c>
+      <c r="AH10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>1712</v>
+      </c>
+      <c r="AJ10" s="21">
+        <v>45209</v>
+      </c>
+      <c r="AK10" s="4">
+        <v>46368</v>
+      </c>
+      <c r="AL10">
+        <v>2026</v>
+      </c>
+      <c r="AM10">
+        <v>544900</v>
+      </c>
+      <c r="AN10">
+        <v>4900</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B11" t="s">
         <v>273</v>
       </c>
       <c r="F11" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="H11" t="s">
         <v>1645</v>
@@ -12365,22 +12694,28 @@
       <c r="AA11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B12" t="s">
         <v>273</v>
       </c>
       <c r="F12" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="H12" t="s">
         <v>1640</v>
       </c>
       <c r="I12" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="P12" t="s">
         <v>200</v>
@@ -12403,16 +12738,22 @@
       <c r="AA12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="B13" t="s">
         <v>273</v>
       </c>
       <c r="F13" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="H13" t="s">
         <v>1500</v>
@@ -12439,6 +12780,12 @@
         <v>0</v>
       </c>
       <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>0</v>
       </c>
     </row>
@@ -12854,9 +13201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE90B83-E126-4D39-94E6-B33283C8DC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12874,33 +13219,33 @@
         <v>112</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1791</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>1792</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>1793</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>1794</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>1795</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1796</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>1797</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>1798</v>
-      </c>
       <c r="C2" s="20" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="D2" s="21">
         <v>45352</v>
@@ -12912,18 +13257,18 @@
         <v>550000</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="D3" s="21">
         <v>45352</v>
@@ -12935,18 +13280,18 @@
         <v>550000</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="D4" s="21">
         <v>45463</v>
@@ -12958,7 +13303,7 @@
         <v>1200.5</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -12976,11 +13321,121 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAD653A-DB80-460C-86DB-ACD85A6EF957}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C5" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C6" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EAAF30-BD78-4D23-AEBC-1D6C37D138A6}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13160,10 +13615,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B12" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="C12" t="s">
         <v>1385</v>
@@ -13174,13 +13629,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B13" t="s">
         <v>850</v>
       </c>
       <c r="C13" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D13" t="s">
         <v>736</v>
@@ -13188,13 +13643,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B14" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="C14" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D14" t="s">
         <v>736</v>
@@ -13202,7 +13657,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B15" t="s">
         <v>851</v>
@@ -13219,13 +13674,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B16" t="s">
         <v>908</v>
       </c>
       <c r="C16" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -13236,30 +13691,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B17" t="s">
         <v>853</v>
       </c>
       <c r="C17" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B18" t="s">
         <v>852</v>
       </c>
       <c r="C18" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
@@ -13270,13 +13725,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C19" t="s">
         <v>1715</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1716</v>
       </c>
       <c r="D19" t="s">
         <v>736</v>
@@ -13287,12 +13742,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13440,7 +13895,7 @@
         <v>1002</v>
       </c>
       <c r="E10" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -13592,7 +14047,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B26" t="s">
         <v>1303</v>
@@ -13604,12 +14059,12 @@
         <v>801</v>
       </c>
       <c r="E26" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B27" t="s">
         <v>804</v>
@@ -13617,7 +14072,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B28" t="s">
         <v>925</v>
@@ -13625,7 +14080,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B29" t="s">
         <v>379</v>
@@ -13637,7 +14092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
@@ -13711,7 +14166,7 @@
         <v>253</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>254</v>
@@ -13931,31 +14386,31 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B6" t="s">
         <v>1730</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>1731</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1732</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1733</v>
       </c>
       <c r="F6" t="s">
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="I6" t="s">
         <v>198</v>
       </c>
       <c r="J6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="K6" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="L6" t="s">
         <v>301</v>
@@ -13964,16 +14419,16 @@
         <v>301</v>
       </c>
       <c r="N6" t="s">
+        <v>1737</v>
+      </c>
+      <c r="O6" t="s">
         <v>1738</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>1739</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>1740</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1741</v>
       </c>
       <c r="R6" t="s">
         <v>303</v>
@@ -13991,7 +14446,7 @@
         <v>874</v>
       </c>
       <c r="Y6" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
   </sheetData>
@@ -14000,7 +14455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F40B5-89DA-4741-9D93-0338FA3A7E2C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -14149,113 +14604,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1469</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1526</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1491</v>
-      </c>
-      <c r="C2" t="s">
-        <v>736</v>
-      </c>
-      <c r="D2" t="s">
-        <v>738</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>856</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1490</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C4" t="s">
-        <v>736</v>
-      </c>
-      <c r="D4" t="s">
-        <v>738</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1532</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1492</v>
-      </c>
-      <c r="C5" t="s">
-        <v>736</v>
-      </c>
-      <c r="D5" t="s">
-        <v>738</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14340,6 +14688,113 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F1C7F-C3A7-4EC8-A468-AE1E52A9CDFA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C2" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2" t="s">
+        <v>738</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D4" t="s">
+        <v>738</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C5" t="s">
+        <v>736</v>
+      </c>
+      <c r="D5" t="s">
+        <v>738</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900FA95B-8B00-4597-9C9C-B9D179841747}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -14614,7 +15069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD92D06B-F8ED-4433-B13A-26AE77A867A4}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -14727,7 +15182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -15195,7 +15650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69AB3B-3A11-477C-A201-8388519D3807}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -15344,7 +15799,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B13">
         <v>72</v>
@@ -15355,7 +15810,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B14">
         <v>83</v>
@@ -15369,7 +15824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:AX84"/>
   <sheetViews>
@@ -16856,7 +17311,7 @@
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="B73" t="s">
         <v>513</v>
@@ -16877,21 +17332,21 @@
         <v>12</v>
       </c>
       <c r="V73" t="s">
+        <v>1757</v>
+      </c>
+      <c r="W73" t="s">
         <v>1758</v>
       </c>
-      <c r="W73" t="s">
+      <c r="Z73" t="s">
         <v>1759</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="AP73" t="s">
         <v>1760</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>1761</v>
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B74" t="s">
         <v>510</v>
@@ -16902,7 +17357,7 @@
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B75" t="s">
         <v>502</v>
@@ -16911,7 +17366,7 @@
         <v>561</v>
       </c>
       <c r="E75" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="T75" t="s">
         <v>574</v>
@@ -16925,7 +17380,7 @@
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B76" t="s">
         <v>922</v>
@@ -16934,12 +17389,12 @@
         <v>562</v>
       </c>
       <c r="AS76" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B77" t="s">
         <v>503</v>
@@ -16954,12 +17409,12 @@
         <v>123</v>
       </c>
       <c r="U77" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B78" t="s">
         <v>511</v>
@@ -16971,7 +17426,7 @@
         <v>900</v>
       </c>
       <c r="L78" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="U78" t="s">
         <v>574</v>
@@ -16979,7 +17434,7 @@
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B79" t="s">
         <v>507</v>
@@ -16988,24 +17443,24 @@
         <v>564</v>
       </c>
       <c r="E79" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="G79" s="13">
         <v>44053</v>
       </c>
       <c r="AD79" t="s">
+        <v>1781</v>
+      </c>
+      <c r="AM79" t="s">
         <v>1782</v>
       </c>
-      <c r="AM79" t="s">
+      <c r="AS79" t="s">
         <v>1783</v>
-      </c>
-      <c r="AS79" t="s">
-        <v>1784</v>
       </c>
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B80" t="s">
         <v>516</v>
@@ -17014,12 +17469,12 @@
         <v>559</v>
       </c>
       <c r="AS80" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B81" t="s">
         <v>512</v>
@@ -17028,12 +17483,12 @@
         <v>560</v>
       </c>
       <c r="AS81" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B82" t="s">
         <v>520</v>
@@ -17048,18 +17503,18 @@
         <v>8900999</v>
       </c>
       <c r="Y82" t="s">
+        <v>1786</v>
+      </c>
+      <c r="AF82" t="s">
         <v>1787</v>
       </c>
-      <c r="AF82" t="s">
+      <c r="AP82" t="s">
         <v>1788</v>
-      </c>
-      <c r="AP82" t="s">
-        <v>1789</v>
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B83" t="s">
         <v>521</v>
@@ -17068,12 +17523,12 @@
         <v>562</v>
       </c>
       <c r="AF83" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="B84" t="s">
         <v>513</v>
@@ -17091,19 +17546,19 @@
         <v>44866</v>
       </c>
       <c r="Q84" t="s">
+        <v>1764</v>
+      </c>
+      <c r="V84" t="s">
         <v>1765</v>
       </c>
-      <c r="V84" t="s">
+      <c r="W84" t="s">
         <v>1766</v>
-      </c>
-      <c r="W84" t="s">
-        <v>1767</v>
       </c>
       <c r="Z84">
         <v>909000</v>
       </c>
       <c r="AP84" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
   </sheetData>
@@ -17112,7 +17567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0191B-A695-44B6-B8DB-539DF91B46C4}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -17200,7 +17655,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B10" t="s">
         <v>386</v>
@@ -17208,10 +17663,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B11" t="s">
         <v>1751</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1752</v>
       </c>
     </row>
   </sheetData>
@@ -18724,7 +19179,7 @@
         <v>640</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="AK1" s="3" t="s">
         <v>641</v>

</xml_diff>

<commit_message>
Adding or improving list views and pagination
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE945748-A0C6-41E9-A1F0-1BB42B11BECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77267F4B-6665-43A9-8E26-7BB4571C82B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="5" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -6070,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12A4D20-CBEC-42E3-9A24-C9C857FE01F3}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7942,7 +7942,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8782,7 +8782,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -10033,7 +10033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247DFAE7-4496-4934-B20F-D611E033A94F}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -12293,7 +12293,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -18515,8 +18515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC9B3A8-42C1-4A9C-B1C1-5E5E07CE0539}">
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update image references and fixed tests
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE945748-A0C6-41E9-A1F0-1BB42B11BECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77267F4B-6665-43A9-8E26-7BB4571C82B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="5" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -6070,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12A4D20-CBEC-42E3-9A24-C9C857FE01F3}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -7942,7 +7942,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -8782,7 +8782,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -10033,7 +10033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247DFAE7-4496-4934-B20F-D611E033A94F}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -12293,7 +12293,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -18515,8 +18515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC9B3A8-42C1-4A9C-B1C1-5E5E07CE0539}">
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changes on automation IS84
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5AC96D-F80D-41D9-A0AA-D4DD92B6B100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6A1D08-73D0-4571-8CC8-8EA3F5201910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="24" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" tabRatio="950" firstSheet="28" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -8474,7 +8474,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -8679,7 +8679,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -9202,7 +9202,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -13314,7 +13314,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45478</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -14854,7 +14854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -15255,8 +15255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15402,6 +15402,12 @@
       <c r="D2" t="s">
         <v>260</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -15419,6 +15425,12 @@
       <c r="I3" t="s">
         <v>264</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
       <c r="N3" t="s">
         <v>190</v>
       </c>
@@ -15570,6 +15582,12 @@
       <c r="I5" t="s">
         <v>810</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
       <c r="T5" t="s">
         <v>811</v>
       </c>
@@ -15619,6 +15637,12 @@
       </c>
       <c r="I6" t="s">
         <v>1654</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
       </c>
       <c r="N6" t="s">
         <v>190</v>
@@ -18095,7 +18119,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18387,7 +18411,7 @@
         <v>1819</v>
       </c>
       <c r="F15" s="22">
-        <v>642614.75249999994</v>
+        <v>642614.75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Changes on automation test cases IS84
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6A1D08-73D0-4571-8CC8-8EA3F5201910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241E086C-3B1F-44D6-BBAC-152A25DF2F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" tabRatio="950" firstSheet="28" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3499" uniqueCount="2036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3499" uniqueCount="2037">
   <si>
     <t>FirstName</t>
   </si>
@@ -5896,9 +5896,6 @@
     <t>LIS: LOT 5, EXCEPT: PART ON SRW PLAN 45999A DISTRICT LOT 175 GROUP 2 NEW WESTMINSTER DISTRICT PLAN 30099 ||| PAIMS: Lot 5 District Lot 175 Group 2 New Westminster District Plan 30099</t>
   </si>
   <si>
-    <t>Automated Acquisition File - Takes Logic IS81</t>
-  </si>
-  <si>
     <t>028-928-563</t>
   </si>
   <si>
@@ -5998,9 +5995,6 @@
     <t>NEP13998</t>
   </si>
   <si>
-    <t>721 Howser Ridge FSR, Howser, BC</t>
-  </si>
-  <si>
     <t>6840 Daisy Lane, Whistler, BC</t>
   </si>
   <si>
@@ -6185,6 +6179,15 @@
   </si>
   <si>
     <t>000-000-999</t>
+  </si>
+  <si>
+    <t>Automated Acquisition File - Takes Logic IS84</t>
+  </si>
+  <si>
+    <t>33925 Boyd Rd</t>
+  </si>
+  <si>
+    <t>Northern Region, South Coast Region</t>
   </si>
 </sst>
 </file>
@@ -6275,7 +6278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6318,6 +6321,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7311,8 +7315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3C62D2-095D-41C7-8E12-52D5164F6230}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7320,7 +7324,7 @@
     <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
@@ -7463,7 +7467,7 @@
         <v>246</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>2036</v>
       </c>
       <c r="I3" s="4"/>
       <c r="M3" s="4"/>
@@ -7557,7 +7561,7 @@
         <v>246</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>2036</v>
       </c>
       <c r="M6" s="4"/>
       <c r="O6" t="b">
@@ -7973,8 +7977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8263,7 +8267,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45478</v>
+        <v>45482</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -8474,7 +8478,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45478</v>
+        <v>45482</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -8679,7 +8683,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45478</v>
+        <v>45482</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -9202,7 +9206,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45478</v>
+        <v>45482</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -9515,7 +9519,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45478</v>
+        <v>45482</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -9901,7 +9905,7 @@
         <v>246</v>
       </c>
       <c r="L20" t="s">
-        <v>1939</v>
+        <v>2034</v>
       </c>
       <c r="O20" t="s">
         <v>795</v>
@@ -13148,7 +13152,7 @@
         <v>1000</v>
       </c>
       <c r="X2" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="Y2" s="8">
         <v>5000</v>
@@ -13314,7 +13318,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45478</v>
+        <v>45482</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -14855,7 +14859,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14901,7 +14905,7 @@
         <v>239</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1830</v>
@@ -14912,16 +14916,16 @@
         <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="C2">
         <v>4361431</v>
       </c>
       <c r="D2" t="s">
-        <v>1973</v>
+        <v>2035</v>
       </c>
       <c r="E2" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="F2" t="s">
         <v>257</v>
@@ -14946,7 +14950,7 @@
         <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -14954,7 +14958,7 @@
         <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -14962,7 +14966,7 @@
         <v>284</v>
       </c>
       <c r="B6" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="F6" t="s">
         <v>258</v>
@@ -14970,13 +14974,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B7" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="D7" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -14984,7 +14988,7 @@
         <v>276</v>
       </c>
       <c r="B8" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -14992,7 +14996,7 @@
         <v>277</v>
       </c>
       <c r="B9" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -15000,13 +15004,13 @@
         <v>1817</v>
       </c>
       <c r="B10" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="C10">
         <v>1821391</v>
       </c>
       <c r="D10" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="E10" t="s">
         <v>1626</v>
@@ -15017,7 +15021,7 @@
         <v>403</v>
       </c>
       <c r="B11" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -15025,19 +15029,19 @@
         <v>1578</v>
       </c>
       <c r="B12" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="C12">
         <v>8540071</v>
       </c>
       <c r="D12" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="E12" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="F12" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -15045,7 +15049,7 @@
         <v>1576</v>
       </c>
       <c r="B13" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -15053,7 +15057,7 @@
         <v>1579</v>
       </c>
       <c r="B14" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -15061,7 +15065,7 @@
         <v>1577</v>
       </c>
       <c r="B15" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -15069,19 +15073,19 @@
         <v>806</v>
       </c>
       <c r="B16" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="C16">
         <v>1821391</v>
       </c>
       <c r="D16" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E16" t="s">
         <v>1626</v>
       </c>
       <c r="F16" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -15089,7 +15093,7 @@
         <v>1580</v>
       </c>
       <c r="B17" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -15097,7 +15101,7 @@
         <v>1581</v>
       </c>
       <c r="B18" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -15105,7 +15109,7 @@
         <v>814</v>
       </c>
       <c r="B19" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -15113,7 +15117,7 @@
         <v>1582</v>
       </c>
       <c r="B20" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -15129,7 +15133,7 @@
         <v>1584</v>
       </c>
       <c r="B22" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -15137,7 +15141,7 @@
         <v>1585</v>
       </c>
       <c r="B23" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -15145,7 +15149,7 @@
         <v>1586</v>
       </c>
       <c r="B24" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -15153,10 +15157,10 @@
         <v>1587</v>
       </c>
       <c r="B25" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D25" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -15164,13 +15168,13 @@
         <v>1622</v>
       </c>
       <c r="B26" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C26">
         <v>1821391</v>
       </c>
       <c r="D26" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="E26" t="s">
         <v>1626</v>
@@ -15181,7 +15185,7 @@
         <v>1623</v>
       </c>
       <c r="B27" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -15189,7 +15193,7 @@
         <v>1624</v>
       </c>
       <c r="B28" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -15197,7 +15201,7 @@
         <v>1625</v>
       </c>
       <c r="B29" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -15205,7 +15209,7 @@
         <v>1816</v>
       </c>
       <c r="B30" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="C30">
         <v>90054549</v>
@@ -15222,27 +15226,27 @@
         <v>1831</v>
       </c>
       <c r="G31" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
     </row>
   </sheetData>
@@ -15255,8 +15259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15551,7 +15555,7 @@
         <v>1</v>
       </c>
       <c r="AA4" s="32" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="AB4" t="s">
         <v>272</v>
@@ -15810,10 +15814,10 @@
         <v>1927</v>
       </c>
       <c r="B2" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C2" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -16499,8 +16503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16688,7 +16692,7 @@
       <c r="G3" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="30">
         <v>1200</v>
       </c>
       <c r="I3" s="17" t="s">
@@ -16707,8 +16711,8 @@
       <c r="N3" t="s">
         <v>1258</v>
       </c>
-      <c r="O3" s="30">
-        <v>3207.0003000000002</v>
+      <c r="O3" s="34">
+        <v>3207.0001999999999</v>
       </c>
       <c r="P3" s="4">
         <v>39077</v>
@@ -16762,7 +16766,7 @@
       <c r="G4" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="30">
         <v>1604</v>
       </c>
       <c r="I4" s="17" t="s">
@@ -16817,7 +16821,7 @@
       <c r="G5" s="16" t="s">
         <v>1267</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="17" t="s">
         <v>1267</v>
       </c>
@@ -16869,8 +16873,8 @@
       <c r="G6" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H6" s="6">
-        <v>2205.3000000000002</v>
+      <c r="H6" s="30">
+        <v>2205.9090000000001</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>1268</v>
@@ -16894,7 +16898,7 @@
         <v>1268</v>
       </c>
       <c r="R6" s="30">
-        <v>1346.9901</v>
+        <v>1346.9999</v>
       </c>
       <c r="S6" s="4">
         <v>43717</v>
@@ -16932,7 +16936,7 @@
       <c r="G7" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="30">
         <v>3800.9</v>
       </c>
       <c r="I7" s="17" t="s">
@@ -17011,7 +17015,7 @@
         <v>1268</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="V8" s="4">
         <v>44083</v>
@@ -17251,9 +17255,6 @@
       <c r="J13" s="15" t="s">
         <v>1268</v>
       </c>
-      <c r="K13">
-        <v>1000.8901</v>
-      </c>
       <c r="L13" s="4">
         <v>44988</v>
       </c>
@@ -17306,9 +17307,6 @@
       <c r="J14" s="15" t="s">
         <v>1268</v>
       </c>
-      <c r="K14">
-        <v>2339.9092000000001</v>
-      </c>
       <c r="L14" s="4">
         <v>47545</v>
       </c>
@@ -17367,9 +17365,6 @@
       <c r="N15" t="s">
         <v>1257</v>
       </c>
-      <c r="O15">
-        <v>100.0001</v>
-      </c>
       <c r="P15" s="4">
         <v>47545</v>
       </c>
@@ -17425,9 +17420,6 @@
       <c r="N16" t="s">
         <v>1849</v>
       </c>
-      <c r="O16">
-        <v>200.00020000000001</v>
-      </c>
       <c r="P16" s="4">
         <v>47545</v>
       </c>
@@ -17483,9 +17475,6 @@
       <c r="N17" t="s">
         <v>1850</v>
       </c>
-      <c r="O17">
-        <v>300.00029999999998</v>
-      </c>
       <c r="P17" s="4">
         <v>47545</v>
       </c>
@@ -17541,9 +17530,6 @@
       <c r="N18" t="s">
         <v>1258</v>
       </c>
-      <c r="O18">
-        <v>400.00040000000001</v>
-      </c>
       <c r="P18" s="4">
         <v>47545</v>
       </c>
@@ -17599,9 +17585,6 @@
       <c r="N19" t="s">
         <v>1259</v>
       </c>
-      <c r="O19">
-        <v>500.00510000000003</v>
-      </c>
       <c r="P19" s="4">
         <v>47545</v>
       </c>
@@ -17657,9 +17640,6 @@
       <c r="N20" t="s">
         <v>1851</v>
       </c>
-      <c r="O20">
-        <v>600.00609999999995</v>
-      </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="15" t="s">
         <v>1267</v>
@@ -17713,9 +17693,6 @@
       <c r="N21" t="s">
         <v>1871</v>
       </c>
-      <c r="O21">
-        <v>700.00710000000004</v>
-      </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="15" t="s">
         <v>1267</v>
@@ -17769,9 +17746,7 @@
       <c r="Q22" s="15" t="s">
         <v>1268</v>
       </c>
-      <c r="R22" s="30">
-        <v>8900.991</v>
-      </c>
+      <c r="R22" s="30"/>
       <c r="S22" s="4">
         <v>47545</v>
       </c>
@@ -17830,9 +17805,7 @@
       <c r="T23" s="28" t="s">
         <v>1268</v>
       </c>
-      <c r="U23" s="30">
-        <v>9000.0022000000008</v>
-      </c>
+      <c r="U23" s="30"/>
       <c r="V23" s="4">
         <v>44936</v>
       </c>
@@ -17978,9 +17951,6 @@
       </c>
       <c r="N26" t="s">
         <v>1257</v>
-      </c>
-      <c r="O26">
-        <v>800.00810000000001</v>
       </c>
       <c r="P26" s="4">
         <v>47545</v>
@@ -18160,10 +18130,10 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>1819</v>
@@ -18180,10 +18150,10 @@
         <v>1813</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>246</v>
@@ -18200,10 +18170,10 @@
         <v>1813</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>246</v>
@@ -18220,10 +18190,10 @@
         <v>1812</v>
       </c>
       <c r="C5" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="D5" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E5" t="s">
         <v>1819</v>
@@ -18240,10 +18210,10 @@
         <v>1813</v>
       </c>
       <c r="C6" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="D6" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E6" t="s">
         <v>246</v>
@@ -18260,10 +18230,10 @@
         <v>1813</v>
       </c>
       <c r="C7" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E7" t="s">
         <v>246</v>
@@ -18294,7 +18264,7 @@
         <v>1813</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -18308,7 +18278,7 @@
         <v>1813</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -18322,10 +18292,10 @@
         <v>1812</v>
       </c>
       <c r="C11" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="D11" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E11" t="s">
         <v>1819</v>
@@ -18342,10 +18312,10 @@
         <v>1812</v>
       </c>
       <c r="C12" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="D12" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E12" t="s">
         <v>1819</v>
@@ -18362,10 +18332,10 @@
         <v>1813</v>
       </c>
       <c r="C13" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="D13" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E13" t="s">
         <v>246</v>
@@ -18382,10 +18352,10 @@
         <v>1812</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>2030</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>2032</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>1819</v>
@@ -18402,10 +18372,10 @@
         <v>1812</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>1819</v>
@@ -18422,10 +18392,10 @@
         <v>1813</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>2030</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>2032</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>246</v>
@@ -18442,7 +18412,7 @@
         <v>1812</v>
       </c>
       <c r="C17" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -18453,7 +18423,7 @@
         <v>1812</v>
       </c>
       <c r="C18" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -18464,7 +18434,7 @@
         <v>1813</v>
       </c>
       <c r="C19" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="J19" s="11"/>
     </row>
@@ -18476,7 +18446,7 @@
         <v>1812</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -18490,7 +18460,7 @@
         <v>1812</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -18504,7 +18474,7 @@
         <v>1813</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -18518,7 +18488,7 @@
         <v>1812</v>
       </c>
       <c r="C23" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -18537,7 +18507,7 @@
         <v>1813</v>
       </c>
       <c r="C25" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -18548,7 +18518,7 @@
         <v>1812</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -18562,7 +18532,7 @@
         <v>1813</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -18576,7 +18546,7 @@
         <v>1813</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -18590,7 +18560,7 @@
         <v>1812</v>
       </c>
       <c r="C29" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -18601,7 +18571,7 @@
         <v>1812</v>
       </c>
       <c r="C30" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -22166,7 +22136,7 @@
         <v>1620</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="AL1" s="3" t="s">
         <v>598</v>
@@ -22691,7 +22661,7 @@
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="D4" t="s">
         <v>519</v>
@@ -22707,16 +22677,16 @@
         <v>191</v>
       </c>
       <c r="L4" t="s">
+        <v>1977</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1978</v>
+      </c>
+      <c r="P4" t="s">
         <v>1979</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>1980</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1981</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1982</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -23076,84 +23046,84 @@
         <v>964</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>1984</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1985</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>1986</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1987</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1988</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1989</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1990</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1991</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1992</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1993</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1994</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1995</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1996</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1997</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1998</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>1999</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>2000</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>2001</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>2002</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>2003</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>2004</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>2005</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>2006</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>2007</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>987</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="B2" t="s">
         <v>996</v>
@@ -23248,7 +23218,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="B3" t="s">
         <v>997</v>

</xml_diff>

<commit_message>
PSP-8826: Automation test case update for IS84 (#4173)
* IS82 automation updates

* Automation changes

* Changes on automation IS84

* Changes on automation test cases IS84

* Additional validation on Property Management Tab

---------

Co-authored-by: Alejandro Sanchez <emailforasr@gmail.com>
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5AC96D-F80D-41D9-A0AA-D4DD92B6B100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241E086C-3B1F-44D6-BBAC-152A25DF2F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="24" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3499" uniqueCount="2036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3499" uniqueCount="2037">
   <si>
     <t>FirstName</t>
   </si>
@@ -5896,9 +5896,6 @@
     <t>LIS: LOT 5, EXCEPT: PART ON SRW PLAN 45999A DISTRICT LOT 175 GROUP 2 NEW WESTMINSTER DISTRICT PLAN 30099 ||| PAIMS: Lot 5 District Lot 175 Group 2 New Westminster District Plan 30099</t>
   </si>
   <si>
-    <t>Automated Acquisition File - Takes Logic IS81</t>
-  </si>
-  <si>
     <t>028-928-563</t>
   </si>
   <si>
@@ -5998,9 +5995,6 @@
     <t>NEP13998</t>
   </si>
   <si>
-    <t>721 Howser Ridge FSR, Howser, BC</t>
-  </si>
-  <si>
     <t>6840 Daisy Lane, Whistler, BC</t>
   </si>
   <si>
@@ -6185,6 +6179,15 @@
   </si>
   <si>
     <t>000-000-999</t>
+  </si>
+  <si>
+    <t>Automated Acquisition File - Takes Logic IS84</t>
+  </si>
+  <si>
+    <t>33925 Boyd Rd</t>
+  </si>
+  <si>
+    <t>Northern Region, South Coast Region</t>
   </si>
 </sst>
 </file>
@@ -6275,7 +6278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6318,6 +6321,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7311,8 +7315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3C62D2-095D-41C7-8E12-52D5164F6230}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7320,7 +7324,7 @@
     <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
@@ -7463,7 +7467,7 @@
         <v>246</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>2036</v>
       </c>
       <c r="I3" s="4"/>
       <c r="M3" s="4"/>
@@ -7557,7 +7561,7 @@
         <v>246</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>2036</v>
       </c>
       <c r="M6" s="4"/>
       <c r="O6" t="b">
@@ -7973,8 +7977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8263,7 +8267,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45482</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -8474,7 +8478,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45482</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -8679,7 +8683,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45482</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -9202,7 +9206,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45482</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -9515,7 +9519,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45482</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -9901,7 +9905,7 @@
         <v>246</v>
       </c>
       <c r="L20" t="s">
-        <v>1939</v>
+        <v>2034</v>
       </c>
       <c r="O20" t="s">
         <v>795</v>
@@ -13148,7 +13152,7 @@
         <v>1000</v>
       </c>
       <c r="X2" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="Y2" s="8">
         <v>5000</v>
@@ -13314,7 +13318,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45467</v>
+        <v>45482</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -14854,8 +14858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14901,7 +14905,7 @@
         <v>239</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1830</v>
@@ -14912,16 +14916,16 @@
         <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="C2">
         <v>4361431</v>
       </c>
       <c r="D2" t="s">
-        <v>1973</v>
+        <v>2035</v>
       </c>
       <c r="E2" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="F2" t="s">
         <v>257</v>
@@ -14946,7 +14950,7 @@
         <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -14954,7 +14958,7 @@
         <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -14962,7 +14966,7 @@
         <v>284</v>
       </c>
       <c r="B6" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="F6" t="s">
         <v>258</v>
@@ -14970,13 +14974,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B7" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="D7" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -14984,7 +14988,7 @@
         <v>276</v>
       </c>
       <c r="B8" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -14992,7 +14996,7 @@
         <v>277</v>
       </c>
       <c r="B9" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -15000,13 +15004,13 @@
         <v>1817</v>
       </c>
       <c r="B10" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="C10">
         <v>1821391</v>
       </c>
       <c r="D10" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="E10" t="s">
         <v>1626</v>
@@ -15017,7 +15021,7 @@
         <v>403</v>
       </c>
       <c r="B11" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -15025,19 +15029,19 @@
         <v>1578</v>
       </c>
       <c r="B12" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="C12">
         <v>8540071</v>
       </c>
       <c r="D12" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="E12" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="F12" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -15045,7 +15049,7 @@
         <v>1576</v>
       </c>
       <c r="B13" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -15053,7 +15057,7 @@
         <v>1579</v>
       </c>
       <c r="B14" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -15061,7 +15065,7 @@
         <v>1577</v>
       </c>
       <c r="B15" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -15069,19 +15073,19 @@
         <v>806</v>
       </c>
       <c r="B16" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="C16">
         <v>1821391</v>
       </c>
       <c r="D16" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E16" t="s">
         <v>1626</v>
       </c>
       <c r="F16" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -15089,7 +15093,7 @@
         <v>1580</v>
       </c>
       <c r="B17" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -15097,7 +15101,7 @@
         <v>1581</v>
       </c>
       <c r="B18" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -15105,7 +15109,7 @@
         <v>814</v>
       </c>
       <c r="B19" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -15113,7 +15117,7 @@
         <v>1582</v>
       </c>
       <c r="B20" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -15129,7 +15133,7 @@
         <v>1584</v>
       </c>
       <c r="B22" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -15137,7 +15141,7 @@
         <v>1585</v>
       </c>
       <c r="B23" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -15145,7 +15149,7 @@
         <v>1586</v>
       </c>
       <c r="B24" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -15153,10 +15157,10 @@
         <v>1587</v>
       </c>
       <c r="B25" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D25" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -15164,13 +15168,13 @@
         <v>1622</v>
       </c>
       <c r="B26" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C26">
         <v>1821391</v>
       </c>
       <c r="D26" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="E26" t="s">
         <v>1626</v>
@@ -15181,7 +15185,7 @@
         <v>1623</v>
       </c>
       <c r="B27" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -15189,7 +15193,7 @@
         <v>1624</v>
       </c>
       <c r="B28" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -15197,7 +15201,7 @@
         <v>1625</v>
       </c>
       <c r="B29" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -15205,7 +15209,7 @@
         <v>1816</v>
       </c>
       <c r="B30" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="C30">
         <v>90054549</v>
@@ -15222,27 +15226,27 @@
         <v>1831</v>
       </c>
       <c r="G31" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="G39" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
     </row>
   </sheetData>
@@ -15255,8 +15259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15402,6 +15406,12 @@
       <c r="D2" t="s">
         <v>260</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -15419,6 +15429,12 @@
       <c r="I3" t="s">
         <v>264</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
       <c r="N3" t="s">
         <v>190</v>
       </c>
@@ -15539,7 +15555,7 @@
         <v>1</v>
       </c>
       <c r="AA4" s="32" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="AB4" t="s">
         <v>272</v>
@@ -15570,6 +15586,12 @@
       <c r="I5" t="s">
         <v>810</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
       <c r="T5" t="s">
         <v>811</v>
       </c>
@@ -15619,6 +15641,12 @@
       </c>
       <c r="I6" t="s">
         <v>1654</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
       </c>
       <c r="N6" t="s">
         <v>190</v>
@@ -15786,10 +15814,10 @@
         <v>1927</v>
       </c>
       <c r="B2" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C2" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -16475,8 +16503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA05679-694C-4F3E-B058-118DE368DBE0}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16664,7 +16692,7 @@
       <c r="G3" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="30">
         <v>1200</v>
       </c>
       <c r="I3" s="17" t="s">
@@ -16683,8 +16711,8 @@
       <c r="N3" t="s">
         <v>1258</v>
       </c>
-      <c r="O3" s="30">
-        <v>3207.0003000000002</v>
+      <c r="O3" s="34">
+        <v>3207.0001999999999</v>
       </c>
       <c r="P3" s="4">
         <v>39077</v>
@@ -16738,7 +16766,7 @@
       <c r="G4" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="30">
         <v>1604</v>
       </c>
       <c r="I4" s="17" t="s">
@@ -16793,7 +16821,7 @@
       <c r="G5" s="16" t="s">
         <v>1267</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="17" t="s">
         <v>1267</v>
       </c>
@@ -16845,8 +16873,8 @@
       <c r="G6" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H6" s="6">
-        <v>2205.3000000000002</v>
+      <c r="H6" s="30">
+        <v>2205.9090000000001</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>1268</v>
@@ -16870,7 +16898,7 @@
         <v>1268</v>
       </c>
       <c r="R6" s="30">
-        <v>1346.9901</v>
+        <v>1346.9999</v>
       </c>
       <c r="S6" s="4">
         <v>43717</v>
@@ -16908,7 +16936,7 @@
       <c r="G7" s="16" t="s">
         <v>1268</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="30">
         <v>3800.9</v>
       </c>
       <c r="I7" s="17" t="s">
@@ -16987,7 +17015,7 @@
         <v>1268</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="V8" s="4">
         <v>44083</v>
@@ -17227,9 +17255,6 @@
       <c r="J13" s="15" t="s">
         <v>1268</v>
       </c>
-      <c r="K13">
-        <v>1000.8901</v>
-      </c>
       <c r="L13" s="4">
         <v>44988</v>
       </c>
@@ -17282,9 +17307,6 @@
       <c r="J14" s="15" t="s">
         <v>1268</v>
       </c>
-      <c r="K14">
-        <v>2339.9092000000001</v>
-      </c>
       <c r="L14" s="4">
         <v>47545</v>
       </c>
@@ -17343,9 +17365,6 @@
       <c r="N15" t="s">
         <v>1257</v>
       </c>
-      <c r="O15">
-        <v>100.0001</v>
-      </c>
       <c r="P15" s="4">
         <v>47545</v>
       </c>
@@ -17401,9 +17420,6 @@
       <c r="N16" t="s">
         <v>1849</v>
       </c>
-      <c r="O16">
-        <v>200.00020000000001</v>
-      </c>
       <c r="P16" s="4">
         <v>47545</v>
       </c>
@@ -17459,9 +17475,6 @@
       <c r="N17" t="s">
         <v>1850</v>
       </c>
-      <c r="O17">
-        <v>300.00029999999998</v>
-      </c>
       <c r="P17" s="4">
         <v>47545</v>
       </c>
@@ -17517,9 +17530,6 @@
       <c r="N18" t="s">
         <v>1258</v>
       </c>
-      <c r="O18">
-        <v>400.00040000000001</v>
-      </c>
       <c r="P18" s="4">
         <v>47545</v>
       </c>
@@ -17575,9 +17585,6 @@
       <c r="N19" t="s">
         <v>1259</v>
       </c>
-      <c r="O19">
-        <v>500.00510000000003</v>
-      </c>
       <c r="P19" s="4">
         <v>47545</v>
       </c>
@@ -17633,9 +17640,6 @@
       <c r="N20" t="s">
         <v>1851</v>
       </c>
-      <c r="O20">
-        <v>600.00609999999995</v>
-      </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="15" t="s">
         <v>1267</v>
@@ -17689,9 +17693,6 @@
       <c r="N21" t="s">
         <v>1871</v>
       </c>
-      <c r="O21">
-        <v>700.00710000000004</v>
-      </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="15" t="s">
         <v>1267</v>
@@ -17745,9 +17746,7 @@
       <c r="Q22" s="15" t="s">
         <v>1268</v>
       </c>
-      <c r="R22" s="30">
-        <v>8900.991</v>
-      </c>
+      <c r="R22" s="30"/>
       <c r="S22" s="4">
         <v>47545</v>
       </c>
@@ -17806,9 +17805,7 @@
       <c r="T23" s="28" t="s">
         <v>1268</v>
       </c>
-      <c r="U23" s="30">
-        <v>9000.0022000000008</v>
-      </c>
+      <c r="U23" s="30"/>
       <c r="V23" s="4">
         <v>44936</v>
       </c>
@@ -17954,9 +17951,6 @@
       </c>
       <c r="N26" t="s">
         <v>1257</v>
-      </c>
-      <c r="O26">
-        <v>800.00810000000001</v>
       </c>
       <c r="P26" s="4">
         <v>47545</v>
@@ -18095,7 +18089,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18136,10 +18130,10 @@
         <v>1812</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>1819</v>
@@ -18156,10 +18150,10 @@
         <v>1813</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>246</v>
@@ -18176,10 +18170,10 @@
         <v>1813</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>246</v>
@@ -18196,10 +18190,10 @@
         <v>1812</v>
       </c>
       <c r="C5" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="D5" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E5" t="s">
         <v>1819</v>
@@ -18216,10 +18210,10 @@
         <v>1813</v>
       </c>
       <c r="C6" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="D6" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E6" t="s">
         <v>246</v>
@@ -18236,10 +18230,10 @@
         <v>1813</v>
       </c>
       <c r="C7" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="D7" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E7" t="s">
         <v>246</v>
@@ -18270,7 +18264,7 @@
         <v>1813</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -18284,7 +18278,7 @@
         <v>1813</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -18298,10 +18292,10 @@
         <v>1812</v>
       </c>
       <c r="C11" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="D11" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E11" t="s">
         <v>1819</v>
@@ -18318,10 +18312,10 @@
         <v>1812</v>
       </c>
       <c r="C12" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="D12" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E12" t="s">
         <v>1819</v>
@@ -18338,10 +18332,10 @@
         <v>1813</v>
       </c>
       <c r="C13" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="D13" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E13" t="s">
         <v>246</v>
@@ -18358,10 +18352,10 @@
         <v>1812</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>2030</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>2032</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>1819</v>
@@ -18378,16 +18372,16 @@
         <v>1812</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>1819</v>
       </c>
       <c r="F15" s="22">
-        <v>642614.75249999994</v>
+        <v>642614.75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -18398,10 +18392,10 @@
         <v>1813</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>2030</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>2032</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>246</v>
@@ -18418,7 +18412,7 @@
         <v>1812</v>
       </c>
       <c r="C17" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -18429,7 +18423,7 @@
         <v>1812</v>
       </c>
       <c r="C18" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -18440,7 +18434,7 @@
         <v>1813</v>
       </c>
       <c r="C19" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="J19" s="11"/>
     </row>
@@ -18452,7 +18446,7 @@
         <v>1812</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -18466,7 +18460,7 @@
         <v>1812</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -18480,7 +18474,7 @@
         <v>1813</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -18494,7 +18488,7 @@
         <v>1812</v>
       </c>
       <c r="C23" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -18513,7 +18507,7 @@
         <v>1813</v>
       </c>
       <c r="C25" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -18524,7 +18518,7 @@
         <v>1812</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
@@ -18538,7 +18532,7 @@
         <v>1813</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -18552,7 +18546,7 @@
         <v>1813</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -18566,7 +18560,7 @@
         <v>1812</v>
       </c>
       <c r="C29" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -18577,7 +18571,7 @@
         <v>1812</v>
       </c>
       <c r="C30" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -22142,7 +22136,7 @@
         <v>1620</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="AL1" s="3" t="s">
         <v>598</v>
@@ -22667,7 +22661,7 @@
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="D4" t="s">
         <v>519</v>
@@ -22683,16 +22677,16 @@
         <v>191</v>
       </c>
       <c r="L4" t="s">
+        <v>1977</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1978</v>
+      </c>
+      <c r="P4" t="s">
         <v>1979</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>1980</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1981</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1982</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -23052,84 +23046,84 @@
         <v>964</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>1984</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1985</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>1986</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1987</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1988</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1989</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1990</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1991</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1992</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1993</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1994</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1995</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1996</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1997</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1998</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>1999</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>2000</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>2001</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>2002</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>2003</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>2004</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>2005</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>2006</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>2007</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>987</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="B2" t="s">
         <v>996</v>
@@ -23224,7 +23218,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="B3" t="s">
         <v>997</v>

</xml_diff>

<commit_message>
Period and payments test cases fix
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1DFD12-EB7B-40A9-BFF9-29225AE2B5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9152D32C-2C62-450E-AAC7-59E332CE7EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7547,8 +7547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC2A471-385A-4133-9FB5-E00CEEFCFD2D}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7845,7 +7845,7 @@
         <v>1240</v>
       </c>
       <c r="K5" s="17">
-        <f t="shared" ref="K3:K6" si="2">I5*0.05</f>
+        <f t="shared" ref="K5" si="2">I5*0.05</f>
         <v>6000</v>
       </c>
       <c r="L5" s="17">
@@ -7938,7 +7938,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8052,7 +8052,7 @@
         <v>9.56</v>
       </c>
       <c r="I3" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -9162,7 +9162,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9373,7 +9373,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -9578,7 +9578,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10101,7 +10101,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10414,7 +10414,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -14213,7 +14213,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">

</xml_diff>

<commit_message>
Changes on Digital files to accomodate updates
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DF7BF7-620B-49DF-A591-5E840B7D32FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2E6E94-7FDF-4846-986F-47510C32C2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="23" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="2113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3624" uniqueCount="2114">
   <si>
     <t>FirstName</t>
   </si>
@@ -6418,6 +6418,9 @@
   </si>
   <si>
     <t>UNIT 19 -- 171 17 St SE, Salmon Arm, BC</t>
+  </si>
+  <si>
+    <t>MinistryProduct</t>
   </si>
 </sst>
 </file>
@@ -9162,7 +9165,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45555</v>
+        <v>45561</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9373,7 +9376,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45555</v>
+        <v>45561</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -9578,7 +9581,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45555</v>
+        <v>45561</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10101,7 +10104,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45555</v>
+        <v>45561</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10414,7 +10417,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45555</v>
+        <v>45561</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -14213,7 +14216,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45555</v>
+        <v>45561</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -15832,7 +15835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -20415,8 +20418,8 @@
   <dimension ref="A1:AX84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21897,105 +21900,96 @@
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>1641</v>
+        <v>1644</v>
       </c>
       <c r="B73" t="s">
-        <v>472</v>
+        <v>827</v>
       </c>
       <c r="C73" t="s">
-        <v>518</v>
-      </c>
-      <c r="N73" s="13">
-        <v>45178</v>
-      </c>
-      <c r="O73">
-        <v>3</v>
-      </c>
-      <c r="P73" s="13">
-        <v>44866</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>7</v>
-      </c>
-      <c r="V73" t="s">
-        <v>1646</v>
-      </c>
-      <c r="W73" t="s">
-        <v>1647</v>
-      </c>
-      <c r="Z73" t="s">
-        <v>1648</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>1649</v>
+        <v>521</v>
+      </c>
+      <c r="AS73" t="s">
+        <v>1651</v>
       </c>
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="B74" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="C74" t="s">
-        <v>519</v>
+        <v>520</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1650</v>
+      </c>
+      <c r="T74" t="s">
+        <v>533</v>
+      </c>
+      <c r="AQ74">
+        <v>122</v>
+      </c>
+      <c r="AW74">
+        <v>2000</v>
       </c>
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>1643</v>
+        <v>1662</v>
       </c>
       <c r="B75" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C75" t="s">
-        <v>520</v>
-      </c>
-      <c r="E75" t="s">
-        <v>1650</v>
-      </c>
-      <c r="T75" t="s">
-        <v>533</v>
-      </c>
-      <c r="AQ75">
-        <v>122</v>
-      </c>
-      <c r="AW75">
-        <v>2000</v>
+        <v>522</v>
+      </c>
+      <c r="I75">
+        <v>1223</v>
+      </c>
+      <c r="L75">
+        <v>123</v>
+      </c>
+      <c r="U75" t="s">
+        <v>1652</v>
       </c>
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>1644</v>
+        <v>1663</v>
       </c>
       <c r="B76" t="s">
-        <v>827</v>
+        <v>466</v>
       </c>
       <c r="C76" t="s">
-        <v>521</v>
+        <v>523</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1669</v>
+      </c>
+      <c r="G76" s="13">
+        <v>44053</v>
+      </c>
+      <c r="AD76" t="s">
+        <v>1670</v>
+      </c>
+      <c r="AM76" t="s">
+        <v>1671</v>
       </c>
       <c r="AS76" t="s">
-        <v>1651</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>1662</v>
+        <v>1642</v>
       </c>
       <c r="B77" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C77" t="s">
-        <v>522</v>
-      </c>
-      <c r="I77">
-        <v>1223</v>
-      </c>
-      <c r="L77">
-        <v>123</v>
-      </c>
-      <c r="U77" t="s">
-        <v>1652</v>
+        <v>519</v>
       </c>
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
@@ -22020,56 +22014,65 @@
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>1663</v>
+        <v>1665</v>
       </c>
       <c r="B79" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="C79" t="s">
-        <v>523</v>
-      </c>
-      <c r="E79" t="s">
-        <v>1669</v>
-      </c>
-      <c r="G79" s="13">
-        <v>44053</v>
-      </c>
-      <c r="AD79" t="s">
-        <v>1670</v>
-      </c>
-      <c r="AM79" t="s">
-        <v>1671</v>
+        <v>519</v>
       </c>
       <c r="AS79" t="s">
-        <v>1672</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>1664</v>
+        <v>1641</v>
       </c>
       <c r="B80" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C80" t="s">
         <v>518</v>
       </c>
-      <c r="AS80" t="s">
-        <v>1673</v>
+      <c r="N80" s="13">
+        <v>45178</v>
+      </c>
+      <c r="O80">
+        <v>3</v>
+      </c>
+      <c r="P80" s="13">
+        <v>44866</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>7</v>
+      </c>
+      <c r="V80" t="s">
+        <v>1646</v>
+      </c>
+      <c r="W80" t="s">
+        <v>1647</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>1648</v>
+      </c>
+      <c r="AP80" t="s">
+        <v>1649</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B81" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C81" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AS81" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.35">
@@ -22824,10 +22827,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
-  <dimension ref="A1:CT21"/>
+  <dimension ref="A1:CU21"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22835,103 +22838,104 @@
     <col min="1" max="1" width="29.81640625" customWidth="1"/>
     <col min="2" max="2" width="28.453125" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.453125" customWidth="1"/>
-    <col min="19" max="19" width="39.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="47" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28.6328125" customWidth="1"/>
-    <col min="37" max="37" width="23.81640625" customWidth="1"/>
-    <col min="38" max="38" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="56" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="33.81640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="50" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="40.453125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="57.54296875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="42.54296875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="18.54296875" customWidth="1"/>
-    <col min="73" max="73" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="42.26953125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="34.453125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="37.7265625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="48.81640625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="41.453125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="53.26953125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.453125" customWidth="1"/>
+    <col min="20" max="20" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="47" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.6328125" customWidth="1"/>
+    <col min="38" max="38" width="23.81640625" customWidth="1"/>
+    <col min="39" max="39" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="50" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="49.453125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="18.54296875" customWidth="1"/>
+    <col min="74" max="74" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="42.26953125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="53.26953125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:99" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
@@ -22942,292 +22946,295 @@
         <v>570</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2020</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1856</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1854</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>2003</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>2004</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1476</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>2000</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>2012</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>2013</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>2014</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>2015</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>1590</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>2057</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>2056</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>1940</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>1996</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>733</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>734</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>1843</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>1844</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>1845</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>1846</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>1847</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>1848</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>1849</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>1850</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="CL1" s="3" t="s">
+      <c r="CM1" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>2083</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>2084</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>2078</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>2079</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1766</v>
       </c>
@@ -23238,113 +23245,113 @@
         <v>1198</v>
       </c>
       <c r="D2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E2" t="s">
         <v>523</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>1855</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>628</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>44614</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>45373</v>
       </c>
-      <c r="K2" s="8">
+      <c r="L2" s="8">
         <v>1</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>3</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>629</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>190</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>2022</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>2060</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>2105</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>2090</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>631</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>447</v>
       </c>
-      <c r="W2" s="4">
+      <c r="X2" s="4">
         <v>44615</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>632</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>2001</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>633</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>299</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>634</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>635</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>633</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>299</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>633</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>636</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>266</v>
       </c>
       <c r="AI2" t="s">
         <v>266</v>
       </c>
       <c r="AJ2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AK2" t="s">
         <v>2016</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>2017</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>266</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>268</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>637</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>638</v>
       </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
       <c r="AQ2">
         <v>0</v>
       </c>
@@ -23352,235 +23359,235 @@
         <v>0</v>
       </c>
       <c r="AS2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT2">
         <v>1</v>
       </c>
       <c r="AU2">
+        <v>1</v>
+      </c>
+      <c r="AV2">
         <v>4</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <v>2</v>
-      </c>
-      <c r="AW2">
-        <v>1</v>
       </c>
       <c r="AX2">
         <v>1</v>
       </c>
       <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="AZ2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="s">
         <v>639</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>640</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>641</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>642</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>643</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>644</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>645</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" t="s">
         <v>646</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BI2" t="s">
         <v>647</v>
       </c>
-      <c r="BI2">
+      <c r="BJ2">
         <v>3</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>266</v>
       </c>
-      <c r="BK2">
+      <c r="BL2">
         <v>100000</v>
       </c>
-      <c r="BL2" s="4">
+      <c r="BM2" s="4">
         <v>44449</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>1852</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>268</v>
       </c>
-      <c r="BO2">
+      <c r="BP2">
         <v>25000</v>
       </c>
-      <c r="BP2" s="4">
+      <c r="BQ2" s="4">
         <v>46003</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
         <v>648</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BS2" t="s">
         <v>299</v>
       </c>
-      <c r="BS2">
+      <c r="BT2">
         <v>205000</v>
       </c>
-      <c r="BT2" s="4">
+      <c r="BU2" s="4">
         <v>46368</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
         <v>649</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BW2" t="s">
         <v>266</v>
       </c>
-      <c r="BW2">
+      <c r="BX2">
         <v>125000</v>
       </c>
-      <c r="BX2" s="4">
+      <c r="BY2" s="4">
         <v>46733</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
         <v>650</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CA2" t="s">
         <v>268</v>
       </c>
-      <c r="CA2">
+      <c r="CB2">
         <v>1290</v>
       </c>
-      <c r="CB2" s="4">
+      <c r="CC2" s="4">
         <v>47828</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CD2" t="s">
         <v>1851</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>299</v>
       </c>
-      <c r="CE2">
+      <c r="CF2">
         <v>11000</v>
       </c>
-      <c r="CF2" s="4">
+      <c r="CG2" s="4">
         <v>45272</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CH2" t="s">
         <v>651</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
         <v>652</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CJ2" t="s">
         <v>266</v>
       </c>
-      <c r="CJ2">
+      <c r="CK2">
         <v>100000</v>
       </c>
-      <c r="CK2" s="4">
+      <c r="CL2" s="4">
         <v>45729</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CM2" t="s">
         <v>653</v>
       </c>
-      <c r="CM2">
+      <c r="CN2">
         <v>7</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CO2" t="s">
         <v>654</v>
       </c>
-      <c r="CO2">
+      <c r="CP2">
         <v>1</v>
       </c>
-      <c r="CP2">
+      <c r="CQ2">
         <v>2</v>
       </c>
-      <c r="CQ2">
+      <c r="CR2">
         <v>1</v>
       </c>
-      <c r="CR2">
+      <c r="CS2">
         <v>4</v>
       </c>
-      <c r="CS2">
+      <c r="CT2">
         <v>1</v>
       </c>
-      <c r="CT2">
+      <c r="CU2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1767</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>666</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>45495</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>1853</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>663</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>44614</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>45373</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>4</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>743</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>2106</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>655</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>2002</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>635</v>
       </c>
       <c r="AA3" t="s">
         <v>635</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AB3" t="s">
+        <v>635</v>
+      </c>
+      <c r="AI3" t="s">
         <v>268</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>266</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>2019</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>2018</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>266</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>656</v>
       </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
       <c r="AQ3">
         <v>0</v>
       </c>
@@ -23608,102 +23615,102 @@
       <c r="AY3">
         <v>0</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BG3" t="s">
         <v>657</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BH3" t="s">
         <v>658</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="BI3" t="s">
         <v>659</v>
       </c>
-      <c r="BI3">
+      <c r="BJ3">
         <v>3</v>
       </c>
-      <c r="CD3" t="s">
+      <c r="CE3" t="s">
         <v>268</v>
       </c>
-      <c r="CE3">
-        <v>0</v>
-      </c>
-      <c r="CF3" s="4">
+      <c r="CF3">
+        <v>0</v>
+      </c>
+      <c r="CG3" s="4">
         <v>44897</v>
       </c>
-      <c r="CG3" t="s">
+      <c r="CH3" t="s">
         <v>660</v>
       </c>
-      <c r="CM3">
+      <c r="CN3">
         <v>6</v>
       </c>
-      <c r="CN3" t="s">
+      <c r="CO3" t="s">
         <v>661</v>
       </c>
-      <c r="CO3">
+      <c r="CP3">
         <v>3</v>
       </c>
-      <c r="CP3">
+      <c r="CQ3">
         <v>1</v>
       </c>
-      <c r="CQ3">
+      <c r="CR3">
         <v>5</v>
       </c>
-      <c r="CR3">
+      <c r="CS3">
         <v>1</v>
       </c>
-      <c r="CS3">
+      <c r="CT3">
         <v>6</v>
       </c>
-      <c r="CT3">
+      <c r="CU3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2021</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>518</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="H4" t="s">
+      <c r="F4" s="4"/>
+      <c r="I4" t="s">
         <v>665</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>45495</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>45910</v>
       </c>
-      <c r="K4" s="8">
-        <v>0</v>
-      </c>
       <c r="L4" s="8">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>190</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>2058</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>2061</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>2023</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>11</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>1</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>5</v>
       </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
       <c r="AT4">
         <v>0</v>
       </c>
@@ -23722,14 +23729,14 @@
       <c r="AY4">
         <v>0</v>
       </c>
-      <c r="BI4">
-        <v>0</v>
-      </c>
-      <c r="CF4" s="4"/>
-      <c r="CM4">
-        <v>0</v>
-      </c>
-      <c r="CO4">
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="CG4" s="4"/>
+      <c r="CN4">
         <v>0</v>
       </c>
       <c r="CP4">
@@ -23747,38 +23754,38 @@
       <c r="CT4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.35">
+      <c r="CU4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2024</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>518</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="8">
-        <v>0</v>
-      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="8">
         <v>0</v>
       </c>
-      <c r="S5" t="s">
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
         <v>2107</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>12</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>6</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>1</v>
       </c>
-      <c r="AS5">
-        <v>0</v>
-      </c>
       <c r="AT5">
         <v>0</v>
       </c>
@@ -23797,14 +23804,14 @@
       <c r="AY5">
         <v>0</v>
       </c>
-      <c r="BI5">
-        <v>0</v>
-      </c>
-      <c r="CF5" s="4"/>
-      <c r="CM5">
-        <v>0</v>
-      </c>
-      <c r="CO5">
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BJ5">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="4"/>
+      <c r="CN5">
         <v>0</v>
       </c>
       <c r="CP5">
@@ -23822,44 +23829,44 @@
       <c r="CT5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.35">
+      <c r="CU5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:99" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>664</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>518</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>665</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>45064</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>45373</v>
       </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
       <c r="L6" s="8">
         <v>0</v>
       </c>
-      <c r="O6" t="s">
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
         <v>2059</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>2062</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>744</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>13</v>
       </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
       <c r="AR6">
         <v>0</v>
       </c>
@@ -23884,13 +23891,13 @@
       <c r="AY6">
         <v>0</v>
       </c>
-      <c r="BI6">
-        <v>0</v>
-      </c>
-      <c r="CM6">
-        <v>0</v>
-      </c>
-      <c r="CO6">
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BJ6">
+        <v>0</v>
+      </c>
+      <c r="CN6">
         <v>0</v>
       </c>
       <c r="CP6">
@@ -23900,74 +23907,77 @@
         <v>0</v>
       </c>
       <c r="CR6">
+        <v>0</v>
+      </c>
+      <c r="CS6">
         <v>1</v>
       </c>
-      <c r="CS6">
+      <c r="CT6">
         <v>4</v>
       </c>
-      <c r="CT6">
+      <c r="CU6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K7" s="8"/>
+    <row r="7" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K8" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K9" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K10" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K11" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K12" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K13" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K14" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K15" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:98" x14ac:dyDescent="0.35">
-      <c r="K16" s="8"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:99" x14ac:dyDescent="0.35">
       <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K17" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K18" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K19" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K20" s="8"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K21" s="8"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Leases consolidations and consultations test cases corrections
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F1A0F0-A397-43A9-A7C4-246CF09D86B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB34F714-D62C-431A-A2D9-F08945064F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="1080" windowWidth="29040" windowHeight="17520" tabRatio="950" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -6574,9 +6574,6 @@
     <t>First Nation</t>
   </si>
   <si>
-    <t>Headquarters (HQ)</t>
-  </si>
-  <si>
     <t>Regional planning</t>
   </si>
   <si>
@@ -6653,6 +6650,9 @@
   </si>
   <si>
     <t>Updated Engineering Automated test</t>
+  </si>
+  <si>
+    <t>Headquarter (HQ)</t>
   </si>
 </sst>
 </file>
@@ -9827,7 +9827,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -10038,7 +10038,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10243,7 +10243,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10766,7 +10766,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -11079,7 +11079,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -15050,7 +15050,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -23663,8 +23663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CY21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24376,6 +24376,12 @@
       <c r="CV2">
         <v>5</v>
       </c>
+      <c r="CW2">
+        <v>0</v>
+      </c>
+      <c r="CX2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -24528,6 +24534,12 @@
       <c r="CV3">
         <v>1</v>
       </c>
+      <c r="CW3">
+        <v>0</v>
+      </c>
+      <c r="CX3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -24634,6 +24646,12 @@
       <c r="CV4">
         <v>0</v>
       </c>
+      <c r="CW4">
+        <v>0</v>
+      </c>
+      <c r="CX4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -24727,6 +24745,12 @@
       <c r="CV5">
         <v>0</v>
       </c>
+      <c r="CW5">
+        <v>0</v>
+      </c>
+      <c r="CX5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -24828,6 +24852,12 @@
       <c r="CV6">
         <v>1</v>
       </c>
+      <c r="CW6">
+        <v>0</v>
+      </c>
+      <c r="CX6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -24929,6 +24959,12 @@
       <c r="CV7">
         <v>0</v>
       </c>
+      <c r="CW7">
+        <v>0</v>
+      </c>
+      <c r="CX7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -25055,6 +25091,12 @@
         <v>0</v>
       </c>
       <c r="CV8">
+        <v>0</v>
+      </c>
+      <c r="CW8">
+        <v>0</v>
+      </c>
+      <c r="CX8">
         <v>0</v>
       </c>
     </row>
@@ -25642,8 +25684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408261CA-1BB0-4036-BE95-18F8D8636D54}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25669,7 +25711,7 @@
         <v>2145</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2146</v>
@@ -25710,7 +25752,7 @@
         <v>663</v>
       </c>
       <c r="F2" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="H2" t="s">
         <v>266</v>
@@ -25722,7 +25764,7 @@
         <v>1210</v>
       </c>
       <c r="K2" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -25739,17 +25781,17 @@
         <v>663</v>
       </c>
       <c r="F3" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="H3" t="s">
         <v>268</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="K3" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -25766,7 +25808,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="H4" t="s">
         <v>266</v>
@@ -25775,10 +25817,10 @@
         <v>45563</v>
       </c>
       <c r="J4" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="K4" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -25786,7 +25828,7 @@
         <v>2157</v>
       </c>
       <c r="B5" t="s">
-        <v>2164</v>
+        <v>2190</v>
       </c>
       <c r="D5" s="4">
         <v>45546</v>
@@ -25795,7 +25837,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="H5" t="s">
         <v>266</v>
@@ -25804,10 +25846,10 @@
         <v>45562</v>
       </c>
       <c r="J5" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="K5" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -25815,7 +25857,7 @@
         <v>2158</v>
       </c>
       <c r="B6" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D6" s="4">
         <v>45547</v>
@@ -25824,17 +25866,17 @@
         <v>663</v>
       </c>
       <c r="F6" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="H6" t="s">
         <v>268</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="K6" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -25842,7 +25884,7 @@
         <v>2159</v>
       </c>
       <c r="B7" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D7" s="4">
         <v>45548</v>
@@ -25851,7 +25893,7 @@
         <v>663</v>
       </c>
       <c r="F7" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="H7" t="s">
         <v>266</v>
@@ -25863,7 +25905,7 @@
         <v>1210</v>
       </c>
       <c r="K7" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -25871,7 +25913,7 @@
         <v>2160</v>
       </c>
       <c r="B8" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="D8" s="4">
         <v>45549</v>
@@ -25892,10 +25934,10 @@
         <v>45559</v>
       </c>
       <c r="J8" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="K8" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -25906,7 +25948,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="D9" s="4">
         <v>45550</v>
@@ -25925,15 +25967,15 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="K9" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B10" t="s">
         <v>2162</v>
@@ -25945,7 +25987,7 @@
         <v>663</v>
       </c>
       <c r="F10" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="H10" t="s">
         <v>266</v>
@@ -25954,10 +25996,10 @@
         <v>45557</v>
       </c>
       <c r="J10" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="K10" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes on automation branch IS92
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB34F714-D62C-431A-A2D9-F08945064F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81993C9B-7C6B-42CC-926A-57B9D3B11D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="1080" windowWidth="29040" windowHeight="17520" tabRatio="950" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3807" uniqueCount="2191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3807" uniqueCount="2192">
   <si>
     <t>FirstName</t>
   </si>
@@ -6574,9 +6574,6 @@
     <t>First Nation</t>
   </si>
   <si>
-    <t>Regional planning</t>
-  </si>
-  <si>
     <t>Regional property services</t>
   </si>
   <si>
@@ -6653,6 +6650,12 @@
   </si>
   <si>
     <t>Headquarter (HQ)</t>
+  </si>
+  <si>
+    <t>001 Hyderbad</t>
+  </si>
+  <si>
+    <t>Regional Planning</t>
   </si>
 </sst>
 </file>
@@ -9537,8 +9540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AL34" sqref="AL34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9827,7 +9830,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -10038,7 +10041,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10243,7 +10246,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10766,7 +10769,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -11079,7 +11082,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -15050,7 +15053,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -21078,7 +21081,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21252,8 +21255,8 @@
   <dimension ref="A1:AX84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68:XFD72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23663,8 +23666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CY21"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AP2" sqref="AP2"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BG6" sqref="BG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24095,7 +24098,7 @@
         <v>1186</v>
       </c>
       <c r="D2" t="s">
-        <v>385</v>
+        <v>2190</v>
       </c>
       <c r="E2" t="s">
         <v>523</v>
@@ -25111,7 +25114,7 @@
         <v>1186</v>
       </c>
       <c r="D9" t="s">
-        <v>385</v>
+        <v>2190</v>
       </c>
       <c r="E9" t="s">
         <v>518</v>
@@ -25685,7 +25688,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25711,7 +25714,7 @@
         <v>2145</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2146</v>
@@ -25752,7 +25755,7 @@
         <v>663</v>
       </c>
       <c r="F2" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="H2" t="s">
         <v>266</v>
@@ -25764,7 +25767,7 @@
         <v>1210</v>
       </c>
       <c r="K2" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -25781,17 +25784,17 @@
         <v>663</v>
       </c>
       <c r="F3" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="H3" t="s">
         <v>268</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="K3" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -25808,7 +25811,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="H4" t="s">
         <v>266</v>
@@ -25817,10 +25820,10 @@
         <v>45563</v>
       </c>
       <c r="J4" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="K4" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -25828,7 +25831,7 @@
         <v>2157</v>
       </c>
       <c r="B5" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="D5" s="4">
         <v>45546</v>
@@ -25837,7 +25840,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="H5" t="s">
         <v>266</v>
@@ -25846,10 +25849,10 @@
         <v>45562</v>
       </c>
       <c r="J5" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="K5" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -25857,7 +25860,7 @@
         <v>2158</v>
       </c>
       <c r="B6" t="s">
-        <v>2164</v>
+        <v>2191</v>
       </c>
       <c r="D6" s="4">
         <v>45547</v>
@@ -25866,17 +25869,17 @@
         <v>663</v>
       </c>
       <c r="F6" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="H6" t="s">
         <v>268</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="K6" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -25884,7 +25887,7 @@
         <v>2159</v>
       </c>
       <c r="B7" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D7" s="4">
         <v>45548</v>
@@ -25893,7 +25896,7 @@
         <v>663</v>
       </c>
       <c r="F7" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="H7" t="s">
         <v>266</v>
@@ -25905,7 +25908,7 @@
         <v>1210</v>
       </c>
       <c r="K7" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -25913,7 +25916,7 @@
         <v>2160</v>
       </c>
       <c r="B8" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D8" s="4">
         <v>45549</v>
@@ -25934,10 +25937,10 @@
         <v>45559</v>
       </c>
       <c r="J8" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="K8" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -25948,7 +25951,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="D9" s="4">
         <v>45550</v>
@@ -25967,15 +25970,15 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="K9" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="B10" t="s">
         <v>2162</v>
@@ -25987,7 +25990,7 @@
         <v>663</v>
       </c>
       <c r="F10" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="H10" t="s">
         <v>266</v>
@@ -25996,10 +25999,10 @@
         <v>45557</v>
       </c>
       <c r="J10" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="K10" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes on automation branch IS92 (#4425)
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB34F714-D62C-431A-A2D9-F08945064F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81993C9B-7C6B-42CC-926A-57B9D3B11D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="1080" windowWidth="29040" windowHeight="17520" tabRatio="950" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3807" uniqueCount="2191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3807" uniqueCount="2192">
   <si>
     <t>FirstName</t>
   </si>
@@ -6574,9 +6574,6 @@
     <t>First Nation</t>
   </si>
   <si>
-    <t>Regional planning</t>
-  </si>
-  <si>
     <t>Regional property services</t>
   </si>
   <si>
@@ -6653,6 +6650,12 @@
   </si>
   <si>
     <t>Headquarter (HQ)</t>
+  </si>
+  <si>
+    <t>001 Hyderbad</t>
+  </si>
+  <si>
+    <t>Regional Planning</t>
   </si>
 </sst>
 </file>
@@ -9537,8 +9540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AL34" sqref="AL34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9827,7 +9830,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -10038,7 +10041,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10243,7 +10246,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10766,7 +10769,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -11079,7 +11082,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -15050,7 +15053,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45574</v>
+        <v>45595</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -21078,7 +21081,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21252,8 +21255,8 @@
   <dimension ref="A1:AX84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68:XFD72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23663,8 +23666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CY21"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AP2" sqref="AP2"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BG6" sqref="BG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24095,7 +24098,7 @@
         <v>1186</v>
       </c>
       <c r="D2" t="s">
-        <v>385</v>
+        <v>2190</v>
       </c>
       <c r="E2" t="s">
         <v>523</v>
@@ -25111,7 +25114,7 @@
         <v>1186</v>
       </c>
       <c r="D9" t="s">
-        <v>385</v>
+        <v>2190</v>
       </c>
       <c r="E9" t="s">
         <v>518</v>
@@ -25685,7 +25688,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25711,7 +25714,7 @@
         <v>2145</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2146</v>
@@ -25752,7 +25755,7 @@
         <v>663</v>
       </c>
       <c r="F2" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="H2" t="s">
         <v>266</v>
@@ -25764,7 +25767,7 @@
         <v>1210</v>
       </c>
       <c r="K2" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -25781,17 +25784,17 @@
         <v>663</v>
       </c>
       <c r="F3" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="H3" t="s">
         <v>268</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="K3" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -25808,7 +25811,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="H4" t="s">
         <v>266</v>
@@ -25817,10 +25820,10 @@
         <v>45563</v>
       </c>
       <c r="J4" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="K4" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -25828,7 +25831,7 @@
         <v>2157</v>
       </c>
       <c r="B5" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="D5" s="4">
         <v>45546</v>
@@ -25837,7 +25840,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="H5" t="s">
         <v>266</v>
@@ -25846,10 +25849,10 @@
         <v>45562</v>
       </c>
       <c r="J5" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="K5" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -25857,7 +25860,7 @@
         <v>2158</v>
       </c>
       <c r="B6" t="s">
-        <v>2164</v>
+        <v>2191</v>
       </c>
       <c r="D6" s="4">
         <v>45547</v>
@@ -25866,17 +25869,17 @@
         <v>663</v>
       </c>
       <c r="F6" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="H6" t="s">
         <v>268</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="K6" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -25884,7 +25887,7 @@
         <v>2159</v>
       </c>
       <c r="B7" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D7" s="4">
         <v>45548</v>
@@ -25893,7 +25896,7 @@
         <v>663</v>
       </c>
       <c r="F7" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="H7" t="s">
         <v>266</v>
@@ -25905,7 +25908,7 @@
         <v>1210</v>
       </c>
       <c r="K7" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -25913,7 +25916,7 @@
         <v>2160</v>
       </c>
       <c r="B8" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D8" s="4">
         <v>45549</v>
@@ -25934,10 +25937,10 @@
         <v>45559</v>
       </c>
       <c r="J8" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="K8" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -25948,7 +25951,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="D9" s="4">
         <v>45550</v>
@@ -25967,15 +25970,15 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="K9" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="B10" t="s">
         <v>2162</v>
@@ -25987,7 +25990,7 @@
         <v>663</v>
       </c>
       <c r="F10" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="H10" t="s">
         <v>266</v>
@@ -25996,10 +25999,10 @@
         <v>45557</v>
       </c>
       <c r="J10" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="K10" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes on automation test set - IS94
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD87F51-8E89-4A39-8148-FBD252E0E20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F7A2E-F3A4-4999-A5FD-6FFDC0568C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="27" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -5908,9 +5908,6 @@
     <t>0948523 B.C.LTD.</t>
   </si>
   <si>
-    <t>Automated Acquisition File - Takes Logic IS89</t>
-  </si>
-  <si>
     <t>UNIT 19 -- 171 17 St SE, Salmon Arm, BC</t>
   </si>
   <si>
@@ -6527,6 +6524,9 @@
   </si>
   <si>
     <t>Automated Test - Minimum Insurance test</t>
+  </si>
+  <si>
+    <t>Automated Acquisition File - Takes Logic IS94</t>
   </si>
 </sst>
 </file>
@@ -7605,7 +7605,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7635,7 +7635,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B2" t="s">
         <v>607</v>
@@ -7652,7 +7652,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -7681,12 +7681,12 @@
         <v>614</v>
       </c>
       <c r="E4" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -7698,7 +7698,7 @@
         <v>617</v>
       </c>
       <c r="E5" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -7737,7 +7737,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B8" t="s">
         <v>607</v>
@@ -7749,12 +7749,12 @@
         <v>609</v>
       </c>
       <c r="E8" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -7771,7 +7771,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -7788,7 +7788,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B12" t="s">
         <v>607</v>
@@ -7822,7 +7822,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B13" t="s">
         <v>607</v>
@@ -8201,7 +8201,7 @@
         <v>2500</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="K2" s="17">
         <f>I2*0.05</f>
@@ -8218,7 +8218,7 @@
         <v>1500.5</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P2" s="16"/>
       <c r="Q2" s="17">
@@ -8232,7 +8232,7 @@
         <v>200.79</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="U2" s="6">
         <v>10.029999999999999</v>
@@ -8270,7 +8270,7 @@
         <v>3500</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="K3" s="17"/>
       <c r="L3" s="17">
@@ -8284,7 +8284,7 @@
         <v>1500.99</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="17">
@@ -8293,7 +8293,7 @@
       </c>
       <c r="S3" s="6"/>
       <c r="T3" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -8327,7 +8327,7 @@
         <v>3000</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="17">
@@ -8336,13 +8336,13 @@
       </c>
       <c r="N4" s="6"/>
       <c r="O4" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="17"/>
       <c r="S4" s="6"/>
       <c r="T4" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -8376,7 +8376,7 @@
         <v>120000</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" ref="K5" si="2">I5*0.05</f>
@@ -8388,13 +8388,13 @@
       </c>
       <c r="N5" s="6"/>
       <c r="O5" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="17"/>
       <c r="S5" s="6"/>
       <c r="T5" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -8428,7 +8428,7 @@
         <v>3000</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17">
@@ -8442,7 +8442,7 @@
         <v>150.78</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="P6" s="16">
         <v>8</v>
@@ -8458,7 +8458,7 @@
         <v>1000</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="U6" s="6">
         <v>20</v>
@@ -9413,7 +9413,7 @@
   <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AL34" sqref="AL34"/>
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9555,13 +9555,13 @@
         <v>901</v>
       </c>
       <c r="AG1" s="3" t="s">
+        <v>1961</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>1962</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1963</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>1964</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>1155</v>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10954,7 +10954,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -11340,7 +11340,7 @@
         <v>246</v>
       </c>
       <c r="L20" t="s">
-        <v>1942</v>
+        <v>2148</v>
       </c>
       <c r="O20" t="s">
         <v>702</v>
@@ -13737,7 +13737,7 @@
         <v>45241</v>
       </c>
       <c r="K2" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="L2" t="s">
         <v>1692</v>
@@ -13872,7 +13872,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B5" s="11">
         <v>56700.89</v>
@@ -13887,28 +13887,28 @@
         <v>496</v>
       </c>
       <c r="F5" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="G5" s="4">
         <v>45569</v>
       </c>
       <c r="K5" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="L5" t="s">
         <v>1692</v>
       </c>
       <c r="M5" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="N5" t="s">
         <v>959</v>
       </c>
       <c r="O5" t="s">
+        <v>1978</v>
+      </c>
+      <c r="P5" t="s">
         <v>1979</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1980</v>
       </c>
       <c r="Q5" t="s">
         <v>812</v>
@@ -13920,7 +13920,7 @@
         <v>1508</v>
       </c>
       <c r="T5" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="U5">
         <v>6</v>
@@ -13931,7 +13931,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -14097,10 +14097,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B7" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="C7">
         <v>5000</v>
@@ -14118,10 +14118,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B8" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="C8">
         <v>1200.8900000000001</v>
@@ -14136,10 +14136,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B9" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="C9">
         <v>50500</v>
@@ -14157,7 +14157,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B10" t="s">
         <v>1078</v>
@@ -14184,7 +14184,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -16088,7 +16088,7 @@
         <v>1547</v>
       </c>
       <c r="B3" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -16124,7 +16124,7 @@
         <v>1547</v>
       </c>
       <c r="B6" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C6" t="s">
         <v>607</v>
@@ -16512,7 +16512,7 @@
         <v>706</v>
       </c>
       <c r="C18" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
@@ -16644,7 +16644,7 @@
         <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -16666,7 +16666,7 @@
         <v>1742</v>
       </c>
       <c r="D7" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -16724,7 +16724,7 @@
         <v>1770</v>
       </c>
       <c r="E12" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="F12" t="s">
         <v>1768</v>
@@ -20953,7 +20953,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21126,9 +21126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21178,7 +21178,7 @@
         <v>510</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>452</v>
@@ -21292,10 +21292,10 @@
         <v>440</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>2089</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>2090</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>2091</v>
       </c>
       <c r="AR1" s="3" t="s">
         <v>441</v>
@@ -21382,7 +21382,7 @@
         <v>502</v>
       </c>
       <c r="T4" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.35">
@@ -21427,7 +21427,7 @@
         <v>500</v>
       </c>
       <c r="AV7" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.35">
@@ -21442,7 +21442,7 @@
         <v>501</v>
       </c>
       <c r="AV8" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.35">
@@ -21457,7 +21457,7 @@
         <v>495</v>
       </c>
       <c r="AV9" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.35">
@@ -21472,18 +21472,18 @@
         <v>496</v>
       </c>
       <c r="AE10" t="s">
+        <v>2065</v>
+      </c>
+      <c r="AG10" t="s">
         <v>2066</v>
       </c>
-      <c r="AG10" t="s">
-        <v>2067</v>
-      </c>
       <c r="AX10" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="11" spans="1:53" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>462</v>
@@ -21497,7 +21497,7 @@
       <c r="O11" s="36"/>
       <c r="Q11" s="36"/>
       <c r="AV11" s="23" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="AW11" s="36"/>
     </row>
@@ -21585,7 +21585,7 @@
         <v>496</v>
       </c>
       <c r="AV16" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.35">
@@ -21603,13 +21603,13 @@
         <v>45245</v>
       </c>
       <c r="W17" t="s">
+        <v>2071</v>
+      </c>
+      <c r="AA17" t="s">
         <v>2072</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AV17" t="s">
         <v>2073</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>2074</v>
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.35">
@@ -21627,19 +21627,19 @@
         <v>36509</v>
       </c>
       <c r="P18" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="Q18" s="13">
         <v>36778</v>
       </c>
       <c r="R18" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="W18" s="9" t="s">
         <v>508</v>
       </c>
       <c r="X18" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="AA18" t="s">
         <v>509</v>
@@ -21648,7 +21648,7 @@
       <c r="AP18" s="4"/>
       <c r="AQ18" s="4"/>
       <c r="AS18" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.35">
@@ -21666,13 +21666,13 @@
         <v>47045</v>
       </c>
       <c r="N19" t="s">
+        <v>2078</v>
+      </c>
+      <c r="AF19" t="s">
         <v>2079</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AU19" t="s">
         <v>2080</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>2081</v>
       </c>
       <c r="AW19" s="13">
         <v>42988</v>
@@ -21684,18 +21684,18 @@
         <v>Research File - Lease / License agreement</v>
       </c>
       <c r="B20" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="C20" t="s">
         <v>501</v>
       </c>
       <c r="AV20" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="21" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>474</v>
@@ -21709,7 +21709,7 @@
       <c r="O21" s="36"/>
       <c r="Q21" s="36"/>
       <c r="AV21" s="23" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="AW21" s="36"/>
     </row>
@@ -21763,16 +21763,16 @@
         <v>Acquisition File - Agricultural Land Commission (ALC)</v>
       </c>
       <c r="B24" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C24" t="s">
         <v>496</v>
       </c>
       <c r="D24" t="s">
+        <v>2084</v>
+      </c>
+      <c r="AV24" t="s">
         <v>2085</v>
-      </c>
-      <c r="AV24" t="s">
-        <v>2086</v>
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.35">
@@ -21781,13 +21781,13 @@
         <v>Acquisition File - Form 5 - Approval of expropriation</v>
       </c>
       <c r="B25" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C25" t="s">
         <v>497</v>
       </c>
       <c r="AV25" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.35">
@@ -21802,7 +21802,7 @@
         <v>498</v>
       </c>
       <c r="AV26" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.35">
@@ -21811,13 +21811,13 @@
         <v>Acquisition File - Compensation requisition (H-120)</v>
       </c>
       <c r="B27" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="C27" t="s">
         <v>499</v>
       </c>
       <c r="AV27" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.35">
@@ -21826,19 +21826,19 @@
         <v>Acquisition File - Land Act Tenure/Reserves</v>
       </c>
       <c r="B28" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C28" t="s">
         <v>500</v>
       </c>
       <c r="AP28" t="s">
+        <v>2091</v>
+      </c>
+      <c r="AQ28" t="s">
         <v>2092</v>
       </c>
-      <c r="AQ28" t="s">
+      <c r="AV28" t="s">
         <v>2093</v>
-      </c>
-      <c r="AV28" t="s">
-        <v>2094</v>
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.35">
@@ -21853,7 +21853,7 @@
         <v>501</v>
       </c>
       <c r="AV29" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.35">
@@ -21868,13 +21868,13 @@
         <v>495</v>
       </c>
       <c r="W30" t="s">
+        <v>2095</v>
+      </c>
+      <c r="AA30" t="s">
         <v>2096</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AI30" t="s">
         <v>2097</v>
-      </c>
-      <c r="AI30" t="s">
-        <v>2098</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.35">
@@ -21889,7 +21889,7 @@
         <v>496</v>
       </c>
       <c r="AV31" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.35">
@@ -21907,16 +21907,16 @@
         <v>36850</v>
       </c>
       <c r="Y32" t="s">
+        <v>2099</v>
+      </c>
+      <c r="Z32" t="s">
         <v>2100</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AN32" t="s">
         <v>2101</v>
       </c>
-      <c r="AN32" t="s">
+      <c r="AS32" t="s">
         <v>2102</v>
-      </c>
-      <c r="AS32" t="s">
-        <v>2103</v>
       </c>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.35">
@@ -21925,18 +21925,18 @@
         <v>Acquisition File - Form 7 - Notice of abandonement</v>
       </c>
       <c r="B33" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C33" t="s">
         <v>498</v>
       </c>
       <c r="AV33" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="34" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>761</v>
@@ -21950,7 +21950,7 @@
       <c r="O34" s="36"/>
       <c r="Q34" s="36"/>
       <c r="AV34" s="23" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="AW34" s="36"/>
     </row>
@@ -21990,7 +21990,7 @@
         <v>777</v>
       </c>
       <c r="AN36" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="AV36" t="s">
         <v>778</v>
@@ -22002,7 +22002,7 @@
         <v>Project -Financial records (invoices, journal vouchers, received cheques etc.)</v>
       </c>
       <c r="B37" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C37" t="s">
         <v>495</v>
@@ -22026,19 +22026,19 @@
         <v>780</v>
       </c>
       <c r="W38" t="s">
+        <v>2106</v>
+      </c>
+      <c r="Z38" t="s">
         <v>2107</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="AA38" t="s">
         <v>2108</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>2109</v>
       </c>
       <c r="AO38" s="13">
         <v>43757</v>
       </c>
       <c r="AR38" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.35">
@@ -22056,10 +22056,10 @@
         <v>7190089</v>
       </c>
       <c r="AN39" t="s">
+        <v>2110</v>
+      </c>
+      <c r="AV39" t="s">
         <v>2111</v>
-      </c>
-      <c r="AV39" t="s">
-        <v>2112</v>
       </c>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.35">
@@ -22080,16 +22080,16 @@
         <v>781</v>
       </c>
       <c r="AI40" t="s">
+        <v>2112</v>
+      </c>
+      <c r="AJ40" t="s">
         <v>2113</v>
       </c>
-      <c r="AJ40" t="s">
+      <c r="AL40" t="s">
         <v>2114</v>
       </c>
-      <c r="AL40" t="s">
+      <c r="AM40" t="s">
         <v>2115</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>2116</v>
       </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.35">
@@ -22104,7 +22104,7 @@
         <v>499</v>
       </c>
       <c r="F41" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="H41" s="13">
         <v>32301</v>
@@ -22119,16 +22119,16 @@
         <v>784</v>
       </c>
       <c r="AE41" t="s">
+        <v>2117</v>
+      </c>
+      <c r="AN41" t="s">
         <v>2118</v>
-      </c>
-      <c r="AN41" t="s">
-        <v>2119</v>
       </c>
       <c r="AO41" s="4"/>
       <c r="AP41" s="4"/>
       <c r="AQ41" s="4"/>
       <c r="AV41" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.35">
@@ -22143,7 +22143,7 @@
         <v>500</v>
       </c>
       <c r="AV42" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.35">
@@ -22158,12 +22158,12 @@
         <v>501</v>
       </c>
       <c r="AV43" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="44" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>462</v>
@@ -22187,7 +22187,7 @@
         <v>Disposition File -Certificate of Compliance</v>
       </c>
       <c r="B45" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C45" t="s">
         <v>496</v>
@@ -22202,13 +22202,13 @@
         <v>Disposition File -Enhanced Referral Records</v>
       </c>
       <c r="B46" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="C46" t="s">
         <v>497</v>
       </c>
       <c r="AV46" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.35">
@@ -22217,13 +22217,13 @@
         <v>Disposition File -First Nations Strength of Claim Report</v>
       </c>
       <c r="B47" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C47" t="s">
         <v>498</v>
       </c>
       <c r="AV47" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.35">
@@ -22238,7 +22238,7 @@
         <v>499</v>
       </c>
       <c r="AG48" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.35">
@@ -22253,7 +22253,7 @@
         <v>500</v>
       </c>
       <c r="AV49" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.35">
@@ -22271,13 +22271,13 @@
         <v>89997</v>
       </c>
       <c r="AC50" t="s">
+        <v>2126</v>
+      </c>
+      <c r="AD50" t="s">
         <v>2127</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AS50" t="s">
         <v>2128</v>
-      </c>
-      <c r="AS50" t="s">
-        <v>2129</v>
       </c>
       <c r="AZ50">
         <v>1997</v>
@@ -22289,13 +22289,13 @@
         <v>Disposition File -Purchase and Sale Agreement</v>
       </c>
       <c r="B51" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C51" t="s">
         <v>495</v>
       </c>
       <c r="AV51" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="52" spans="1:53" x14ac:dyDescent="0.35">
@@ -22310,7 +22310,7 @@
         <v>496</v>
       </c>
       <c r="AV52" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.35">
@@ -22325,12 +22325,12 @@
         <v>497</v>
       </c>
       <c r="AV53" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="54" spans="1:53" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="23" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>764</v>
@@ -22346,14 +22346,14 @@
       <c r="O54" s="36"/>
       <c r="Q54" s="36"/>
       <c r="Z54" s="23" t="s">
+        <v>2132</v>
+      </c>
+      <c r="AS54" s="23" t="s">
         <v>2133</v>
-      </c>
-      <c r="AS54" s="23" t="s">
-        <v>2134</v>
       </c>
       <c r="AW54" s="36"/>
       <c r="AY54" s="23" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="55" spans="1:53" x14ac:dyDescent="0.35">
@@ -22362,13 +22362,13 @@
         <v>Property Management -Approval/sign-off</v>
       </c>
       <c r="B55" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="C55" t="s">
         <v>499</v>
       </c>
       <c r="AV55" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="56" spans="1:53" x14ac:dyDescent="0.35">
@@ -22377,13 +22377,13 @@
         <v>Property Management -Form 8 - Notice of advanced payment </v>
       </c>
       <c r="B56" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="C56" t="s">
         <v>500</v>
       </c>
       <c r="AV56" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.35">
@@ -22392,13 +22392,13 @@
         <v>Property Management -Form 1 - Notice of expropriation </v>
       </c>
       <c r="B57" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="C57" t="s">
         <v>501</v>
       </c>
       <c r="AV57" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.35">
@@ -22413,7 +22413,7 @@
         <v>495</v>
       </c>
       <c r="AV58" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="59" spans="1:53" x14ac:dyDescent="0.35">
@@ -22428,7 +22428,7 @@
         <v>496</v>
       </c>
       <c r="AV59" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="60" spans="1:53" x14ac:dyDescent="0.35">
@@ -22443,7 +22443,7 @@
         <v>497</v>
       </c>
       <c r="AV60" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.35">
@@ -22473,7 +22473,7 @@
         <v>499</v>
       </c>
       <c r="AV62" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="63" spans="1:53" x14ac:dyDescent="0.35">
@@ -22491,16 +22491,16 @@
         <v>32874</v>
       </c>
       <c r="Z63" t="s">
+        <v>2138</v>
+      </c>
+      <c r="AN63" t="s">
         <v>2139</v>
-      </c>
-      <c r="AN63" t="s">
-        <v>2140</v>
       </c>
       <c r="AS63" t="s">
         <v>1509</v>
       </c>
       <c r="AY63" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="64" spans="1:53" x14ac:dyDescent="0.35">
@@ -22509,18 +22509,18 @@
         <v>Property Management -Form 9 - Vesting notice (Form 9)</v>
       </c>
       <c r="B64" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C64" t="s">
         <v>501</v>
       </c>
       <c r="AV64" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="23" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="B65" s="23" t="s">
         <v>487</v>
@@ -22534,7 +22534,7 @@
       <c r="O65" s="36"/>
       <c r="Q65" s="36"/>
       <c r="AV65" s="23" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="AW65" s="36"/>
     </row>
@@ -23217,8 +23217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CY21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="CV6" sqref="CV6"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AZ8" sqref="AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23338,7 +23338,7 @@
         <v>515</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>516</v>
@@ -23452,10 +23452,10 @@
         <v>1887</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>1987</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>1988</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>1989</v>
       </c>
       <c r="AR1" s="3" t="s">
         <v>1773</v>
@@ -23467,7 +23467,7 @@
         <v>537</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>538</v>
@@ -23482,10 +23482,10 @@
         <v>1829</v>
       </c>
       <c r="AZ1" s="3" t="s">
+        <v>1949</v>
+      </c>
+      <c r="BA1" s="3" t="s">
         <v>1950</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>1951</v>
       </c>
       <c r="BB1" s="3" t="s">
         <v>541</v>
@@ -23629,13 +23629,13 @@
         <v>1910</v>
       </c>
       <c r="CW1" s="3" t="s">
+        <v>1964</v>
+      </c>
+      <c r="CX1" s="3" t="s">
         <v>1965</v>
       </c>
-      <c r="CX1" s="3" t="s">
+      <c r="CY1" s="3" t="s">
         <v>1966</v>
-      </c>
-      <c r="CY1" s="3" t="s">
-        <v>1967</v>
       </c>
     </row>
     <row r="2" spans="1:103" x14ac:dyDescent="0.35">
@@ -23649,7 +23649,7 @@
         <v>1081</v>
       </c>
       <c r="D2" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="E2" t="s">
         <v>501</v>
@@ -24359,7 +24359,7 @@
         <v>0</v>
       </c>
       <c r="AS6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AT6">
         <v>1</v>
@@ -24374,7 +24374,7 @@
         <v>0</v>
       </c>
       <c r="AX6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY6">
         <v>0</v>
@@ -24398,7 +24398,7 @@
         <v>44114</v>
       </c>
       <c r="BO6" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="CO6">
         <v>1</v>
@@ -24430,7 +24430,7 @@
     </row>
     <row r="7" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="E7" t="s">
         <v>496</v>
@@ -24451,13 +24451,13 @@
         <v>192</v>
       </c>
       <c r="P7" t="s">
+        <v>1952</v>
+      </c>
+      <c r="R7" t="s">
         <v>1953</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>1954</v>
-      </c>
-      <c r="T7" t="s">
-        <v>1955</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -24537,7 +24537,7 @@
     </row>
     <row r="8" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="E8" t="s">
         <v>496</v>
@@ -24671,7 +24671,7 @@
     </row>
     <row r="9" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B9" t="s">
         <v>1082</v>
@@ -24680,7 +24680,7 @@
         <v>1081</v>
       </c>
       <c r="D9" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="E9" t="s">
         <v>496</v>
@@ -24701,13 +24701,13 @@
         <v>191</v>
       </c>
       <c r="P9" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R9" t="s">
         <v>1969</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>1970</v>
-      </c>
-      <c r="T9" t="s">
-        <v>1971</v>
       </c>
       <c r="AI9" t="s">
         <v>299</v>
@@ -24799,7 +24799,7 @@
     </row>
     <row r="10" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="E10" t="s">
         <v>496</v>
@@ -24820,13 +24820,13 @@
         <v>191</v>
       </c>
       <c r="P10" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R10" t="s">
         <v>1969</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>1970</v>
-      </c>
-      <c r="T10" t="s">
-        <v>1971</v>
       </c>
       <c r="AM10">
         <v>22</v>
@@ -25068,7 +25068,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25209,7 +25209,7 @@
         <v>1601</v>
       </c>
       <c r="K5" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -25220,7 +25220,7 @@
         <v>1883</v>
       </c>
       <c r="K6" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -25282,39 +25282,39 @@
         <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1990</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2010</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1991</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1992</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1993</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1994</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1995</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1996</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1997</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1998</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B2" t="s">
         <v>532</v>
@@ -25326,7 +25326,7 @@
         <v>607</v>
       </c>
       <c r="F2" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H2" t="s">
         <v>266</v>
@@ -25338,15 +25338,15 @@
         <v>1105</v>
       </c>
       <c r="K2" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B3" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D3" s="4">
         <v>45544</v>
@@ -25355,25 +25355,25 @@
         <v>607</v>
       </c>
       <c r="F3" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H3" t="s">
         <v>268</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K3" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B4" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D4" s="4">
         <v>45545</v>
@@ -25382,7 +25382,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="H4" t="s">
         <v>266</v>
@@ -25391,18 +25391,18 @@
         <v>45563</v>
       </c>
       <c r="J4" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K4" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B5" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D5" s="4">
         <v>45546</v>
@@ -25411,7 +25411,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="H5" t="s">
         <v>266</v>
@@ -25420,18 +25420,18 @@
         <v>45562</v>
       </c>
       <c r="J5" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K5" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B6" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D6" s="4">
         <v>45547</v>
@@ -25440,25 +25440,25 @@
         <v>607</v>
       </c>
       <c r="F6" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H6" t="s">
         <v>268</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="K6" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B7" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="D7" s="4">
         <v>45548</v>
@@ -25467,7 +25467,7 @@
         <v>607</v>
       </c>
       <c r="F7" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H7" t="s">
         <v>266</v>
@@ -25479,15 +25479,15 @@
         <v>1105</v>
       </c>
       <c r="K7" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B8" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D8" s="4">
         <v>45549</v>
@@ -25508,21 +25508,21 @@
         <v>45559</v>
       </c>
       <c r="J8" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K8" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D9" s="4">
         <v>45550</v>
@@ -25541,18 +25541,18 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K9" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B10" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D10" s="4">
         <v>45551</v>
@@ -25561,7 +25561,7 @@
         <v>607</v>
       </c>
       <c r="F10" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H10" t="s">
         <v>266</v>
@@ -25570,10 +25570,10 @@
         <v>45557</v>
       </c>
       <c r="J10" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K10" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PSP-9565: Automation test set update IS94 and Changes on Github action (#4509)
* data changes

* Testing browsers

* changing .net 6.0 to .net 8.0

* Deleting EdgeDriver nuget package

* Changes on webdriver config

* Update integration-test.yml

* Changes on automation test set - IS94
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD87F51-8E89-4A39-8148-FBD252E0E20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F7A2E-F3A4-4999-A5FD-6FFDC0568C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="27" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -5908,9 +5908,6 @@
     <t>0948523 B.C.LTD.</t>
   </si>
   <si>
-    <t>Automated Acquisition File - Takes Logic IS89</t>
-  </si>
-  <si>
     <t>UNIT 19 -- 171 17 St SE, Salmon Arm, BC</t>
   </si>
   <si>
@@ -6527,6 +6524,9 @@
   </si>
   <si>
     <t>Automated Test - Minimum Insurance test</t>
+  </si>
+  <si>
+    <t>Automated Acquisition File - Takes Logic IS94</t>
   </si>
 </sst>
 </file>
@@ -7605,7 +7605,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7635,7 +7635,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B2" t="s">
         <v>607</v>
@@ -7652,7 +7652,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -7681,12 +7681,12 @@
         <v>614</v>
       </c>
       <c r="E4" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -7698,7 +7698,7 @@
         <v>617</v>
       </c>
       <c r="E5" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -7737,7 +7737,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B8" t="s">
         <v>607</v>
@@ -7749,12 +7749,12 @@
         <v>609</v>
       </c>
       <c r="E8" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -7771,7 +7771,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -7788,7 +7788,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B12" t="s">
         <v>607</v>
@@ -7822,7 +7822,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B13" t="s">
         <v>607</v>
@@ -8201,7 +8201,7 @@
         <v>2500</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="K2" s="17">
         <f>I2*0.05</f>
@@ -8218,7 +8218,7 @@
         <v>1500.5</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P2" s="16"/>
       <c r="Q2" s="17">
@@ -8232,7 +8232,7 @@
         <v>200.79</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="U2" s="6">
         <v>10.029999999999999</v>
@@ -8270,7 +8270,7 @@
         <v>3500</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="K3" s="17"/>
       <c r="L3" s="17">
@@ -8284,7 +8284,7 @@
         <v>1500.99</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="17">
@@ -8293,7 +8293,7 @@
       </c>
       <c r="S3" s="6"/>
       <c r="T3" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -8327,7 +8327,7 @@
         <v>3000</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="17">
@@ -8336,13 +8336,13 @@
       </c>
       <c r="N4" s="6"/>
       <c r="O4" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="17"/>
       <c r="S4" s="6"/>
       <c r="T4" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -8376,7 +8376,7 @@
         <v>120000</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" ref="K5" si="2">I5*0.05</f>
@@ -8388,13 +8388,13 @@
       </c>
       <c r="N5" s="6"/>
       <c r="O5" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="17"/>
       <c r="S5" s="6"/>
       <c r="T5" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -8428,7 +8428,7 @@
         <v>3000</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17">
@@ -8442,7 +8442,7 @@
         <v>150.78</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="P6" s="16">
         <v>8</v>
@@ -8458,7 +8458,7 @@
         <v>1000</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="U6" s="6">
         <v>20</v>
@@ -9413,7 +9413,7 @@
   <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AL34" sqref="AL34"/>
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9555,13 +9555,13 @@
         <v>901</v>
       </c>
       <c r="AG1" s="3" t="s">
+        <v>1961</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>1962</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>1963</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>1964</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>1155</v>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10954,7 +10954,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -11340,7 +11340,7 @@
         <v>246</v>
       </c>
       <c r="L20" t="s">
-        <v>1942</v>
+        <v>2148</v>
       </c>
       <c r="O20" t="s">
         <v>702</v>
@@ -13737,7 +13737,7 @@
         <v>45241</v>
       </c>
       <c r="K2" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="L2" t="s">
         <v>1692</v>
@@ -13872,7 +13872,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B5" s="11">
         <v>56700.89</v>
@@ -13887,28 +13887,28 @@
         <v>496</v>
       </c>
       <c r="F5" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="G5" s="4">
         <v>45569</v>
       </c>
       <c r="K5" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="L5" t="s">
         <v>1692</v>
       </c>
       <c r="M5" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="N5" t="s">
         <v>959</v>
       </c>
       <c r="O5" t="s">
+        <v>1978</v>
+      </c>
+      <c r="P5" t="s">
         <v>1979</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1980</v>
       </c>
       <c r="Q5" t="s">
         <v>812</v>
@@ -13920,7 +13920,7 @@
         <v>1508</v>
       </c>
       <c r="T5" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="U5">
         <v>6</v>
@@ -13931,7 +13931,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -14097,10 +14097,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B7" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="C7">
         <v>5000</v>
@@ -14118,10 +14118,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B8" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="C8">
         <v>1200.8900000000001</v>
@@ -14136,10 +14136,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B9" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="C9">
         <v>50500</v>
@@ -14157,7 +14157,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B10" t="s">
         <v>1078</v>
@@ -14184,7 +14184,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45614</v>
+        <v>45623</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -16088,7 +16088,7 @@
         <v>1547</v>
       </c>
       <c r="B3" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -16124,7 +16124,7 @@
         <v>1547</v>
       </c>
       <c r="B6" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C6" t="s">
         <v>607</v>
@@ -16512,7 +16512,7 @@
         <v>706</v>
       </c>
       <c r="C18" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
@@ -16644,7 +16644,7 @@
         <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -16666,7 +16666,7 @@
         <v>1742</v>
       </c>
       <c r="D7" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -16724,7 +16724,7 @@
         <v>1770</v>
       </c>
       <c r="E12" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="F12" t="s">
         <v>1768</v>
@@ -20953,7 +20953,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21126,9 +21126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21178,7 +21178,7 @@
         <v>510</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>452</v>
@@ -21292,10 +21292,10 @@
         <v>440</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>2089</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>2090</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>2091</v>
       </c>
       <c r="AR1" s="3" t="s">
         <v>441</v>
@@ -21382,7 +21382,7 @@
         <v>502</v>
       </c>
       <c r="T4" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.35">
@@ -21427,7 +21427,7 @@
         <v>500</v>
       </c>
       <c r="AV7" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.35">
@@ -21442,7 +21442,7 @@
         <v>501</v>
       </c>
       <c r="AV8" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.35">
@@ -21457,7 +21457,7 @@
         <v>495</v>
       </c>
       <c r="AV9" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.35">
@@ -21472,18 +21472,18 @@
         <v>496</v>
       </c>
       <c r="AE10" t="s">
+        <v>2065</v>
+      </c>
+      <c r="AG10" t="s">
         <v>2066</v>
       </c>
-      <c r="AG10" t="s">
-        <v>2067</v>
-      </c>
       <c r="AX10" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="11" spans="1:53" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>462</v>
@@ -21497,7 +21497,7 @@
       <c r="O11" s="36"/>
       <c r="Q11" s="36"/>
       <c r="AV11" s="23" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="AW11" s="36"/>
     </row>
@@ -21585,7 +21585,7 @@
         <v>496</v>
       </c>
       <c r="AV16" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.35">
@@ -21603,13 +21603,13 @@
         <v>45245</v>
       </c>
       <c r="W17" t="s">
+        <v>2071</v>
+      </c>
+      <c r="AA17" t="s">
         <v>2072</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AV17" t="s">
         <v>2073</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>2074</v>
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.35">
@@ -21627,19 +21627,19 @@
         <v>36509</v>
       </c>
       <c r="P18" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="Q18" s="13">
         <v>36778</v>
       </c>
       <c r="R18" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="W18" s="9" t="s">
         <v>508</v>
       </c>
       <c r="X18" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="AA18" t="s">
         <v>509</v>
@@ -21648,7 +21648,7 @@
       <c r="AP18" s="4"/>
       <c r="AQ18" s="4"/>
       <c r="AS18" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.35">
@@ -21666,13 +21666,13 @@
         <v>47045</v>
       </c>
       <c r="N19" t="s">
+        <v>2078</v>
+      </c>
+      <c r="AF19" t="s">
         <v>2079</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AU19" t="s">
         <v>2080</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>2081</v>
       </c>
       <c r="AW19" s="13">
         <v>42988</v>
@@ -21684,18 +21684,18 @@
         <v>Research File - Lease / License agreement</v>
       </c>
       <c r="B20" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="C20" t="s">
         <v>501</v>
       </c>
       <c r="AV20" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="21" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>474</v>
@@ -21709,7 +21709,7 @@
       <c r="O21" s="36"/>
       <c r="Q21" s="36"/>
       <c r="AV21" s="23" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="AW21" s="36"/>
     </row>
@@ -21763,16 +21763,16 @@
         <v>Acquisition File - Agricultural Land Commission (ALC)</v>
       </c>
       <c r="B24" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C24" t="s">
         <v>496</v>
       </c>
       <c r="D24" t="s">
+        <v>2084</v>
+      </c>
+      <c r="AV24" t="s">
         <v>2085</v>
-      </c>
-      <c r="AV24" t="s">
-        <v>2086</v>
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.35">
@@ -21781,13 +21781,13 @@
         <v>Acquisition File - Form 5 - Approval of expropriation</v>
       </c>
       <c r="B25" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C25" t="s">
         <v>497</v>
       </c>
       <c r="AV25" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.35">
@@ -21802,7 +21802,7 @@
         <v>498</v>
       </c>
       <c r="AV26" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.35">
@@ -21811,13 +21811,13 @@
         <v>Acquisition File - Compensation requisition (H-120)</v>
       </c>
       <c r="B27" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="C27" t="s">
         <v>499</v>
       </c>
       <c r="AV27" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.35">
@@ -21826,19 +21826,19 @@
         <v>Acquisition File - Land Act Tenure/Reserves</v>
       </c>
       <c r="B28" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C28" t="s">
         <v>500</v>
       </c>
       <c r="AP28" t="s">
+        <v>2091</v>
+      </c>
+      <c r="AQ28" t="s">
         <v>2092</v>
       </c>
-      <c r="AQ28" t="s">
+      <c r="AV28" t="s">
         <v>2093</v>
-      </c>
-      <c r="AV28" t="s">
-        <v>2094</v>
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.35">
@@ -21853,7 +21853,7 @@
         <v>501</v>
       </c>
       <c r="AV29" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.35">
@@ -21868,13 +21868,13 @@
         <v>495</v>
       </c>
       <c r="W30" t="s">
+        <v>2095</v>
+      </c>
+      <c r="AA30" t="s">
         <v>2096</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AI30" t="s">
         <v>2097</v>
-      </c>
-      <c r="AI30" t="s">
-        <v>2098</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.35">
@@ -21889,7 +21889,7 @@
         <v>496</v>
       </c>
       <c r="AV31" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.35">
@@ -21907,16 +21907,16 @@
         <v>36850</v>
       </c>
       <c r="Y32" t="s">
+        <v>2099</v>
+      </c>
+      <c r="Z32" t="s">
         <v>2100</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AN32" t="s">
         <v>2101</v>
       </c>
-      <c r="AN32" t="s">
+      <c r="AS32" t="s">
         <v>2102</v>
-      </c>
-      <c r="AS32" t="s">
-        <v>2103</v>
       </c>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.35">
@@ -21925,18 +21925,18 @@
         <v>Acquisition File - Form 7 - Notice of abandonement</v>
       </c>
       <c r="B33" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C33" t="s">
         <v>498</v>
       </c>
       <c r="AV33" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="34" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>761</v>
@@ -21950,7 +21950,7 @@
       <c r="O34" s="36"/>
       <c r="Q34" s="36"/>
       <c r="AV34" s="23" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="AW34" s="36"/>
     </row>
@@ -21990,7 +21990,7 @@
         <v>777</v>
       </c>
       <c r="AN36" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="AV36" t="s">
         <v>778</v>
@@ -22002,7 +22002,7 @@
         <v>Project -Financial records (invoices, journal vouchers, received cheques etc.)</v>
       </c>
       <c r="B37" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C37" t="s">
         <v>495</v>
@@ -22026,19 +22026,19 @@
         <v>780</v>
       </c>
       <c r="W38" t="s">
+        <v>2106</v>
+      </c>
+      <c r="Z38" t="s">
         <v>2107</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="AA38" t="s">
         <v>2108</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>2109</v>
       </c>
       <c r="AO38" s="13">
         <v>43757</v>
       </c>
       <c r="AR38" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.35">
@@ -22056,10 +22056,10 @@
         <v>7190089</v>
       </c>
       <c r="AN39" t="s">
+        <v>2110</v>
+      </c>
+      <c r="AV39" t="s">
         <v>2111</v>
-      </c>
-      <c r="AV39" t="s">
-        <v>2112</v>
       </c>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.35">
@@ -22080,16 +22080,16 @@
         <v>781</v>
       </c>
       <c r="AI40" t="s">
+        <v>2112</v>
+      </c>
+      <c r="AJ40" t="s">
         <v>2113</v>
       </c>
-      <c r="AJ40" t="s">
+      <c r="AL40" t="s">
         <v>2114</v>
       </c>
-      <c r="AL40" t="s">
+      <c r="AM40" t="s">
         <v>2115</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>2116</v>
       </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.35">
@@ -22104,7 +22104,7 @@
         <v>499</v>
       </c>
       <c r="F41" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="H41" s="13">
         <v>32301</v>
@@ -22119,16 +22119,16 @@
         <v>784</v>
       </c>
       <c r="AE41" t="s">
+        <v>2117</v>
+      </c>
+      <c r="AN41" t="s">
         <v>2118</v>
-      </c>
-      <c r="AN41" t="s">
-        <v>2119</v>
       </c>
       <c r="AO41" s="4"/>
       <c r="AP41" s="4"/>
       <c r="AQ41" s="4"/>
       <c r="AV41" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.35">
@@ -22143,7 +22143,7 @@
         <v>500</v>
       </c>
       <c r="AV42" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.35">
@@ -22158,12 +22158,12 @@
         <v>501</v>
       </c>
       <c r="AV43" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="44" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>462</v>
@@ -22187,7 +22187,7 @@
         <v>Disposition File -Certificate of Compliance</v>
       </c>
       <c r="B45" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C45" t="s">
         <v>496</v>
@@ -22202,13 +22202,13 @@
         <v>Disposition File -Enhanced Referral Records</v>
       </c>
       <c r="B46" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="C46" t="s">
         <v>497</v>
       </c>
       <c r="AV46" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.35">
@@ -22217,13 +22217,13 @@
         <v>Disposition File -First Nations Strength of Claim Report</v>
       </c>
       <c r="B47" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C47" t="s">
         <v>498</v>
       </c>
       <c r="AV47" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.35">
@@ -22238,7 +22238,7 @@
         <v>499</v>
       </c>
       <c r="AG48" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.35">
@@ -22253,7 +22253,7 @@
         <v>500</v>
       </c>
       <c r="AV49" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.35">
@@ -22271,13 +22271,13 @@
         <v>89997</v>
       </c>
       <c r="AC50" t="s">
+        <v>2126</v>
+      </c>
+      <c r="AD50" t="s">
         <v>2127</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AS50" t="s">
         <v>2128</v>
-      </c>
-      <c r="AS50" t="s">
-        <v>2129</v>
       </c>
       <c r="AZ50">
         <v>1997</v>
@@ -22289,13 +22289,13 @@
         <v>Disposition File -Purchase and Sale Agreement</v>
       </c>
       <c r="B51" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C51" t="s">
         <v>495</v>
       </c>
       <c r="AV51" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="52" spans="1:53" x14ac:dyDescent="0.35">
@@ -22310,7 +22310,7 @@
         <v>496</v>
       </c>
       <c r="AV52" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.35">
@@ -22325,12 +22325,12 @@
         <v>497</v>
       </c>
       <c r="AV53" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="54" spans="1:53" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="23" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>764</v>
@@ -22346,14 +22346,14 @@
       <c r="O54" s="36"/>
       <c r="Q54" s="36"/>
       <c r="Z54" s="23" t="s">
+        <v>2132</v>
+      </c>
+      <c r="AS54" s="23" t="s">
         <v>2133</v>
-      </c>
-      <c r="AS54" s="23" t="s">
-        <v>2134</v>
       </c>
       <c r="AW54" s="36"/>
       <c r="AY54" s="23" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="55" spans="1:53" x14ac:dyDescent="0.35">
@@ -22362,13 +22362,13 @@
         <v>Property Management -Approval/sign-off</v>
       </c>
       <c r="B55" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="C55" t="s">
         <v>499</v>
       </c>
       <c r="AV55" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="56" spans="1:53" x14ac:dyDescent="0.35">
@@ -22377,13 +22377,13 @@
         <v>Property Management -Form 8 - Notice of advanced payment </v>
       </c>
       <c r="B56" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="C56" t="s">
         <v>500</v>
       </c>
       <c r="AV56" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.35">
@@ -22392,13 +22392,13 @@
         <v>Property Management -Form 1 - Notice of expropriation </v>
       </c>
       <c r="B57" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="C57" t="s">
         <v>501</v>
       </c>
       <c r="AV57" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.35">
@@ -22413,7 +22413,7 @@
         <v>495</v>
       </c>
       <c r="AV58" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="59" spans="1:53" x14ac:dyDescent="0.35">
@@ -22428,7 +22428,7 @@
         <v>496</v>
       </c>
       <c r="AV59" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="60" spans="1:53" x14ac:dyDescent="0.35">
@@ -22443,7 +22443,7 @@
         <v>497</v>
       </c>
       <c r="AV60" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.35">
@@ -22473,7 +22473,7 @@
         <v>499</v>
       </c>
       <c r="AV62" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="63" spans="1:53" x14ac:dyDescent="0.35">
@@ -22491,16 +22491,16 @@
         <v>32874</v>
       </c>
       <c r="Z63" t="s">
+        <v>2138</v>
+      </c>
+      <c r="AN63" t="s">
         <v>2139</v>
-      </c>
-      <c r="AN63" t="s">
-        <v>2140</v>
       </c>
       <c r="AS63" t="s">
         <v>1509</v>
       </c>
       <c r="AY63" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="64" spans="1:53" x14ac:dyDescent="0.35">
@@ -22509,18 +22509,18 @@
         <v>Property Management -Form 9 - Vesting notice (Form 9)</v>
       </c>
       <c r="B64" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C64" t="s">
         <v>501</v>
       </c>
       <c r="AV64" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="23" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="B65" s="23" t="s">
         <v>487</v>
@@ -22534,7 +22534,7 @@
       <c r="O65" s="36"/>
       <c r="Q65" s="36"/>
       <c r="AV65" s="23" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="AW65" s="36"/>
     </row>
@@ -23217,8 +23217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CY21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="CV6" sqref="CV6"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AZ8" sqref="AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23338,7 +23338,7 @@
         <v>515</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>516</v>
@@ -23452,10 +23452,10 @@
         <v>1887</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>1987</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>1988</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>1989</v>
       </c>
       <c r="AR1" s="3" t="s">
         <v>1773</v>
@@ -23467,7 +23467,7 @@
         <v>537</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>538</v>
@@ -23482,10 +23482,10 @@
         <v>1829</v>
       </c>
       <c r="AZ1" s="3" t="s">
+        <v>1949</v>
+      </c>
+      <c r="BA1" s="3" t="s">
         <v>1950</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>1951</v>
       </c>
       <c r="BB1" s="3" t="s">
         <v>541</v>
@@ -23629,13 +23629,13 @@
         <v>1910</v>
       </c>
       <c r="CW1" s="3" t="s">
+        <v>1964</v>
+      </c>
+      <c r="CX1" s="3" t="s">
         <v>1965</v>
       </c>
-      <c r="CX1" s="3" t="s">
+      <c r="CY1" s="3" t="s">
         <v>1966</v>
-      </c>
-      <c r="CY1" s="3" t="s">
-        <v>1967</v>
       </c>
     </row>
     <row r="2" spans="1:103" x14ac:dyDescent="0.35">
@@ -23649,7 +23649,7 @@
         <v>1081</v>
       </c>
       <c r="D2" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="E2" t="s">
         <v>501</v>
@@ -24359,7 +24359,7 @@
         <v>0</v>
       </c>
       <c r="AS6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AT6">
         <v>1</v>
@@ -24374,7 +24374,7 @@
         <v>0</v>
       </c>
       <c r="AX6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY6">
         <v>0</v>
@@ -24398,7 +24398,7 @@
         <v>44114</v>
       </c>
       <c r="BO6" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="CO6">
         <v>1</v>
@@ -24430,7 +24430,7 @@
     </row>
     <row r="7" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="E7" t="s">
         <v>496</v>
@@ -24451,13 +24451,13 @@
         <v>192</v>
       </c>
       <c r="P7" t="s">
+        <v>1952</v>
+      </c>
+      <c r="R7" t="s">
         <v>1953</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>1954</v>
-      </c>
-      <c r="T7" t="s">
-        <v>1955</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -24537,7 +24537,7 @@
     </row>
     <row r="8" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="E8" t="s">
         <v>496</v>
@@ -24671,7 +24671,7 @@
     </row>
     <row r="9" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B9" t="s">
         <v>1082</v>
@@ -24680,7 +24680,7 @@
         <v>1081</v>
       </c>
       <c r="D9" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="E9" t="s">
         <v>496</v>
@@ -24701,13 +24701,13 @@
         <v>191</v>
       </c>
       <c r="P9" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R9" t="s">
         <v>1969</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>1970</v>
-      </c>
-      <c r="T9" t="s">
-        <v>1971</v>
       </c>
       <c r="AI9" t="s">
         <v>299</v>
@@ -24799,7 +24799,7 @@
     </row>
     <row r="10" spans="1:103" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="E10" t="s">
         <v>496</v>
@@ -24820,13 +24820,13 @@
         <v>191</v>
       </c>
       <c r="P10" t="s">
+        <v>1968</v>
+      </c>
+      <c r="R10" t="s">
         <v>1969</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>1970</v>
-      </c>
-      <c r="T10" t="s">
-        <v>1971</v>
       </c>
       <c r="AM10">
         <v>22</v>
@@ -25068,7 +25068,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25209,7 +25209,7 @@
         <v>1601</v>
       </c>
       <c r="K5" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -25220,7 +25220,7 @@
         <v>1883</v>
       </c>
       <c r="K6" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -25282,39 +25282,39 @@
         <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1990</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2010</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1991</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1992</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1993</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1994</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1995</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1996</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1997</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>1998</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B2" t="s">
         <v>532</v>
@@ -25326,7 +25326,7 @@
         <v>607</v>
       </c>
       <c r="F2" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H2" t="s">
         <v>266</v>
@@ -25338,15 +25338,15 @@
         <v>1105</v>
       </c>
       <c r="K2" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B3" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D3" s="4">
         <v>45544</v>
@@ -25355,25 +25355,25 @@
         <v>607</v>
       </c>
       <c r="F3" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H3" t="s">
         <v>268</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K3" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B4" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D4" s="4">
         <v>45545</v>
@@ -25382,7 +25382,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="H4" t="s">
         <v>266</v>
@@ -25391,18 +25391,18 @@
         <v>45563</v>
       </c>
       <c r="J4" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K4" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B5" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D5" s="4">
         <v>45546</v>
@@ -25411,7 +25411,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="H5" t="s">
         <v>266</v>
@@ -25420,18 +25420,18 @@
         <v>45562</v>
       </c>
       <c r="J5" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K5" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B6" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D6" s="4">
         <v>45547</v>
@@ -25440,25 +25440,25 @@
         <v>607</v>
       </c>
       <c r="F6" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H6" t="s">
         <v>268</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="K6" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B7" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="D7" s="4">
         <v>45548</v>
@@ -25467,7 +25467,7 @@
         <v>607</v>
       </c>
       <c r="F7" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H7" t="s">
         <v>266</v>
@@ -25479,15 +25479,15 @@
         <v>1105</v>
       </c>
       <c r="K7" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B8" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D8" s="4">
         <v>45549</v>
@@ -25508,21 +25508,21 @@
         <v>45559</v>
       </c>
       <c r="J8" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="K8" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D9" s="4">
         <v>45550</v>
@@ -25541,18 +25541,18 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="K9" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B10" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D10" s="4">
         <v>45551</v>
@@ -25561,7 +25561,7 @@
         <v>607</v>
       </c>
       <c r="F10" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H10" t="s">
         <v>266</v>
@@ -25570,10 +25570,10 @@
         <v>45557</v>
       </c>
       <c r="J10" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K10" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to adapt GHA
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F7A2E-F3A4-4999-A5FD-6FFDC0568C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFE89D7-3ACE-4A6B-811A-B2A53FD7754D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="27" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="2149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3717" uniqueCount="2149">
   <si>
     <t>FirstName</t>
   </si>
@@ -9412,8 +9412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10954,7 +10954,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -20201,7 +20201,7 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20933,6 +20933,9 @@
       <c r="E9" t="s">
         <v>153</v>
       </c>
+      <c r="G9" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -21126,7 +21129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
     </sheetView>

</xml_diff>

<commit_message>
PSP-9565: Changes on automation test set to accomodate GHA (#4516)
* data changes

* Testing browsers

* changing .net 6.0 to .net 8.0

* Deleting EdgeDriver nuget package

* Changes on webdriver config

* Update integration-test.yml

* Changes on automation test set - IS94

* Changes to adapt GHA

* Changing checklist button to explicit path

* Correcting a research file element
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F7A2E-F3A4-4999-A5FD-6FFDC0568C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFE89D7-3ACE-4A6B-811A-B2A53FD7754D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="27" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="2149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3717" uniqueCount="2149">
   <si>
     <t>FirstName</t>
   </si>
@@ -9412,8 +9412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ABE440-1217-4524-8B92-D6A2E8FC0332}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10954,7 +10954,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45623</v>
+        <v>45628</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -20201,7 +20201,7 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20933,6 +20933,9 @@
       <c r="E9" t="s">
         <v>153</v>
       </c>
+      <c r="G9" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -21126,7 +21129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665AEC9-C942-4A65-984C-CAD52F4E2CCE}">
   <dimension ref="A1:BA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
     </sheetView>

</xml_diff>

<commit_message>
Changes on Automation branch IS95
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFE89D7-3ACE-4A6B-811A-B2A53FD7754D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F91E57-F52E-4B12-A233-D0859774085D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6526,7 +6526,7 @@
     <t>Automated Test - Minimum Insurance test</t>
   </si>
   <si>
-    <t>Automated Acquisition File - Takes Logic IS94</t>
+    <t>Automated Acquisition File - Takes Logic IS95</t>
   </si>
 </sst>
 </file>
@@ -9413,7 +9413,7 @@
   <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="I3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="J3" s="4">
         <v>45318</v>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="I5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="J5" s="4">
         <v>45318</v>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="I7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="J7" s="4">
         <v>45318</v>
@@ -10641,7 +10641,7 @@
       </c>
       <c r="I12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="J12" s="4">
         <v>45318</v>
@@ -10954,7 +10954,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="J15" s="4">
         <v>45318</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">

</xml_diff>

<commit_message>
PSP-9937: IS98 Updating automation test cases (#4630)
* Changes on automation branch

* Changes on existing automated test based on last changes from IS98

* Update Acquisition Details file

---------

Co-authored-by: Alejandro Sanchez <emailforasr@gmail.com>
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6287798-B498-41FB-8ED9-09F94D863CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4687E609-D0AB-405D-AE75-7A72DE73EB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="950" firstSheet="15" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="950" firstSheet="11" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3824" uniqueCount="2210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3832" uniqueCount="2219">
   <si>
     <t>FirstName</t>
   </si>
@@ -6181,9 +6181,6 @@
     <t>THAT PART OF LOT 2 DISTRICT LOT 71 CARIBOO DISTRICT PLAN BCP49571 EXCEPT PLAN BCP49574 SHOWN ON PLAN BCP49575</t>
   </si>
   <si>
-    <t>012-041-530</t>
-  </si>
-  <si>
     <t>Lease / License agreement</t>
   </si>
   <si>
@@ -6643,9 +6640,6 @@
     <t>Compensation 2 for Acquisition Subfile</t>
   </si>
   <si>
-    <t>Devin Smith (MoTI Solicitor),Juan Manrique (Owner),Praveen Kumar (Owner's Solicitor)</t>
-  </si>
-  <si>
     <t>AcquisitionCompensationSubfilesMainFileTotal</t>
   </si>
   <si>
@@ -6710,6 +6704,39 @@
   </si>
   <si>
     <t>Ali Thomson,Ellicott Joe</t>
+  </si>
+  <si>
+    <t>Devin Smith,Juan Manrique,Bobbi Bjornholt</t>
+  </si>
+  <si>
+    <t>Devin Smith (MoTI Solicitor),Juan Manrique (Owner),Bobbi Bjornholt (Owner's Solicitor)</t>
+  </si>
+  <si>
+    <t>Devin Smith (MoTI Solicitor),TRANS MOUNTAIN PIPELINE INC. (Agriculture Credit Act)</t>
+  </si>
+  <si>
+    <t>Devin Smith,TRANS MOUNTAIN PIPELINE INC.</t>
+  </si>
+  <si>
+    <t>BELL MOBILITY INC.</t>
+  </si>
+  <si>
+    <t>BELL MOBILITY INC., Inc. No. (Owner's Representative)</t>
+  </si>
+  <si>
+    <t>ProjectTeamMembers</t>
+  </si>
+  <si>
+    <t>Allison Kay Cameron,Robert Arthur Meredith,Carmen Jacobson,Catharina Theodora Cornelia Maria Goossen-Jacobs</t>
+  </si>
+  <si>
+    <t>Doris Evelyn Jacobson</t>
+  </si>
+  <si>
+    <t>Allison E Morton,Elizabeth Allison Jopp,Jean Allison Krebs</t>
+  </si>
+  <si>
+    <t>011-333-855</t>
   </si>
 </sst>
 </file>
@@ -6800,7 +6827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6853,6 +6880,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7135,10 +7172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12A4D20-CBEC-42E3-9A24-C9C857FE01F3}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7153,11 +7190,12 @@
     <col min="8" max="10" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" style="5" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>160</v>
       </c>
@@ -7200,8 +7238,11 @@
       <c r="N1" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -7239,8 +7280,11 @@
       <c r="N2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -7279,7 +7323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -7318,7 +7362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>171</v>
       </c>
@@ -7362,8 +7406,11 @@
       <c r="N5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>350</v>
       </c>
@@ -7398,8 +7445,11 @@
       <c r="N6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1226</v>
       </c>
@@ -7435,7 +7485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1227</v>
       </c>
@@ -7794,12 +7844,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
@@ -7817,7 +7867,7 @@
         <v>167</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>604</v>
@@ -7828,16 +7878,16 @@
         <v>1942</v>
       </c>
       <c r="B2" t="s">
-        <v>605</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>807</v>
+        <v>2212</v>
       </c>
       <c r="D2" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="E2" t="s">
-        <v>418</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7845,13 +7895,13 @@
         <v>1942</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>605</v>
       </c>
       <c r="C3" t="s">
-        <v>609</v>
+        <v>807</v>
       </c>
       <c r="D3" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E3" t="s">
         <v>418</v>
@@ -7865,13 +7915,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E4" t="s">
-        <v>1940</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -7882,10 +7932,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D5" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E5" t="s">
         <v>1940</v>
@@ -9371,14 +9421,14 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.85546875" bestFit="1" customWidth="1"/>
@@ -9603,10 +9653,10 @@
   <dimension ref="A1:AV46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="27" topLeftCell="AO28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="27" topLeftCell="Y28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="AR24" sqref="AR24"/>
+      <selection pane="bottomRight" activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9686,31 +9736,31 @@
         <v>724</v>
       </c>
       <c r="I1" s="38" t="s">
+        <v>2146</v>
+      </c>
+      <c r="J1" s="38" t="s">
         <v>2147</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="K1" s="38" t="s">
         <v>2148</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="L1" s="38" t="s">
         <v>2149</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="M1" s="38" t="s">
         <v>2150</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="N1" s="38" t="s">
         <v>2151</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="O1" s="38" t="s">
         <v>2152</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="P1" s="38" t="s">
         <v>2153</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="Q1" s="38" t="s">
         <v>2154</v>
-      </c>
-      <c r="Q1" s="38" t="s">
-        <v>2155</v>
       </c>
       <c r="R1" s="38" t="s">
         <v>684</v>
@@ -9725,10 +9775,10 @@
         <v>687</v>
       </c>
       <c r="V1" s="38" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="W1" s="38" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="X1" s="38" t="s">
         <v>786</v>
@@ -9791,13 +9841,13 @@
         <v>1957</v>
       </c>
       <c r="AR1" s="38" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="AS1" s="38" t="s">
-        <v>2188</v>
+        <v>2186</v>
       </c>
       <c r="AT1" s="38" t="s">
-        <v>2189</v>
+        <v>2187</v>
       </c>
       <c r="AU1" s="38" t="s">
         <v>1150</v>
@@ -9829,19 +9879,19 @@
         <v>696</v>
       </c>
       <c r="I2" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="J2" t="s">
         <v>575</v>
       </c>
       <c r="K2" t="s">
+        <v>2156</v>
+      </c>
+      <c r="L2" t="s">
         <v>2157</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>2158</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2159</v>
       </c>
       <c r="N2" s="4">
         <v>45170</v>
@@ -9960,23 +10010,23 @@
         <v>959</v>
       </c>
       <c r="I3" t="s">
+        <v>2159</v>
+      </c>
+      <c r="J3" t="s">
         <v>2160</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>2161</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>2162</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>2163</v>
-      </c>
-      <c r="M3" t="s">
-        <v>2164</v>
       </c>
       <c r="N3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45681</v>
+        <v>45688</v>
       </c>
       <c r="O3" s="4">
         <v>45318</v>
@@ -10199,7 +10249,7 @@
       </c>
       <c r="N5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45681</v>
+        <v>45688</v>
       </c>
       <c r="O5" s="4">
         <v>45318</v>
@@ -10412,7 +10462,7 @@
       </c>
       <c r="N7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45681</v>
+        <v>45688</v>
       </c>
       <c r="O7" s="4">
         <v>45318</v>
@@ -10955,7 +11005,7 @@
       </c>
       <c r="N12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45681</v>
+        <v>45688</v>
       </c>
       <c r="O12" s="4">
         <v>45318</v>
@@ -11280,7 +11330,7 @@
       </c>
       <c r="N15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45681</v>
+        <v>45688</v>
       </c>
       <c r="O15" s="4">
         <v>45318</v>
@@ -11682,7 +11732,7 @@
         <v>246</v>
       </c>
       <c r="R20" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="U20" t="s">
         <v>698</v>
@@ -11903,7 +11953,7 @@
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="B23" t="s">
         <v>246</v>
@@ -11927,7 +11977,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="U23" t="s">
         <v>744</v>
@@ -11999,7 +12049,7 @@
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="C24">
         <v>5512570</v>
@@ -12017,19 +12067,19 @@
         <v>1338</v>
       </c>
       <c r="I24" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="J24" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="K24" t="s">
         <v>575</v>
       </c>
       <c r="L24" t="s">
+        <v>2175</v>
+      </c>
+      <c r="M24" t="s">
         <v>2176</v>
-      </c>
-      <c r="M24" t="s">
-        <v>2177</v>
       </c>
       <c r="N24" s="4">
         <v>45036</v>
@@ -12044,10 +12094,10 @@
         <v>45829</v>
       </c>
       <c r="R24" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="S24" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="T24" t="s">
         <v>743</v>
@@ -12056,7 +12106,7 @@
         <v>744</v>
       </c>
       <c r="V24" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="X24" t="s">
         <v>191</v>
@@ -12077,13 +12127,13 @@
         <v>706</v>
       </c>
       <c r="AD24" t="s">
+        <v>2167</v>
+      </c>
+      <c r="AE24" t="s">
         <v>2168</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AF24" t="s">
         <v>2169</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>2170</v>
       </c>
       <c r="AG24">
         <v>16</v>
@@ -12134,7 +12184,7 @@
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="C25">
         <v>5512570</v>
@@ -12149,22 +12199,22 @@
         <v>924</v>
       </c>
       <c r="G25" t="s">
+        <v>2178</v>
+      </c>
+      <c r="I25" t="s">
         <v>2179</v>
-      </c>
-      <c r="I25" t="s">
-        <v>2180</v>
       </c>
       <c r="J25" t="s">
         <v>575</v>
       </c>
       <c r="K25" t="s">
+        <v>2161</v>
+      </c>
+      <c r="L25" t="s">
         <v>2162</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>2163</v>
-      </c>
-      <c r="M25" t="s">
-        <v>2164</v>
       </c>
       <c r="N25" s="4">
         <v>45432</v>
@@ -12179,13 +12229,13 @@
         <v>45737</v>
       </c>
       <c r="R25" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="V25" t="s">
         <v>7</v>
       </c>
       <c r="W25" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="X25" t="s">
         <v>192</v>
@@ -13980,7 +14030,7 @@
         <v>898</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>899</v>
@@ -14304,8 +14354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CC3795-F36B-4D0F-8244-A4F4C3935686}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14325,8 +14375,8 @@
     <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="80.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.7109375" customWidth="1"/>
+    <col min="16" max="16" width="122.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="83.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="42.5703125" bestFit="1" customWidth="1"/>
@@ -14449,10 +14499,10 @@
         <v>955</v>
       </c>
       <c r="P2" t="s">
-        <v>2187</v>
+        <v>2209</v>
       </c>
       <c r="Q2" t="s">
-        <v>250</v>
+        <v>2208</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -14489,6 +14539,12 @@
       <c r="K3" t="s">
         <v>1071</v>
       </c>
+      <c r="P3" t="s">
+        <v>2210</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2211</v>
+      </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
@@ -14567,97 +14623,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>1965</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="39">
         <v>56700.89</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="39">
         <v>2775</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="39">
         <v>59475.89</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="23" t="s">
         <v>496</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="23" t="s">
         <v>1980</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="27">
         <v>45569</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="23" t="s">
         <v>1970</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="23" t="s">
         <v>1686</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="23" t="s">
         <v>2031</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="23" t="s">
         <v>954</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="23" t="s">
         <v>1972</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="23" t="s">
         <v>1973</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="23" t="s">
         <v>807</v>
       </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="R5" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="23" t="s">
         <v>1502</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="23" t="s">
         <v>1974</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="23">
         <v>6</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="23">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>1977</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="23" t="s">
         <v>499</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="41">
         <v>45178</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" t="s">
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="23" t="s">
         <v>1071</v>
       </c>
-      <c r="R6" t="b">
+      <c r="P6" s="23" t="s">
+        <v>2213</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>2212</v>
+      </c>
+      <c r="R6" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="23">
         <v>9</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2205</v>
+        <v>2203</v>
       </c>
       <c r="B7" s="37">
         <v>56789.98</v>
@@ -14702,10 +14764,10 @@
         <v>955</v>
       </c>
       <c r="P7" t="s">
-        <v>2208</v>
+        <v>2206</v>
       </c>
       <c r="Q7" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="R7" t="b">
         <v>1</v>
@@ -14725,7 +14787,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="B8" s="37">
         <v>10000</v>
@@ -14744,7 +14806,7 @@
         <v>44845</v>
       </c>
       <c r="K8" t="s">
-        <v>2190</v>
+        <v>2188</v>
       </c>
       <c r="L8" t="s">
         <v>1687</v>
@@ -14753,25 +14815,25 @@
         <v>2031</v>
       </c>
       <c r="N8" t="s">
+        <v>2191</v>
+      </c>
+      <c r="O8" t="s">
+        <v>2192</v>
+      </c>
+      <c r="P8" t="s">
+        <v>2194</v>
+      </c>
+      <c r="Q8" t="s">
         <v>2193</v>
-      </c>
-      <c r="O8" t="s">
-        <v>2194</v>
-      </c>
-      <c r="P8" t="s">
-        <v>2196</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>2195</v>
       </c>
       <c r="R8" t="b">
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>2197</v>
+        <v>2195</v>
       </c>
       <c r="T8" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
       <c r="U8">
         <v>11</v>
@@ -14782,7 +14844,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="B9" s="37">
         <v>2000</v>
@@ -14798,22 +14860,22 @@
         <v>45650</v>
       </c>
       <c r="K9" t="s">
-        <v>2191</v>
+        <v>2189</v>
       </c>
       <c r="L9" t="s">
         <v>1687</v>
       </c>
       <c r="M9" t="s">
+        <v>2199</v>
+      </c>
+      <c r="N9" t="s">
+        <v>2200</v>
+      </c>
+      <c r="O9" t="s">
         <v>2201</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>2202</v>
-      </c>
-      <c r="O9" t="s">
-        <v>2203</v>
-      </c>
-      <c r="P9" t="s">
-        <v>2204</v>
       </c>
       <c r="Q9" t="s">
         <v>903</v>
@@ -14822,10 +14884,10 @@
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="T9" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="U9">
         <v>12</v>
@@ -15051,7 +15113,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
       <c r="B11" t="s">
         <v>952</v>
@@ -15071,7 +15133,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
       <c r="B12" t="s">
         <v>950</v>
@@ -15091,7 +15153,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2192</v>
+        <v>2190</v>
       </c>
       <c r="B13" t="s">
         <v>951</v>
@@ -15858,7 +15920,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45681</v>
+        <v>45688</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -17166,7 +17228,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17477,8 +17539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17577,7 +17639,7 @@
         <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>2033</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -21205,7 +21267,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -22114,7 +22176,7 @@
         <v>510</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>452</v>
@@ -22228,10 +22290,10 @@
         <v>440</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>2081</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>2082</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>2083</v>
       </c>
       <c r="AR1" s="3" t="s">
         <v>441</v>
@@ -22318,7 +22380,7 @@
         <v>502</v>
       </c>
       <c r="T4" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
@@ -22363,7 +22425,7 @@
         <v>500</v>
       </c>
       <c r="AV7" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
@@ -22378,7 +22440,7 @@
         <v>501</v>
       </c>
       <c r="AV8" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
@@ -22393,7 +22455,7 @@
         <v>495</v>
       </c>
       <c r="AV9" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
@@ -22408,18 +22470,18 @@
         <v>496</v>
       </c>
       <c r="AE10" t="s">
+        <v>2057</v>
+      </c>
+      <c r="AG10" t="s">
         <v>2058</v>
       </c>
-      <c r="AG10" t="s">
-        <v>2059</v>
-      </c>
       <c r="AX10" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="11" spans="1:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>462</v>
@@ -22433,7 +22495,7 @@
       <c r="O11" s="36"/>
       <c r="Q11" s="36"/>
       <c r="AV11" s="23" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="AW11" s="36"/>
     </row>
@@ -22521,7 +22583,7 @@
         <v>496</v>
       </c>
       <c r="AV16" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
@@ -22539,13 +22601,13 @@
         <v>45245</v>
       </c>
       <c r="W17" t="s">
+        <v>2063</v>
+      </c>
+      <c r="AA17" t="s">
         <v>2064</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AV17" t="s">
         <v>2065</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>2066</v>
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
@@ -22563,19 +22625,19 @@
         <v>36509</v>
       </c>
       <c r="P18" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="Q18" s="13">
         <v>36778</v>
       </c>
       <c r="R18" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="W18" s="9" t="s">
         <v>508</v>
       </c>
       <c r="X18" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="AA18" t="s">
         <v>509</v>
@@ -22584,7 +22646,7 @@
       <c r="AP18" s="4"/>
       <c r="AQ18" s="4"/>
       <c r="AS18" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
@@ -22602,13 +22664,13 @@
         <v>47045</v>
       </c>
       <c r="N19" t="s">
+        <v>2070</v>
+      </c>
+      <c r="AF19" t="s">
         <v>2071</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AU19" t="s">
         <v>2072</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>2073</v>
       </c>
       <c r="AW19" s="13">
         <v>42988</v>
@@ -22620,18 +22682,18 @@
         <v>Research File - Lease / License agreement</v>
       </c>
       <c r="B20" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C20" t="s">
         <v>501</v>
       </c>
       <c r="AV20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="21" spans="1:52" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>474</v>
@@ -22645,7 +22707,7 @@
       <c r="O21" s="36"/>
       <c r="Q21" s="36"/>
       <c r="AV21" s="23" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="AW21" s="36"/>
     </row>
@@ -22699,16 +22761,16 @@
         <v>Acquisition File - Agricultural Land Commission (ALC)</v>
       </c>
       <c r="B24" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C24" t="s">
         <v>496</v>
       </c>
       <c r="D24" t="s">
+        <v>2076</v>
+      </c>
+      <c r="AV24" t="s">
         <v>2077</v>
-      </c>
-      <c r="AV24" t="s">
-        <v>2078</v>
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
@@ -22717,13 +22779,13 @@
         <v>Acquisition File - Form 5 - Approval of expropriation</v>
       </c>
       <c r="B25" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C25" t="s">
         <v>497</v>
       </c>
       <c r="AV25" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
@@ -22738,7 +22800,7 @@
         <v>498</v>
       </c>
       <c r="AV26" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
@@ -22747,13 +22809,13 @@
         <v>Acquisition File - Compensation requisition (H-120)</v>
       </c>
       <c r="B27" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C27" t="s">
         <v>499</v>
       </c>
       <c r="AV27" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
@@ -22762,19 +22824,19 @@
         <v>Acquisition File - Land Act Tenure/Reserves</v>
       </c>
       <c r="B28" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C28" t="s">
         <v>500</v>
       </c>
       <c r="AP28" t="s">
+        <v>2083</v>
+      </c>
+      <c r="AQ28" t="s">
         <v>2084</v>
       </c>
-      <c r="AQ28" t="s">
+      <c r="AV28" t="s">
         <v>2085</v>
-      </c>
-      <c r="AV28" t="s">
-        <v>2086</v>
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
@@ -22789,7 +22851,7 @@
         <v>501</v>
       </c>
       <c r="AV29" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
@@ -22804,13 +22866,13 @@
         <v>495</v>
       </c>
       <c r="W30" t="s">
+        <v>2087</v>
+      </c>
+      <c r="AA30" t="s">
         <v>2088</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AI30" t="s">
         <v>2089</v>
-      </c>
-      <c r="AI30" t="s">
-        <v>2090</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
@@ -22825,7 +22887,7 @@
         <v>496</v>
       </c>
       <c r="AV31" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
@@ -22843,16 +22905,16 @@
         <v>36850</v>
       </c>
       <c r="Y32" t="s">
+        <v>2091</v>
+      </c>
+      <c r="Z32" t="s">
         <v>2092</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AN32" t="s">
         <v>2093</v>
       </c>
-      <c r="AN32" t="s">
+      <c r="AS32" t="s">
         <v>2094</v>
-      </c>
-      <c r="AS32" t="s">
-        <v>2095</v>
       </c>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.25">
@@ -22861,18 +22923,18 @@
         <v>Acquisition File - Form 7 - Notice of abandonement</v>
       </c>
       <c r="B33" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C33" t="s">
         <v>498</v>
       </c>
       <c r="AV33" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="34" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>757</v>
@@ -22886,7 +22948,7 @@
       <c r="O34" s="36"/>
       <c r="Q34" s="36"/>
       <c r="AV34" s="23" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="AW34" s="36"/>
     </row>
@@ -22926,7 +22988,7 @@
         <v>773</v>
       </c>
       <c r="AN36" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="AV36" t="s">
         <v>774</v>
@@ -22938,7 +23000,7 @@
         <v>Project -Financial records (invoices, journal vouchers, received cheques etc.)</v>
       </c>
       <c r="B37" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="C37" t="s">
         <v>495</v>
@@ -22962,19 +23024,19 @@
         <v>776</v>
       </c>
       <c r="W38" t="s">
+        <v>2098</v>
+      </c>
+      <c r="Z38" t="s">
         <v>2099</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="AA38" t="s">
         <v>2100</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>2101</v>
       </c>
       <c r="AO38" s="13">
         <v>43757</v>
       </c>
       <c r="AR38" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.25">
@@ -22992,10 +23054,10 @@
         <v>7190089</v>
       </c>
       <c r="AN39" t="s">
+        <v>2102</v>
+      </c>
+      <c r="AV39" t="s">
         <v>2103</v>
-      </c>
-      <c r="AV39" t="s">
-        <v>2104</v>
       </c>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.25">
@@ -23016,16 +23078,16 @@
         <v>777</v>
       </c>
       <c r="AI40" t="s">
+        <v>2104</v>
+      </c>
+      <c r="AJ40" t="s">
         <v>2105</v>
       </c>
-      <c r="AJ40" t="s">
+      <c r="AL40" t="s">
         <v>2106</v>
       </c>
-      <c r="AL40" t="s">
+      <c r="AM40" t="s">
         <v>2107</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>2108</v>
       </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.25">
@@ -23040,7 +23102,7 @@
         <v>499</v>
       </c>
       <c r="F41" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="H41" s="13">
         <v>32301</v>
@@ -23055,16 +23117,16 @@
         <v>780</v>
       </c>
       <c r="AE41" t="s">
+        <v>2109</v>
+      </c>
+      <c r="AN41" t="s">
         <v>2110</v>
-      </c>
-      <c r="AN41" t="s">
-        <v>2111</v>
       </c>
       <c r="AO41" s="4"/>
       <c r="AP41" s="4"/>
       <c r="AQ41" s="4"/>
       <c r="AV41" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.25">
@@ -23079,7 +23141,7 @@
         <v>500</v>
       </c>
       <c r="AV42" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.25">
@@ -23094,12 +23156,12 @@
         <v>501</v>
       </c>
       <c r="AV43" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="44" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>462</v>
@@ -23123,7 +23185,7 @@
         <v>Disposition File -Certificate of Compliance</v>
       </c>
       <c r="B45" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="C45" t="s">
         <v>496</v>
@@ -23138,13 +23200,13 @@
         <v>Disposition File -Enhanced Referral Records</v>
       </c>
       <c r="B46" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="C46" t="s">
         <v>497</v>
       </c>
       <c r="AV46" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.25">
@@ -23153,13 +23215,13 @@
         <v>Disposition File -First Nations Strength of Claim Report</v>
       </c>
       <c r="B47" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="C47" t="s">
         <v>498</v>
       </c>
       <c r="AV47" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.25">
@@ -23174,7 +23236,7 @@
         <v>499</v>
       </c>
       <c r="AG48" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.25">
@@ -23189,7 +23251,7 @@
         <v>500</v>
       </c>
       <c r="AV49" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.25">
@@ -23207,13 +23269,13 @@
         <v>89997</v>
       </c>
       <c r="AC50" t="s">
+        <v>2118</v>
+      </c>
+      <c r="AD50" t="s">
         <v>2119</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AS50" t="s">
         <v>2120</v>
-      </c>
-      <c r="AS50" t="s">
-        <v>2121</v>
       </c>
       <c r="AZ50">
         <v>1997</v>
@@ -23225,13 +23287,13 @@
         <v>Disposition File -Purchase and Sale Agreement</v>
       </c>
       <c r="B51" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C51" t="s">
         <v>495</v>
       </c>
       <c r="AV51" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="52" spans="1:53" x14ac:dyDescent="0.25">
@@ -23246,7 +23308,7 @@
         <v>496</v>
       </c>
       <c r="AV52" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.25">
@@ -23261,12 +23323,12 @@
         <v>497</v>
       </c>
       <c r="AV53" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="54" spans="1:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>760</v>
@@ -23282,14 +23344,14 @@
       <c r="O54" s="36"/>
       <c r="Q54" s="36"/>
       <c r="Z54" s="23" t="s">
+        <v>2124</v>
+      </c>
+      <c r="AS54" s="23" t="s">
         <v>2125</v>
-      </c>
-      <c r="AS54" s="23" t="s">
-        <v>2126</v>
       </c>
       <c r="AW54" s="36"/>
       <c r="AY54" s="23" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="55" spans="1:53" x14ac:dyDescent="0.25">
@@ -23298,13 +23360,13 @@
         <v>Property Management -Approval/sign-off</v>
       </c>
       <c r="B55" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="C55" t="s">
         <v>499</v>
       </c>
       <c r="AV55" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="56" spans="1:53" x14ac:dyDescent="0.25">
@@ -23313,13 +23375,13 @@
         <v>Property Management -Form 8 - Notice of advanced payment </v>
       </c>
       <c r="B56" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C56" t="s">
         <v>500</v>
       </c>
       <c r="AV56" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.25">
@@ -23328,13 +23390,13 @@
         <v>Property Management -Form 1 - Notice of expropriation </v>
       </c>
       <c r="B57" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C57" t="s">
         <v>501</v>
       </c>
       <c r="AV57" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.25">
@@ -23349,7 +23411,7 @@
         <v>495</v>
       </c>
       <c r="AV58" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="59" spans="1:53" x14ac:dyDescent="0.25">
@@ -23364,7 +23426,7 @@
         <v>496</v>
       </c>
       <c r="AV59" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="60" spans="1:53" x14ac:dyDescent="0.25">
@@ -23379,7 +23441,7 @@
         <v>497</v>
       </c>
       <c r="AV60" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.25">
@@ -23409,7 +23471,7 @@
         <v>499</v>
       </c>
       <c r="AV62" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="63" spans="1:53" x14ac:dyDescent="0.25">
@@ -23427,16 +23489,16 @@
         <v>32874</v>
       </c>
       <c r="Z63" t="s">
+        <v>2130</v>
+      </c>
+      <c r="AN63" t="s">
         <v>2131</v>
-      </c>
-      <c r="AN63" t="s">
-        <v>2132</v>
       </c>
       <c r="AS63" t="s">
         <v>1503</v>
       </c>
       <c r="AY63" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="64" spans="1:53" x14ac:dyDescent="0.25">
@@ -23445,18 +23507,18 @@
         <v>Property Management -Form 9 - Vesting notice (Form 9)</v>
       </c>
       <c r="B64" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C64" t="s">
         <v>501</v>
       </c>
       <c r="AV64" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B65" s="23" t="s">
         <v>487</v>
@@ -23470,7 +23532,7 @@
       <c r="O65" s="36"/>
       <c r="Q65" s="36"/>
       <c r="AV65" s="23" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="AW65" s="36"/>
     </row>
@@ -23656,7 +23718,7 @@
         <v>64</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1030</v>
@@ -24157,7 +24219,7 @@
   <dimension ref="A1:CY21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24588,7 +24650,7 @@
         <v>1076</v>
       </c>
       <c r="D2" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="E2" t="s">
         <v>501</v>
@@ -25337,7 +25399,7 @@
         <v>44114</v>
       </c>
       <c r="BO6" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="CO6">
         <v>1</v>
@@ -25619,7 +25681,7 @@
         <v>1076</v>
       </c>
       <c r="D9" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="E9" t="s">
         <v>496</v>
@@ -25900,7 +25962,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes on automation test set
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A12E2A3-571B-4A81-985C-D784286CF7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25B217-6566-4784-96B1-C72A79649437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38580" yWindow="1140" windowWidth="28800" windowHeight="15225" tabRatio="950" firstSheet="27" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38310" yWindow="5520" windowWidth="28800" windowHeight="15225" tabRatio="950" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="2227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="2226">
   <si>
     <t>FirstName</t>
   </si>
@@ -6668,9 +6668,6 @@
   </si>
   <si>
     <t>006-093-914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joe Ellicott </t>
   </si>
   <si>
     <t>Joe Ellicott (MoTI Solicitor)</t>
@@ -7311,7 +7308,7 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -7437,7 +7434,7 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -9120,7 +9117,7 @@
         <v>246</v>
       </c>
       <c r="E2" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="F2" t="s">
         <v>248</v>
@@ -9129,7 +9126,7 @@
         <v>249</v>
       </c>
       <c r="H2" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="I2" s="4">
         <v>44625</v>
@@ -9229,13 +9226,13 @@
         <v>247</v>
       </c>
       <c r="E5" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="G5" t="s">
         <v>254</v>
       </c>
       <c r="H5" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="L5" t="s">
         <v>255</v>
@@ -9910,7 +9907,7 @@
         <v>691</v>
       </c>
       <c r="I2" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="J2" t="s">
         <v>571</v>
@@ -9919,7 +9916,7 @@
         <v>2039</v>
       </c>
       <c r="L2" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="M2" t="s">
         <v>2040</v>
@@ -10057,7 +10054,7 @@
       </c>
       <c r="N3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="O3" s="4">
         <v>45318</v>
@@ -10280,7 +10277,7 @@
       </c>
       <c r="N5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="O5" s="4">
         <v>45318</v>
@@ -10493,7 +10490,7 @@
       </c>
       <c r="N7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="O7" s="4">
         <v>45318</v>
@@ -11036,7 +11033,7 @@
       </c>
       <c r="N12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="O12" s="4">
         <v>45318</v>
@@ -11361,7 +11358,7 @@
       </c>
       <c r="N15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="O15" s="4">
         <v>45318</v>
@@ -12104,7 +12101,7 @@
         <v>1281</v>
       </c>
       <c r="I24" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="J24" t="s">
         <v>2039</v>
@@ -12113,7 +12110,7 @@
         <v>571</v>
       </c>
       <c r="L24" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="M24" t="s">
         <v>2056</v>
@@ -14391,8 +14388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CC3795-F36B-4D0F-8244-A4F4C3935686}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14536,10 +14533,10 @@
         <v>903</v>
       </c>
       <c r="P2" t="s">
+        <v>2201</v>
+      </c>
+      <c r="Q2" t="s">
         <v>2202</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>2203</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -14577,10 +14574,10 @@
         <v>1019</v>
       </c>
       <c r="P3" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="Q3" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
@@ -14639,10 +14636,10 @@
         <v>903</v>
       </c>
       <c r="P4" t="s">
+        <v>2196</v>
+      </c>
+      <c r="Q4" t="s">
         <v>2197</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>2196</v>
       </c>
       <c r="R4" t="b">
         <v>1</v>
@@ -14801,10 +14798,10 @@
         <v>903</v>
       </c>
       <c r="P7" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="Q7" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="R7" t="b">
         <v>1</v>
@@ -14858,10 +14855,10 @@
         <v>2072</v>
       </c>
       <c r="P8" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="Q8" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="R8" t="b">
         <v>1</v>
@@ -15957,7 +15954,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -17437,7 +17434,7 @@
         <v>695</v>
       </c>
       <c r="C11" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="D11" t="s">
         <v>600</v>
@@ -17576,7 +17573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -17933,7 +17930,7 @@
         <v>1521</v>
       </c>
       <c r="B30" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="C30">
         <v>90054549</v>
@@ -17950,7 +17947,7 @@
         <v>1536</v>
       </c>
       <c r="G31" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
@@ -18176,7 +18173,7 @@
         <v>269</v>
       </c>
       <c r="U3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="V3" t="s">
         <v>804</v>
@@ -18262,7 +18259,7 @@
         <v>1301</v>
       </c>
       <c r="V4" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="W4" t="s">
         <v>736</v>
@@ -18546,7 +18543,7 @@
         <v>1182</v>
       </c>
       <c r="B2" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="C2" t="s">
         <v>266</v>
@@ -18853,7 +18850,7 @@
         <v>1214</v>
       </c>
       <c r="H2" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="I2" t="s">
         <v>1228</v>
@@ -18909,7 +18906,7 @@
         <v>1229</v>
       </c>
       <c r="J3" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="K3" t="s">
         <v>1219</v>
@@ -23606,7 +23603,7 @@
         <v>340</v>
       </c>
       <c r="B2" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -23622,7 +23619,7 @@
         <v>342</v>
       </c>
       <c r="B4" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -23646,7 +23643,7 @@
         <v>1170</v>
       </c>
       <c r="B7" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -23670,7 +23667,7 @@
         <v>1409</v>
       </c>
       <c r="B10" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -24723,7 +24720,7 @@
         <v>1771</v>
       </c>
       <c r="T2" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="U2" t="s">
         <v>1801</v>

</xml_diff>

<commit_message>
Lease Active indicator test cases
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F22C643-3D73-4C8F-98ED-2BF57EAEABC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04C5DEF-EEE3-461F-9680-1CCAD9C8896D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="26" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="18" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3877" uniqueCount="2244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3961" uniqueCount="2250">
   <si>
     <t>FirstName</t>
   </si>
@@ -6812,6 +6812,24 @@
   </si>
   <si>
     <t>Consolidation Source - Retired Parent</t>
+  </si>
+  <si>
+    <t>Property Management Active Lease Status</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Terminated</t>
+  </si>
+  <si>
+    <t>Testing Active lease status from Property Management</t>
+  </si>
+  <si>
+    <t>009-670-301</t>
+  </si>
+  <si>
+    <t>Property Management Lease Active status</t>
   </si>
 </sst>
 </file>
@@ -17913,13 +17931,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E382B1-281B-4434-81AA-04C8D5F3D2FB}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.81640625" bestFit="1" customWidth="1"/>
@@ -18304,6 +18322,14 @@
       </c>
       <c r="B33" s="14" t="s">
         <v>2240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>2249</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2248</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -21081,7 +21107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76AD87F-398D-4043-9616-B8AC430B9A08}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
@@ -24648,20 +24674,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:CY21"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AK18" sqref="AK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="1" max="1" width="37.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.453125" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.26953125" customWidth="1"/>
     <col min="9" max="9" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
@@ -26336,46 +26362,957 @@
       </c>
     </row>
     <row r="11" spans="1:103" x14ac:dyDescent="0.35">
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="A11" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E11" t="s">
+        <v>492</v>
+      </c>
+      <c r="I11" t="s">
+        <v>597</v>
+      </c>
+      <c r="J11" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>190</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T11" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM11">
+        <v>33</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>0</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BK11">
+        <v>0</v>
+      </c>
+      <c r="CO11">
+        <v>0</v>
+      </c>
+      <c r="CQ11">
+        <v>0</v>
+      </c>
+      <c r="CR11">
+        <v>0</v>
+      </c>
+      <c r="CS11">
+        <v>0</v>
+      </c>
+      <c r="CT11">
+        <v>0</v>
+      </c>
+      <c r="CU11">
+        <v>0</v>
+      </c>
+      <c r="CV11">
+        <v>0</v>
+      </c>
+      <c r="CW11">
+        <v>0</v>
+      </c>
+      <c r="CX11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:103" x14ac:dyDescent="0.35">
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="A12" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E12" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" t="s">
+        <v>597</v>
+      </c>
+      <c r="J12" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>190</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R12" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T12" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM12">
+        <v>33</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>0</v>
+      </c>
+      <c r="AV12">
+        <v>0</v>
+      </c>
+      <c r="AW12">
+        <v>0</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12">
+        <v>0</v>
+      </c>
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BK12">
+        <v>0</v>
+      </c>
+      <c r="CO12">
+        <v>0</v>
+      </c>
+      <c r="CQ12">
+        <v>0</v>
+      </c>
+      <c r="CR12">
+        <v>0</v>
+      </c>
+      <c r="CS12">
+        <v>0</v>
+      </c>
+      <c r="CT12">
+        <v>0</v>
+      </c>
+      <c r="CU12">
+        <v>0</v>
+      </c>
+      <c r="CV12">
+        <v>0</v>
+      </c>
+      <c r="CW12">
+        <v>0</v>
+      </c>
+      <c r="CX12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:103" x14ac:dyDescent="0.35">
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="A13" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E13" t="s">
+        <v>497</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2247</v>
+      </c>
+      <c r="I13" t="s">
+        <v>597</v>
+      </c>
+      <c r="J13" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>190</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T13" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM13">
+        <v>33</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>0</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <v>0</v>
+      </c>
+      <c r="AW13">
+        <v>0</v>
+      </c>
+      <c r="AX13">
+        <v>0</v>
+      </c>
+      <c r="AY13">
+        <v>0</v>
+      </c>
+      <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BK13">
+        <v>0</v>
+      </c>
+      <c r="CO13">
+        <v>0</v>
+      </c>
+      <c r="CQ13">
+        <v>0</v>
+      </c>
+      <c r="CR13">
+        <v>0</v>
+      </c>
+      <c r="CS13">
+        <v>0</v>
+      </c>
+      <c r="CT13">
+        <v>0</v>
+      </c>
+      <c r="CU13">
+        <v>0</v>
+      </c>
+      <c r="CV13">
+        <v>0</v>
+      </c>
+      <c r="CW13">
+        <v>0</v>
+      </c>
+      <c r="CX13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:103" x14ac:dyDescent="0.35">
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="A14" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2245</v>
+      </c>
+      <c r="I14" t="s">
+        <v>597</v>
+      </c>
+      <c r="J14" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>190</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T14" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM14">
+        <v>33</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>0</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14">
+        <v>0</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BK14">
+        <v>0</v>
+      </c>
+      <c r="CO14">
+        <v>0</v>
+      </c>
+      <c r="CQ14">
+        <v>0</v>
+      </c>
+      <c r="CR14">
+        <v>0</v>
+      </c>
+      <c r="CS14">
+        <v>0</v>
+      </c>
+      <c r="CT14">
+        <v>0</v>
+      </c>
+      <c r="CU14">
+        <v>0</v>
+      </c>
+      <c r="CV14">
+        <v>0</v>
+      </c>
+      <c r="CW14">
+        <v>0</v>
+      </c>
+      <c r="CX14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:103" x14ac:dyDescent="0.35">
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="A15" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E15" t="s">
+        <v>692</v>
+      </c>
+      <c r="I15" t="s">
+        <v>597</v>
+      </c>
+      <c r="J15" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>190</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T15" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM15">
+        <v>33</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>0</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AU15">
+        <v>0</v>
+      </c>
+      <c r="AV15">
+        <v>0</v>
+      </c>
+      <c r="AW15">
+        <v>0</v>
+      </c>
+      <c r="AX15">
+        <v>0</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>0</v>
+      </c>
+      <c r="BA15">
+        <v>0</v>
+      </c>
+      <c r="BK15">
+        <v>0</v>
+      </c>
+      <c r="CO15">
+        <v>0</v>
+      </c>
+      <c r="CQ15">
+        <v>0</v>
+      </c>
+      <c r="CR15">
+        <v>0</v>
+      </c>
+      <c r="CS15">
+        <v>0</v>
+      </c>
+      <c r="CT15">
+        <v>0</v>
+      </c>
+      <c r="CU15">
+        <v>0</v>
+      </c>
+      <c r="CV15">
+        <v>0</v>
+      </c>
+      <c r="CW15">
+        <v>0</v>
+      </c>
+      <c r="CX15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:103" x14ac:dyDescent="0.35">
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-    </row>
-    <row r="17" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-    </row>
-    <row r="18" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-    </row>
-    <row r="19" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2246</v>
+      </c>
+      <c r="F16" s="4">
+        <v>45750</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2247</v>
+      </c>
+      <c r="I16" t="s">
+        <v>597</v>
+      </c>
+      <c r="J16" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>190</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R16" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T16" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM16">
+        <v>33</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+      <c r="AU16">
+        <v>0</v>
+      </c>
+      <c r="AV16">
+        <v>0</v>
+      </c>
+      <c r="AW16">
+        <v>0</v>
+      </c>
+      <c r="AX16">
+        <v>0</v>
+      </c>
+      <c r="AY16">
+        <v>0</v>
+      </c>
+      <c r="AZ16">
+        <v>0</v>
+      </c>
+      <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BK16">
+        <v>0</v>
+      </c>
+      <c r="CO16">
+        <v>0</v>
+      </c>
+      <c r="CQ16">
+        <v>0</v>
+      </c>
+      <c r="CR16">
+        <v>0</v>
+      </c>
+      <c r="CS16">
+        <v>0</v>
+      </c>
+      <c r="CT16">
+        <v>0</v>
+      </c>
+      <c r="CU16">
+        <v>0</v>
+      </c>
+      <c r="CV16">
+        <v>0</v>
+      </c>
+      <c r="CW16">
+        <v>0</v>
+      </c>
+      <c r="CX16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:102" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E17" t="s">
+        <v>246</v>
+      </c>
+      <c r="I17" t="s">
+        <v>597</v>
+      </c>
+      <c r="J17" s="4">
+        <v>42462</v>
+      </c>
+      <c r="K17" s="4">
+        <v>45749</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>190</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T17" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM17">
+        <v>33</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>0</v>
+      </c>
+      <c r="AU17">
+        <v>0</v>
+      </c>
+      <c r="AV17">
+        <v>0</v>
+      </c>
+      <c r="AW17">
+        <v>0</v>
+      </c>
+      <c r="AX17">
+        <v>0</v>
+      </c>
+      <c r="AY17">
+        <v>0</v>
+      </c>
+      <c r="AZ17">
+        <v>0</v>
+      </c>
+      <c r="BA17">
+        <v>0</v>
+      </c>
+      <c r="BK17">
+        <v>0</v>
+      </c>
+      <c r="CO17">
+        <v>0</v>
+      </c>
+      <c r="CQ17">
+        <v>0</v>
+      </c>
+      <c r="CR17">
+        <v>0</v>
+      </c>
+      <c r="CS17">
+        <v>0</v>
+      </c>
+      <c r="CT17">
+        <v>0</v>
+      </c>
+      <c r="CU17">
+        <v>0</v>
+      </c>
+      <c r="CV17">
+        <v>0</v>
+      </c>
+      <c r="CW17">
+        <v>0</v>
+      </c>
+      <c r="CX17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:102" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E18" t="s">
+        <v>246</v>
+      </c>
+      <c r="I18" t="s">
+        <v>597</v>
+      </c>
+      <c r="J18" s="4">
+        <v>45749</v>
+      </c>
+      <c r="K18" s="4">
+        <v>72777</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>190</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1769</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1772</v>
+      </c>
+      <c r="T18" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>299</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>299</v>
+      </c>
+      <c r="AM18">
+        <v>33</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18">
+        <v>0</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>0</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>0</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>0</v>
+      </c>
+      <c r="BK18">
+        <v>0</v>
+      </c>
+      <c r="CO18">
+        <v>0</v>
+      </c>
+      <c r="CQ18">
+        <v>0</v>
+      </c>
+      <c r="CR18">
+        <v>0</v>
+      </c>
+      <c r="CS18">
+        <v>0</v>
+      </c>
+      <c r="CT18">
+        <v>0</v>
+      </c>
+      <c r="CU18">
+        <v>0</v>
+      </c>
+      <c r="CV18">
+        <v>0</v>
+      </c>
+      <c r="CW18">
+        <v>0</v>
+      </c>
+      <c r="CX18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:102" x14ac:dyDescent="0.35">
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:102" x14ac:dyDescent="0.35">
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:102" x14ac:dyDescent="0.35">
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>

</xml_diff>

<commit_message>
Automation - adding default province name test
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248BC590-5275-485B-BD9A-BF29FBDF3806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E9CD76-65B4-4E02-8840-7439012FBA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="28" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4082" uniqueCount="2327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4083" uniqueCount="2328">
   <si>
     <t>FirstName</t>
   </si>
@@ -7062,6 +7062,9 @@
   </si>
   <si>
     <t>MoTT contact</t>
+  </si>
+  <si>
+    <t>PropertyProvince</t>
   </si>
 </sst>
 </file>
@@ -10416,7 +10419,7 @@
       </c>
       <c r="N3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="O3" s="4">
         <v>45318</v>
@@ -10639,7 +10642,7 @@
       </c>
       <c r="N5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="O5" s="4">
         <v>45318</v>
@@ -10852,7 +10855,7 @@
       </c>
       <c r="N7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="O7" s="4">
         <v>45318</v>
@@ -11395,7 +11398,7 @@
       </c>
       <c r="N12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="O12" s="4">
         <v>45318</v>
@@ -11720,7 +11723,7 @@
       </c>
       <c r="N15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="O15" s="4">
         <v>45318</v>
@@ -16591,7 +16594,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45792</v>
+        <v>45810</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -18986,10 +18989,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC28AC-6E43-4E72-BAB6-024FC197C5A5}">
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19000,46 +19003,47 @@
     <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="60" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.453125" customWidth="1"/>
-    <col min="25" max="25" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="63.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="42" max="45" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="60" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.453125" customWidth="1"/>
+    <col min="26" max="26" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="63.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="46" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
@@ -19065,84 +19069,87 @@
         <v>1595</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>1596</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1597</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1599</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>1600</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>1601</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1598</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>1602</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1603</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>1604</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>1605</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>1606</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>1607</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>1608</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>1609</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>1610</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1611</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>1612</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>1613</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1614</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1615</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>1616</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>328</v>
       </c>
       <c r="D2" t="s">
         <v>259</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>264</v>
       </c>
@@ -19155,62 +19162,62 @@
       <c r="H3" t="s">
         <v>262</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>263</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>190</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>265</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>267</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>268</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>266</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>330</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>269</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>2204</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>802</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>270</v>
       </c>
-      <c r="Y3" s="30">
+      <c r="Z3" s="30">
         <v>100.0001</v>
       </c>
-      <c r="Z3" t="b">
+      <c r="AA3" t="b">
         <v>1</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>50.988799999999998</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>271</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>394</v>
       </c>
@@ -19232,68 +19239,68 @@
       <c r="H4" t="s">
         <v>1635</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>396</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>1617</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>1636</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>190</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>1618</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>1619</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>266</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>268</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>1620</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>397</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>1296</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>2205</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>735</v>
       </c>
-      <c r="Y4" s="30">
+      <c r="Z4" s="30">
         <v>65.898600000000002</v>
       </c>
-      <c r="Z4" t="b">
+      <c r="AA4" t="b">
         <v>1</v>
       </c>
-      <c r="AA4" s="32" t="s">
+      <c r="AB4" s="32" t="s">
         <v>1672</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>271</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>687</v>
       </c>
@@ -19312,47 +19319,47 @@
       <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>707</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="T5" t="s">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
         <v>708</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>733</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>734</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>735</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>2240</v>
       </c>
-      <c r="Y5" s="30">
+      <c r="Z5" s="30">
         <v>89.87</v>
       </c>
-      <c r="Z5" t="b">
+      <c r="AA5" t="b">
         <v>1</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>125.7801</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>710</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1387</v>
       </c>
@@ -19368,58 +19375,58 @@
       <c r="H6" t="s">
         <v>66</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>1391</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="N6" t="s">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
         <v>190</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>1514</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>1392</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>268</v>
       </c>
       <c r="R6" t="s">
         <v>268</v>
       </c>
       <c r="S6" t="s">
+        <v>268</v>
+      </c>
+      <c r="T6" t="s">
         <v>1393</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>1394</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>2245</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>1395</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>270</v>
       </c>
-      <c r="Y6" s="30">
+      <c r="Z6" s="30">
         <v>1200.1212</v>
       </c>
-      <c r="Z6" t="b">
+      <c r="AA6" t="b">
         <v>1</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>8900.9876999999997</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>710</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>1396</v>
       </c>
     </row>
@@ -24487,7 +24494,7 @@
     </row>
     <row r="56" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
-        <f t="shared" ref="A56:A70" si="6">_xlfn.CONCAT("Property Management -",B56)</f>
+        <f t="shared" ref="A56:A64" si="6">_xlfn.CONCAT("Property Management -",B56)</f>
         <v>Property Management -Form 8 - Notice of advanced payment </v>
       </c>
       <c r="B56" t="s">
@@ -25485,7 +25492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49A716-1E6E-4D56-8BE1-20B354C9F88C}">
   <dimension ref="A1:DA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First commit for playwright project and changes on Frontend to add data-testid and consistency on messages
</commit_message>
<xml_diff>
--- a/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
+++ b/testing/PIMS.Tests.Automation/Data/PIMS_Testing_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueT\projects\PSP\testing\PIMS.Tests.Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E431184-B963-4693-8FBB-38F4E9D4B682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5B1408-10EC-4065-8E40-021BEC4A041A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="950" firstSheet="29" activeTab="42" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10690,7 +10690,7 @@
       </c>
       <c r="N3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45841</v>
+        <v>45866</v>
       </c>
       <c r="O3" s="4">
         <v>45318</v>
@@ -10928,7 +10928,7 @@
       </c>
       <c r="N5" s="4">
         <f ca="1">TODAY()</f>
-        <v>45841</v>
+        <v>45866</v>
       </c>
       <c r="O5" s="4">
         <v>45318</v>
@@ -11153,7 +11153,7 @@
       </c>
       <c r="N7" s="4">
         <f ca="1">TODAY()</f>
-        <v>45841</v>
+        <v>45866</v>
       </c>
       <c r="O7" s="4">
         <v>45318</v>
@@ -11726,7 +11726,7 @@
       </c>
       <c r="N12" s="4">
         <f ca="1">TODAY()</f>
-        <v>45841</v>
+        <v>45866</v>
       </c>
       <c r="O12" s="4">
         <v>45318</v>
@@ -12069,7 +12069,7 @@
       </c>
       <c r="N15" s="4">
         <f ca="1">TODAY()</f>
-        <v>45841</v>
+        <v>45866</v>
       </c>
       <c r="O15" s="4">
         <v>45318</v>
@@ -16859,7 +16859,7 @@
       </c>
       <c r="F4" s="4">
         <f ca="1">TODAY()</f>
-        <v>45841</v>
+        <v>45866</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" t="s">
@@ -18933,7 +18933,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19986,8 +19986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718AA1BD-8944-4A5E-BDA4-69421020A1DE}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20655,7 +20655,7 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21112,7 +21112,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24285,7 +24285,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24494,7 +24494,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>